<commit_message>
ASTRO Suite safe store
</commit_message>
<xml_diff>
--- a/Astronomy Utilities/Astronomy Utlities.xlsx
+++ b/Astronomy Utilities/Astronomy Utlities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profmc/Library/CloudStorage/Dropbox/Lambda-Update-Project/Lambda-Development/Astronomy Utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{649B3404-EA47-9646-87C5-83413B39C09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5C87B4-C01D-1740-91AC-403925B346C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="1100" windowWidth="33260" windowHeight="19560" activeTab="2" xr2:uid="{7A445647-2974-6942-9320-70750788AE91}"/>
   </bookViews>
@@ -18,24 +18,28 @@
     <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="ASTRO_APPARENT_SOLAR_SIZE">_xlfn.LAMBDA(_xlpm.radius,_xlpm.distance,_xlop.format,_xlop.prec, _xlfn.LET(_xlpm.p, IF(_xlfn.ISOMITTED(_xlpm.prec), 4, _xlpm.prec), _xlpm.raw, _xlpm.radius / _xlpm.distance, _xlpm.result, IF(OR(_xlfn.ISOMITTED(_xlpm.format), _xlpm.format = "formatted"), TEXT(_xlpm.raw, "0." &amp; REPT("0", _xlpm.p)) &amp; "☉", _xlpm.raw), _xlpm.result))</definedName>
     <definedName name="ASTRO_CALC_TEMP">_xlfn.LAMBDA(_xlpm.subclass, _xlfn.LET(_xlpm.arrTypes, {"O3";"O4";"O5";"O6";"O7";"O8";"O9";"B0";"B1";"B2";"B3";"B4";"B5";"B6";"B7";"B8";"B9";"A0";"A1";"A2";"A3";"A4";"A5";"A6";"A7";"A8";"A9";"F0";"F1";"F2";"F3";"F4";"F5";"F6";"F7";"F8";"F9";"G0";"G1";"G2";"G3";"G4";"G5";"G6";"G7";"G8";"G9";"K0";"K1";"K2";"K3";"K4";"K5";"K6";"K7";"K8";"K9";"M0";"M1";"M2";"M3";"M4";"M5";"M6";"M7";"M8";"M9"}, _xlpm.arrTHigh, {44900;42900;41400;39500;37100;35100;33300;31400;26000;20600;17000;16400;15700;14500;14000;12300;10700;9700;9300;8800;8600;8250;8100;7910;7760;7590;7400;7220;7020;6820;6750;6670;6550;6350;6280;6180;6050;5930;5860;5770;5720;5680;5660;5600;5550;5480;5380;5270;5170;5100;4830;4600;4440;4300;4100;3990;3930;3850;3660;3560;3430;3210;3060;2810;2680;2570;2380}, _xlpm.arrSpan, {2000;1500;1900;2400;2000;1800;1900;5400;5400;3600;600;700;1200;500;1700;1600;1000;400;500;200;350;150;190;150;170;190;180;200;200;70;80;120;200;70;100;130;120;70;90;50;40;20;60;50;70;100;110;100;70;270;230;160;140;200;110;60;80;190;100;130;220;150;250;130;110;190;280}, _xlpm.mtxStars, _xlfn.HSTACK(_xlpm.arrTypes, _xlpm.arrTHigh, _xlpm.arrSpan), _xlpm.no_space, SUBSTITUTE(_xlpm.subclass, " ", ""), _xlpm.dot_pos, FIND(".", _xlpm.no_space &amp; ".0"), _xlpm.base, LEFT(_xlpm.no_space, _xlpm.dot_pos - 1), _xlpm.f, VALUE("0." &amp; MID(_xlpm.no_space, _xlpm.dot_pos + 1, LEN(_xlpm.no_space))), _xlpm.T_high, _xlfn.XLOOKUP(_xlpm.base, INDEX(_xlpm.mtxStars, , 1), INDEX(_xlpm.mtxStars, , 2)), _xlpm.span, _xlfn.XLOOKUP(_xlpm.base, INDEX(_xlpm.mtxStars, , 1), INDEX(_xlpm.mtxStars, , 3)), _xlpm.result, _xlpm.T_high - (_xlpm.f * _xlpm.span), _xlpm.result))</definedName>
+    <definedName name="ASTRO_CARTESIAN_TO_SPHERICAL">_xlfn.LAMBDA(_xlpm.x,_xlpm.y,_xlpm.z,_xlpm.prec, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec) + (_xlpm.prec &lt; 0), 3, _xlpm.prec), _xlpm.r, SQRT(_xlpm.x ^ 2 + _xlpm.y ^ 2 + _xlpm.z ^ 2), _xlpm.phi, DEGREES(ACOS(_xlpm.z / _xlpm.r)), _xlpm.theta, MOD(DEGREES(ATAN2(_xlpm.y, _xlpm.x)), 360), _xlpm.phi_out, ROUND(_xlpm.phi, _xlpm.prec), _xlpm.theta_out, ROUND(_xlpm.theta, _xlpm.prec), _xlpm.r_out, ROUND(_xlpm.r, _xlpm.prec), _xlfn.HSTACK(_xlpm.phi_out, _xlpm.theta_out, _xlpm.r_out)))</definedName>
     <definedName name="ASTRO_DISPLAY_SPECTRAL">_xlfn.LAMBDA(_xlop.type, _xlfn.LET(_xlpm.Types, {"O";"B";"A";"F";"G";"K";"M"}, _xlpm.Headers, TRANSPOSE(_xlfn.VSTACK(" ", _xlpm.Types)), _xlpm.FindCol, _xlfn.MAKEARRAY(COUNTA(_xlpm.Types), 2, _xlfn.LAMBDA(_xlpm.r,_xlpm.c, IF(_xlpm.c = 1, INDEX(_xlpm.Types, _xlpm.r), _xlpm.r))), _xlpm.arrTypes, {"O";"O";"O";"O3";"O4";"O5";"O6";"O7";"O8";"O9";"B0";"B1";"B2";"B3";"B4";"B5";"B6";"B7";"B8";"B9";"A0";"A1";"A2";"A3";"A4";"A5";"A6";"A7";"A8";"A9";"F0";"F1";"F2";"F3";"F4";"F5";"F6";"F7";"F8";"F9";"G0";"G1";"G2";"G3";"G4";"G5";"G6";"G7";"G8";"G9";"K0";"K1";"K2";"K3";"K4";"K5";"K6";"K7";"K8";"K9";"M0";"M1";"M2";"M3";"M4";"M5";"M6";"M7";"M8";"M9"}, _xlpm.arrTHigh, {"";"";"";44900;42900;41400;39500;37100;35100;33300;31400;26000;20600;17000;16400;15700;14500;14000;12300;10700;9700;9300;8800;8600;8250;8100;7910;7760;7590;7400;7220;7020;6820;6750;6670;6550;6350;6280;6180;6050;5930;5860;5770;5720;5680;5660;5600;5550;5480;5380;5270;5170;5100;4830;4600;4440;4300;4100;3990;3930;3850;3660;3560;3430;3210;3060;2810;2680;2570;2380}, _xlpm.arrSpan, {"";"";"";2000;1500;1900;2400;2000;1800;1900;5400;5400;3600;600;700;1200;500;1700;1600;1000;400;500;200;350;150;190;150;170;190;180;200;200;70;80;120;200;70;100;130;120;70;90;50;40;20;60;50;70;100;110;100;70;270;230;160;140;200;110;60;80;190;100;130;220;150;250;130;110;190;280}, _xlpm.formattedData, _xlfn.BYROW(_xlfn.HSTACK(_xlpm.arrTypes, _xlpm.arrTHigh, _xlpm.arrSpan), _xlfn.LAMBDA(_xlpm.row, _xlfn.TEXTJOIN("; ", TRUE, TEXT(INDEX(_xlpm.row, 2), "0"), TEXT(INDEX(_xlpm.row, 3), "0")))), _xlpm.Numbers, _xlfn.SEQUENCE(10, 1, 0, 1), _xlpm.O_Stars, _xlfn._xlws.FILTER(_xlpm.formattedData, LEFT(_xlpm.arrTypes, 1) = "O"), _xlpm.B_Stars, _xlfn._xlws.FILTER(_xlpm.formattedData, LEFT(_xlpm.arrTypes, 1) = "B"), _xlpm.A_Stars, _xlfn._xlws.FILTER(_xlpm.formattedData, LEFT(_xlpm.arrTypes, 1) = "A"), _xlpm.F_Stars, _xlfn._xlws.FILTER(_xlpm.formattedData, LEFT(_xlpm.arrTypes, 1) = "F"), _xlpm.G_Stars, _xlfn._xlws.FILTER(_xlpm.formattedData, LEFT(_xlpm.arrTypes, 1) = "G"), _xlpm.K_Stars, _xlfn._xlws.FILTER(_xlpm.formattedData, LEFT(_xlpm.arrTypes, 1) = "K"), _xlpm.M_Stars, _xlfn._xlws.FILTER(_xlpm.formattedData, LEFT(_xlpm.arrTypes, 1) = "M"), _xlpm.fullTable, _xlfn.VSTACK(_xlpm.Headers, _xlfn.HSTACK(_xlpm.Numbers, _xlpm.O_Stars, _xlpm.B_Stars, _xlpm.A_Stars, _xlpm.F_Stars, _xlpm.G_Stars, _xlpm.K_Stars, _xlpm.M_Stars)), _xlpm.temps, _xlfn._xlws.FILTER(_xlpm.arrTHigh, LEFT(_xlpm.arrTypes, 1) = _xlpm.type), _xlpm.spans, _xlfn._xlws.FILTER(_xlpm.arrSpan, LEFT(_xlpm.arrTypes, 1) = _xlpm.type), _xlpm.typeHead, _xlfn.HSTACK(_xlpm.type, "span"), _xlpm.slimTable, _xlfn.VSTACK(_xlpm.typeHead, _xlfn.HSTACK(_xlpm.temps, _xlpm.spans)), _xlpm.result, IF(ISBLANK(_xlpm.type), _xlpm.fullTable, _xlpm.slimTable), _xlpm.result))</definedName>
     <definedName name="ASTRO_HAB_INDEX">_xlfn.LAMBDA(_xlpm.orbital_dist,_xlop.nucleal_radius,_xlop.prec, _xlfn.LET(_xlpm.rounding_precision, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.nucleal_radius, IF(_xlfn.ISOMITTED(_xlpm.nucleal_radius), 1, _xlpm.nucleal_radius), _xlpm.is_inner_orbit, IF(_xlpm.orbital_dist &lt; _xlpm.nucleal_radius, TRUE, FALSE), _xlpm.habitability_index, IF(_xlpm.is_inner_orbit, (2 * _xlpm.orbital_dist / _xlpm.nucleal_radius) - 1, (_xlpm.orbital_dist / (-3.85 * _xlpm.nucleal_radius)) + (4.85 / 3.85)), _xlpm.final_result, IF(_xlpm.habitability_index &lt;= 0, "U/I", ROUND(_xlpm.habitability_index, _xlpm.rounding_precision)), _xlpm.final_result))</definedName>
     <definedName name="ASTRO_HABITABLE_ZONES">_xlfn.LAMBDA(_xlpm.mode,_xlop.lum,_xlop.precision, _xlfn.LET(_xlpm.mode, UPPER(_xlpm.mode), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.precision), 3, _xlpm.precision), _xlpm.zone_labels, {"Z0";"Z1";"Z2";"Z3";"Z4";"Z5"}, _xlpm.inner_factors, {0;0.5;0.75;0.95;1.385;1.77}, _xlpm.outer_factors, {0.5;0.75;0.95;1.385;1.77;4.85}, _xlpm.avg_factors, (_xlpm.inner_factors + _xlpm.outer_factors) / 2, _xlpm.span_factors, _xlpm.outer_factors - _xlpm.inner_factors, _xlpm.nucleal, SQRT(IF(_xlfn.ISOMITTED(_xlpm.lum), 1, _xlpm.lum)), _xlpm.inner_scaled, ROUND(_xlpm.nucleal * _xlpm.inner_factors, _xlpm.prec), _xlpm.outer_scaled, ROUND(_xlpm.nucleal * _xlpm.outer_factors, _xlpm.prec), _xlpm.avg_scaled, ROUND(_xlpm.nucleal * _xlpm.avg_factors, _xlpm.prec), _xlpm.span_scaled, ROUND(_xlpm.nucleal * _xlpm.span_factors, _xlpm.prec), _xlpm.vertical_labels, {"0: ","1: ","2: ","N ➔","3: ","4: ","5: "}, _xlpm.vertical_values, _xlfn.VSTACK(ROUND(INDEX(_xlpm.inner_factors, 2) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.inner_factors, 3) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.inner_factors, 4) * _xlpm.nucleal, _xlpm.prec), ROUND(_xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.outer_factors, 4) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.outer_factors, 5) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.outer_factors, 6) * _xlpm.nucleal, _xlpm.prec)), _xlpm.result, _xlfn.SWITCH(_xlpm.mode, "STANDARD", CHOOSE({1,2,3,4,5}, _xlfn.VSTACK("Zone", _xlpm.zone_labels), _xlfn.VSTACK("Inner", _xlpm.inner_factors), _xlfn.VSTACK("Outer", _xlpm.outer_factors), _xlfn.VSTACK("Average", _xlpm.avg_factors), _xlfn.VSTACK("Span", _xlpm.span_factors)), "VERTICAL", _xlfn.LET(_xlpm.labels, {"0:","1:","2:","N ➔","3:","4:","5:"}, _xlpm.scaled_values, ROUND(_xlpm.nucleal * {0.5,0.75,0.95,1,1.385,1.77,4.85}, _xlpm.prec), TRANSPOSE(_xlfn.VSTACK(_xlpm.labels, _xlpm.scaled_values))), "HORIZONTAL", _xlfn.HSTACK(ROUND(INDEX(_xlpm.inner_factors, 2) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.inner_factors, 3) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.inner_factors, 4) * _xlpm.nucleal, _xlpm.prec), ROUND(_xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.outer_factors, 4) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.outer_factors, 5) * _xlpm.nucleal, _xlpm.prec), ROUND(INDEX(_xlpm.outer_factors, 6) * _xlpm.nucleal, _xlpm.prec)), "Invalid mode"), _xlpm.result))</definedName>
+    <definedName name="ASTRO_ORBIT_AXIS">_xlfn.LAMBDA(_xlpm.mass1,_xlpm.mass2,_xlpm.period, _xlfn.LET(_xlpm.m_2, IF((_xlfn.ISOMITTED(_xlpm.mass2)) + (_xlpm.mass2 = 1), 0, _xlpm.mass2 * 0.000003003), _xlpm.axis, POWER((POWER(_xlpm.period, 2) * (_xlpm.mass1 + _xlpm.m_2)), 1 / 3), _xlpm.axis))</definedName>
+    <definedName name="ASTRO_ORBIT_CONFIGURATION_INDEX">_xlfn.LAMBDA(_xlpm.mass1,_xlpm.mass2, ABS(_xlpm.mass1 - _xlpm.mass2) / (_xlpm.mass1 + _xlpm.mass2))</definedName>
+    <definedName name="ASTRO_ORBIT_PERIOD">_xlfn.LAMBDA(_xlpm.mass1,_xlpm.mass2,_xlpm.axis, _xlfn.LET(_xlpm.m_2, IF((_xlfn.ISOMITTED(_xlpm.mass2)) + (_xlpm.mass2 = 1), 0, _xlpm.mass2 * 0.00000300273), _xlpm.period, SQRT(POWER(_xlpm.axis, 3) / (_xlpm.mass1 + _xlpm.m_2)), _xlpm.period))</definedName>
+    <definedName name="ASTRO_ORBIT_SOLVER">_xlfn.LAMBDA(_xlpm.mode,_xlpm.val_1,_xlpm.val_2,_xlpm.mass2,_xlpm.precision, _xlfn.LET(_xlpm.m_2, IF(_xlfn.ISOMITTED(_xlpm.mass2) + (_xlpm.mass2 = 1), 0, _xlpm.mass2 * 0.000003003), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.precision), 4, _xlpm.precision), _xlpm.result, _xlfn.SWITCH(LOWER(_xlpm.mode), "axis", POWER((POWER(_xlpm.val_2, 2) * (_xlpm.val_1 + _xlpm.m_2)), 1 / 3), "period", SQRT(POWER(_xlpm.val_2, 3) / (_xlpm.val_1 + _xlpm.m_2)), "mass", POWER(_xlpm.val_1, 3) / POWER(_xlpm.val_2, 2), NA()), _xlpm.label, _xlfn.SWITCH(LOWER(_xlpm.mode), "axis", "Axis = ", "period", "Period = ", "mass", "Mass = ", "?"), TEXT(_xlpm.result, "0." &amp; REPT("0", _xlpm.prec)) &amp; " " &amp; _xlpm.label))</definedName>
+    <definedName name="ASTRO_ORBIT_SUM_MASSES">_xlfn.LAMBDA(_xlpm.axis,_xlpm.period, POWER(_xlpm.axis, 3) / POWER(_xlpm.period, 2))</definedName>
     <definedName name="ASTRO_PLANET_METRICS">_xlfn.LAMBDA(_xlpm.mode,_xlpm.param_1,_xlpm.param_2,_xlop.prec, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 5, _xlpm.prec), _xlpm.mode, LOWER(_xlpm.mode), _xlpm.output, _xlfn.SWITCH(_xlpm.mode, "md", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.d, _xlpm.param_2, _xlpm.R, (_xlpm.M / _xlpm.d) ^ (1 / 3), _xlpm.g, (_xlpm.M * _xlpm.d ^ 2) ^ (1 / 3), _xlpm.v, (_xlpm.M * SQRT(_xlpm.d)) ^ (1 / 3), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "mr", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.R, _xlpm.param_2, _xlpm.d, _xlpm.M / _xlpm.R ^ 3, _xlpm.g, _xlpm.M / _xlpm.R ^ 2, _xlpm.v, SQRT(_xlpm.M / _xlpm.R), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "mg", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.g, _xlpm.param_2, _xlpm.R, SQRT(_xlpm.M / _xlpm.g), _xlpm.d, SQRT(_xlpm.g ^ 3 / _xlpm.M), _xlpm.v, (_xlpm.M * _xlpm.g) ^ 0.25, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "rd", _xlfn.LET(_xlpm.R, _xlpm.param_1, _xlpm.d, _xlpm.param_2, _xlpm.M, _xlpm.d * _xlpm.R ^ 3, _xlpm.g, _xlpm.d * _xlpm.R, _xlpm.v, _xlpm.R * SQRT(_xlpm.d), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "rg", _xlfn.LET(_xlpm.R, _xlpm.param_1, _xlpm.g, _xlpm.param_2, _xlpm.M, _xlpm.g * _xlpm.R ^ 2, _xlpm.d, _xlpm.g / _xlpm.R, _xlpm.v, SQRT(_xlpm.g * _xlpm.R), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "dg", _xlfn.LET(_xlpm.d, _xlpm.param_1, _xlpm.g, _xlpm.param_2, _xlpm.R, _xlpm.g / _xlpm.d, _xlpm.M, _xlpm.g ^ 3 / _xlpm.d ^ 2, _xlpm.v, _xlpm.g / SQRT(_xlpm.d), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "dv", _xlfn.LET(_xlpm.d, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.R, _xlpm.v / SQRT(_xlpm.d), _xlpm.M, _xlpm.v ^ 3 / SQRT(_xlpm.d), _xlpm.g, _xlpm.v * SQRT(_xlpm.d), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "gv", _xlfn.LET(_xlpm.g, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.R, _xlpm.v ^ 2 / _xlpm.g, _xlpm.M, _xlpm.v ^ 4 / _xlpm.g, _xlpm.d, (_xlpm.g / _xlpm.v) ^ 2, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "mv", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.R, _xlpm.M / _xlpm.v ^ 2, _xlpm.g, _xlpm.v ^ 4 / _xlpm.M, _xlpm.d, _xlpm.v ^ 6 / _xlpm.M ^ 2, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "rv", _xlfn.LET(_xlpm.R, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.g, _xlpm.v ^ 2 / _xlpm.R, _xlpm.M, _xlpm.R * _xlpm.v ^ 2, _xlpm.d, (_xlpm.v / _xlpm.R) ^ 2, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), NA()), _xlpm.headers, _xlfn.SWITCH(_xlpm.mode, "md", {"M ➔","R","d ➔","g","v"}, "mr", {"M ➔","R ➔","d","g","v"}, "mg", {"M ➔","R","d","g ➔","v"}, "rd", {"M","R ➔","d ➔","g","v"}, "rg", {"M","R ➔","d","g ➔","v"}, "dg", {"M","R","d ➔","g ➔","v"}, "dv", {"M","R","d ➔","g","v ➔"}, "gv", {"M","R","d","g ➔","v ➔"}, "mv", {"M ➔","R","d","g","v ➔"}, "rv", {"M","R ➔","d","g","v ➔"}, {"M","R","d","g","v"}), _xlpm.values, ROUND(_xlpm.output, _xlpm.prec), CHOOSE({1,2}, TRANSPOSE(_xlpm.headers), TRANSPOSE(_xlpm.values))))</definedName>
     <definedName name="ASTRO_PLANET_METRICS_SAFETY">_xlfn.LAMBDA(_xlpm.mode,_xlpm.param_1,_xlpm.param_2,_xlop.prec, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 5, _xlpm.prec), _xlpm.mode, LOWER(_xlpm.mode), _xlpm.output, _xlfn.SWITCH(_xlpm.mode, "md", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.d, _xlpm.param_2, _xlpm.R, (_xlpm.M / _xlpm.d) ^ (1 / 3), _xlpm.g, (_xlpm.M * _xlpm.d ^ 2) ^ (1 / 3), _xlpm.v, (_xlpm.M * SQRT(_xlpm.d)) ^ (1 / 3), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "mr", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.R, _xlpm.param_2, _xlpm.d, _xlpm.M / _xlpm.R ^ 3, _xlpm.g, _xlpm.M / _xlpm.R ^ 2, _xlpm.v, SQRT(_xlpm.M / _xlpm.R), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "mg", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.g, _xlpm.param_2, _xlpm.R, SQRT(_xlpm.M / _xlpm.g), _xlpm.d, SQRT(_xlpm.g ^ 3 / _xlpm.M), _xlpm.v, (_xlpm.M * _xlpm.g) ^ 0.25, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "rd", _xlfn.LET(_xlpm.R, _xlpm.param_1, _xlpm.d, _xlpm.param_2, _xlpm.M, _xlpm.d * _xlpm.R ^ 3, _xlpm.g, _xlpm.d * _xlpm.R, _xlpm.v, _xlpm.R * SQRT(_xlpm.d), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "rg", _xlfn.LET(_xlpm.R, _xlpm.param_1, _xlpm.g, _xlpm.param_2, _xlpm.M, _xlpm.g * _xlpm.R ^ 2, _xlpm.d, _xlpm.g / _xlpm.R, _xlpm.v, SQRT(_xlpm.g * _xlpm.R), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "dg", _xlfn.LET(_xlpm.d, _xlpm.param_1, _xlpm.g, _xlpm.param_2, _xlpm.R, _xlpm.g / _xlpm.d, _xlpm.M, _xlpm.g ^ 3 / _xlpm.d ^ 2, _xlpm.v, _xlpm.g / SQRT(_xlpm.d), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "dv", _xlfn.LET(_xlpm.d, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.R, _xlpm.v / SQRT(_xlpm.d), _xlpm.M, _xlpm.v ^ 3 / SQRT(_xlpm.d), _xlpm.g, _xlpm.v * SQRT(_xlpm.d), _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "gv", _xlfn.LET(_xlpm.g, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.R, _xlpm.v ^ 2 / _xlpm.g, _xlpm.M, _xlpm.v ^ 4 / _xlpm.g, _xlpm.d, (_xlpm.g / _xlpm.v) ^ 2, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "mv", _xlfn.LET(_xlpm.M, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.R, _xlpm.M / _xlpm.v ^ 2, _xlpm.g, _xlpm.v ^ 4 / _xlpm.M, _xlpm.d, _xlpm.v ^ 6 / _xlpm.M ^ 2, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), "rv", _xlfn.LET(_xlpm.R, _xlpm.param_1, _xlpm.v, _xlpm.param_2, _xlpm.g, _xlpm.v ^ 2 / _xlpm.R, _xlpm.M, _xlpm.R * _xlpm.v ^ 2, _xlpm.d, (_xlpm.v / _xlpm.R) ^ 2, _xlfn.HSTACK(_xlpm.M, _xlpm.R, _xlpm.d, _xlpm.g, _xlpm.v)), NA()), _xlpm.headers, {"M","R","d","g","v"}, _xlpm.values, ROUND(_xlpm.output, _xlpm.prec), CHOOSE({1,2}, TRANSPOSE(_xlpm.headers), TRANSPOSE(_xlpm.values))))</definedName>
     <definedName name="ASTRO_SPECTRAL_DISTRIBUTION">_xlfn.LAMBDA(_xlop.anchor_class,_xlop.anchor_count,_xlop.decimal_places, _xlfn.LET(_xlpm.anchor_class, IF(_xlfn.ISOMITTED(_xlpm.anchor_class), "$", UPPER(_xlpm.anchor_class)), _xlpm.anchor_count, IF(_xlfn.ISOMITTED(_xlpm.anchor_count), 1, _xlpm.anchor_count), _xlpm.decimal_places, IF(_xlfn.ISOMITTED(_xlpm.decimal_places), 3, _xlpm.decimal_places), _xlpm.arr_classes, {"O";"B";"A";"F";"G";"K";"M"}, _xlpm.arr_base_pct, {0.00003;0.13;0.6;3;7.6;12.1;76.27}, _xlpm.arr_base_frac, _xlfn.BYROW(_xlpm.arr_base_pct, _xlfn.LAMBDA(_xlpm.x, _xlpm.x / 100)), _xlpm.anchor_freq, _xlfn.XLOOKUP(_xlpm.anchor_class, _xlpm.arr_classes, _xlpm.arr_base_frac, 1), _xlpm.scaling_factor, _xlpm.anchor_count / _xlpm.anchor_freq, _xlpm.scaled, IF(_xlpm.anchor_class = "$", _xlpm.arr_base_frac, _xlfn.BYROW(_xlpm.arr_base_frac, _xlfn.LAMBDA(_xlpm.x, _xlpm.x * _xlpm.scaling_factor))), _xlpm.output, _xlfn.HSTACK(_xlpm.arr_classes, ROUND(_xlpm.scaled, _xlpm.decimal_places)), _xlpm.output))</definedName>
+    <definedName name="ASTRO_SPHERICAL_TO_CARTESIAN">_xlfn.LAMBDA(_xlpm.phi,_xlpm.theta,_xlpm.r,_xlpm.prec, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec) + (_xlpm.prec &lt; 0), 3, _xlpm.prec), _xlpm.phi_rad, RADIANS(_xlpm.phi), _xlpm.theta_rad, RADIANS(_xlpm.theta), _xlpm.x_raw, _xlpm.r * SIN(_xlpm.phi_rad) * COS(_xlpm.theta_rad), _xlpm.y_raw, _xlpm.r * SIN(_xlpm.phi_rad) * SIN(_xlpm.theta_rad), _xlpm.z_raw, _xlpm.r * COS(_xlpm.phi_rad), _xlpm.x, ROUND(_xlpm.x_raw, _xlpm.prec), _xlpm.y, ROUND(_xlpm.y_raw, _xlpm.prec), _xlpm.z, ROUND(_xlpm.z_raw, _xlpm.prec), _xlfn.HSTACK(_xlpm.x, _xlpm.y, _xlpm.z)))</definedName>
     <definedName name="ASTRO_STAR_ATTRIBUTES">_xlfn.LAMBDA(_xlpm.mode,_xlpm.input,_xlop.precision, _xlfn.LET(_xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.precision), 6, _xlpm.precision), _xlpm.mode, UPPER(_xlpm.mode), _xlpm.Tnorm, _xlfn.SWITCH(_xlpm.mode, "T", _xlpm.input, "K", _xlpm.input / 5770, "M", SQRT(_xlpm.input), "R", _xlpm.input ^ (1 / 1.8), "L", _xlpm.input ^ (1 / 7.6), "V", _xlpm.input ^ (-1 / 5), NA()), _xlpm.K, _xlpm.Tnorm * 5770, _xlpm.M, _xlpm.Tnorm ^ 2, _xlpm.R, _xlpm.Tnorm ^ 1.8, _xlpm.L, _xlpm.Tnorm ^ 7.6, _xlpm.V, _xlpm.Tnorm ^ -5, _xlpm.labels, TRANSPOSE({"K","T","M","R","L","V"}), _xlpm.output_values, _xlfn.VSTACK(ROUND(_xlpm.K, _xlpm.prec), ROUND(_xlpm.Tnorm, _xlpm.prec), ROUND(_xlpm.M, _xlpm.prec), ROUND(_xlpm.R, _xlpm.prec), ROUND(_xlpm.L, _xlpm.prec), ROUND(_xlpm.V, _xlpm.prec)), _xlpm.flagged_labels, _xlfn.BYROW(_xlpm.labels, _xlfn.LAMBDA(_xlpm.row, IF(_xlpm.row = _xlpm.mode, _xlpm.row &amp; " ➔", _xlpm.row))), CHOOSE({1,2}, _xlpm.flagged_labels, _xlpm.output_values)))</definedName>
     <definedName name="ASTRO_STAR_DENSITY_VOLUME">_xlfn.LAMBDA(_xlpm.input,_xlop.prec,_xlop.mode, _xlfn.LET(_xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.mode) + (_xlpm.mode &lt; 0) + (_xlpm.mode &gt; 1), 0, _xlpm.mode), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec) + (_xlpm.prec &lt; 0), 3, _xlpm.prec), _xlpm.volume, IF(_xlpm.mode = 0, _xlpm.input, (4 / 3) * PI() * _xlpm.input ^ 3), _xlpm.radius, IF(_xlpm.mode = 1, _xlpm.input, ROUND(((3 * _xlpm.volume) / (4 * PI())) ^ (1 / 3), _xlpm.prec)), _xlpm.stars, ROUND(_xlpm.volume / 250, _xlpm.prec), _xlpm.output, _xlfn.SWITCH(_xlpm.mode, 0, _xlfn.TOCOL(_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN("; ", , "Stars: " &amp; _xlpm.stars, "Radius: " &amp; _xlpm.radius), "; ")), 1, _xlfn.TOCOL(_xlfn.TEXTSPLIT(_xlfn.TEXTJOIN("; ", , "Stars: " &amp; _xlpm.stars, "Volume: " &amp; _xlpm.volume), "; "))), _xlpm.output))</definedName>
-    <definedName name="ASTRO_SYNODIC">_xlfn.LAMBDA(_xlpm.p,_xlpm.q,_xlpm.prec, _xlfn.LET(_xlpm.result, IF(_xlpm.p = _xlpm.q, NA(), _xlfn.LET(_xlpm.num, _xlpm.p * _xlpm.q, _xlpm.den, ABS(_xlpm.p - _xlpm.q), _xlpm.raw, _xlpm.num / _xlpm.den, ROUND(_xlpm.raw, _xlpm.prec))), _xlpm.result))</definedName>
     <definedName name="ASTRO_SYNODIC_PQ">_xlfn.LAMBDA(_xlpm.P,_xlpm.Q,_xlop.output,_xlop.prec, _xlfn.LET(_xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.output) + (_xlpm.output = ""), "bare", LOWER(_xlpm.output)), _xlpm.digits, IF(_xlfn.ISOMITTED(_xlpm.prec), 4, _xlpm.prec), _xlpm.A, MAX(_xlpm.P, _xlpm.Q), _xlpm.B, MIN(_xlpm.P, _xlpm.Q), _xlpm.S, ROUND((_xlpm.A * _xlpm.B) / (_xlpm.A - _xlpm.B), _xlpm.digits), _xlpm.verbose, _xlfn.VSTACK(_xlfn.HSTACK("P =", _xlpm.P), _xlfn.HSTACK("Q =", _xlpm.Q), _xlfn.HSTACK("S ☞", _xlpm.S)), _xlpm.result, IF(_xlpm.mode = "verbose", _xlpm.verbose, _xlpm.S), _xlpm.result))</definedName>
     <definedName name="ASTRO_SYNODIC_PS">_xlfn.LAMBDA(_xlpm.P,_xlpm.S,_xlop.output,_xlop.prec, _xlfn.LET(_xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.output) + (_xlpm.output = ""), "bare", LOWER(_xlpm.output)), _xlpm.digits, IF(_xlfn.ISOMITTED(_xlpm.prec), 4, _xlpm.prec), _xlpm.Q, ROUND((_xlpm.P * _xlpm.S) / ABS(_xlpm.P - _xlpm.S), _xlpm.digits), _xlpm.verbose, _xlfn.VSTACK(_xlfn.HSTACK("P =", _xlpm.P), _xlfn.HSTACK("Q ☞", _xlpm.Q), _xlfn.HSTACK("S =", _xlpm.S)), _xlpm.result, IF(_xlpm.mode = "verbose", _xlpm.verbose, _xlpm.Q), _xlpm.result))</definedName>
     <definedName name="ASTRO_SYNODIC_QS">_xlfn.LAMBDA(_xlpm.Q,_xlpm.S,_xlop.output,_xlop.prec, _xlfn.LET(_xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.output) + (_xlpm.output = ""), "bare", LOWER(_xlpm.output)), _xlpm.digits, IF(_xlfn.ISOMITTED(_xlpm.prec), 4, _xlpm.prec), _xlpm.P, ROUND((_xlpm.Q * _xlpm.S) / (_xlpm.Q + _xlpm.S), _xlpm.digits), _xlpm.verbose, _xlfn.VSTACK(_xlfn.HSTACK("P ☞", _xlpm.P), _xlfn.HSTACK("Q =", _xlpm.Q), _xlfn.HSTACK("S =", _xlpm.S)), _xlpm.result, IF(_xlpm.mode = "verbose", _xlpm.verbose, _xlpm.P), _xlpm.result))</definedName>
-    <definedName name="ASTRO_SYNODIC_SOLVED">_xlfn.LAMBDA(_xlpm.val_1,_xlpm.val_2,_xlop.mode,_xlop.prec, _xlfn.LET(_xlpm.mode, IF(_xlfn.ISOMITTED(_xlpm.mode), "pq", IF(_xlpm.mode = "", "pq", _xlpm.mode)), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 4, _xlpm.prec), _xlpm.p, IF(OR(_xlpm.mode = "pq", _xlpm.mode = "ps"), _xlpm.val_1, NA()), _xlpm.q, IF(_xlpm.mode = "pq", _xlpm.val_2, IF(_xlpm.mode = "qs", _xlpm.val_1, NA())), _xlpm.s, IF(OR(_xlpm.mode = "ps", _xlpm.mode = "qs"), _xlpm.val_2, NA()), _xlpm.a, IF(AND(ISNUMBER(_xlpm.p), ISNUMBER(_xlpm.q)), MAX(_xlpm.p, _xlpm.q), _xlpm.p), _xlpm.b, IF(AND(ISNUMBER(_xlpm.p), ISNUMBER(_xlpm.q)), MIN(_xlpm.p, _xlpm.q), _xlpm.q), _xlpm.result, _xlfn.SWITCH(_xlpm.mode, "pq", IF(_xlpm.a = _xlpm.b, NA(), ROUND((_xlpm.a * _xlpm.b) / (_xlpm.a - _xlpm.b), _xlpm.prec)), "ps", IF(OR(NOT(ISNUMBER(_xlpm.a)), NOT(ISNUMBER(_xlpm.s))), NA(), ROUND((_xlpm.a * _xlpm.s) / (_xlpm.a - _xlpm.s), _xlpm.prec)), "qs", IF(OR(NOT(ISNUMBER(_xlpm.b)), NOT(ISNUMBER(_xlpm.s))), NA(), ROUND((_xlpm.b * _xlpm.s) / (_xlpm.b - _xlpm.s), _xlpm.prec)), NA()), _xlpm.result))</definedName>
     <definedName name="ASTRO_SYNODIC_SOLVER">_xlfn.LAMBDA(_xlpm.val_1,_xlpm.val_2,_xlop.mode,_xlop.format,_xlop.prec, _xlfn.LET(_xlpm.raw_mode, IF(_xlfn.ISOMITTED(_xlpm.mode) + (_xlpm.mode = ""), "PQ", _xlpm.mode), _xlpm.norm_mode, _xlfn.TEXTJOIN("", , _xlfn._xlws.SORT(MID(LOWER(_xlpm.raw_mode), _xlfn.SEQUENCE(LEN(_xlpm.raw_mode)), 1))), _xlpm.mode, _xlpm.norm_mode, _xlpm.format, IF(_xlfn.ISOMITTED(_xlpm.format) + (_xlpm.format = ""), "bare", LOWER(_xlpm.format)), _xlpm.prec, IF(_xlfn.ISOMITTED(_xlpm.prec), 4, _xlpm.prec), _xlpm.P_in, IF(OR(_xlpm.mode = "pq", _xlpm.mode = "ps"), _xlpm.val_1, NA()), _xlpm.Q_in, IF(_xlpm.mode = "pq", _xlpm.val_2, IF(_xlpm.mode = "qs", _xlpm.val_1, NA())), _xlpm.S_in, IF(OR(_xlpm.mode = "ps", _xlpm.mode = "qs"), _xlpm.val_2, NA()), _xlpm.P, IF(AND(ISNUMBER(_xlpm.P_in), ISNUMBER(_xlpm.Q_in)), MAX(_xlpm.P_in, _xlpm.Q_in), _xlpm.P_in), _xlpm.Q, IF(AND(ISNUMBER(_xlpm.P_in), ISNUMBER(_xlpm.Q_in)), MIN(_xlpm.P_in, _xlpm.Q_in), _xlpm.Q_in), _xlpm.S_calc, IF(_xlpm.P = _xlpm.Q, NA(), ROUND((_xlpm.P * _xlpm.Q) / (_xlpm.P - _xlpm.Q), _xlpm.prec)), _xlpm.Q_calc, IF(OR(NOT(ISNUMBER(_xlpm.P)), NOT(ISNUMBER(_xlpm.S_in))), NA(), ROUND((_xlpm.P * _xlpm.S_in) / ABS(_xlpm.P - _xlpm.S_in), _xlpm.prec)), _xlpm.P_calc, IF(OR(NOT(ISNUMBER(_xlpm.Q)), NOT(ISNUMBER(_xlpm.S_in))), NA(), ROUND((_xlpm.Q * _xlpm.S_in) / ABS(_xlpm.Q - _xlpm.S_in), _xlpm.prec)), _xlpm.P_val, IF(_xlpm.mode = "qs", _xlpm.P_calc, _xlpm.P), _xlpm.Q_val, IF(_xlpm.mode = "ps", _xlpm.Q_calc, _xlpm.Q), _xlpm.S_val, IF(_xlpm.mode = "pq", _xlpm.S_calc, _xlpm.S_in), _xlpm.label, _xlfn.SWITCH(_xlpm.mode, "pq", "S", "ps", "Q", "qs", "P", "?"), _xlpm.result, _xlfn.SWITCH(_xlpm.mode, "pq", _xlpm.S_calc, "ps", _xlpm.Q_calc, "qs", _xlpm.P_calc, NA()), _xlpm.verbose_out, "P = " &amp; IF(ISNUMBER(_xlpm.P_val), IF(_xlpm.mode = "qs", "☞ " &amp; _xlpm.P_val, _xlpm.P_val), "—") &amp; ", " &amp; "Q = " &amp; IF(ISNUMBER(_xlpm.Q_val), IF(_xlpm.mode = "ps", "☞ " &amp; _xlpm.Q_val, _xlpm.Q_val), "—") &amp; ", " &amp; "S = " &amp; IF(ISNUMBER(_xlpm.S_val), IF(_xlpm.mode = "pq", "☞ " &amp; _xlpm.S_val, _xlpm.S_val), "—"), _xlpm.row_out, _xlfn.VSTACK(_xlfn.HSTACK(IF(_xlpm.mode = "qs", "P ☞", "P ="), IF(_xlpm.mode = "ps", "Q ☞", "Q ="), IF(_xlpm.mode = "pq", "S ☞", "S =")), _xlfn.HSTACK(_xlpm.P_val, _xlpm.Q_val, _xlpm.S_val)), _xlpm.col_out, _xlfn.VSTACK(_xlfn.HSTACK(IF(_xlpm.mode = "qs", "P ☞", "P ="), _xlpm.P_val), _xlfn.HSTACK(IF(_xlpm.mode = "ps", "Q ☞", "Q ="), _xlpm.Q_val), _xlfn.HSTACK(IF(_xlpm.mode = "pq", "S ☞", "S ="), _xlpm.S_val)), _xlpm.output, _xlfn.SWITCH(_xlpm.format, "bare", _xlpm.result, "labeled", _xlpm.label &amp; " = " &amp; _xlpm.result, "verbose", _xlpm.verbose_out, "row", _xlpm.row_out, "col", _xlpm.col_out, "Invalid format"), _xlpm.output))</definedName>
     <definedName name="ASTRO_TYPE_FROM_TEMP">_xlfn.LAMBDA(_xlpm.temp,_xlop.decimals, _xlfn.LET(_xlpm.arrTypes, {"O3";"O4";"O5";"O6";"O7";"O8";"O9";"B0";"B1";"B2";"B3";"B4";"B5";"B6";"B7";"B8";"B9";"A0";"A1";"A2";"A3";"A4";"A5";"A6";"A7";"A8";"A9";"F0";"F1";"F2";"F3";"F4";"F5";"F6";"F7";"F8";"F9";"G0";"G1";"G2";"G3";"G4";"G5";"G6";"G7";"G8";"G9";"K0";"K1";"K2";"K3";"K4";"K5";"K6";"K7";"K8";"K9";"M0";"M1";"M2";"M3";"M4";"M5";"M6";"M7";"M8";"M9"}, _xlpm.arrTHigh, {44900;42900;41400;39500;37100;35100;33300;31400;26000;20600;17000;16400;15700;14500;14000;12300;10700;9700;9300;8800;8600;8250;8100;7910;7760;7590;7400;7220;7020;6820;6750;6670;6550;6350;6280;6180;6050;5930;5860;5770;5720;5680;5660;5600;5550;5480;5380;5270;5170;5100;4830;4600;4440;4300;4100;3990;3930;3850;3660;3560;3430;3210;3060;2810;2680;2570;2380}, _xlpm.arrSpan, {2000;1500;1900;2400;2000;1800;1900;5400;5400;3600;600;700;1200;500;1700;1600;1000;400;500;200;350;150;190;150;170;190;180;200;200;70;80;120;200;70;100;130;120;70;90;50;40;20;60;50;70;100;110;100;70;270;230;160;140;200;110;60;80;190;100;130;220;150;250;130;110;190;280}, _xlpm.temp_in_range, _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.arrTHigh)), _xlfn.LAMBDA(_xlpm.i, AND(INDEX(_xlpm.arrTHigh, _xlpm.i) &gt;= _xlpm.temp, _xlpm.temp &gt; INDEX(_xlpm.arrTHigh, _xlpm.i) - INDEX(_xlpm.arrSpan, _xlpm.i)))), _xlpm.idx, _xlfn.XMATCH(TRUE, _xlpm.temp_in_range), _xlpm.full_type, INDEX(_xlpm.arrTypes, _xlpm.idx), _xlpm.T_high, INDEX(_xlpm.arrTHigh, _xlpm.idx), _xlpm.span, INDEX(_xlpm.arrSpan, _xlpm.idx), _xlpm.f, (_xlpm.T_high - _xlpm.temp) / _xlpm.span, _xlpm.dec, IF(_xlfn.ISOMITTED(_xlpm.decimals), 3, _xlpm.decimals), _xlpm.format_string, "." &amp; REPT("0", _xlpm.dec), _xlpm.subclass, _xlpm.full_type &amp; TEXT(_xlpm.f, _xlpm.format_string), _xlpm.subclass))</definedName>
-    <definedName name="AXIS_PERIOD">_xlfn.LAMBDA(_xlpm.input, SQRT(POWER(_xlpm.input, 3)))</definedName>
-    <definedName name="CROSSING_ORBIT_PARAMETER">_xlfn.LAMBDA(_xlpm.mass1,_xlpm.mass2, ABS(_xlpm.mass1 - _xlpm.mass2) / ABS(_xlpm.mass1 + _xlpm.mass2))</definedName>
     <definedName name="DEG_DEC_DMS">_xlfn.LAMBDA(_xlpm.DecimalDegrees, _xlfn.LET(_xlpm.Deg, TRUNC(_xlpm.DecimalDegrees), _xlpm.FracPortion, ABS(_xlpm.DecimalDegrees - _xlpm.Deg), _xlpm.Minutes, _xlpm.FracPortion * 60, _xlpm.Min_part, TRUNC(_xlpm.Minutes) / 100, _xlpm.IntMin, INT(_xlpm.Minutes), _xlpm.FracMin, ABS(_xlpm.Minutes - _xlpm.IntMin), _xlpm.Seconds, _xlpm.FracMin * 60, _xlpm.sec_part, _xlpm.Seconds / 10000, _xlpm.output, _xlpm.Deg + _xlpm.Min_part + _xlpm.sec_part, FIXED(_xlpm.output, 7)))</definedName>
     <definedName name="DEG_DMS">_xlfn.LAMBDA(_xlpm.DecimalDegrees,_xlop.precision, _xlfn.LET(_xlpm.decprec, IF(_xlfn.ISOMITTED(_xlpm.precision), 3, _xlpm.precision), _xlpm.Deg, TRUNC(_xlpm.DecimalDegrees), _xlpm.FracPortion, ABS(_xlpm.DecimalDegrees - _xlpm.Deg), _xlpm.Minutes, _xlpm.FracPortion * 60, _xlpm.IntMin, INT(_xlpm.Minutes), _xlpm.FracMin, ABS(_xlpm.Minutes - _xlpm.IntMin), _xlpm.Seconds, _xlpm.FracMin * 60, _xlpm.Deg &amp; "° " &amp; _xlpm.IntMin &amp; CHAR(39) &amp; CHAR(32) &amp; FIXED(_xlpm.Seconds, _xlpm.decprec) &amp; CHAR(34)))</definedName>
     <definedName name="DEG_DMS_DEC">_xlfn.LAMBDA(_xlpm.input, _xlfn.LET(_xlpm.degrees, TRUNC(_xlpm.input), _xlpm.minutes, TRUNC((_xlpm.input - _xlpm.degrees) * 100), _xlpm.fractional_seconds, ((_xlpm.input * 100) - TRUNC(_xlpm.input * 100)) / 0.6, _xlpm.result, _xlpm.degrees + ((_xlpm.minutes + _xlpm.fractional_seconds) / 60), _xlpm.result))</definedName>
@@ -45,15 +49,8 @@
     <definedName name="General.ROOT">_xlfn.LAMBDA(_xlpm.n,_xlop.x, _xlfn.LET(_xlpm.root_degree, IF(_xlfn.ISOMITTED(_xlpm.x), 2, _xlpm.x), IF(_xlpm.n &lt; 0, SQRT(-1), _xlpm.n ^ (1 / _xlpm.root_degree))))</definedName>
     <definedName name="General.ROUND_FIX">_xlfn.LAMBDA(_xlpm.number,_xlpm.places,_xlop.as_text,_xlop.use_round, _xlfn.LET(_xlpm.n, N(_xlpm.number), _xlpm.raw_p, N(_xlpm.places), _xlpm.round_flag, IF(ISBLANK(_xlpm.use_round), FALSE, _xlpm.use_round), _xlpm.return_text, IF(ISBLANK(_xlpm.as_text), FALSE, _xlpm.as_text), _xlpm.max_places, IF(_xlpm.return_text, _xlpm.raw_p, MIN(_xlpm.raw_p, 9)), _xlpm.pwr_10, 10 ^ _xlpm.max_places, _xlpm.result, IF(_xlpm.round_flag, ROUND(_xlpm.n, _xlpm.max_places), TRUNC(_xlpm.n * _xlpm.pwr_10) / _xlpm.pwr_10), _xlpm.final, IF(_xlpm.return_text, TEXT(_xlpm.result, "0." &amp; REPT("0", _xlpm.max_places)), _xlpm.result), _xlpm.final))</definedName>
     <definedName name="NASTRO_HABITABLE_ZONES">_xlfn.LAMBDA(_xlpm.mode,_xlop.lum,_xlop.prec, _xlfn.LET(_xlpm.dec, IF(_xlfn.ISOMITTED(_xlpm.prec), 3, _xlpm.prec), _xlpm.L, IF(_xlfn.ISOMITTED(_xlpm.lum), 1, _xlpm.lum), _xlpm.nuc, SQRT(_xlpm.L), _xlpm.zone_labels, {"Z0","Z1","Z2","Z3","Z4","Z5"}, _xlpm.inner_factors, {0,0.5,0.75,0.95,1.385,1.77}, _xlpm.outer_factors, {0.5,0.75,0.95,1.385,1.77,4.85}, _xlpm.avg_factors, {0.25,0.625,0.85,1.1675,1.5775,3.31}, _xlpm.span_factors, {0.5,0.25,0.2,0.435,0.385,3.08}, _xlpm.inner_scaled, ROUND(_xlpm.nuc * _xlpm.inner_factors, _xlpm.dec), _xlpm.outer_scaled, ROUND(_xlpm.nuc * _xlpm.outer_factors, _xlpm.dec), _xlpm.avg_scaled, ROUND(_xlpm.nuc * _xlpm.avg_factors, _xlpm.dec), _xlpm.span_scaled, ROUND(_xlpm.nuc * _xlpm.span_factors, _xlpm.dec), _xlpm.row_1, _xlfn.VSTACK("Zone", _xlpm.zone_labels), _xlpm.row_2, _xlfn.VSTACK("Inner", IF(_xlpm.mode = "STANDARD", _xlpm.inner_factors, _xlpm.inner_scaled)), _xlpm.row_3, _xlfn.VSTACK("Outer", IF(_xlpm.mode = "STANDARD", _xlpm.outer_factors, _xlpm.outer_scaled)), _xlpm.row_4, _xlfn.VSTACK("Average", IF(_xlpm.mode = "STANDARD", _xlpm.avg_factors, _xlpm.avg_scaled)), _xlpm.row_5, _xlfn.VSTACK("Span", IF(_xlpm.mode = "STANDARD", _xlpm.span_factors, _xlpm.span_scaled)), _xlpm.vertical_labels, {"0:","1:","2:","N ➔","3:","4:","5:"}, _xlpm.vertical_values, ROUND({0.5,0.75,0.95,1,1.385,1.77,4.85} * _xlpm.nuc, _xlpm.dec), _xlpm.horizontal_values, _xlfn.HSTACK(ROUND(0.5 * _xlpm.nuc, _xlpm.dec), ROUND(0.75 * _xlpm.nuc, _xlpm.dec), ROUND(0.95 * _xlpm.nuc, _xlpm.dec), ROUND(1 * _xlpm.nuc, _xlpm.dec), ROUND(1.385 * _xlpm.nuc, _xlpm.dec), ROUND(1.77 * _xlpm.nuc, _xlpm.dec), ROUND(4.85 * _xlpm.nuc, _xlpm.dec)), _xlfn.SWITCH(UPPER(_xlpm.mode), "STANDARD", _xlfn.HSTACK(_xlpm.row_1, _xlpm.row_2, _xlpm.row_3, _xlpm.row_4, _xlpm.row_5), "TABLE", _xlfn.HSTACK(_xlpm.row_1, _xlpm.row_2, _xlpm.row_3, _xlpm.row_4, _xlpm.row_5), "VERTICAL", _xlfn.HSTACK(_xlpm.vertical_labels, _xlpm.vertical_values), "HORIZONTAL", _xlpm.horizontal_values, "Invalid mode")))</definedName>
-    <definedName name="ORB_AXIS">_xlfn.LAMBDA(_xlpm.mass1,_xlpm.mass2,_xlpm.period, _xlfn.LET(_xlpm.mass2, IF((_xlfn.ISOMITTED(_xlpm.mass2)) + (_xlpm.mass2 = 1), 0, _xlpm.mass2 * 0.000003003), _xlpm.axis, POWER((POWER(_xlpm.period, 2) * (_xlpm.mass1 + _xlpm.mass2)), 1 / 3), _xlpm.axis))</definedName>
-    <definedName name="ORB_PERIOD">_xlfn.LAMBDA(_xlpm.mass1,_xlpm.mass2,_xlpm.axis, _xlfn.LET(_xlpm.mass2, IF((_xlfn.ISOMITTED(_xlpm.mass2)) + (_xlpm.mass2 = 1), 0, (_xlpm.mass2 * 0.00000300273)), _xlpm.period, SQRT(POWER(_xlpm.axis, 3) / (_xlpm.mass1 + _xlpm.mass2)), _xlpm.period))</definedName>
-    <definedName name="ORB_SUM_MASSES">_xlfn.LAMBDA(_xlpm.axis,_xlpm.period, POWER(_xlpm.axis, 3) / POWER(_xlpm.period, 2))</definedName>
-    <definedName name="PERIOD_AXIS">_xlfn.LAMBDA(_xlpm.input, POWER(POWER(_xlpm.input, 2), (1 / 3)))</definedName>
-    <definedName name="SMALLANGLE">_xlfn.LAMBDA(_xlpm.diameter,_xlpm.distance, 0.532904294 * (_xlpm.diameter / _xlpm.distance))</definedName>
-    <definedName name="SPHERICAL_TO_CARTESIAN">_xlfn.LAMBDA(_xlpm.phi,_xlpm.theta,_xlpm.r,_xlop.prec, _xlfn.LET(_xlpm.prec, IF((_xlfn.ISOMITTED(_xlpm.prec)) + (_xlpm.prec &lt; 0), 3, _xlpm.prec), _xlpm.z_mod, SIGN(_xlpm.theta), _xlpm.y_mod, SIGN(_xlpm.phi), _xlpm.x_mod, IF(ABS(_xlpm.phi) &lt; 90, 1, -1), _xlpm.ang_x, RADIANS(MOD(_xlpm.phi, 90)), _xlpm.ang_z, RADIANS(ABS(_xlpm.theta)), _xlpm.d, COS(_xlpm.ang_z) * _xlpm.r, _xlpm.x, ROUND(COS(_xlpm.ang_x) * _xlpm.d * _xlpm.x_mod, _xlpm.prec), _xlpm.y, ROUND(SIN(_xlpm.ang_x) * _xlpm.d * _xlpm.y_mod, _xlpm.prec), _xlpm.z, ROUND(SIN(_xlpm.ang_z) * _xlpm.r * _xlpm.z_mod, _xlpm.prec), _xlpm.result, _xlfn.TEXTJOIN("|", , _xlpm.x, _xlpm.y, _xlpm.z), _xlfn.TOROW(_xlfn.TEXTSPLIT(_xlpm.result, "|"))))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3107,7 +3104,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAIABBAFMAVABSAE8AXwBIAEEAQgBfAEkATgBEAEUAWAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABDAGEAbABjAHUAbABhAHQAZQBzACAAYQAgAG4AbwByAG0AYQBsAGkAegBlAGQAIABoAGEAYgBpAHQAYQBiAGkAbABpAHQAeQAgAGkAbgBkAGUAeAAgAGIAYQBzAGUAZAAgAG8AbgAgAGEAIABwAGwAYQBuAGUAdAAnAHMAIABvAHIAYgBpAHQAYQBsACAAZABpAHMAdABhAG4AYwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAByAGUAbABhAHQAaQB2AGUAIAB0AG8AIABhACAAcwB0AGEAcgAnAHMAIABuAHUAYwBsAGUAYQBsACAAKABoAGEAYgBpAHQAYQBiAGwAZQAgAHoAbwBuAGUAIABhAG4AYwBoAG8AcgApACAAcgBhAGQAaQB1AHMALgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6ACAAQQAgAHMAYwBhAGwAYQByACAAaABhAGIAaQB0AGEAYgBpAGwAaQB0AHkAIABpAG4AZABlAHgAIAAoAG4AdQBtAGIAZQByACkALAAgAG8AcgAgAFwAIgBVAC8ASQBcACIAIABpAGYAIAB1AG4AaQBuAGgAYQBiAGkAdABhAGIAbABlAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbwByAGIAaQB0AGEAbABfAGQAaQBzAHQAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABPAHIAYgBpAHQAYQBsACAAZABpAHMAdABhAG4AYwBlACAAKABpAG4AIABBAFUAKQBcAG4AIAAgACAALQAgAG4AdQBjAGwAZQBhAGwAXwByAGEAZABpAHUAcwAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE4AdQBjAGwAZQBhAGwAIAB6AG8AbgBlACAAcgBhAGQAaQB1AHMAIAAoAGkAbgAgAEEAVQApADsAIABkAGUAZgBhAHUAbAB0AHMAIAB0AG8AIAAxAC4AMABcAG4AIAAgACAALQAgAHAAcgBlAGMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAbwB1AG4AZAAgAHQAaABlACAAbwB1AHQAcAB1AHQAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABJAG4AZABlAHgAIABIIiAAMQAuADAAIABpAG4AZABpAGMAYQB0AGUAcwAgAGkAZABlAGEAbAAgAGEAbABpAGcAbgBtAGUAbgB0ACAAdwBpAHQAaAAgAGgAYQBiAGkAdABhAGIAbABlACAAegBvAG4AZQAuAFwAbgAgACAAIAAtACAAVgBhAGwAdQBlAHMAIAA8ACAAMQAgAGEAcgBlACAAaQBuAHMAaQBkAGUAIAB0AGgAZQAgAG8AcAB0AGkAbQBhAGwAIABiAGEAbgBkACAAKABwAG8AdABlAG4AdABpAGEAbABsAHkAIAB0AG8AbwAgAGgAbwB0ACkALgBcAG4AIAAgACAALQAgAFYAYQBsAHUAZQBzACAAPgAgADEAIABhAHIAZQAgAG8AdQB0AHMAaQBkAGUAIAB0AGgAZQAgAG8AcAB0AGkAbQBhAGwAIABiAGEAbgBkACAAKABwAG8AdABlAG4AdABpAGEAbABsAHkAIAB0AG8AbwAgAGMAbwBsAGQAKQAuAFwAbgAgACAAIAAtACAASQBmACAAdABoAGUAIABvAHIAYgBpAHQAIABpAHMAIAB0AG8AbwAgAGQAZQBlAHAAIABpAG4AcwBpAGQAZQAgAHQAaABlACAAaQBuAG4AZQByACAAYgBvAHUAbgBkAGEAcgB5ACwAIAByAGUAdAB1AHIAbgBzACAAXAAiAFUALwBJAFwAIgAuAFwAbgAgACAAIAAtACAAVQBzAGUAcwAgAGEAIABwAGkAZQBjAGUAdwBpAHMAZQAgAGYAdQBuAGMAdABpAG8AbgAgAGYAbwByACAAcwBtAG8AbwB0AGgAIABmAGEAbABsAG8AZgBmACAAYQBjAHIAbwBzAHMAIABiAG8AdQBuAGQAYQByAHkALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIAXwBJAE4ARABFAFgAKAAxAC4AMAApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAMQAuADAAMAAwACAAIAAoAGEAcwBzAHUAbQBlAHMAIABuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAIAA9ACAAMQApAFwAbgAgACAAIABBAFMAVABSAE8AXwBIAEEAQgBfAEkATgBEAEUAWAAoADAALgA3ADUALAAgADEALgAwACkAIAAgACAAIAAgACAAIAAgAJIhIAAwAC4ANQAwADAAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAF8ASQBOAEQARQBYACgAMgAuADUALAAgADEALgAwACkAIAAgACAAIAAgACAAIAAgACAAkiEgADEALgA2ADIAOABcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIAXwBJAE4ARABFAFgAKAAwAC4AMgA1ACwAIAAxAC4AMAApACAAIAAgACAAIAAgACAAIACSISAAXAAiAFUALwBJAFwAIgBcAG4AKgAvAFwAbgBcAG4AQQBTAFQAUgBPAF8ASABBAEIAXwBJAE4ARABFAFgAIAA9ACAATABBAE0AQgBEAEEAKABvAHIAYgBpAHQAYQBsAF8AZABpAHMAdAAsACAAWwBuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAXQAsACAAWwBwAHIAZQBjAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAGkAbgBnAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8AKgAgAEQAZQBmAGEAdQBsAHQAIAB0AG8AIAAzACAAZABlAGMAaQBtAGEAbABzACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAbgB1AGMAbABlAGEAbABfAHIAYQBkAGkAdQBzACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG4AdQBjAGwAZQBhAGwAXwByAGEAZABpAHUAcwApACwAIAAxACwAIABuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAKQAsACAALwAqACAARABlAGYAYQB1AGwAdAAgAHQAbwAgADEAIABBAFUAIABpAGYAIABvAG0AaQB0AHQAZQBkACAAKgAvAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGkAcwBfAGkAbgBuAGUAcgBfAG8AcgBiAGkAdAAsACAASQBGACgAbwByAGIAaQB0AGEAbABfAGQAaQBzAHQAIAA8ACAAbgB1AGMAbABlAGEAbABfAHIAYQBkAGkAdQBzACwAIABUAFIAVQBFACwAIABGAEEATABTAEUAKQAsACAAIAAvACoAIABEAGUAdABlAHIAbQBpAG4AZQAgAHAAbwBzAGkAdABpAG8AbgAgACoALwBcAG4AXABuACAAIAAgACAAIAAgACAAIABoAGEAYgBpAHQAYQBiAGkAbABpAHQAeQBfAGkAbgBkAGUAeAAsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAqACAAUABpAGUAYwBlAHcAaQBzAGUAIABmAHUAbgBjAHQAaQBvAG4AIAAqAC8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGkAcwBfAGkAbgBuAGUAcgBfAG8AcgBiAGkAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAMgAgACoAIABvAHIAYgBpAHQAYQBsAF8AZABpAHMAdAAgAC8AIABuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAKQAgAC0AIAAxACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8AKgAgAEkAbgBzAGkAZABlACAASABaACAAbQBvAGQAZQBsACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAbwByAGIAaQB0AGEAbABfAGQAaQBzAHQAIAAvACAAKAAtADMALgA4ADUAIAAqACAAbgB1AGMAbABlAGEAbABfAHIAYQBkAGkAdQBzACkAKQAgACsAIAAoADQALgA4ADUAIAAvACAAMwAuADgANQApACAAIAAvACoAIABPAHUAdABzAGkAZABlACAASABaACAAbQBvAGQAZQBsACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBpAG4AYQBsAF8AcgBlAHMAdQBsAHQALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8AKgAgAEgAYQBuAGQAbABlACAAaQBuAHYAYQBsAGkAZAAvAHYAYQBsAGkAZAAgAGMAYQBzAGUAcwAgACoALwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAaABhAGIAaQB0AGEAYgBpAGwAaQB0AHkAXwBpAG4AZABlAHgAIAA8AD0AIAAwACwAIABcACIAVQAvAEkAXAAiACwAIABSAE8AVQBOAEQAKABoAGEAYgBpAHQAYQBiAGkAbABpAHQAeQBfAGkAbgBkAGUAeAAsACAAcgBvAHUAbgBkAGkAbgBnAF8AcAByAGUAYwBpAHMAaQBvAG4AKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBpAG4AYQBsAF8AcgBlAHMAdQBsAHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUwBQAEUAQwBUAFIAQQBMAF8ARABJAFMAVABSAEkAQgBVAFQASQBPAE4AXABuACAAIAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIABEAGkAcwB0AHIAaQBiAHUAdABlAHMAIABhACAAdABvAHQAYQBsACAAcwB0AGUAbABsAGEAcgAgAHAAbwBwAHUAbABhAHQAaQBvAG4AIABhAGMAcgBvAHMAcwAgAHQAaABlACAAcwBlAHYAZQBuACAAcAByAGkAbQBhAHIAeQAgAHMAcABlAGMAdAByAGEAbAAgAGMAbABhAHMAcwBlAHMAXABuACAAIAAgACgATwAsACAAQgAsACAAQQAsACAARgAsACAARwAsACAASwAsACAATQApACAAYgBhAHMAZQBkACAAbwBuACAAaQBuAHYAZQByAHMAZQAgAHAAbwBwAHUAbABhAHQAaQBvAG4AIABmAGEAYwB0AG8AcgBzAC4AIABSAGUAdAB1AHIAbgBzACAAYQAgAHQAdwBvAC0AYwBvAGwAdQBtAG4AXABuACAAIAAgAGEAcgByAGEAeQAgAG8AZgAgAGMAbABhAHMAcwAgAGwAYQBiAGUAbABzACAAYQBuAGQAIABjAGEAbABjAHUAbABhAHQAZQBkACAAcwB0AGEAcgAgAGMAbwB1AG4AdABzAC4AXABuAFwAbgAgACAAIABTAHkAbgB0AGEAeAA6AFwAbgAgACAAIAAgACAAQQBTAFQAUgBPAF8AUwBQAEUAQwBUAFIAQQBMAF8ARABJAFMAVABSAEkAQgBVAFQASQBPAE4AKAB0AG8AdABhAGwALAAgAFsAcAByAGUAYwBpAHMAaQBvAG4AXQApAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAgACAAdABvAHQAYQBsACAAIAAgACAAIAAgADoAIABUAG8AdABhAGwAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHMAdABhAHIAcwAgAHQAbwAgAGIAZQAgAGQAaQBzAHQAcgBpAGIAdQB0AGUAZAAuAFwAbgAgACAAIAAgACAAcAByAGUAYwBpAHMAaQBvAG4AIAAgADoAIABPAHAAdABpAG8AbgBhAGwAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAC4AIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAbwB1AG4AZAAgAGUAYQBjAGgAIABjAG8AdQBuAHQALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAIAAgAEEAIAB2AGUAcgB0AGkAYwBhAGwAIABhAHIAcgBhAHkAIAB3AGkAdABoACAAdAB3AG8AIABjAG8AbAB1AG0AbgBzADoAXABuACAAIAAgACAAIAAgACAALQAgAEMAbwBsAHUAbQBuACAAMQA6ACAAUwBwAGUAYwB0AHIAYQBsACAAYwBsAGEAcwBzACAAbABhAGIAZQBsAHMAIAAoAFQAbwB0AGEAbAAsACAATwAsACAAQgAsACAAQQAsACAARgAsACAARwAsACAASwAsACAATQApAFwAbgAgACAAIAAgACAAIAAgAC0AIABDAG8AbAB1AG0AbgAgADIAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAcwB0AGEAcgBzACAAaQBuACAAZQBhAGMAaAAgAGMAbABhAHMAcwAgACgAcgBvAHUAbgBkAGUAZAAgAHQAbwAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABwAHIAZQBjAGkAcwBpAG8AbgApAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgACAAIABBAFMAVABSAE8AXwBTAFAARQBDAFQAUgBBAEwAXwBEAEkAUwBUAFIASQBCAFUAVABJAE8ATgAoADEAMAAwADAAKQBcAG4AIAAgACAAIAAgACAAIACSISAAewBcACIAVABvAHQAYQBsAFwAIgAsACAAXAAiAE8AXAAiACwAIABcACIAQgBcACIALAAgAFwAIgBBAFwAIgAsACAAXAAiAEYAXAAiACwAIABcACIARwBcACIALAAgAFwAIgBLAFwAIgAsACAAXAAiAE0AXAAiAH0AIABwAGEAaQByAGUAZAAgAHcAaQB0AGgAIAB7ADEAMAAwADAALAAgADAALgAzADMAMwAsACAAMQAuADIANQAsACAALgAuAC4AfQBcAG4AXABuACAAIAAgACAAIABBAFMAVABSAE8AXwBTAFAARQBDAFQAUgBBAEwAXwBEAEkAUwBUAFIASQBCAFUAVABJAE8ATgAoADUAMAAwADAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIACSISAAewBcACIAVABvAHQAYQBsAFwAIgAsACAAXAAiAE8AXAAiACwAIABcACIAQgBcACIALAAgAFwAIgBBAFwAIgAsACAAXAAiAEYAXAAiACwAIABcACIARwBcACIALAAgAFwAIgBLAFwAIgAsACAAXAAiAE0AXAAiAH0AIABwAGEAaQByAGUAZAAgAHcAaQB0AGgAIAByAG8AdQBuAGQAZQBkACAAaQBuAHQAZQBnAGUAcgBzAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgACAAIAAtACAAVABoAGUAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgAGkAcwAgAGIAYQBzAGUAZAAgAG8AbgAgAGkAbgB2AGUAcgBzAGUAIAB3AGUAaQBnAGgAdABpAG4AZwAgAGYAYQBjAHQAbwByAHMAOgBcAG4AIAAgACAAIAAgACAAIAAgACAATwA6ACAAMQAvADMAMAAwADAAMAAwADAAXABuACAAIAAgACAAIAAgACAAIAAgAEIAOgAgADEALwA4ADAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAQQA6ACAAMQAvADEANgAwAFwAbgAgACAAIAAgACAAIAAgACAAIABGADoAIAAxAC8AMwAzAFwAbgAgACAAIAAgACAAIAAgACAAIABHADoAIAAxAC8AMQAzAFwAbgAgACAAIAAgACAAIAAgACAAIABLADoAIAAxAC8AOABcAG4AIAAgACAAIAAgACAAIAAgACAATQA6ACAAMQAvADEALgAzADEANQAzAC4ALgAuAFwAbgAgACAAIAAgACAALQAgAFQAaABlAHMAZQAgAHYAYQBsAHUAZQBzACAAYQBwAHAAcgBvAHgAaQBtAGEAdABlACAAcgBlAGwAYQB0AGkAdgBlACAAZgByAGUAcQB1AGUAbgBjAHkAIABhAG4AZAAgAGEAYgB1AG4AZABhAG4AYwBlACAAbwBmACAAcwB0AGEAcgAgAHQAeQBwAGUAcwAuAFwAbgAgACAAIAAgACAALQAgAFwAIgBUAG8AdABhAGwAXAAiACAAaQBzACAAaQBuAGMAbAB1AGQAZQBkACAAYQBzACAAdABoAGUAIABmAGkAcgBzAHQAIAByAG8AdwAgAG8AZgAgAHQAaABlACAAbwB1AHQAcAB1AHQAIABmAG8AcgAgAGUAYQBzAHkAIABzAHUAbQBtAGEAdABpAG8AbgAvAGEAdQBkAGkAdAAuAFwAbgAgACAAIAAgACAALQAgAEkAbgB0AGUAbgBkAGUAZAAgAGYAbwByACAAdQBzAGUAIABpAG4AIABtAG8AZABlAGwAaQBuAGcAIABzAHQAYQByACAAcwB5AHMAdABlAG0AIABwAG8AcAB1AGwAYQB0AGkAbwBuAHMALAAgAGcAYQBsAGEAeAB5ACAAcwBlAGUAZABpAG4AZwAsACAAbwByACAAdABlAGEAYwBoAGkAbgBnACAAdABoAGUAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgAG8AZgAgAHMAdABlAGwAbABhAHIAIAB0AHkAcABlAHMALgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFMAUABFAEMAVABSAEEATABfAEQASQBTAFQAUgBJAEIAVQBUAEkATwBOACAAPQAgAEwAQQBNAEIARABBACgAWwBhAG4AYwBoAG8AcgBfAGMAbABhAHMAcwBdACwAIABbAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0AF0ALAAgAFsAZABlAGMAaQBtAGEAbABfAHAAbABhAGMAZQBzAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAPQA9AD0AIABEAGUAZgBhAHUAbAB0ACAAcABhAHIAYQBtAGUAdABlAHIAcwAgAD0APQA9AFwAbgAgACAAIAAgACAAIAAgACAAYQBuAGMAaABvAHIAXwBjAGwAYQBzAHMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAYQBuAGMAaABvAHIAXwBjAGwAYQBzAHMAKQAsACAAXAAiACQAXAAiACwAIABVAFAAUABFAFIAKABhAG4AYwBoAG8AcgBfAGMAbABhAHMAcwApACkALABcAG4AIAAgACAAIAAgACAAIAAgAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACkALAAgADEALAAgAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAGQAZQBjAGkAbQBhAGwAXwBwAGwAYQBjAGUAcwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBpAG0AYQBsAF8AcABsAGEAYwBlAHMAKQAsACAAMwAsACAAZABlAGMAaQBtAGEAbABfAHAAbABhAGMAZQBzACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAA9AD0APQAgAFMAcABlAGMAdAByAGEAbAAgAGMAbABhAHMAcwAgAGEAcgByAGEAeQAgAGEAbgBkACAAYgBhAHMAZQAgAGYAcgBlAHEAdQBlAG4AYwBpAGUAcwAgACgAZQBtAHAAaQByAGkAYwBhAGwAKQAgAD0APQA9AFwAbgAgACAAIAAgACAAIAAgACAAYQByAHIAXwBjAGwAYQBzAHMAZQBzACwAIAB7AFwAIgBPAFwAIgA7ACAAXAAiAEIAXAAiADsAIABcACIAQQBcACIAOwAgAFwAIgBGAFwAIgA7ACAAXAAiAEcAXAAiADsAIABcACIASwBcACIAOwAgAFwAIgBNAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABhAHIAcgBfAGIAYQBzAGUAXwBwAGMAdAAsACAAewAwAC4AMAAwADAAMAAzADsAIAAwAC4AMQAzADsAIAAwAC4ANgA7ACAAMwAuADAAOwAgADcALgA2ADsAIAAxADIALgAxADsAIAA3ADYALgAyADcAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAAQgBZAFIATwBXACgAYQByAHIAXwBiAGEAcwBlAF8AcABjAHQALAAgAEwAQQBNAEIARABBACgAeAAsACAAeAAgAC8AIAAxADAAMAApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAA9AD0APQAgAEwAbwBvAGsAdQBwACAAcwBjAGEAbABpAG4AZwAgAGYAYQBjAHQAbwByACAAZgBvAHIAIABhACAAcwBwAGUAYwBpAGYAaQBjACAAYQBuAGMAaABvAHIAIAB0AHkAcABlAFwAbgAgACAAIAAgACAAIAAgACAAYQBuAGMAaABvAHIAXwBmAHIAZQBxACwAIABYAEwATwBPAEsAVQBQACgAYQBuAGMAaABvAHIAXwBjAGwAYQBzAHMALAAgAGEAcgByAF8AYwBsAGEAcwBzAGUAcwAsACAAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIABzAGMAYQBsAGkAbgBnAF8AZgBhAGMAdABvAHIALAAgAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACAALwAgAGEAbgBjAGgAbwByAF8AZgByAGUAcQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAD0APQA9ACAAUwBjAGEAbABlAGQAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgABQgIABuAG8AcgBtAGEAbABpAHoAZQAgAG8AcgAgAGEAcABwAGwAeQAgAHUAcwBlAHIALQBkAGUAZgBpAG4AZQBkACAAcwBjAGEAbABlAFwAbgAgACAAIAAgACAAIAAgACAAcwBjAGEAbABlAGQALAAgAEkARgAoAGEAbgBjAGgAbwByAF8AYwBsAGEAcwBzACAAPQAgAFwAIgAkAFwAIgAsACAAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAAQgBZAFIATwBXACgAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAATABBAE0AQgBEAEEAKAB4ACwAIAB4ACAAKgAgAHMAYwBhAGwAaQBuAGcAXwBmAGEAYwB0AG8AcgApACkAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAD0APQA9ACAARgBpAG4AYQBsACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAsACAASABTAFQAQQBDAEsAKABhAHIAcgBfAGMAbABhAHMAcwBlAHMALAAgAFIATwBVAE4ARAAoAHMAYwBhAGwAZQBkACwAIABkAGUAYwBpAG0AYQBsAF8AcABsAGEAYwBlAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AQwBBAEwAQwBfAFQARQBNAFAAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6ACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaQBuAHQAZQByAHAAbwBsAGEAdABlAGQAIABlAGYAZgBlAGMAdABpAHYAZQAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgACgAaQBuACAASwBlAGwAdgBpAG4AKQAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAHMAdABlAGwAbABhAHIAIABzAHUAYgBjAGwAYQBzAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAZQAuAGcALgAgAFwAIgBHADcALgAzAFwAIgApACwAIAB1AHMAaQBuAGcAIABoAGEAcgBkAGMAbwBkAGUAZAAgAGgAaQBnAGgALQB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIABhAG4AYwBoAG8AcgBzACAAYQBuAGQAIABzAHAAYQBuACAAdgBhAGwAdQBlAHMAIABiAGUAdAB3AGUAZQBuACAAcwB1AGIAYwBsAGEAcwBzAGUAcwAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6ACAAQQAgAG4AdQBtAGUAcgBpAGMAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIABpAG4AIABLAGUAbAB2AGkAbgAsACAAaQBuAHQAZQByAHAAbwBsAGEAdABlAGQAIAB1AHMAaQBuAGcAIABsAGkAbgBlAGEAcgAgAHMAYwBhAGwAaQBuAGcAIAB3AGkAdABoAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABzAHUAYgBjAGwAYQBzAHMALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAHMAdQBiAGMAbABhAHMAcwAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAIABzAHQAcgBpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAYQAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAuACAAQQBjAGMAZQBwAHQAcwAgAGYAbwByAG0AYQB0AHMAIABsAGkAawBlACAAXAAiAEYANQBcACIALAAgAFwAIgBLADIALgA2AFwAIgAsACAAXAAiAE0AOAAuADkAXAAiACwAIABlAHQAYwAuAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABUAGUAbQBwAGUAcgBhAHQAdQByAGUAIABkAGEAdABhACAAaQBzACAAYgBhAHMAZQBkACAAbwBuACAAZQBtAHAAaQByAGkAYwBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIABhAG4AYwBoAG8AcgBzACAAZgBvAHIAIAB0AHkAcABlAHMAIABPADMAIAB0AGgAcgBvAHUAZwBoACAATQA5AC4AXABuACAAIAAgAC0AIABUAGgAZQAgAGYAdQBuAGMAdABpAG8AbgAgAHMAdQBwAHAAbwByAHQAcwAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIABpAG4AcAB1AHQAIABhAG4AZAAgAGEAcwBzAHUAbQBlAHMAIABsAGkAbgBlAGEAcgAgAGYAYQBsAGwAbwBmAGYAIABiAGUAdAB3AGUAZQBuACAAcwB1AGIAYwBsAGEAcwBzACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAYQBuAGMAaABvAHIAcwAuAFwAbgAgACAAIAAtACAAVABoAGUAIABoAGkAZwBoACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAKABgAFQAXwBoAGkAZwBoAGAAKQAgAGkAcwAgAHIAZQB0AHIAaQBlAHYAZQBkACAAZgBvAHIAIAB0AGgAZQAgAGIAYQBzAGUAIABzAHUAYgBjAGwAYQBzAHMAIAAoAGUALgBnAC4ALAAgAFwAIgBHADcAXAAiACkALAAgAGEAbgBkACAAaQBuAHQAZQByAHAAbwBsAGEAdABpAG8AbgAgAHUAcwBlAHMAOgBcAG4AIAAgACAAIAAgACAAIABUACAAPQAgAFQAXwBoAGkAZwBoACAALQAgACgAZgByAGEAYwB0AGkAbwBuACAAKgAgAHMAcABhAG4AKQBcAG4AIAAgACAALQAgAEgAYQBuAGQAbABlAHMAIABpAG4AcAB1AHQAcwAgAHcAaQB0AGgAIABvAHIAIAB3AGkAdABoAG8AdQB0ACAAYQAgAGQAZQBjAGkAbQBhAGwAIABwAG8AaQBuAHQAIAAoAGUALgBnAC4ALAAgAFwAIgBGADYAXAAiACAAPQAgAFwAIgBGADYALgAwAFwAIgApAC4AXABuACAAIAAgAC0AIABJAG4AdABlAHIAbgBhAGwAbAB5ACAAdQBzAGUAcwAgAFgATABPAE8ASwBVAFAAIABvAHYAZQByACAAYQAgAG0AYQB0AHIAaQB4ACAAYgB1AGkAbAB0ACAAZgByAG8AbQAgAGgAYQByAGQAYwBvAGQAZQBkACAAcwB1AGIAYwBsAGEAcwBzACAAbABhAGIAZQBsAHMALAAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQBzACwAIABhAG4AZAAgAHMAcABhAG4AcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBDAEEATABDAF8AVABFAE0AUAAoAFwAIgBHADcALgAzAFwAIgApACAAIAAgAJIhIAA1ADUAMgA5AFwAbgAgACAAIABBAFMAVABSAE8AXwBDAEEATABDAF8AVABFAE0AUAAoAFwAIgBPADQALgA0AFwAIgApACAAIAAgAJIhIAA0ADIAMwAwADAAXABuACAAIAAgAEEAUwBUAFIATwBfAEMAQQBMAEMAXwBUAEUATQBQACgAXAAiAEYAOAAuADQANQBcACIAKQAgACAAkiEgADYAMQAyADEALgA1AFwAbgAgACAAIABBAFMAVABSAE8AXwBDAEEATABDAF8AVABFAE0AUAAoAFwAIgBNADgALgA2AFwAIgApACAAIAAgAJIhIAAyADQANQA2AFwAbgAqAC8AXABuAFwAbgBcAG4AQQBTAFQAUgBPAF8AQwBBAEwAQwBfAFQARQBNAFAAIAA9ACAATABBAE0AQgBEAEEAKABzAHUAYgBjAGwAYQBzAHMALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAALQAtAC0AIABIAGEAcgBkAGMAbwBkAGUAZAAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAgAGEAcgByAGEAeQBzACAALQAtAC0AXABuAFwAbgAgACAAIAAgAGEAcgByAFQAeQBwAGUAcwAsACAAewBcAG4AIAAgACAAIAAgACAAXAAiAE8AMwBcACIAOwAgAFwAIgBPADQAXAAiADsAIABcACIATwA1AFwAIgA7ACAAXAAiAE8ANgBcACIAOwAgAFwAIgBPADcAXAAiADsAIABcACIATwA4AFwAIgA7ACAAXAAiAE8AOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEIAMABcACIAOwAgAFwAIgBCADEAXAAiADsAIABcACIAQgAyAFwAIgA7ACAAXAAiAEIAMwBcACIAOwAgAFwAIgBCADQAXAAiADsAIABcACIAQgA1AFwAIgA7ACAAXAAiAEIANgBcACIAOwAgAFwAIgBCADcAXAAiADsAIABcACIAQgA4AFwAIgA7ACAAXAAiAEIAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEEAMABcACIAOwAgAFwAIgBBADEAXAAiADsAIABcACIAQQAyAFwAIgA7ACAAXAAiAEEAMwBcACIAOwAgAFwAIgBBADQAXAAiADsAIABcACIAQQA1AFwAIgA7ACAAXAAiAEEANgBcACIAOwAgAFwAIgBBADcAXAAiADsAIABcACIAQQA4AFwAIgA7ACAAXAAiAEEAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEYAMABcACIAOwAgAFwAIgBGADEAXAAiADsAIABcACIARgAyAFwAIgA7ACAAXAAiAEYAMwBcACIAOwAgAFwAIgBGADQAXAAiADsAIABcACIARgA1AFwAIgA7ACAAXAAiAEYANgBcACIAOwAgAFwAIgBGADcAXAAiADsAIABcACIARgA4AFwAIgA7ACAAXAAiAEYAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEcAMABcACIAOwAgAFwAIgBHADEAXAAiADsAIABcACIARwAyAFwAIgA7ACAAXAAiAEcAMwBcACIAOwAgAFwAIgBHADQAXAAiADsAIABcACIARwA1AFwAIgA7ACAAXAAiAEcANgBcACIAOwAgAFwAIgBHADcAXAAiADsAIABcACIARwA4AFwAIgA7ACAAXAAiAEcAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEsAMABcACIAOwAgAFwAIgBLADEAXAAiADsAIABcACIASwAyAFwAIgA7ACAAXAAiAEsAMwBcACIAOwAgAFwAIgBLADQAXAAiADsAIABcACIASwA1AFwAIgA7ACAAXAAiAEsANgBcACIAOwAgAFwAIgBLADcAXAAiADsAIABcACIASwA4AFwAIgA7ACAAXAAiAEsAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAE0AMABcACIAOwAgAFwAIgBNADEAXAAiADsAIABcACIATQAyAFwAIgA7ACAAXAAiAE0AMwBcACIAOwAgAFwAIgBNADQAXAAiADsAIABcACIATQA1AFwAIgA7ACAAXAAiAE0ANgBcACIAOwAgAFwAIgBNADcAXAAiADsAIABcACIATQA4AFwAIgA7ACAAXAAiAE0AOQBcACIAXABuACAAIAAgACAAfQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABIAGkAZwBoACAAZQBmAGYAZQBjAHQAaQB2AGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAcwAgACgASwApACAAZgBvAHIAIABlAGEAYwBoACAAcwB1AGIAYwBsAGEAcwBzAFwAbgAgACAAIAAgAGEAcgByAFQASABpAGcAaAAsACAAewBcAG4AIAAgACAAIAAgACAANAA0ADkAMAAwADsAIAA0ADIAOQAwADAAOwAgADQAMQA0ADAAMAA7ACAAMwA5ADUAMAAwADsAIAAzADcAMQAwADAAOwAgADMANQAxADAAMAA7ACAAMwAzADMAMAAwADsAXABuACAAIAAgACAAIAAgADMAMQA0ADAAMAA7ACAAMgA2ADAAMAAwADsAIAAyADAANgAwADAAOwAgADEANwAwADAAMAA7ACAAMQA2ADQAMAAwADsAIAAxADUANwAwADAAOwAgADEANAA1ADAAMAA7ACAAMQA0ADAAMAAwADsAIAAxADIAMwAwADAAOwAgADEAMAA3ADAAMAA7AFwAbgAgACAAIAAgACAAIAA5ADcAMAAwADsAIAA5ADMAMAAwADsAIAA4ADgAMAAwADsAIAA4ADYAMAAwADsAIAA4ADIANQAwADsAIAA4ADEAMAAwADsAIAA3ADkAMQAwADsAIAA3ADcANgAwADsAIAA3ADUAOQAwADsAIAA3ADQAMAAwADsAXABuACAAIAAgACAAIAAgADcAMgAyADAAOwAgADcAMAAyADAAOwAgADYAOAAyADAAOwAgADYANwA1ADAAOwAgADYANgA3ADAAOwAgADYANQA1ADAAOwAgADYAMwA1ADAAOwAgADYAMgA4ADAAOwAgADYAMQA4ADAAOwBcAG4AIAAgACAAIAAgACAANgAwADUAMAA7ACAANQA5ADMAMAA7ACAANQA4ADYAMAA7ACAANQA3ADcAMAA7ACAANQA3ADIAMAA7ACAANQA2ADgAMAA7ACAANQA2ADYAMAA7ACAANQA2ADAAMAA7ACAANQA1ADUAMAA7ACAANQA0ADgAMAA7AFwAbgAgACAAIAAgACAAIAA1ADMAOAAwADsAIAA1ADIANwAwADsAIAA1ADEANwAwADsAIAA1ADEAMAAwADsAIAA0ADgAMwAwADsAIAA0ADYAMAAwADsAIAA0ADQANAAwADsAIAA0ADMAMAAwADsAIAA0ADEAMAAwADsAIAAzADkAOQAwADsAXABuACAAIAAgACAAIAAgADMAOQAzADAAOwAgADMAOAA1ADAAOwAgADMANgA2ADAAOwAgADMANQA2ADAAOwAgADMANAAzADAAOwAgADMAMgAxADAAOwAgADMAMAA2ADAAOwAgADIAOAAxADAAOwAgADIANgA4ADAAOwAgADIANQA3ADAAOwAgADIAMwA4ADAAXABuACAAIAAgACAAfQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABUAGUAbQBwAGUAcgBhAHQAdQByAGUAIABzAHAAYQBuACAAdABvACAAdABoAGUAIABuAGUAeAB0ACAAcwB1AGIAYwBsAGEAcwBzACAAKABLACkAXABuACAAIAAgACAAYQByAHIAUwBwAGEAbgAsACAAewBcAG4AIAAgACAAIAAgACAAMgAwADAAMAA7ACAAMQA1ADAAMAA7ACAAMQA5ADAAMAA7ACAAMgA0ADAAMAA7ACAAMgAwADAAMAA7ACAAMQA4ADAAMAA7ACAAMQA5ADAAMAA7AFwAbgAgACAAIAAgACAAIAA1ADQAMAAwADsAIAA1ADQAMAAwADsAIAAzADYAMAAwADsAIAA2ADAAMAA7ACAANwAwADAAOwAgADEAMgAwADAAOwAgADUAMAAwADsAIAAxADcAMAAwADsAIAAxADYAMAAwADsAIAAxADAAMAAwADsAXABuACAAIAAgACAAIAAgADQAMAAwADsAIAA1ADAAMAA7ACAAMgAwADAAOwAgADMANQAwADsAIAAxADUAMAA7ACAAMQA5ADAAOwAgADEANQAwADsAIAAxADcAMAA7ACAAMQA5ADAAOwAgADEAOAAwADsAXABuACAAIAAgACAAIAAgADIAMAAwADsAIAAyADAAMAA7ACAANwAwADsAIAA4ADAAOwAgADEAMgAwADsAIAAyADAAMAA7ACAANwAwADsAIAAxADAAMAA7ACAAMQAzADAAOwBcAG4AIAAgACAAIAAgACAAMQAyADAAOwAgADcAMAA7ACAAOQAwADsAIAA1ADAAOwAgADQAMAA7ACAAMgAwADsAIAA2ADAAOwAgADUAMAA7ACAANwAwADsAIAAxADAAMAA7AFwAbgAgACAAIAAgACAAIAAxADEAMAA7ACAAMQAwADAAOwAgADcAMAA7ACAAMgA3ADAAOwAgADIAMwAwADsAIAAxADYAMAA7ACAAMQA0ADAAOwAgADIAMAAwADsAIAAxADEAMAA7ACAANgAwADsAXABuACAAIAAgACAAIAAgADgAMAA7ACAAMQA5ADAAOwAgADEAMAAwADsAIAAxADMAMAA7ACAAMgAyADAAOwAgADEANQAwADsAIAAyADUAMAA7ACAAMQAzADAAOwAgADEAMQAwADsAIAAxADkAMAA7ACAAMgA4ADAAXABuACAAIAAgACAAfQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABCAHUAbgBkAGwAZQAgAGkAbgB0AG8AIABhACAAcwBpAG4AZwBsAGUAIABtAGEAdAByAGkAeAAgAGYAbwByACAAYwBsAGUAYQBuACAAbABvAG8AawB1AHAAXABuACAAIAAgACAAbQB0AHgAUwB0AGEAcgBzACwAIABIAFMAVABBAEMASwAoAGEAcgByAFQAeQBwAGUAcwAsACAAYQByAHIAVABIAGkAZwBoACwAIABhAHIAcgBTAHAAYQBuACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABJAG4AcAB1AHQAIABuAG8AcgBtAGEAbABpAHoAYQB0AGkAbwBuACAAYQBuAGQAIABwAGEAcgBzAGkAbgBnACAALQAtAC0AXABuAFwAbgAgACAAIAAgAG4AbwBfAHMAcABhAGMAZQAsACAAUwBVAEIAUwBUAEkAVABVAFQARQAoAHMAdQBiAGMAbABhAHMAcwAsACAAXAAiACAAXAAiACwAIABcACIAXAAiACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABUAHIAaQBtACAAdwBoAGkAdABlAHMAcABhAGMAZQBcAG4AIAAgACAAIABkAG8AdABfAHAAbwBzACwAIABGAEkATgBEACgAXAAiAC4AXAAiACwAIABuAG8AXwBzAHAAYQBjAGUAIAAmACAAXAAiAC4AMABcACIAKQAsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAARQBuAHMAdQByAGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGkAcwAgAGQAZQB0AGUAYwB0AGUAZAAgAGUAdgBlAG4AIABmAG8AcgAgAHcAaABvAGwAZQAgAHMAdQBiAGMAbABhAHMAcwBlAHMAXABuACAAIAAgACAAYgBhAHMAZQAsACAATABFAEYAVAAoAG4AbwBfAHMAcABhAGMAZQAsACAAZABvAHQAXwBwAG8AcwAgAC0AIAAxACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABFAHgAdAByAGEAYwB0ACAAcgBvAG8AdAAgAHMAdQBiAGMAbABhAHMAcwAsACAAZQAuAGcALgAsACAAXAAiAEcANwBcACIAIABmAHIAbwBtACAAXAAiAEcANwAuADMAXAAiAFwAbgAgACAAIAAgAGYALAAgAFYAQQBMAFUARQAoAFwAIgAwAC4AXAAiACAAJgAgAE0ASQBEACgAbgBvAF8AcwBwAGEAYwBlACwAIABkAG8AdABfAHAAbwBzACAAKwAgADEALAAgAEwARQBOACgAbgBvAF8AcwBwAGEAYwBlACkAKQApACwAIAAvAC8AIABDAG8AbgB2AGUAcgB0ACAAZABlAGMAaQBtAGEAbAAgAHMAdAByAGkAbgBnACAAdABvACAAbgB1AG0AZQByAGkAYwAgACgAZQAuAGcALgAsACAAMAAuADMAKQBcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABMAG8AbwBrAHUAcAAgAGgAaQBnAGgAIAB0AGUAbQBwACAAYQBuAGQAIABzAHAAYQBuACAAZgByAG8AbQAgAG0AYQB0AHIAaQB4ACAALQAtAC0AXABuAFwAbgAgACAAIAAgAFQAXwBoAGkAZwBoACwAIABYAEwATwBPAEsAVQBQACgAYgBhAHMAZQAsACAASQBOAEQARQBYACgAbQB0AHgAUwB0AGEAcgBzACwALAAxACkALAAgAEkATgBEAEUAWAAoAG0AdAB4AFMAdABhAHIAcwAsACwAMgApACkALAAgAC8ALwAgAGUALgBnAC4AIAA1ADUANQAwACAAZgBvAHIAIABcACIARwA3AFwAIgBcAG4AIAAgACAAIABzAHAAYQBuACwAIAAgACAAWABMAE8ATwBLAFUAUAAoAGIAYQBzAGUALAAgAEkATgBEAEUAWAAoAG0AdAB4AFMAdABhAHIAcwAsACwAMQApACwAIABJAE4ARABFAFgAKABtAHQAeABTAHQAYQByAHMALAAsADMAKQApACwAIAAvAC8AIABlAC4AZwAuACAANwAwACAAZgBvAHIAIABcACIARwA3AFwAIgBcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABJAG4AdABlAHIAcABvAGwAYQB0AGkAbwBuADoAIABUACAAPQAgAFQAXwBoAGkAZwBoACAALQAgAGYAIAAqACAAcwBwAGEAbgAgAC0ALQAtAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsACAAVABfAGgAaQBnAGgAIAAtACAAKABmACAAKgAgAHMAcABhAG4AKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFQAWQBQAEUAXwBGAFIATwBNAF8AVABFAE0AUAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AdABlAHIAcABvAGwAYQB0AGUAZAAgAHMAdABlAGwAbABhAHIAIABzAHAAZQBjAHQAcgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIAAoAGUALgBnAC4AIABcACIARwA3AC4AMwBcACIAKQAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAGUAZgBmAGUAYwB0AGkAdgBlACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAaQBuACAASwBlAGwAdgBpAG4ALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgAgAEEAIABzAHQAcgBpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAdABoAGUAIABlAHMAdABpAG0AYQB0AGUAZAAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAsACAAbwBwAHQAaQBvAG4AYQBsAGwAeQAgAHcAaQB0AGgAIABkAGUAYwBpAG0AYQBsACAAcAByAGUAYwBpAHMAaQBvAG4ALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAHQAZQBtAHAAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABBACAAbgB1AG0AZQByAGkAYwAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgAGkAbgAgAEsAZQBsAHYAaQBuAC4AXABuACAAIAAgAC0AIABkAGUAYwBpAG0AYQBsAHMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAGkAbgBjAGwAdQBkAGUAIABpAG4AIAB0AGgAZQAgAHMAdQBiAGMAbABhAHMAcwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAzACkALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAVABoAGUAIABmAHUAbgBjAHQAaQBvAG4AIABtAGEAdABjAGgAZQBzACAAdABoAGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAB0AG8AIAB0AGgAZQAgAGMAbwByAHIAZQBjAHQAIABzAHAAZQBjAHQAcgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIAByAGEAbgBnAGUAIABiAHkAIABjAGgAZQBjAGsAaQBuAGcAIAB3AGgAaQBjAGgAIABoAGkAZwBoAC0AdABlAG0AcAAgAGIAYQBuAGQAIABpAHQAIABmAGEAbABsAHMAIAB3AGkAdABoAGkAbgAuAFwAbgAgACAAIAAtACAASQB0ACAAdABoAGUAbgAgAGwAaQBuAGUAYQByAGwAeQAgAGkAbgB0AGUAcgBwAG8AbABhAHQAZQBzACAAdABoAGUAIABkAGUAYwBpAG0AYQBsACAAcABvAHIAdABpAG8AbgAgAG8AZgAgAHQAaABlACAAcwB1AGIAYwBsAGEAcwBzACAAdQBzAGkAbgBnADoAXABuACAAIAAgACAAIAAgACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAD0AIAAoAFQAXwBoAGkAZwBoACAALQAgAHQAZQBtAHAAKQAgAC8AIABzAHAAYQBuAFwAbgAgACAAIAAtACAAVQBzAGUAcwAgAGgAYQByAGQAYwBvAGQAZQBkACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAYQBuAGMAaABvAHIAcwAgAGEAbgBkACAAcwBwAGEAbgBzACAAYQBjAHIAbwBzAHMAIABzAHAAZQBjAHQAcgBhAGwAIAB0AHkAcABlAHMAIABPADMAEyBNADkALgBcAG4AIAAgACAALQAgAFMAdQBwAHAAbwByAHQAcwAgAGgAaQBnAGgAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGEAbgBkACAAbgBvAHIAbQBhAGwAaQB6AGEAdABpAG8AbgAgAGYAbwByACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHMAdQBiAGMAbABhAHMAcwBlAHMAIABsAGkAawBlACAAXAAiAEsANAAuADMANwA2AFwAIgAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBUAFkAUABFAF8ARgBSAE8ATQBfAFQARQBNAFAAKAA0ADIAMwAwADAAKQAgACAAIACSISAAXAAiAE8ANAAuADQAMAAwAFwAIgBcAG4AIAAgACAAQQBTAFQAUgBPAF8AVABZAFAARQBfAEYAUgBPAE0AXwBUAEUATQBQACgANQA1ADIAOQApACAAIAAgACAAkiEgAFwAIgBHADcALgAzADAAMABcACIAXABuACAAIAAgAEEAUwBUAFIATwBfAFQAWQBQAEUAXwBGAFIATwBNAF8AVABFAE0AUAAoADYAMQAyADEALgA1ACkAIAAgAJIhIABcACIARgA4AC4ANAA1ADAAXAAiAFwAbgAgACAAIABBAFMAVABSAE8AXwBUAFkAUABFAF8ARgBSAE8ATQBfAFQARQBNAFAAKAAyADQANQA2ACwAIAAxACkAIACSISAAXAAiAE0AOAAuADYAXAAiAFwAbgBcAG4AIAAgACAARABlAHAAZQBuAGQAZQBuAGMAaQBlAHMAOgBcAG4AIAAgACAALQAgAFUAcwBlAHMAIABYAE0AQQBUAEMASAAgACsAIABNAEEAUAAgAGYAbwByACAAbABvAGcAaQBjAGEAbAAgAHIAYQBuAGcAZQAgAGQAZQB0AGUAYwB0AGkAbwBuAC4AXABuACAAIAAgAC0AIABBAHMAcwB1AG0AZQBzACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAZABlAGMAcgBlAGEAcwBlAHMAIABtAG8AbgBvAHQAbwBuAGkAYwBhAGwAbAB5ACAAYQBjAHIAbwBzAHMAIABzAHUAYgBjAGwAYQBzAHMAIABzAGUAcQB1AGUAbgBjAGUALgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFQAWQBQAEUAXwBGAFIATwBNAF8AVABFAE0AUAAgAD0AIABMAEEATQBCAEQAQQAoAHQAZQBtAHAALAAgAFsAZABlAGMAaQBtAGEAbABzAF0ALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAALQAtAC0AIABIAGEAcgBkAGMAbwBkAGUAZAAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAgAGQAYQB0AGEAIAAtAC0ALQBcAG4AIAAgACAAIABhAHIAcgBUAHkAcABlAHMALAAgAHsAXABuACAAIAAgACAAIAAgAFwAIgBPADMAXAAiADsAIABcACIATwA0AFwAIgA7ACAAXAAiAE8ANQBcACIAOwAgAFwAIgBPADYAXAAiADsAIABcACIATwA3AFwAIgA7ACAAXAAiAE8AOABcACIAOwAgAFwAIgBPADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBCADAAXAAiADsAIABcACIAQgAxAFwAIgA7ACAAXAAiAEIAMgBcACIAOwAgAFwAIgBCADMAXAAiADsAIABcACIAQgA0AFwAIgA7ACAAXAAiAEIANQBcACIAOwAgAFwAIgBCADYAXAAiADsAIABcACIAQgA3AFwAIgA7ACAAXAAiAEIAOABcACIAOwAgAFwAIgBCADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBBADAAXAAiADsAIABcACIAQQAxAFwAIgA7ACAAXAAiAEEAMgBcACIAOwAgAFwAIgBBADMAXAAiADsAIABcACIAQQA0AFwAIgA7ACAAXAAiAEEANQBcACIAOwAgAFwAIgBBADYAXAAiADsAIABcACIAQQA3AFwAIgA7ACAAXAAiAEEAOABcACIAOwAgAFwAIgBBADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBGADAAXAAiADsAIABcACIARgAxAFwAIgA7ACAAXAAiAEYAMgBcACIAOwAgAFwAIgBGADMAXAAiADsAIABcACIARgA0AFwAIgA7ACAAXAAiAEYANQBcACIAOwAgAFwAIgBGADYAXAAiADsAIABcACIARgA3AFwAIgA7ACAAXAAiAEYAOABcACIAOwAgAFwAIgBGADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBHADAAXAAiADsAIABcACIARwAxAFwAIgA7ACAAXAAiAEcAMgBcACIAOwAgAFwAIgBHADMAXAAiADsAIABcACIARwA0AFwAIgA7ACAAXAAiAEcANQBcACIAOwAgAFwAIgBHADYAXAAiADsAIABcACIARwA3AFwAIgA7ACAAXAAiAEcAOABcACIAOwAgAFwAIgBHADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBLADAAXAAiADsAIABcACIASwAxAFwAIgA7ACAAXAAiAEsAMgBcACIAOwAgAFwAIgBLADMAXAAiADsAIABcACIASwA0AFwAIgA7ACAAXAAiAEsANQBcACIAOwAgAFwAIgBLADYAXAAiADsAIABcACIASwA3AFwAIgA7ACAAXAAiAEsAOABcACIAOwAgAFwAIgBLADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBNADAAXAAiADsAIABcACIATQAxAFwAIgA7ACAAXAAiAE0AMgBcACIAOwAgAFwAIgBNADMAXAAiADsAIABcACIATQA0AFwAIgA7ACAAXAAiAE0ANQBcACIAOwAgAFwAIgBNADYAXAAiADsAIABcACIATQA3AFwAIgA7ACAAXAAiAE0AOABcACIAOwAgAFwAIgBNADkAXAAiAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAAYQByAHIAVABIAGkAZwBoACwAIAB7AFwAbgAgACAAIAAgACAAIAA0ADQAOQAwADAAOwAgADQAMgA5ADAAMAA7ACAANAAxADQAMAAwADsAIAAzADkANQAwADAAOwAgADMANwAxADAAMAA7ACAAMwA1ADEAMAAwADsAIAAzADMAMwAwADAAOwBcAG4AIAAgACAAIAAgACAAMwAxADQAMAAwADsAIAAyADYAMAAwADAAOwAgADIAMAA2ADAAMAA7ACAAMQA3ADAAMAAwADsAIAAxADYANAAwADAAOwAgADEANQA3ADAAMAA7ACAAMQA0ADUAMAAwADsAIAAxADQAMAAwADAAOwAgADEAMgAzADAAMAA7ACAAMQAwADcAMAAwADsAXABuACAAIAAgACAAIAAgADkANwAwADAAOwAgADkAMwAwADAAOwAgADgAOAAwADAAOwAgADgANgAwADAAOwAgADgAMgA1ADAAOwAgADgAMQAwADAAOwAgADcAOQAxADAAOwAgADcANwA2ADAAOwAgADcANQA5ADAAOwAgADcANAAwADAAOwBcAG4AIAAgACAAIAAgACAANwAyADIAMAA7ACAANwAwADIAMAA7ACAANgA4ADIAMAA7ACAANgA3ADUAMAA7ACAANgA2ADcAMAA7ACAANgA1ADUAMAA7ACAANgAzADUAMAA7ACAANgAyADgAMAA7ACAANgAxADgAMAA7AFwAbgAgACAAIAAgACAAIAA2ADAANQAwADsAIAA1ADkAMwAwADsAIAA1ADgANgAwADsAIAA1ADcANwAwADsAIAA1ADcAMgAwADsAIAA1ADYAOAAwADsAIAA1ADYANgAwADsAIAA1ADYAMAAwADsAIAA1ADUANQAwADsAIAA1ADQAOAAwADsAXABuACAAIAAgACAAIAAgADUAMwA4ADAAOwAgADUAMgA3ADAAOwAgADUAMQA3ADAAOwAgADUAMQAwADAAOwAgADQAOAAzADAAOwAgADQANgAwADAAOwAgADQANAA0ADAAOwAgADQAMwAwADAAOwAgADQAMQAwADAAOwAgADMAOQA5ADAAOwBcAG4AIAAgACAAIAAgACAAMwA5ADMAMAA7ACAAMwA4ADUAMAA7ACAAMwA2ADYAMAA7ACAAMwA1ADYAMAA7ACAAMwA0ADMAMAA7ACAAMwAyADEAMAA7ACAAMwAwADYAMAA7ACAAMgA4ADEAMAA7ACAAMgA2ADgAMAA7ACAAMgA1ADcAMAA7ACAAMgAzADgAMABcAG4AIAAgACAAIAB9ACwAXABuAFwAbgAgACAAIAAgAGEAcgByAFMAcABhAG4ALAAgAHsAXABuACAAIAAgACAAIAAgADIAMAAwADAAOwAgADEANQAwADAAOwAgADEAOQAwADAAOwAgADIANAAwADAAOwAgADIAMAAwADAAOwAgADEAOAAwADAAOwAgADEAOQAwADAAOwBcAG4AIAAgACAAIAAgACAANQA0ADAAMAA7ACAANQA0ADAAMAA7ACAAMwA2ADAAMAA7ACAANgAwADAAOwAgADcAMAAwADsAIAAxADIAMAAwADsAIAA1ADAAMAA7ACAAMQA3ADAAMAA7ACAAMQA2ADAAMAA7ACAAMQAwADAAMAA7AFwAbgAgACAAIAAgACAAIAA0ADAAMAA7ACAANQAwADAAOwAgADIAMAAwADsAIAAzADUAMAA7ACAAMQA1ADAAOwAgADEAOQAwADsAIAAxADUAMAA7ACAAMQA3ADAAOwAgADEAOQAwADsAIAAxADgAMAA7AFwAbgAgACAAIAAgACAAIAAyADAAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAOAAwADsAIAAxADIAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAMQAwADAAOwAgADEAMwAwADsAXABuACAAIAAgACAAIAAgADEAMgAwADsAIAA3ADAAOwAgADkAMAA7ACAANQAwADsAIAA0ADAAOwAgADIAMAA7ACAANgAwADsAIAA1ADAAOwAgADcAMAA7ACAAMQAwADAAOwBcAG4AIAAgACAAIAAgACAAMQAxADAAOwAgADEAMAAwADsAIAA3ADAAOwAgADIANwAwADsAIAAyADMAMAA7ACAAMQA2ADAAOwAgADEANAAwADsAIAAyADAAMAA7ACAAMQAxADAAOwAgADYAMAA7AFwAbgAgACAAIAAgACAAIAA4ADAAOwAgADEAOQAwADsAIAAxADAAMAA7ACAAMQAzADAAOwAgADIAMgAwADsAIAAxADUAMAA7ACAAMgA1ADAAOwAgADEAMwAwADsAIAAxADEAMAA7ACAAMQA5ADAAOwAgADIAOAAwAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABEAGUAdABlAHIAbQBpAG4AZQAgAG0AYQB0AGMAaAAgAGkAbgBkAGUAeAAgAC0ALQAtAFwAbgAgACAAIAAgAHQAZQBtAHAAXwBpAG4AXwByAGEAbgBnAGUALABcAG4AIAAgACAAIAAgACAATQBBAFAAKABTAEUAUQBVAEUATgBDAEUAKABSAE8AVwBTACgAYQByAHIAVABIAGkAZwBoACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABpACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAQQBOAEQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAYQByAHIAVABIAGkAZwBoACwAIABpACkAIAA+AD0AIAB0AGUAbQBwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHQAZQBtAHAAIAA+ACAASQBOAEQARQBYACgAYQByAHIAVABIAGkAZwBoACwAIABpACkAIAAtACAASQBOAEQARQBYACgAYQByAHIAUwBwAGEAbgAsACAAaQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAaQBkAHgALAAgAFgATQBBAFQAQwBIACgAVABSAFUARQAsACAAdABlAG0AcABfAGkAbgBfAHIAYQBuAGcAZQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAATABvAG8AawB1AHAAIAB0AHkAcABlACAAYQBuAGQAIABjAG8AbQBwAHUAdABlACAAZgByAGEAYwB0AGkAbwBuACAALQAtAC0AXABuACAAIAAgACAAZgB1AGwAbABfAHQAeQBwAGUALAAgAEkATgBEAEUAWAAoAGEAcgByAFQAeQBwAGUAcwAsACAAaQBkAHgAKQAsAFwAbgAgACAAIAAgAFQAXwBoAGkAZwBoACwAIABJAE4ARABFAFgAKABhAHIAcgBUAEgAaQBnAGgALAAgAGkAZAB4ACkALABcAG4AIAAgACAAIABzAHAAYQBuACwAIABJAE4ARABFAFgAKABhAHIAcgBTAHAAYQBuACwAIABpAGQAeAApACwAXABuACAAIAAgACAAZgAsACAAKABUAF8AaABpAGcAaAAgAC0AIAB0AGUAbQBwACkAIAAvACAAcwBwAGEAbgAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIAAtAC0ALQAgAEYAbwByAG0AYQB0ACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIAAtAC0ALQBcAG4AIAAgACAAIABkAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBpAG0AYQBsAHMAKQAsACAAMwAsACAAZABlAGMAaQBtAGEAbABzACkALABcAG4AIAAgACAAIABmAG8AcgBtAGEAdABfAHMAdAByAGkAbgBnACwAIABcACIALgBcACIAIAAmACAAUgBFAFAAVAAoAFwAIgAwAFwAIgAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgAHMAdQBiAGMAbABhAHMAcwAsACAAZgB1AGwAbABfAHQAeQBwAGUAIAAmACAAVABFAFgAVAAoAGYALAAgAGYAbwByAG0AYQB0AF8AcwB0AHIAaQBuAGcAKQAsAFwAbgBcAG4AIAAgACAAIABzAHUAYgBjAGwAYQBzAHMAXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8ARABJAFMAUABMAEEAWQBfAFMAUABFAEMAVABSAEEATAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABEAGkAcwBwAGwAYQB5AHMAIABzAHAAZQBjAHQAcgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIABhAG4AZAAgAHMAcABhAG4AIABkAGEAdABhACAAYQBjAHIAbwBzAHMAIABzAHQAZQBsAGwAYQByACAAYwBsAGEAcwBzAGkAZgBpAGMAYQB0AGkAbwBuAHMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBhAG4AIAByAGUAdAB1AHIAbgAgAGUAaQB0AGgAZQByACAAdABoAGUAIABmAHUAbABsACAAcwBwAGUAYwB0AHIAYQBsACAAbQBhAHQAcgBpAHgAIAAoAE8AMwATIE0AOQApACAAbwByACAAYQAgAGYAaQBsAHQAZQByAGUAZAAgAHQAdwBvAC0AYwBvAGwAdQBtAG4AIAB2AGkAZQB3AC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAIABcAG4AIAAgACAALQAgAEkAZgAgAHQAeQBwAGUAIABpAHMAIABvAG0AaQB0AHQAZQBkADoAIABXAGkAZABlACAAbQBhAHQAcgBpAHgAIABvAGYAIABzAHAAZQBjAHQAcgBhAGwAIABjAGwAYQBzAHMAZQBzACAAKABPACAAdABvACAATQApACwAIAAxADAAIABzAHUAYgBjAGwAYQBzAHMAZQBzACAAZQBhAGMAaABcAG4AIAAgACAALQAgAEkAZgAgAHQAeQBwAGUAIABpAHMAIABwAHIAbwB2AGkAZABlAGQAOgAgAFQAdwBvAC0AYwBvAGwAdQBtAG4AIAB0AGEAYgBsAGUAIAB3AGkAdABoACAAVABlAG0AcABlAHIAYQB0AHUAcgBlACAAYQBuAGQAIABTAHAAYQBuACAAZgBvAHIAIAB0AGgAZQAgAHIAZQBxAHUAZQBzAHQAZQBkACAAYwBsAGEAcwBzAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAdAB5AHAAZQAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AbgBlACAAbwBmACAAewBcACIATwBcACIALABcACIAQgBcACIALABcACIAQQBcACIALABcACIARgBcACIALABcACIARwBcACIALABcACIASwBcACIALABcACIATQBcACIAfQAgAHQAbwAgAGwAaQBtAGkAdAAgAG8AdQB0AHAAdQB0ACAAdABvACAAdABoAGEAdAAgAHMAcABlAGMAdAByAGEAbAAgAGcAcgBvAHUAcABcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAVABlAG0AcABlAHIAYQB0AHUAcgBlAHMAIABhAHIAZQAgAGgAaQBnAGgALQBlAG4AZAAgAHYAYQBsAHUAZQBzACAAZgBvAHIAIABlAGEAYwBoACAAcwB1AGIAYwBsAGEAcwBzACAAKAByAGUAYQBsAC0AdwBvAHIAbABkACAAaQBuAHMAcABpAHIAZQBkACwAIABzAG0AbwBvAHQAaABlAGQAIABkAGEAdABhACkALgBcAG4AIAAgACAALQAgAFMAcABhAG4AIABpAHMAIAB0AGgAZQAgAEsAZQBsAHYAaQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABhACAAcwB1AGIAYwBsAGEAcwBzACAAYQBuAGQAIAB0AGgAZQAgAG4AZQB4AHQAIABjAG8AbwBsAGUAcgAgAG8AbgBlAC4AXABuACAAIAAgAC0AIABJAGYAIABuAG8AIAB0AHkAcABlACAAaQBzACAAcwBwAGUAYwBpAGYAaQBlAGQALAAgAG8AdQB0AHAAdQB0ACAAaQBzACAAbwByAGcAYQBuAGkAegBlAGQAIABhAHMAIABhACAAdgBpAHMAdQBhAGwAIAByAGUAZgBlAHIAZQBuAGMAZQAgAHQAYQBiAGwAZQAuAFwAbgAgACAAIAAtACAAVQBzAGUAcwAgAFYAUwBUAEEAQwBLACAAYQBuAGQAIABIAFMAVABBAEMASwAgAGkAbgB0AGUAcgBuAGEAbABsAHkAIABmAG8AcgAgAGMAbABlAGEAbgAgAHMAdAByAHUAYwB0AHUAcgBlADsAIAByAGUAcABsAGEAYwBlAHMAIABwAHIAZQB2AGkAbwB1AHMAIABzAGUAcABhAHIAYQB0AGUAZAAgAHYAZQByAHMAaQBvAG4AcwAuAFwAbgAgACAAIAAtACAAVABoAGkAcwAgAGYAdQBuAGMAdABpAG8AbgAgAHMAdQBwAGUAcgBzAGUAZABlAHMAOgAgAEEAUwBUAFIATwBfAEQASQBTAFAATABBAFkAXwBCAEEAUwBFAF8ARABBAFQAQQAsACAAXwBTAEUAUABBAFIAQQBUAEUARAAsACAAYQBuAGQAIABfAEIAWQBfAFQAWQBQAEUALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8ARABJAFMAUABMAEEAWQBfAFMAUABFAEMAVABSAEEATAAoACkAIAAgACAAIAAgACAAIAAgAJIhIABSAGUAdAB1AHIAbgBzACAAZgB1AGwAbAAgAE8AMwATIE0AOQAgAHMAdQBiAGMAbABhAHMAcwAgAGMAaABhAHIAdABcAG4AIAAgACAAQQBTAFQAUgBPAF8ARABJAFMAUABMAEEAWQBfAFMAUABFAEMAVABSAEEATAAoAFwAIgBHAFwAIgApACAAIAAgACAAIACSISAAUgBlAHQAdQByAG4AcwAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgAGEAbgBkACAAcwBwAGEAbgAgAGYAbwByACAARwAwABMgRwA5AFwAbgAgACAAIABBAFMAVABSAE8AXwBEAEkAUwBQAEwAQQBZAF8AUwBQAEUAQwBUAFIAQQBMACgAXAAiAEYAXAAiACkAIAAgACAAIAAgAJIhIABGADAAEyBGADkAIABjAGwAYQBzAHMAaQBmAGkAYwBhAHQAaQBvAG4AIABtAGUAdAByAGkAYwBzAFwAbgAqAC8AXABuAFwAbgBBAFMAVABSAE8AXwBEAEkAUwBQAEwAQQBZAF8AUwBQAEUAQwBUAFIAQQBMACAAPQAgAEwAQQBNAEIARABBACgAWwB0AHkAcABlAF0ALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAALQAtAC0AIABEAGUAZgBpAG4AZQAgAHMAcABlAGMAdAByAGEAbAAgAHQAeQBwAGUAcwAgAGEAbgBkACAAYgB1AGkAbABkACAAaABlAGwAcABlAHIAcwAgAC0ALQAtAFwAbgAgACAAIAAgAFQAeQBwAGUAcwAsACAAewBcACIATwBcACIAOwBcACIAQgBcACIAOwBcACIAQQBcACIAOwBcACIARgBcACIAOwBcACIARwBcACIAOwBcACIASwBcACIAOwBcACIATQBcACIAfQAsAFwAbgAgACAAIAAgAEgAZQBhAGQAZQByAHMALAAgAFQAUgBBAE4AUwBQAE8AUwBFACgAVgBTAFQAQQBDAEsAKABcACIAIABcACIALAAgAFQAeQBwAGUAcwApACkALABcAG4AIAAgACAAIABGAGkAbgBkAEMAbwBsACwAIABNAEEASwBFAEEAUgBSAEEAWQAoAEMATwBVAE4AVABBACgAVAB5AHAAZQBzACkALAAgADIALAAgAEwAQQBNAEIARABBACgAcgAsACAAYwAsACAASQBGACgAYwAgAD0AIAAxACwAIABJAE4ARABFAFgAKABUAHkAcABlAHMALAAgAHIAKQAsACAAcgApACkAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIAAtAC0ALQAgAFIAYQB3ACAAcwB0AGEAcgAgAHMAdQBiAGMAbABhAHMAcwAgAGQAYQB0AGEAIAAtAC0ALQBcAG4AIAAgACAAIABhAHIAcgBUAHkAcABlAHMALAAgAHsAXABuACAAIAAgACAAIAAgAFwAIgBPAFwAIgA7ACAAXAAiAE8AXAAiADsAIABcACIATwBcACIAOwAgAFwAIgBPADMAXAAiADsAIABcACIATwA0AFwAIgA7ACAAXAAiAE8ANQBcACIAOwAgAFwAIgBPADYAXAAiADsAIABcACIATwA3AFwAIgA7ACAAXAAiAE8AOABcACIAOwAgAFwAIgBPADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBCADAAXAAiADsAIABcACIAQgAxAFwAIgA7ACAAXAAiAEIAMgBcACIAOwAgAFwAIgBCADMAXAAiADsAIABcACIAQgA0AFwAIgA7ACAAXAAiAEIANQBcACIAOwAgAFwAIgBCADYAXAAiADsAIABcACIAQgA3AFwAIgA7ACAAXAAiAEIAOABcACIAOwAgAFwAIgBCADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBBADAAXAAiADsAIABcACIAQQAxAFwAIgA7ACAAXAAiAEEAMgBcACIAOwAgAFwAIgBBADMAXAAiADsAIABcACIAQQA0AFwAIgA7ACAAXAAiAEEANQBcACIAOwAgAFwAIgBBADYAXAAiADsAIABcACIAQQA3AFwAIgA7ACAAXAAiAEEAOABcACIAOwAgAFwAIgBBADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBGADAAXAAiADsAIABcACIARgAxAFwAIgA7ACAAXAAiAEYAMgBcACIAOwAgAFwAIgBGADMAXAAiADsAIABcACIARgA0AFwAIgA7ACAAXAAiAEYANQBcACIAOwAgAFwAIgBGADYAXAAiADsAIABcACIARgA3AFwAIgA7ACAAXAAiAEYAOABcACIAOwAgAFwAIgBGADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBHADAAXAAiADsAIABcACIARwAxAFwAIgA7ACAAXAAiAEcAMgBcACIAOwAgAFwAIgBHADMAXAAiADsAIABcACIARwA0AFwAIgA7ACAAXAAiAEcANQBcACIAOwAgAFwAIgBHADYAXAAiADsAIABcACIARwA3AFwAIgA7ACAAXAAiAEcAOABcACIAOwAgAFwAIgBHADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBLADAAXAAiADsAIABcACIASwAxAFwAIgA7ACAAXAAiAEsAMgBcACIAOwAgAFwAIgBLADMAXAAiADsAIABcACIASwA0AFwAIgA7ACAAXAAiAEsANQBcACIAOwAgAFwAIgBLADYAXAAiADsAIABcACIASwA3AFwAIgA7ACAAXAAiAEsAOABcACIAOwAgAFwAIgBLADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBNADAAXAAiADsAIABcACIATQAxAFwAIgA7ACAAXAAiAE0AMgBcACIAOwAgAFwAIgBNADMAXAAiADsAIABcACIATQA0AFwAIgA7ACAAXAAiAE0ANQBcACIAOwAgAFwAIgBNADYAXAAiADsAIABcACIATQA3AFwAIgA7ACAAXAAiAE0AOABcACIAOwAgAFwAIgBNADkAXAAiAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAAYQByAHIAVABIAGkAZwBoACwAIAB7AFwAbgAgACAAIAAgACAAIABcACIAXAAiADsAIABcACIAXAAiADsAIABcACIAXAAiADsAIAA0ADQAOQAwADAAOwAgADQAMgA5ADAAMAA7ACAANAAxADQAMAAwADsAIAAzADkANQAwADAAOwAgADMANwAxADAAMAA7ACAAMwA1ADEAMAAwADsAIAAzADMAMwAwADAAOwBcAG4AIAAgACAAIAAgACAAMwAxADQAMAAwADsAIAAyADYAMAAwADAAOwAgADIAMAA2ADAAMAA7ACAAMQA3ADAAMAAwADsAIAAxADYANAAwADAAOwAgADEANQA3ADAAMAA7ACAAMQA0ADUAMAAwADsAIAAxADQAMAAwADAAOwAgADEAMgAzADAAMAA7ACAAMQAwADcAMAAwADsAXABuACAAIAAgACAAIAAgADkANwAwADAAOwAgADkAMwAwADAAOwAgADgAOAAwADAAOwAgADgANgAwADAAOwAgADgAMgA1ADAAOwAgADgAMQAwADAAOwAgADcAOQAxADAAOwAgADcANwA2ADAAOwAgADcANQA5ADAAOwAgADcANAAwADAAOwBcAG4AIAAgACAAIAAgACAANwAyADIAMAA7ACAANwAwADIAMAA7ACAANgA4ADIAMAA7ACAANgA3ADUAMAA7ACAANgA2ADcAMAA7ACAANgA1ADUAMAA7ACAANgAzADUAMAA7ACAANgAyADgAMAA7ACAANgAxADgAMAA7AFwAbgAgACAAIAAgACAAIAA2ADAANQAwADsAIAA1ADkAMwAwADsAIAA1ADgANgAwADsAIAA1ADcANwAwADsAIAA1ADcAMgAwADsAIAA1ADYAOAAwADsAIAA1ADYANgAwADsAIAA1ADYAMAAwADsAIAA1ADUANQAwADsAIAA1ADQAOAAwADsAXABuACAAIAAgACAAIAAgADUAMwA4ADAAOwAgADUAMgA3ADAAOwAgADUAMQA3ADAAOwAgADUAMQAwADAAOwAgADQAOAAzADAAOwAgADQANgAwADAAOwAgADQANAA0ADAAOwAgADQAMwAwADAAOwAgADQAMQAwADAAOwAgADMAOQA5ADAAOwBcAG4AIAAgACAAIAAgACAAMwA5ADMAMAA7ACAAMwA4ADUAMAA7ACAAMwA2ADYAMAA7ACAAMwA1ADYAMAA7ACAAMwA0ADMAMAA7ACAAMwAyADEAMAA7ACAAMwAwADYAMAA7ACAAMgA4ADEAMAA7ACAAMgA2ADgAMAA7ACAAMgA1ADcAMAA7ACAAMgAzADgAMABcAG4AIAAgACAAIAB9ACwAXABuAFwAbgAgACAAIAAgAGEAcgByAFMAcABhAG4ALAAgAHsAXABuACAAIAAgACAAIAAgAFwAIgBcACIAOwAgAFwAIgBcACIAOwAgAFwAIgBcACIAOwAgADIAMAAwADAAOwAgADEANQAwADAAOwAgADEAOQAwADAAOwAgADIANAAwADAAOwAgADIAMAAwADAAOwAgADEAOAAwADAAOwAgADEAOQAwADAAOwBcAG4AIAAgACAAIAAgACAANQA0ADAAMAA7ACAANQA0ADAAMAA7ACAAMwA2ADAAMAA7ACAANgAwADAAOwAgADcAMAAwADsAIAAxADIAMAAwADsAIAA1ADAAMAA7ACAAMQA3ADAAMAA7ACAAMQA2ADAAMAA7ACAAMQAwADAAMAA7AFwAbgAgACAAIAAgACAAIAA0ADAAMAA7ACAANQAwADAAOwAgADIAMAAwADsAIAAzADUAMAA7ACAAMQA1ADAAOwAgADEAOQAwADsAIAAxADUAMAA7ACAAMQA3ADAAOwAgADEAOQAwADsAIAAxADgAMAA7AFwAbgAgACAAIAAgACAAIAAyADAAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAOAAwADsAIAAxADIAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAMQAwADAAOwAgADEAMwAwADsAXABuACAAIAAgACAAIAAgADEAMgAwADsAIAA3ADAAOwAgADkAMAA7ACAANQAwADsAIAA0ADAAOwAgADIAMAA7ACAANgAwADsAIAA1ADAAOwAgADcAMAA7ACAAMQAwADAAOwBcAG4AIAAgACAAIAAgACAAMQAxADAAOwAgADEAMAAwADsAIAA3ADAAOwAgADIANwAwADsAIAAyADMAMAA7ACAAMQA2ADAAOwAgADEANAAwADsAIAAyADAAMAA7ACAAMQAxADAAOwAgADYAMAA7AFwAbgAgACAAIAAgACAAIAA4ADAAOwAgADEAOQAwADsAIAAxADAAMAA7ACAAMQAzADAAOwAgADIAMgAwADsAIAAxADUAMAA7ACAAMgA1ADAAOwAgADEAMwAwADsAIAAxADEAMAA7ACAAMQA5ADAAOwAgADIAOAAwAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABJAGYAIABuAG8AIAB0AHkAcABlACAAaQBzACAAcwBwAGUAYwBpAGYAaQBlAGQALAAgAGQAaQBzAHAAbABhAHkAIABmAHUAbABsACAAdABhAGIAbABlACAALQAtAC0AXABuACAAIAAgACAAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAAQgBZAFIATwBXACgASABTAFQAQQBDAEsAKABhAHIAcgBUAHkAcABlAHMALAAgAGEAcgByAFQASABpAGcAaAAsACAAYQByAHIAUwBwAGEAbgApACwAXABuACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAcgBvAHcALAAgAFQARQBYAFQASgBPAEkATgAoAFwAIgA7ACAAXAAiACwAIABUAFIAVQBFACwAIABUAEUAWABUACgASQBOAEQARQBYACgAcgBvAHcALAAgADIAKQAsACAAXAAiADAAXAAiACkALAAgAFQARQBYAFQAKABJAE4ARABFAFgAKAByAG8AdwAsACAAMwApACwAIABcACIAMABcACIAKQApACkAXABuACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIABOAHUAbQBiAGUAcgBzACwAIABTAEUAUQBVAEUATgBDAEUAKAAxADAALAAxACwAMAAsADEAKQAsAFwAbgAgACAAIAAgAE8AXwBTAHQAYQByAHMALAAgAEYASQBMAFQARQBSACgAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAATABFAEYAVAAoAGEAcgByAFQAeQBwAGUAcwAsADEAKQA9AFwAIgBPAFwAIgApACwAXABuACAAIAAgACAAQgBfAFMAdABhAHIAcwAsACAARgBJAEwAVABFAFIAKABmAG8AcgBtAGEAdAB0AGUAZABEAGEAdABhACwAIABMAEUARgBUACgAYQByAHIAVAB5AHAAZQBzACwAMQApAD0AXAAiAEIAXAAiACkALABcAG4AIAAgACAAIABBAF8AUwB0AGEAcgBzACwAIABGAEkATABUAEUAUgAoAGYAbwByAG0AYQB0AHQAZQBkAEQAYQB0AGEALAAgAEwARQBGAFQAKABhAHIAcgBUAHkAcABlAHMALAAxACkAPQBcACIAQQBcACIAKQAsAFwAbgAgACAAIAAgAEYAXwBTAHQAYQByAHMALAAgAEYASQBMAFQARQBSACgAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAATABFAEYAVAAoAGEAcgByAFQAeQBwAGUAcwAsADEAKQA9AFwAIgBGAFwAIgApACwAXABuACAAIAAgACAARwBfAFMAdABhAHIAcwAsACAARgBJAEwAVABFAFIAKABmAG8AcgBtAGEAdAB0AGUAZABEAGEAdABhACwAIABMAEUARgBUACgAYQByAHIAVAB5AHAAZQBzACwAMQApAD0AXAAiAEcAXAAiACkALABcAG4AIAAgACAAIABLAF8AUwB0AGEAcgBzACwAIABGAEkATABUAEUAUgAoAGYAbwByAG0AYQB0AHQAZQBkAEQAYQB0AGEALAAgAEwARQBGAFQAKABhAHIAcgBUAHkAcABlAHMALAAxACkAPQBcACIASwBcACIAKQAsAFwAbgAgACAAIAAgAE0AXwBTAHQAYQByAHMALAAgAEYASQBMAFQARQBSACgAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAATABFAEYAVAAoAGEAcgByAFQAeQBwAGUAcwAsADEAKQA9AFwAIgBNAFwAIgApACwAXABuAFwAbgAgACAAIAAgAGYAdQBsAGwAVABhAGIAbABlACwAIABWAFMAVABBAEMASwAoAEgAZQBhAGQAZQByAHMALAAgAEgAUwBUAEEAQwBLACgATgB1AG0AYgBlAHIAcwAsAE8AXwBTAHQAYQByAHMALAAgAEIAXwBTAHQAYQByAHMALAAgAEEAXwBTAHQAYQByAHMALAAgAEYAXwBTAHQAYQByAHMALAAgAEcAXwBTAHQAYQByAHMALAAgAEsAXwBTAHQAYQByAHMALAAgAE0AXwBTAHQAYQByAHMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAASQBmACAAdAB5AHAAZQAgAGkAcwAgAHMAcABlAGMAaQBmAGkAZQBkACwAIABqAHUAcwB0ACAAcgBlAHQAdQByAG4AIAB0AHcAbwAtAGMAbwBsAHUAbQBuACAAYgByAGUAYQBrAGQAbwB3AG4AIAAtAC0ALQBcAG4AIAAgACAAIAB0AGUAbQBwAHMALAAgAEYASQBMAFQARQBSACgAYQByAHIAVABIAGkAZwBoACwAIABMAEUARgBUACgAYQByAHIAVAB5AHAAZQBzACwAIAAxACkAIAA9ACAAdAB5AHAAZQApACwAXABuACAAIAAgACAAcwBwAGEAbgBzACwAIABGAEkATABUAEUAUgAoAGEAcgByAFMAcABhAG4ALAAgAEwARQBGAFQAKABhAHIAcgBUAHkAcABlAHMALAAgADEAKQAgAD0AIAB0AHkAcABlACkALABcAG4AIAAgACAAIAB0AHkAcABlAEgAZQBhAGQALAAgAEgAUwBUAEEAQwBLACgAdAB5AHAAZQAsACAAXAAiAHMAcABhAG4AXAAiACkALABcAG4AIAAgACAAIABzAGwAaQBtAFQAYQBiAGwAZQAsACAAVgBTAFQAQQBDAEsAKAB0AHkAcABlAEgAZQBhAGQALAAgAEgAUwBUAEEAQwBLACgAdABlAG0AcABzACwAIABzAHAAYQBuAHMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAARgBpAG4AYQBsACAAbwB1AHQAcAB1AHQAOgAgAGYAdQBsAGwAIAB0AGEAYgBsAGUAIABvAHIAIABmAGkAbAB0AGUAcgBlAGQAIABjAG8AbAB1AG0AbgBzAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAdAB5AHAAZQApACwAIABmAHUAbABsAFQAYQBiAGwAZQAsACAAcwBsAGkAbQBUAGEAYgBsAGUAKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFMAVABBAFIAXwBBAFQAVABSAEkAQgBVAFQARQBTAFwAbgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAGEAbABjAHUAbABhAHQAZQBzACAAYQBsAGwAIABrAGUAeQAgAHMAdABlAGwAbABhAHIAIABwAGEAcgBhAG0AZQB0AGUAcgBzACAAZgByAG8AbQAgAGEAIABzAGkAbgBnAGwAZQAgAGsAbgBvAHcAbgAgAHYAYQBsAHUAZQAgABQgIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUALAAgAG0AYQBzAHMALAAgAHIAYQBkAGkAdQBzACwAXABuACAAIAAgAGwAdQBtAGkAbgBvAHMAaQB0AHkALAAgAG8AcgAgAGwAaQBmAGUAdABpAG0AZQAgABQgIAB1AHMAaQBuAGcAIABlAG0AcABpAHIAaQBjAGEAbAAgAHAAbwB3AGUAcgAtAGwAYQB3ACAAcwBjAGEAbABpAG4AZwAgAHIAZQBsAGEAdABpAG8AbgBzAGgAaQBwAHMAIABiAGEAcwBlAGQAIABvAG4AIAB0AGgAZQAgAFMAdQBuAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABtAG8AZABlACAAIAAgACAAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABBACAAcwB0AHIAaQBuAGcAIABpAG4AZABpAGMAYQB0AGkAbgBnACAAdABoAGUAIABpAG4AcAB1AHQAIABhAHQAdAByAGkAYgB1AHQAZQAgAHQAeQBwAGUAOgBcAG4AIAAgACAAIAAgACAAIABcACIASwBcACIAIAAUICAARQBmAGYAZQBjAHQAaQB2AGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAAoAEsAZQBsAHYAaQBuACkAXABuACAAIAAgACAAIAAgACAAXAAiAFQAXAAiACAAFCAgAE4AbwByAG0AYQBsAGkAegBlAGQAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAAoAFQAIAAvACAANQA3ADcAMAAgAEsAKQBcAG4AIAAgACAAIAAgACAAIABcACIATQBcACIAIAAUICAATQBhAHMAcwAgACgAcwBvAGwAYQByACAAdQBuAGkAdABzACkAXABuACAAIAAgACAAIAAgACAAXAAiAFIAXAAiACAAFCAgAFIAYQBkAGkAdQBzACAAKABzAG8AbABhAHIAIAB1AG4AaQB0AHMAKQBcAG4AIAAgACAAIAAgACAAIABcACIATABcACIAIAAUICAATAB1AG0AaQBuAG8AcwBpAHQAeQAgACgAcwBvAGwAYQByACAAdQBuAGkAdABzACkAXABuACAAIAAgACAAIAAgACAAXAAiAFYAXAAiACAAFCAgAE0AYQBpAG4ALQBzAGUAcQB1AGUAbgBjAGUAIABsAGkAZgBlAHQAaQBtAGUAIAAoAHMAbwBsAGEAcgAgAHUAbgBpAHQAcwApAFwAbgAgACAAIAAtACAAaQBuAHAAdQB0ACAAIAAgACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAQQAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAaQBuAHAAdQB0ACAAYQB0AHQAcgBpAGIAdQB0AGUAIAAoAG0AdQBzAHQAIABtAGEAdABjAGgAIAB0AGgAZQAgAG0AbwBkAGUAKQAuAFwAbgAgACAAIAAtACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAbwB1AG4AZAAgAG8AdQB0AHAAdQB0ACAAdgBhAGwAdQBlAHMALgAgAEQAZQBmAGEAdQBsAHQAIAA9ACAANgAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIABBACAAdAB3AG8ALQBjAG8AbAB1AG0AbgAgAGEAcgByAGEAeQAgAHcAaQB0AGgAIABsAGEAYgBlAGwAZQBkACAAcwB0AGUAbABsAGEAcgAgAHAAYQByAGEAbQBlAHQAZQByAHMAIAAoAEsALAAgAFQALAAgAE0ALAAgAFIALAAgAEwALAAgAFYAKQAsAFwAbgAgACAAIAB3AGkAdABoACAAdABoAGUAIABpAG4AcAB1AHQAIABhAHQAdAByAGkAYgB1AHQAZQAgAGYAbABhAGcAZwBlAGQAIAB3AGkAdABoACAAYQAgAJQnIABhAHIAcgBvAHcAIABmAG8AcgAgAGMAbABhAHIAaQB0AHkALgBcAG4AXABuACAAIAAgAE0AZQB0AGgAbwBkADoAXABuACAAIAAgAFQAaABlACAAZgB1AG4AYwB0AGkAbwBuACAAbgBvAHIAbQBhAGwAaQB6AGUAcwAgAHQAaABlACAAaQBuAHAAdQB0ACAAdgBhAGwAdQBlACAAdABvACAAYQAgAHMAbwBsAGEAcgAtAHIAZQBsAGEAdABpAHYAZQAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgACgAYABUAG4AbwByAG0AYAApAFwAbgAgACAAIABhAG4AZAAgAGQAZQByAGkAdgBlAHMAIAB0AGgAZQAgAHIAZQBtAGEAaQBuAGkAbgBnACAAcABhAHIAYQBtAGUAdABlAHIAcwAgAGYAcgBvAG0AIABlAG0AcABpAHIAaQBjAGEAbAAgAGUAeABwAG8AbgBlAG4AdABzADoAXABuAFwAbgAgACAAIAAtACAASwAgAD0AIABUAG4AbwByAG0AIADXACAANQA3ADcAMABcAG4AIAAgACAALQAgAE0AIAA9ACAAVABuAG8AcgBtALIAXABuACAAIAAgAC0AIABSACAAPQAgAFQAbgBvAHIAbQBeADEALgA4AFwAbgAgACAAIAAtACAATAAgAD0AIABUAG4AbwByAG0AXgA3AC4ANgBcAG4AIAAgACAALQAgAFYAIAA9ACAAVABuAG8AcgBtAF4AKAAtADUAKQBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8AUwBUAEEAUgBfAEEAVABUAFIASQBCAFUAVABFAFMAKABcACIASwBcACIALAAgADkAMQA3ADAALgA2ADAANQAyACwAIAAzACkAXABuAFwAbgAgACAAIABPAHUAdABwAHUAdAA6AFwAbgAgACAAIAAgACAASwAgAJQnIAAgACAAOQAxADcAMAAuADYAMAA1AFwAbgAgACAAIAAgACAAVAAgACAAIAAgACAAMQAuADUAOAA4AFwAbgAgACAAIAAgACAATQAgACAAIAAgACAAMgAuADUAMgAzAFwAbgAgACAAIAAgACAAUgAgACAAIAAgACAAMgAuADIAOQA2AFwAbgAgACAAIAAgACAATAAgACAAIAAgACAAMwAzAC4AMAAwADYAXABuACAAIAAgACAAIABWACAAIAAgACAAIAAwAC4AMQAwADEAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAEIAYQBzAGUAZAAgAG8AbgAgAHMAaQBtAHAAbABpAGYAaQBlAGQAIABzAHQAZQBsAGwAYQByACAAcwBjAGEAbABpAG4AZwAgAGwAYQB3AHMAIAB1AHMAZQBkACAAaQBuACAAYQBzAHQAcgBvAHAAaAB5AHMAaQBjAHMAIABhAG4AZAAgAHcAbwByAGwAZABiAHUAaQBsAGQAaQBuAGcALgBcAG4AIAAgACAALQAgAEUAZgBmAGUAYwB0AGkAdgBlACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAaQBzACAAcwBjAGEAbABlAGQAIAB0AG8AIAA1ADcANwAwACAASwAgAGYAbwByACAAdABoAGUAIABTAHUAbgAgACgAcwB0AGEAbgBkAGEAcgBkACAAcwBvAGwAYQByACAAcgBlAGYAZQByAGUAbgBjAGUAKQAuAFwAbgAgACAAIAAtACAATABpAGYAZQB0AGkAbQBlACAAaQBzACAAYQBwAHAAcgBvAHgAaQBtAGEAdABlAGQAIABhAHMAIABhACAAcABvAHcAZQByACAAaQBuAHYAZQByAHMAZQAgAG8AZgAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQA6ACAAVgAgAB0iIABUAHsgdSAuAFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAZgBvAHIAIABlAGQAdQBjAGEAdABpAG8AbgBhAGwALAAgAHMAcABlAGMAdQBsAGEAdABpAHYAZQAsACAAYQBuAGQAIABtAG8AZABlAGwAaQBuAGcAIABwAHUAcgBwAG8AcwBlAHMALgBcAG4AXABuACoALwBcAG4AXABuAEEAUwBUAFIATwBfAFMAVABBAFIAXwBBAFQAVABSAEkAQgBVAFQARQBTACAAPQAgAEwAQQBNAEIARABBACgAbQBvAGQAZQAsACAAaQBuAHAAdQB0ACwAIABbAHAAcgBlAGMAaQBzAGkAbwBuAF0ALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAAUwBlAHQAIABkAGUAZgBhAHUAbAB0ACAAcgBvAHUAbgBkAGkAbgBnACAAcAByAGUAYwBpAHMAaQBvAG4AXABuACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjAGkAcwBpAG8AbgApACwAIAA2ACwAIABwAHIAZQBjAGkAcwBpAG8AbgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAE4AbwByAG0AYQBsAGkAegBlACAAaQBuAHAAdQB0ACAAbQBvAGQAZQAgAHQAbwAgAHUAcABwAGUAcgAtAGMAYQBzAGUAIABmAG8AcgAgAGMAbwBuAHMAaQBzAHQAZQBuAGMAeQBcAG4AIAAgACAAIABtAG8AZABlACwAIABVAFAAUABFAFIAKABtAG8AZABlACkALABcAG4AXABuACAAIAAgACAALwAvACAATgBvAHIAbQBhAGwAaQB6AGUAIABpAG4AcAB1AHQAIAB0AG8AIABzAG8AbABhAHIALQByAGUAbABhAHQAaQB2AGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAAoAFQAbgBvAHIAbQApAFwAbgAgACAAIAAgAFQAbgBvAHIAbQAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIABcACIAVABcACIALAAgAGkAbgBwAHUAdAAsAFwAbgAgACAAIAAgACAAIABcACIASwBcACIALAAgAGkAbgBwAHUAdAAgAC8AIAA1ADcANwAwACwAXABuACAAIAAgACAAIAAgAFwAIgBNAFwAIgAsACAAUwBRAFIAVAAoAGkAbgBwAHUAdAApACwAXABuACAAIAAgACAAIAAgAFwAIgBSAFwAIgAsACAAaQBuAHAAdQB0ACAAXgAgACgAMQAgAC8AIAAxAC4AOAApACwAXABuACAAIAAgACAAIAAgAFwAIgBMAFwAIgAsACAAaQBuAHAAdQB0ACAAXgAgACgAMQAgAC8AIAA3AC4ANgApACwAXABuACAAIAAgACAAIAAgAFwAIgBWAFwAIgAsACAAaQBuAHAAdQB0ACAAXgAgACgALQAxACAALwAgADUAKQAsAFwAbgAgACAAIAAgACAAIABOAEEAKAApAFwAbgAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAATgBvAHcAIABkAGUAcgBpAHYAZQAgAGEAbABsACAAbwB0AGgAZQByACAAYQB0AHQAcgBpAGIAdQB0AGUAcwAgAGYAcgBvAG0AIABUAG4AbwByAG0AXABuACAAIAAgACAASwAsACAAVABuAG8AcgBtACAAKgAgADUANwA3ADAALABcAG4AIAAgACAAIABNACwAIABUAG4AbwByAG0AIABeACAAMgAsAFwAbgAgACAAIAAgAFIALAAgAFQAbgBvAHIAbQAgAF4AIAAxAC4AOAAsAFwAbgAgACAAIAAgAEwALAAgAFQAbgBvAHIAbQAgAF4AIAA3AC4ANgAsAFwAbgAgACAAIAAgAFYALAAgAFQAbgBvAHIAbQAgAF4AIAAtADUALABcAG4AXABuACAAIAAgACAALwAvACAAUgBvAHUAbgBkACAAZQB2AGUAcgB5AHQAaABpAG4AZwAgAGEAbgBkACAAZgBvAHIAbQBhAHQAIABhAHMAIABzAHQAcgBpAG4AZwBzAFwAbgAgACAAIAAgAGwAYQBiAGUAbABzACwAIABUAFIAQQBOAFMAUABPAFMARQAoAHsAXAAiAEsAXAAiACwAIABcACIAVABcACIALAAgAFwAIgBNAFwAIgAsACAAXAAiAFIAXAAiACwAIABcACIATABcACIALAAgAFwAIgBWAFwAIgB9ACkALABcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0AF8AdgBhAGwAdQBlAHMALAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABLACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoAFQAbgBvAHIAbQAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABNACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoAFIALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgATAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABWACwAIABwAHIAZQBjACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAATABhAGIAZQBsAHMAIAB3AGkAdABoACAAYQByAHIAbwB3ACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAbQBvAGQAZQAgAC0ALQAtAFwAbgAgACAAIAAgACAAIAAgACAAZgBsAGEAZwBnAGUAZABfAGwAYQBiAGUAbABzACwAIABCAFkAUgBPAFcAKABsAGEAYgBlAGwAcwAsACAATABBAE0AQgBEAEEAKAByAG8AdwAsACAASQBGACgAcgBvAHcAIAA9ACAAbQBvAGQAZQAsACAAcgBvAHcAIAAmACAAXAAiACAAlCdcACIALAAgAHIAbwB3ACkAKQApACwAXABuAFwAbgBcAG4AIAAgACAAIAAvAC8AIABSAGUAdAB1AHIAbgAgAGwAYQBiAGUAbABlAGQAIAB0AGEAYgBsAGUAXABuACAAIAAgACAAQwBIAE8ATwBTAEUAKAB7ADEALAAgADIAfQAsACAAZgBsAGEAZwBnAGUAZABfAGwAYQBiAGUAbABzACwAIABvAHUAdABwAHUAdABfAHYAYQBsAHUAZQBzACkAXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6ACAAUgBlAHQAdQByAG4AcwAgAGgAYQBiAGkAdABhAGIAbABlACAAegBvAG4AZQAgAGQAYQB0AGEAIABiAGEAcwBlAGQAIABvAG4AIABzAHQAZQBsAGwAYQByACAAbAB1AG0AaQBuAG8AcwBpAHQAeQAuAFwAbgBcAG4AIAAgACAATQBvAGQAZQBzADoAXABuACAAIAAgAC0AIABcACIAVABBAEIATABFAFwAIgAgACAAIAAgAJIhIABSAGUAdAB1AHIAbgBzACAAYQAgAGYAdQBsAGwAIAB0AGEAYgBsAGUAIABvAGYAIABpAG4AbgBlAHIALwBvAHUAdABlAHIALwBhAHYAZwAvAHMAcABhAG4AIABkAGkAcwB0AGEAbgBjAGUAcwAgAGYAbwByACAAegBvAG4AZQBzACAAWgAwABMgWgA1AC4AXABuACAAIAAgAC0AIABcACIAVgBFAFIAVABJAEMAQQBMAFwAIgAgAJIhIABSAGUAdAB1AHIAbgBzACAAYQAgAHYAZQByAHQAaQBjAGEAbAAgAGwAaQBzAHQAIABvAGYAIABzAGMAYQBsAGUAZAAgAGQAaQBzAHQAYQBuAGMAZQBzACwAIAB3AGkAdABoACAATgAtAD4AIABtAGEAcgBrAGkAbgBnACAAdABoAGUAIABuAHUAYwBsAGUAYQBsACAAcgBhAGQAaQB1AHMALgBcAG4AIAAgACAALQAgAFwAIgBIAE8AUgBJAFoATwBOAFQAQQBMAFwAIgAgAJIhIABSAGUAdAB1AHIAbgBzACAAYQAgAGgAbwByAGkAegBvAG4AdABhAGwAIAByAG8AdwAgAG8AZgAgAHQAaABlACAAcwBhAG0AZQAgAHYAYQBsAHUAZQBzACAAZgBvAHIAIAB1AHMAZQAgAGkAbgAgAGkAbgBsAGkAbgBlACAAZABpAHMAcABsAGEAeQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAE8AbgBlACAAbwBmACAAXAAiAFQAQQBCAEwARQBcACIALAAgAFwAIgBWAEUAUgBUAEkAQwBBAEwAXAAiACwAIABvAHIAIABcACIASABPAFIASQBaAE8ATgBUAEEATABcACIALgBcAG4AIAAgACAALQAgAGwAdQBtACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAAUwB0AGUAbABsAGEAcgAgAGwAdQBtAGkAbgBvAHMAaQB0AHkAIABpAG4AIABzAG8AbABhAHIAIAB1AG4AaQB0AHMALgAgAFIAZQBxAHUAaQByAGUAZAAgAGYAbwByACAAVgBFAFIAVABJAEMAQQBMACAAYQBuAGQAIABIAE8AUgBJAFoATwBOAFQAQQBMAC4AXABuACAAIAAgAC0AIABwAHIAZQBjAGkAcwBpAG8AbgAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADMAKQBcAG4AXABuACAAIAAgAFoAbwBuAGUAcwAgACgAWgAwABMgWgA1ACkAIAByAGUAcAByAGUAcwBlAG4AdAAgAG4AZQBzAHQAZQBkACAAYwBpAHIAYwB1AG0AcwB0AGUAbABsAGEAcgAgAGgAYQBiAGkAdABhAGIAaQBsAGkAdAB5ACAAYgBhAG4AZABzADoAXABuACAAIAAgAC0AIABaADAAOgAgACgAdABvAG8AIABoAG8AdAApAFwAbgAgACAAIAAtACAAWgAxADoAIAAoAGkAbgBuAGUAcgAgAGUAZABnAGUAKQBcAG4AIAAgACAALQAgAFoAMgA6ACAAKABpAG4AbgBlAHIAIAB0AGUAbQBwAGUAcgBhAHQAZQApAFwAbgAgACAAIAAtACAAWgAzADoAIAAoAG8AdQB0AGUAcgAgAHQAZQBtAHAAZQByAGEAdABlACkAXABuACAAIAAgAC0AIABaADQAOgAgACgAbwB1AHQAZQByACAAZQBkAGcAZQApAFwAbgAgACAAIAAtACAAWgA1ADoAIAAoAHQAbwBvACAAYwBvAGwAZAApAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQAgAHUAcwBhAGcAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBIAEEAQgBJAFQAQQBCAEwARQBfAFoATwBOAEUAUwAoAFwAIgBUAEEAQgBMAEUAXAAiACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgAFIAZQB0AHUAcgBuAHMAIABiAGEAcwBlACAAcgBlAGYAZQByAGUAbgBjAGUAIABjAGgAYQByAHQAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAEkAVABBAEIATABFAF8AWgBPAE4ARQBTACgAXAAiAFYARQBSAFQASQBDAEEATABcACIALAAgADEALgAyADUAKQAgACAAIACSISAAUgBlAHQAdQByAG4AcwAgAHYAZQByAHQAaQBjAGEAbAAgAGQAaQBzAHQAYQBuAGMAZQBzACAAcwBjAGEAbABlAGQAIAB0AG8AIABzAHQAYQByACAAdwBpAHQAaAAgAEwAIAA9ACAAMQAuADIANQBcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAKABcACIASABPAFIASQBaAE8ATgBUAEEATABcACIALAAgADEALgAyADUAKQAgAJIhIABSAGUAdAB1AHIAbgBzACAAcwBhAG0AZQAgAGEAcwAgAHIAbwB3AFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABOAHUAYwBsAGUAYQBsACAAcgBhAGQAaQB1AHMAIABpAHMAIABzAHEAcgB0ACgATAApACAAYQBuAGQAIAB1AHMAZQBkACAAYQBzACAAYQBuAGMAaABvAHIAIABiAGUAdAB3AGUAZQBuACAAWgAyABMgWgAzAC4AXABuACAAIAAgAC0AIABJAG4AcAB1AHQAIABpAHMAIABpAGcAbgBvAHIAZQBkACAAZgBvAHIAIABtAG8AZABlACAAXAAiAFQAQQBCAEwARQBcACIALgBcAG4AKgAvAFwAbgBcAG4AQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAIAA9ACAATABBAE0AQgBEAEEAKABtAG8AZABlACwAIABbAGwAdQBtAF0ALAAgAFsAcAByAGUAYwBpAHMAaQBvAG4AXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAG8AZABlACwAIABVAFAAUABFAFIAKABtAG8AZABlACkALABcAG4AIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAaQBzAGkAbwBuACkALAAgADMALAAgAHAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AXABuACAAIAAgACAALwAvACAAWgBvAG4AZQAgAGMAbwBlAGYAZgBpAGMAaQBlAG4AdABzAFwAbgAgACAAIAAgAHoAbwBuAGUAXwBsAGEAYgBlAGwAcwAsACAAewBcACIAWgAwAFwAIgA7ACAAXAAiAFoAMQBcACIAOwAgAFwAIgBaADIAXAAiADsAIABcACIAWgAzAFwAIgA7ACAAXAAiAFoANABcACIAOwAgAFwAIgBaADUAXAAiAH0ALABcAG4AIAAgACAAIABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAB7ADAAOwAgADAALgA1ADsAIAAwAC4ANwA1ADsAIAAwAC4AOQA1ADsAIAAxAC4AMwA4ADUAOwAgADEALgA3ADcAfQAsAFwAbgAgACAAIAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAHsAMAAuADUAOwAgADAALgA3ADUAOwAgADAALgA5ADUAOwAgADEALgAzADgANQA7ACAAMQAuADcANwA7ACAANAAuADgANQB9ACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFAAcgBlAGMAbwBtAHAAdQB0AGUAIABhAHYAZQByAGEAZwBlACAAYQBuAGQAIABzAHAAYQBuAFwAbgAgACAAIAAgAGEAdgBnAF8AZgBhAGMAdABvAHIAcwAsACAAKABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACAAKwAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMAKQAgAC8AIAAyACwAXABuACAAIAAgACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMAIAAtACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABOAHUAYwBsAGUAYQBsACAAKABmAG8AcgAgAHMAYwBhAGwAaQBuAGcAKQBcAG4AIAAgACAAIABuAHUAYwBsAGUAYQBsACwAIABTAFEAUgBUACgASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAHUAbQApACwAIAAxACwAIABsAHUAbQApACkALABcAG4AXABuACAAIAAgACAALwAvACAAQwBvAG0AcAB1AHQAZQAgAHMAYwBhAGwAZQBkACAAZABpAHMAdABhAG4AYwBlAHMAXABuACAAIAAgACAAaQBuAG4AZQByAF8AcwBjAGEAbABlAGQALAAgAFIATwBVAE4ARAAoAG4AdQBjAGwAZQBhAGwAIAAqACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAbwB1AHQAZQByAF8AcwBjAGEAbABlAGQALAAgAFIATwBVAE4ARAAoAG4AdQBjAGwAZQBhAGwAIAAqACAAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAYQB2AGcAXwBzAGMAYQBsAGUAZAAsACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAgACoAIABhAHYAZwBfAGYAYQBjAHQAbwByAHMALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgAHMAcABhAG4AXwBzAGMAYQBsAGUAZAAsACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAgACoAIABzAHAAYQBuAF8AZgBhAGMAdABvAHIAcwAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEYAbwByAG0AYQB0AHQAZQBkACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAdgBlAHIAdABpAGMAYQBsAF8AbABhAGIAZQBsAHMALAAgAHsAXAAiADAAOgAgAFwAIgAsACAAXAAiADEAOgAgAFwAIgAsACAAXAAiADIAOgAgAFwAIgAsACAAXAAiAE4AIACUJ1wAIgAsACAAXAAiADMAOgAgAFwAIgAsACAAXAAiADQAOgAgAFwAIgAsACAAXAAiADUAOgAgAFwAIgB9ACwAXABuACAAIAAgACAAdgBlAHIAdABpAGMAYQBsAF8AdgBhAGwAdQBlAHMALAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAMgApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgAFIATwBVAE4ARAAoAEkATgBEAEUAWAAoAGkAbgBuAGUAcgBfAGYAYQBjAHQAbwByAHMALAAgADMAKQAgACoAIABuAHUAYwBsAGUAYQBsACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA0ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwAsACAANAApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgAFIATwBVAE4ARAAoAEkATgBEAEUAWAAoAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgADUAKQAgACoAIABuAHUAYwBsAGUAYQBsACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA2ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApAFwAbgAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAAUgBlAHQAdQByAG4AIABsAG8AZwBpAGMAXABuACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4AIAAgACAAIAAgACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBTAFQAQQBOAEQAQQBSAEQAXAAiACwAIABDAEgATwBPAFMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgAHsAMQAsACAAMgAsACAAMwAsACAANAAsACAANQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIAWgBvAG4AZQBcACIALAAgAHoAbwBuAGUAXwBsAGEAYgBlAGwAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIASQBuAG4AZQByAFwAIgAsACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIATwB1AHQAZQByAFwAIgAsACAAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIAQQB2AGUAcgBhAGcAZQBcACIALAAgAGEAdgBnAF8AZgBhAGMAdABvAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIAUwBwAGEAbgBcACIALAAgAHMAcABhAG4AXwBmAGEAYwB0AG8AcgBzACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAVgBFAFIAVABJAEMAQQBMAFwAIgAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsAHMALAAgAHsAXAAiADAAOgBcACIALAAgAFwAIgAxADoAXAAiACwAIABcACIAMgA6AFwAIgAsACAAXAAiAE4AIACUJ1wAIgAsACAAXAAiADMAOgBcACIALAAgAFwAIgA0ADoAXAAiACwAIABcACIANQA6AFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHMAYwBhAGwAZQBkAF8AdgBhAGwAdQBlAHMALAAgAFIATwBVAE4ARAAoAG4AdQBjAGwAZQBhAGwAIAAqACAAewAwAC4ANQAsACAAMAAuADcANQAsACAAMAAuADkANQAsACAAMQAsACAAMQAuADMAOAA1ACwAIAAxAC4ANwA3ACwAIAA0AC4AOAA1AH0ALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAQQBOAFMAUABPAFMARQAoAFYAUwBUAEEAQwBLACgAbABhAGIAZQBsAHMALAAgAHMAYwBhAGwAZQBkAF8AdgBhAGwAdQBlAHMAKQApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAEgATwBSAEkAWgBPAE4AVABBAEwAXAAiACwAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAMgApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAMwApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAANAApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA0ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA1ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA2ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAEkAbgB2AGEAbABpAGQAIABtAG8AZABlAFwAIgBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAE4AQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6ACAAUAByAG8AdgBpAGQAZQBzACAAaQBuAGYAbwByAG0AYQB0AGkAbwBuACAAYQBiAG8AdQB0ACAAcwB0AGUAbABsAGEAcgAgAGgAYQBiAGkAdABhAGIAbABlACAAegBvAG4AZQBzACAAYQBjAHIAbwBzAHMAIABtAHUAbAB0AGkAcABsAGUAIABkAGkAcwBwAGwAYQB5ACAAbQBvAGQAZQBzADoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC0AIABTAFQAQQBOAEQAQQBSAEQAOgAgAFIAZQB0AHUAcgBuAHMAIABhACAAZgBpAHgAZQBkACAAdABhAGIAbABlACAAbwBmACAAaQBuAG4AZQByAC8AbwB1AHQAZQByACAAYgBvAHUAbgBkAHMAIABmAG8AcgAgAFoAMAATIFoANQAgAHoAbwBuAGUAcwAgAGkAbgAgAEEAVQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAgAFQAQQBCAEwARQA6ACAAUwBjAGEAbABlAHMAIAB0AGgAZQAgAFMAVABBAE4ARABBAFIARAAgAHoAbwBuAGUAcwAgAGIAYQBzAGUAZAAgAG8AbgAgAHMAdABlAGwAbABhAHIAIABsAHUAbQBpAG4AbwBzAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAtACAAVgBFAFIAVABJAEMAQQBMADoAIABSAGUAdAB1AHIAbgBzACAAYQAgAHYAZQByAHQAaQBjAGEAbAAgAGwAaQBzAHQAIABvAGYAIAB6AG8AbgBlACAAbABhAGIAZQBsAHMAIABhAG4AZAAgAGQAaQBzAHQAYQBuAGMAZQBzACAAYgBhAHMAZQBkACAAbwBuACAAbAB1AG0AaQBuAG8AcwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAgAEgATwBSAEkAWgBPAE4AVABBAEwAOgAgAFIAZQB0AHUAcgBuAHMAIABhACAAcwBpAG4AZwBsAGUALQByAG8AdwAgAHMAdQBtAG0AYQByAHkAIABvAGYAIABzAGMAYQBsAGUAZAAgAGQAaQBzAHQAYQBuAGMAZQBzAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFwAIgBTAFQAQQBOAEQAQQBSAEQAXAAiACwAIABcACIAVABBAEIATABFAFwAIgAsACAAXAAiAFYARQBSAFQASQBDAEEATABcACIALAAgAG8AcgAgAFwAIgBIAE8AUgBJAFoATwBOAFQAQQBMAFwAIgBcAG4AIAAgACAALQAgAGwAdQBtACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAAUwB0AGUAbABsAGEAcgAgAGwAdQBtAGkAbgBvAHMAaQB0AHkAIABpAG4AIABzAG8AbABhAHIAIAB1AG4AaQB0AHMAIAAoAG8AbgBsAHkAIAByAGUAcQB1AGkAcgBlAGQAIABmAG8AcgAgAFQAQQBCAEwARQAsACAAVgBFAFIAVABJAEMAQQBMACwAIABvAHIAIABIAE8AUgBJAFoATwBOAFQAQQBMACAAbQBvAGQAZQBzACkAXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAG8AdQBuAGQAIABkAGkAcwB0AGEAbgBjAGUAcwAgAHQAbwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAzACkAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAEkAVABBAEIATABFAF8AWgBPAE4ARQBTACgAXAAiAFMAVABBAE4ARABBAFIARABcACIAKQBcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAKABcACIAVABBAEIATABFAFwAIgAsACAAMwApAFwAbgAgACAAIABBAFMAVABSAE8AXwBIAEEAQgBJAFQAQQBCAEwARQBfAFoATwBOAEUAUwAoAFwAIgBWAEUAUgBUAEkAQwBBAEwAXAAiACwAIAAzACkAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAEkAVABBAEIATABFAF8AWgBPAE4ARQBTACgAXAAiAEgATwBSAEkAWgBPAE4AVABBAEwAXAAiACwAIAAzACkAXABuACoALwBcAG4AXABuAE4AQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAIAA9ACAATABBAE0AQgBEAEEAKABtAG8AZABlACwAIABbAGwAdQBtAF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAARABlAGYAYQB1AGwAdABzACAALQAtAC0AXABuACAAIAAgACAAZABlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABMACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGwAdQBtACkALAAgADEALAAgAGwAdQBtACkALABcAG4AIAAgACAAIABuAHUAYwAsACAAUwBRAFIAVAAoAEwAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIAAtAC0ALQAgAFoAbwBuAGUAIABiAGEAcwBlACAAZABhAHQAYQAgAC0ALQAtAFwAbgAgACAAIAAgAHoAbwBuAGUAXwBsAGEAYgBlAGwAcwAsACAAewBcACIAWgAwAFwAIgAsACAAXAAiAFoAMQBcACIALAAgAFwAIgBaADIAXAAiACwAIABcACIAWgAzAFwAIgAsACAAXAAiAFoANABcACIALAAgAFwAIgBaADUAXAAiAH0ALABcAG4AIAAgACAAIABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAB7ADAALAAgADAALgA1ACwAIAAwAC4ANwA1ACwAIAAwAC4AOQA1ACwAIAAxAC4AMwA4ADUALAAgADEALgA3ADcAfQAsAFwAbgAgACAAIAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAHsAMAAuADUALAAgADAALgA3ADUALAAgADAALgA5ADUALAAgADEALgAzADgANQAsACAAMQAuADcANwAsACAANAAuADgANQB9ACwAXABuACAAIAAgACAAYQB2AGcAXwBmAGEAYwB0AG8AcgBzACwAIAAgACAAewAwAC4AMgA1ACwAIAAwAC4ANgAyADUALAAgADAALgA4ADUALAAgADEALgAxADYANwA1ACwAIAAxAC4ANQA3ADcANQAsACAAMwAuADMAMQB9ACwAXABuACAAIAAgACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgACAAewAwAC4ANQAsACAAMAAuADIANQAsACAAMAAuADIALAAgADAALgA0ADMANQAsACAAMAAuADMAOAA1ACwAIAAzAC4AMAA4AH0ALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABTAGMAYQBsAGUAZAAgAHYAYQBsAHUAZQBzACAALQAtAC0AXABuACAAIAAgACAAaQBuAG4AZQByAF8AcwBjAGEAbABlAGQALAAgAFIATwBVAE4ARAAoAG4AdQBjACAAKgAgAGkAbgBuAGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIABvAHUAdABlAHIAXwBzAGMAYQBsAGUAZAAsACAAUgBPAFUATgBEACgAbgB1AGMAIAAqACAAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgAGEAdgBnAF8AcwBjAGEAbABlAGQALAAgACAAIABSAE8AVQBOAEQAKABuAHUAYwAgACoAIABhAHYAZwBfAGYAYQBjAHQAbwByAHMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIABzAHAAYQBuAF8AcwBjAGEAbABlAGQALAAgACAAUgBPAFUATgBEACgAbgB1AGMAIAAqACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgAGQAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABUAGEAYgBsAGUAOgAgAFMAVABBAE4ARABBAFIARAAgAGEAbgBkACAAVABBAEIATABFACAAbQBvAGQAZQBzACAALQAtAC0AXABuACAAIAAgACAAcgBvAHcAXwAxACwAIABWAFMAVABBAEMASwAoAFwAIgBaAG8AbgBlAFwAIgAsACAAegBvAG4AZQBfAGwAYQBiAGUAbABzACkALABcAG4AIAAgACAAIAByAG8AdwBfADIALAAgAFYAUwBUAEEAQwBLACgAXAAiAEkAbgBuAGUAcgBcACIALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAUwBUAEEATgBEAEEAUgBEAFwAIgAsACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAaQBuAG4AZQByAF8AcwBjAGEAbABlAGQAKQApACwAXABuACAAIAAgACAAcgBvAHcAXwAzACwAIABWAFMAVABBAEMASwAoAFwAIgBPAHUAdABlAHIAXAAiACwAIABJAEYAKABtAG8AZABlAD0AXAAiAFMAVABBAE4ARABBAFIARABcACIALAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAG8AdQB0AGUAcgBfAHMAYwBhAGwAZQBkACkAKQAsAFwAbgAgACAAIAAgAHIAbwB3AF8ANAAsACAAVgBTAFQAQQBDAEsAKABcACIAQQB2AGUAcgBhAGcAZQBcACIALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAUwBUAEEATgBEAEEAUgBEAFwAIgAsACAAYQB2AGcAXwBmAGEAYwB0AG8AcgBzACwAIABhAHYAZwBfAHMAYwBhAGwAZQBkACkAKQAsAFwAbgAgACAAIAAgAHIAbwB3AF8ANQAsACAAVgBTAFQAQQBDAEsAKABcACIAUwBwAGEAbgBcACIALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAUwBUAEEATgBEAEEAUgBEAFwAIgAsACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgAHMAcABhAG4AXwBzAGMAYQBsAGUAZAApACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABWAGUAcgB0AGkAYwBhAGwAIABtAG8AZABlACAAbwB1AHQAcAB1AHQAIAAtAC0ALQBcAG4AIAAgACAAIAB2AGUAcgB0AGkAYwBhAGwAXwBsAGEAYgBlAGwAcwAsACAAewBcACIAMAA6AFwAIgAsACAAXAAiADEAOgBcACIALAAgAFwAIgAyADoAXAAiACwAIABcACIATgAgAJQnXAAiACwAIABcACIAMwA6AFwAIgAsACAAXAAiADQAOgBcACIALAAgAFwAIgA1ADoAXAAiAH0ALABcAG4AIAAgACAAIAB2AGUAcgB0AGkAYwBhAGwAXwB2AGEAbAB1AGUAcwAsACAAUgBPAFUATgBEACgAewAwAC4ANQAsACAAMAAuADcANQAsACAAMAAuADkANQAsACAAMQAsACAAMQAuADMAOAA1ACwAIAAxAC4ANwA3ACwAIAA0AC4AOAA1AH0AIAAqACAAbgB1AGMALAAgAGQAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABIAG8AcgBpAHoAbwBuAHQAYQBsACAAbQBvAGQAZQAgAG8AdQB0AHAAdQB0ACAALQAtAC0AXABuACAAIAAgACAAaABvAHIAaQB6AG8AbgB0AGEAbABfAHYAYQBsAHUAZQBzACwAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAwAC4ANQAgACoAIABuAHUAYwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAwAC4ANwA1ACAAKgAgAG4AdQBjACwAIABkAGUAYwApACwAXABuACAAIAAgACAAIAAgAFIATwBVAE4ARAAoADAALgA5ADUAIAAqACAAbgB1AGMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIAAgACAAUgBPAFUATgBEACgAMQAgACoAIABuAHUAYwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAxAC4AMwA4ADUAIAAqACAAbgB1AGMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIAAgACAAUgBPAFUATgBEACgAMQAuADcANwAgACoAIABuAHUAYwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAA0AC4AOAA1ACAAKgAgAG4AdQBjACwAIABkAGUAYwApAFwAbgAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABGAGkAbgBhAGwAIABvAHUAdABwAHUAdAAgAGIAYQBzAGUAZAAgAG8AbgAgAG0AbwBkAGUAIAAtAC0ALQBcAG4AIAAgACAAIABTAFcASQBUAEMASAAoAFwAbgAgACAAIAAgACAAIABVAFAAUABFAFIAKABtAG8AZABlACkALABcAG4AIAAgACAAIAAgACAAXAAiAFMAVABBAE4ARABBAFIARABcACIALAAgAEgAUwBUAEEAQwBLACgAcgBvAHcAXwAxACwAIAByAG8AdwBfADIALAAgAHIAbwB3AF8AMwAsACAAcgBvAHcAXwA0ACwAIAByAG8AdwBfADUAKQAsAFwAbgAgACAAIAAgACAAIABcACIAVABBAEIATABFAFwAIgAsACAAIAAgACAASABTAFQAQQBDAEsAKAByAG8AdwBfADEALAAgAHIAbwB3AF8AMgAsACAAcgBvAHcAXwAzACwAIAByAG8AdwBfADQALAAgAHIAbwB3AF8ANQApACwAXABuACAAIAAgACAAIAAgAFwAIgBWAEUAUgBUAEkAQwBBAEwAXAAiACwAIABIAFMAVABBAEMASwAoAHYAZQByAHQAaQBjAGEAbABfAGwAYQBiAGUAbABzACwAIAB2AGUAcgB0AGkAYwBhAGwAXwB2AGEAbAB1AGUAcwApACwAXABuACAAIAAgACAAIAAgAFwAIgBIAE8AUgBJAFoATwBOAFQAQQBMAFwAIgAsACAAaABvAHIAaQB6AG8AbgB0AGEAbABfAHYAYQBsAHUAZQBzACwAXABuACAAIAAgACAAIAAgAFwAIgBJAG4AdgBhAGwAaQBkACAAbQBvAGQAZQBcACIAXABuACAAIAAgACAAKQBcAG4AIAAgACkAXABuACkAXABuADsAXABuAFwAbgAvACoAIABBAFMAVABSAE8AXwBTAFQAQQBSAF8ARABFAE4AUwBJAFQAWQBfAFYATwBMAFUATQBFAFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABHAGkAdgBlAG4AIABhACAAcwBwAGgAZQByAGkAYwBhAGwAIAB2AG8AbAB1AG0AZQAgACgAbwByACAAcgBhAGQAaQB1AHMAKQAsACAAYwBhAGwAYwB1AGwAYQB0AGUAIABoAG8AdwAgAG0AYQBuAHkAIABzAHQAYQByAHMAIABmAGkAdAAgAGEAdAAgADEAIABzAHQAYQByACAAcABlAHIAIAAyADUAMAAgAGMAdQBiAGkAYwAgAGwAaQBnAGgAdAAtAHkAZQBhAHIAcwAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAaQBuAHAAdQB0ACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAARQBpAHQAaABlAHIAIABhACAAcwBwAGgAZQByAGkAYwBhAGwAIAByAGEAZABpAHUAcwAgAG8AcgAgAGEAIAB2AG8AbAB1AG0AZQAsACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlAC4AXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAZgBvAHIAIABvAHUAdABwAHUAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADMAKQAuAFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAFwAbgAgACAAIAAgACAAIAAgADAAIAA9ACAAaQBuAHAAdQB0ACAAaQBzACAAYQAgAHYAbwBsAHUAbQBlACAAaQBuACAAYwB1AGIAaQBjACAAbABpAGcAaAB0AC0AeQBlAGEAcgBzACAAKABkAGUAZgBhAHUAbAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAxACAAPQAgAGkAbgBwAHUAdAAgAGkAcwAgAGEAIAByAGEAZABpAHUAcwAgAGkAbgAgAGwAaQBnAGgAdAAtAHkAZQBhAHIAcwAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAQQAgAHYAZQByAHQAaQBjAGEAbAAgAGEAcgByAGEAeQAgAGMAbwBuAHQAYQBpAG4AaQBuAGcAIABlAGkAdABoAGUAcgA6AFwAbgAgACAAIAAgACAAIAAgACIgIABbAG4AdQBtAGIAZQByACAAbwBmACAAcwB0AGEAcgBzADsAIAByAGEAZABpAHUAcwBdACAAaQBmACAAbQBvAGQAZQAgAD0AIAAwAFwAbgAgACAAIAAgACAAIAAgACIgIABbAG4AdQBtAGIAZQByACAAbwBmACAAcwB0AGEAcgBzADsAIAB2AG8AbAB1AG0AZQBdACAAaQBmACAAbQBvAGQAZQAgAD0AIAAxAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBTAFQAQQBSAF8ARABFAE4AUwBJAFQAWQBfAFYATwBMAFUATQBFACgAMQAwADAAMAApACAAIAAgACAAIAAgACAAIAAgACAAkiEgAHsANAAuADAAMAAwADsAIAA2AC4AMgAwADMAfQBcAG4AIAAgACAAQQBTAFQAUgBPAF8AUwBUAEEAUgBfAEQARQBOAFMASQBUAFkAXwBWAE8ATABVAE0ARQAoADUALAAgADIALAAgADEAKQAgACAAIAAgACAAIAAgAJIhIAB7ADIALgA2ADIAOwAgADUAMgAzAC4ANgAwAH0AXABuACoALwBcAG4AXABuAEEAUwBUAFIATwBfAFMAVABBAFIAXwBEAEUATgBTAEkAVABZAF8AVgBPAEwAVQBNAEUAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALAAgAFsAcAByAGUAYwBdACwAIABbAG0AbwBkAGUAXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAgACsAIAAoAG0AbwBkAGUAIAA8ACAAMAApACAAKwAgACgAbQBvAGQAZQAgAD4AIAAxACkALAAgADAALAAgAG0AbwBkAGUAKQAsAFwAbgAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACAAKwAgACgAcAByAGUAYwAgADwAIAAwACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAB2AG8AbAB1AG0AZQAsACAASQBGACgAbQBvAGQAZQAgAD0AIAAwACwAIABpAG4AcAB1AHQALAAgACgANAAvADMAKQAgACoAIABQAEkAKAApACAAKgAgAGkAbgBwAHUAdAAgAF4AIAAzACkALABcAG4AIAAgACAAIAByAGEAZABpAHUAcwAsACAASQBGACgAbQBvAGQAZQAgAD0AIAAxACwAIABpAG4AcAB1AHQALAAgAFIATwBVAE4ARAAoACgAKAAzACAAKgAgAHYAbwBsAHUAbQBlACkAIAAvACAAKAA0ACAAKgAgAFAASQAoACkAKQApACAAXgAgACgAMQAvADMAKQAsACAAcAByAGUAYwApACkALABcAG4AIAAgACAAIABzAHQAYQByAHMALAAgAFIATwBVAE4ARAAoAHYAbwBsAHUAbQBlACAALwAgADIANQAwACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAFMAVwBJAFQAQwBIACgAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIAAwACwAIABUAE8AQwBPAEwAKABUAEUAWABUAFMAUABMAEkAVAAoAFQARQBYAFQASgBPAEkATgAoAFwAIgA7ACAAXAAiACwAIAAsACAAXAAiAFMAdABhAHIAcwA6ACAAXAAiACYAcwB0AGEAcgBzACwAIABcACIAUgBhAGQAaQB1AHMAOgAgAFwAIgAmAHIAYQBkAGkAdQBzACkALAAgAFwAIgA7ACAAXAAiACkAKQAsAFwAbgAgACAAIAAgACAAIAAxACwAIABUAE8AQwBPAEwAKABUAEUAWABUAFMAUABMAEkAVAAoAFQARQBYAFQASgBPAEkATgAoAFwAIgA7ACAAXAAiACwAIAAsACAAXAAiAFMAdABhAHIAcwA6ACAAXAAiACYAcwB0AGEAcgBzACwAIABcACIAVgBvAGwAdQBtAGUAOgAgAFwAIgAmAHYAbwBsAHUAbQBlACkALAAgAFwAIgA7ACAAXAAiACkAKQBcAG4AIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUABMAEEATgBFAFQAXwBNAEUAVABSAEkAQwBTAF8AUwBBAEYARQBUAFkAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgAgAEMAYQBsAGMAdQBsAGEAdABlAHMAIABwAGwAYQBuAGUAdABhAHIAeQAgAG0AYQBzAHMALAAgAHIAYQBkAGkAdQBzACwAIABkAGUAbgBzAGkAdAB5ACwAIABzAHUAcgBmAGEAYwBlACAAZwByAGEAdgBpAHQAeQAsACAAYQBuAGQAIABlAHMAYwBhAHAAZQAgAHYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgByAG8AbQAgAGEAbgB5ACAAdgBhAGwAaQBkACAAcABhAGkAcgAgAG8AZgAgAHQAdwBvACAAawBuAG8AdwBuACAAcABhAHIAYQBtAGUAdABlAHIAcwAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAIABzAHQAcgBpAG4AZwAgAGkAbgBkAGkAYwBhAHQAaQBuAGcAIAB0AGgAZQAgAGsAbgBvAHcAbgAgAGkAbgBwAHUAdAAgAHAAYQBpAHIALgAgAEEAYwBjAGUAcAB0AGEAYgBsAGUAIAB2AGEAbAB1AGUAcwA6AFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAGQAXAAiACAAPQAgAE0AYQBzAHMAIAArACAARABlAG4AcwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAbQByAFwAIgAgAD0AIABNAGEAcwBzACAAKwAgAFIAYQBkAGkAdQBzAFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAGcAXAAiACAAPQAgAE0AYQBzAHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAcgBkAFwAIgAgAD0AIABSAGEAZABpAHUAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgByAGcAXAAiACAAPQAgAFIAYQBkAGkAdQBzACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAGQAZwBcACIAIAA9ACAARABlAG4AcwBpAHQAeQAgACsAIABHAHIAYQB2AGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgBkAHYAXAAiACAAPQAgAEQAZQBuAHMAaQB0AHkAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAGcAdgBcACIAIAA9ACAARwByAGEAdgBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAbQB2AFwAIgAgAD0AIABNAGEAcwBzACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgByAHYAXAAiACAAPQAgAFIAYQBkAGkAdQBzACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAtACAAcABhAHIAYQBtAF8AMQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFQAaABlACAAZgBpAHIAcwB0ACAAbgB1AG0AZQByAGkAYwAgAGkAbgBwAHUAdAAsACAAbQBlAGEAbgBpAG4AZwAgAGQAZQBwAGUAbgBkAHMAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAtACAAcABhAHIAYQBtAF8AMgAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFQAaABlACAAcwBlAGMAbwBuAGQAIABuAHUAbQBlAHIAaQBjACAAaQBuAHAAdQB0ACwAIABtAGUAYQBuAGkAbgBnACAAZABlAHAAZQBuAGQAcwAgAG8AbgAgAG0AbwBkAGUAXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAZgBvAHIAIABvAHUAdABwAHUAdAAgAHIAbwB1AG4AZABpAG4AZwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAA1ACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABBACAAbABhAGIAZQBsAGUAZAAgADUALQByAG8AdwAgAHQAYQBiAGwAZQAgAHcAaQB0AGgAIAB2AGEAbAB1AGUAcwAgAGYAbwByADoAIABNAGEAcwBzACAAKABNACkALAAgAFIAYQBkAGkAdQBzACAAKABSACkALAAgAEQAZQBuAHMAaQB0AHkAIAAoAGQAKQAsAFwAbgAgACAAIAAgACAARwByAGEAdgBpAHQAeQAgACgAZwApACwAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQAgACgAdgApAFwAbgAqAC8AXABuAFwAbgBBAFMAVABSAE8AXwBQAEwAQQBOAEUAVABfAE0ARQBUAFIASQBDAFMAXwBTAEEARgBFAFQAWQAgAD0AIABMAEEATQBCAEQAQQAoAG0AbwBkAGUALAAgAHAAYQByAGEAbQBfADEALAAgAHAAYQByAGEAbQBfADIALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABwAHIAZQBjAGkAcwBpAG8AbgBcAG4AIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANQAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAE4AbwByAG0AYQBsAGkAegBlACAAaQBuAHAAdQB0ACAAbQBvAGQAZQAgAHQAbwAgAGwAbwB3AGUAcgBjAGEAcwBlAFwAbgAgACAAIAAgAG0AbwBkAGUALAAgAEwATwBXAEUAUgAoAG0AbwBkAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAYgBhAHMAZQBkACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAbQBvAGQAZQBcAG4AIAAgACAAIABvAHUAdABwAHUAdAAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAbQBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgACgATQAgAC8AIABkACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAAoAE0AIAAqACAAZABeADIAKQAgAF4AIAAoADEALwAzACkALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgACgATQAgACoAIABTAFEAUgBUACgAZAApACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABSAGEAZABpAHUAcwBcAG4AIAAgACAAIAAgACAAXAAiAG0AcgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABNACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABNACAALwAgAFIAXgAzACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABNACAALwAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABTAFEAUgBUACgATQAgAC8AIABSACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABNAGEAcwBzACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAGcAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAAUwBRAFIAVAAoAE0AIAAvACAAZwApACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABTAFEAUgBUACgAZwBeADMAIAAvACAATQApACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIAAoAE0AIAAqACAAZwApACAAXgAgADAALgAyADUALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAcgBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGQAIAAqACAAUgBeADMALABcAG4AIAAgACAAIAAgACAAIAAgAGcALAAgAGQAIAAqACAAUgAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAUgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAAUgBhAGQAaQB1AHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABnACAAKgAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABnACAALwAgAFIALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAFMAUQBSAFQAKABnACAAKgAgAFIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBuAHMAaQB0AHkAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGQAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABkACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABnACAALwAgAGQALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGcAXgAzACAALwAgAGQAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABnACAALwAgAFMAUQBSAFQAKABkACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABEAGUAbgBzAGkAdAB5ACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAZAB2AFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHYAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAdgBeADMAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAARwByAGEAdgBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGcAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIAB2AF4AMgAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIAB2AF4ANAAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAGcAIAAvACAAdgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAE0AYQBzAHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAHYAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAATQAgAC8AIAB2AF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgBeADQAIAAvACAATQAsAFwAbgAgACAAIAAgACAAIAAgACAAZAAsACAAdgBeADYAIAAvACAATQBeADIALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAB2AF4AMgAgAC8AIABSACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABSACAAKgAgAHYAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAHYAIAAvACAAUgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABmAGEAbABsAGIAYQBjAGsAXABuACAAIAAgACAAIAAgAE4AQQAoACkAXABuACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABGAG8AcgBtAGEAdAAgAHcAaQB0AGgAIABoAGUAYQBkAGUAcgBzACAAYQBuAGQAIAByAG8AdQBuAGQAaQBuAGcAXABuACAAIAAgACAAaABlAGEAZABlAHIAcwAsACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACwAXABuACAAIAAgACAAdgBhAGwAdQBlAHMALAAgAFIATwBVAE4ARAAoAG8AdQB0AHAAdQB0ACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABDAEgATwBPAFMARQAoAHsAMQAsACAAMgB9ACwAIABUAFIAQQBOAFMAUABPAFMARQAoAGgAZQBhAGQAZQByAHMAKQAsACAAVABSAEEATgBTAFAATwBTAEUAKAB2AGEAbAB1AGUAcwApACkAXABuACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABBAFMAVABSAE8AXwBQAEwAQQBOAEUAVABfAE0ARQBUAFIASQBDAFMAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBhAGwAYwB1AGwAYQB0AGUAcwAgAHAAbABhAG4AZQB0AGEAcgB5ACAAbQBhAHMAcwAsACAAcgBhAGQAaQB1AHMALAAgAGQAZQBuAHMAaQB0AHkALAAgAHMAdQByAGYAYQBjAGUAIABnAHIAYQB2AGkAdAB5ACwAIABhAG4AZAAgAGUAcwBjAGEAcABlACAAdgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIABiAGEAcwBlAGQAIABvAG4AIABhAG4AeQAgAHQAdwBvACAAawBuAG8AdwBuACAAdgBhAGwAdQBlAHMALAAgAGEAbgBkACAAZgBsAGEAZwBzACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AcAB1AHQAcwAgAHcAaQB0AGgAIABhAG4AIABhAHIAcgBvAHcAIAAoAJQnKQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAIABzAHQAcgBpAG4AZwAgAGkAbgBkAGkAYwBhAHQAaQBuAGcAIAB0AGgAZQAgAHQAdwBvACAAawBuAG8AdwBuACAAdgBhAGwAdQBlAHMALgAgAEEAYwBjAGUAcAB0AGUAZAAgAHYAYQBsAHUAZQBzADoAXABuACAAIAAgACAAIAAgACAAXAAiAG0AZABcACIAIAA9ACAATQBhAHMAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAHIAXAAiACAAPQAgAE0AYQBzAHMAIAArACAAUgBhAGQAaQB1AHMAXABuACAAIAAgACAAIAAgACAAXAAiAG0AZwBcACIAIAA9ACAATQBhAHMAcwAgACsAIABHAHIAYQB2AGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgByAGQAXAAiACAAPQAgAFIAYQBkAGkAdQBzACAAKwAgAEQAZQBuAHMAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAHIAZwBcACIAIAA9ACAAUgBhAGQAaQB1AHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAZABnAFwAIgAgAD0AIABEAGUAbgBzAGkAdAB5ACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAGQAdgBcACIAIAA9ACAARABlAG4AcwBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAZwB2AFwAIgAgAD0AIABHAHIAYQB2AGkAdAB5ACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAHYAXAAiACAAPQAgAE0AYQBzAHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAHIAdgBcACIAIAA9ACAAUgBhAGQAaQB1AHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgAC0AIABwAGEAcgBhAG0AXwAxACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAARgBpAHIAcwB0ACAAawBuAG8AdwBuACAAcABhAHIAYQBtAGUAdABlAHIAIAAoAG0AZQBhAG4AaQBuAGcAIABkAGUAcABlAG4AZABzACAAbwBuACAAbQBvAGQAZQApAFwAbgAgACAAIAAtACAAcABhAHIAYQBtAF8AMgAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAZQBjAG8AbgBkACAAawBuAG8AdwBuACAAcABhAHIAYQBtAGUAdABlAHIAIAAoAG0AZQBhAG4AaQBuAGcAIABkAGUAcABlAG4AZABzACAAbwBuACAAbQBvAGQAZQApAFwAbgAgACAAIAAtACAAcAByAGUAYwAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAEQAZQBjAGkAbQBhAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGYAbwByACAAbwB1AHQAcAB1AHQAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAANQApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAQQAgADIALQBjAG8AbAB1AG0AbgAgAHYAZQByAHQAaQBjAGEAbAAgAHQAYQBiAGwAZQAgAHcAaQB0AGgAIABoAGUAYQBkAGUAcgBzACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACAAYQBuAGQAIABjAGEAbABjAHUAbABhAHQAZQBkACAAdgBhAGwAdQBlAHMALgBcAG4AIAAgACAAIAAgAEkAbgBwAHUAdAAgAHYAYQBsAHUAZQBzACAAYQByAGUAIABmAGwAYQBnAGcAZQBkACAAdwBpAHQAaAAgAGEAIACUJyAAdABvACAAaQBuAGQAaQBjAGEAdABlACAAdABoAGUAaQByACAAbwByAGkAZwBpAG4ALgBcAG4AIAAgACAAIAAgAFUAbgBpAHQAcwAgAGEAcgBlACAAYQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIABhAG4AZAAgAHIAZQBsAGEAdABpAHYAZQAgACgAZQAuAGcALgAsACAARQBhAHIAdABoACAAPQAgADEALgAwACkALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAZgBvAHIAIAB1AHMAZQAgAGkAbgAgAG0AbwBkAGUAbABpAG4AZwAsACAAcABsAGEAbgBlAHQAYQByAHkAIABwAGgAeQBzAGkAYwBzACAAcwBpAG0AdQBsAGEAdABpAG8AbgBzACwAIABhAG4AZAAgAGUAZAB1AGMAYQB0AGkAbwBuAGEAbAAgAGEAcABwAGwAaQBjAGEAdABpAG8AbgBzAC4AXABuACAAIAAgAC0AIABPAHUAdABwAHUAdABzACAAYQByAGUAIABpAG4AdABlAHIAbgBhAGwAbAB5ACAAYwBhAGwAYwB1AGwAYQB0AGUAZAAgAGIAYQBzAGUAZAAgAG8AbgAgAGIAYQBzAGkAYwAgAHAAaAB5AHMAaQBjAGEAbAAgAHIAZQBsAGEAdABpAG8AbgBzAGgAaQBwAHMAOgBcAG4AIAAgACAAIAAgACAAIAAtACAATQAgAD0AIABtAGEAcwBzAFwAbgAgACAAIAAgACAAIAAgAC0AIABSACAAPQAgAHIAYQBkAGkAdQBzAFwAbgAgACAAIAAgACAAIAAgAC0AIABkACAAPQAgAGQAZQBuAHMAaQB0AHkAXABuACAAIAAgACAAIAAgACAALQAgAGcAIAA9ACAAcwB1AHIAZgBhAGMAZQAgAGcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgACAALQAgAHYAIAA9ACAAZQBzAGMAYQBwAGUAIAB2AGUAbABvAGMAaQB0AHkAXABuACAAIAAgAC0AIABIAGEAbgBkAGwAZQBzACAAaQBuAHAAdQB0ACAAcABlAHIAbQB1AHQAYQB0AGkAbwBuAHMAIABmAGwAZQB4AGkAYgBsAHkAIAB2AGkAYQAgAG0AbwBkAGUAIABzAHQAcgBpAG4AZwAgAHAAYQByAHMAaQBuAGcALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8AUABMAEEATgBFAFQAXwBNAEUAVABSAEkAQwBTAF8ARgBMAEEARwBHAEUARAAoAFwAIgByAGQAXAAiACwAIAAxAC4AMgAsACAAMAAuADcANQApAFwAbgAgACAAIAAgACAAkiFcAG4AIAAgACAAIAAgACAAIABNACAAIAAgACAAIAAgADAALgA2ADcANQBcAG4AIAAgACAAIAAgACAAIABSACAAlCcgACAAIAAgADEALgAyAFwAbgAgACAAIAAgACAAIAAgAGQAIACUJyAAIAAgACAAMAAuADcANQBcAG4AIAAgACAAIAAgACAAIABnACAAIAAgACAAIAAgADAALgA5AFwAbgAgACAAIAAgACAAIAAgAHYAIAAgACAAIAAgACAAMQAuADAAMwA5AFwAbgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFAATABBAE4ARQBUAF8ATQBFAFQAUgBJAEMAUwAgAD0AIABMAEEATQBCAEQAQQAoAG0AbwBkAGUALAAgAHAAYQByAGEAbQBfADEALAAgAHAAYQByAGEAbQBfADIALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABwAHIAZQBjAGkAcwBpAG8AbgBcAG4AIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANQAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAE4AbwByAG0AYQBsAGkAegBlACAAaQBuAHAAdQB0ACAAbQBvAGQAZQAgAHQAbwAgAGwAbwB3AGUAcgBjAGEAcwBlAFwAbgAgACAAIAAgAG0AbwBkAGUALAAgAEwATwBXAEUAUgAoAG0AbwBkAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAYgBhAHMAZQBkACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAbQBvAGQAZQBcAG4AIAAgACAAIABvAHUAdABwAHUAdAAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAbQBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgACgATQAgAC8AIABkACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAAoAE0AIAAqACAAZABeADIAKQAgAF4AIAAoADEALwAzACkALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgACgATQAgACoAIABTAFEAUgBUACgAZAApACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABSAGEAZABpAHUAcwBcAG4AIAAgACAAIAAgACAAXAAiAG0AcgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABNACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABNACAALwAgAFIAXgAzACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABNACAALwAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABTAFEAUgBUACgATQAgAC8AIABSACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABNAGEAcwBzACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAGcAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAAUwBRAFIAVAAoAE0AIAAvACAAZwApACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABTAFEAUgBUACgAZwBeADMAIAAvACAATQApACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIAAoAE0AIAAqACAAZwApACAAXgAgADAALgAyADUALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAcgBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGQAIAAqACAAUgBeADMALABcAG4AIAAgACAAIAAgACAAIAAgAGcALAAgAGQAIAAqACAAUgAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAUgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAAUgBhAGQAaQB1AHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABnACAAKgAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABnACAALwAgAFIALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAFMAUQBSAFQAKABnACAAKgAgAFIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBuAHMAaQB0AHkAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGQAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABkACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABnACAALwAgAGQALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGcAXgAzACAALwAgAGQAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABnACAALwAgAFMAUQBSAFQAKABkACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABEAGUAbgBzAGkAdAB5ACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAZAB2AFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHYAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAdgBeADMAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAARwByAGEAdgBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGcAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIAB2AF4AMgAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIAB2AF4ANAAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAGcAIAAvACAAdgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAE0AYQBzAHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAHYAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAATQAgAC8AIAB2AF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgBeADQAIAAvACAATQAsAFwAbgAgACAAIAAgACAAIAAgACAAZAAsACAAdgBeADYAIAAvACAATQBeADIALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAB2AF4AMgAgAC8AIABSACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABSACAAKgAgAHYAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAHYAIAAvACAAUgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABmAGEAbABsAGIAYQBjAGsAXABuACAAIAAgACAAIAAgAE4AQQAoACkAXABuACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABGAG8AcgBtAGEAdAAgAHcAaQB0AGgAIABoAGUAYQBkAGUAcgBzACAAYQBuAGQAIAByAG8AdQBuAGQAaQBuAGcAXABuACAAIAAgACAAaABlAGEAZABlAHIAcwAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBtAGQAXAAiACwAIAB7AFwAIgBNACAAlCdcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAIACUJ1wAIgAsACAAXAAiAGcAXAAiACwAIABcACIAdgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAG0AcgBcACIALAAgAHsAXAAiAE0AIACUJ1wAIgAsACAAXAAiAFIAIACUJ1wAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABcACIAbQBnAFwAIgAsACAAewBcACIATQAgAJQnXAAiACwAIABcACIAUgBcACIALAAgAFwAIgBkAFwAIgAsACAAXAAiAGcAIACUJ1wAIgAsACAAXAAiAHYAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgByAGQAXAAiACwAIAB7AFwAIgBNAFwAIgAsACAAXAAiAFIAIACUJ1wAIgAsACAAXAAiAGQAIACUJ1wAIgAsACAAXAAiAGcAXAAiACwAIABcACIAdgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAHIAZwBcACIALAAgAHsAXAAiAE0AXAAiACwAIABcACIAUgAgAJQnXAAiACwAIABcACIAZABcACIALAAgAFwAIgBnACAAlCdcACIALAAgAFwAIgB2AFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABcACIAZABnAFwAIgAsACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAIACUJ1wAIgAsACAAXAAiAGcAIACUJ1wAIgAsACAAXAAiAHYAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBkAHYAXAAiACwAIAB7AFwAIgBNAFwAIgAsACAAXAAiAFIAXAAiACwAIABcACIAZAAgAJQnXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2ACAAlCdcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAGcAdgBcACIALAAgAHsAXAAiAE0AXAAiACwAIABcACIAUgBcACIALAAgAFwAIgBkAFwAIgAsACAAXAAiAGcAIACUJ1wAIgAsACAAXAAiAHYAIACUJ1wAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABcACIAbQB2AFwAIgAsACAAewBcACIATQAgAJQnXAAiACwAIABcACIAUgBcACIALAAgAFwAIgBkAFwAIgAsACAAXAAiAGcAXAAiACwAIABcACIAdgAgAJQnXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgByAHYAXAAiACwAIAB7AFwAIgBNAFwAIgAsACAAXAAiAFIAIACUJ1wAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2ACAAlCdcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACAAIAAvAC8AIABmAGEAbABsAGIAYQBjAGsAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAdgBhAGwAdQBlAHMALAAgAFIATwBVAE4ARAAoAG8AdQB0AHAAdQB0ACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABDAEgATwBPAFMARQAoAHsAMQAsACAAMgB9ACwAIABUAFIAQQBOAFMAUABPAFMARQAoAGgAZQBhAGQAZQByAHMAKQAsACAAVABSAEEATgBTAFAATwBTAEUAKAB2AGEAbAB1AGUAcwApACkAXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAFwAbgBcAG4AXABuAFwAbgBBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDACAAPQAgAFwAbgBMAEEATQBCAEQAQQAoAHAALAAgAHEALAAgAHAAcgBlAGMALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4AIAAgACAAIABJAEYAKABwACAAPQAgAHEALABcAG4AIAAgACAAIAAgACAAIABOAEEAKAApACwAXABuACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAbgB1AG0ALAAgAHAAIAAqACAAcQAsAFwAbgAgACAAIAAgACAAIAAgACAAIABkAGUAbgAsACAAQQBCAFMAKABwACAALQAgAHEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAByAGEAdwAsACAAbgB1AG0AIAAvACAAZABlAG4ALABcAG4AIAAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAcgBhAHcALAAgAHAAcgBlAGMAKQBcAG4AIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACkALABcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBTAE8ATABWAEUARAAgAD0AXABuAEwAQQBNAEIARABBACgAdgBhAGwAXwAxACwAIAB2AGEAbABfADIALAAgAFsAbQBvAGQAZQBdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAXAAiAHAAcQBcACIALAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAHAAcQBcACIALAAgAG0AbwBkAGUAKQApACwAXABuACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADQALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIABwACwAIABJAEYAKABPAFIAKABtAG8AZABlAD0AXAAiAHAAcQBcACIALAAgAG0AbwBkAGUAPQBcACIAcABzAFwAIgApACwAIAB2AGEAbABfADEALAAgAE4AQQAoACkAKQAsAFwAbgAgACAAIAAgAHEALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAcABxAFwAIgAsACAAdgBhAGwAXwAyACwAIABJAEYAKABtAG8AZABlAD0AXAAiAHEAcwBcACIALAAgAHYAYQBsAF8AMQAsACAATgBBACgAKQApACkALABcAG4AIAAgACAAIABzACwAIABJAEYAKABPAFIAKABtAG8AZABlAD0AXAAiAHAAcwBcACIALAAgAG0AbwBkAGUAPQBcACIAcQBzAFwAIgApACwAIAB2AGEAbABfADIALAAgAE4AQQAoACkAKQAsAFwAbgBcAG4AIAAgACAAIABhACwAIABJAEYAKABBAE4ARAAoAEkAUwBOAFUATQBCAEUAUgAoAHAAKQAsACAASQBTAE4AVQBNAEIARQBSACgAcQApACkALAAgAE0AQQBYACgAcAAsACAAcQApACwAIABwACkALABcAG4AIAAgACAAIABiACwAIABJAEYAKABBAE4ARAAoAEkAUwBOAFUATQBCAEUAUgAoAHAAKQAsACAASQBTAE4AVQBNAEIARQBSACgAcQApACkALAAgAE0ASQBOACgAcAAsACAAcQApACwAIABxACkALABcAG4AXABuACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4AIAAgACAAIAAgACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBwAHEAXAAiACwAIABJAEYAKABhACAAPQAgAGIALAAgAE4AQQAoACkALAAgAFIATwBVAE4ARAAoACgAYQAgACoAIABiACkAIAAvACAAKABhACAALQAgAGIAKQAsACAAcAByAGUAYwApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBwAHMAXAAiACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAGEAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAHMAKQApACkALAAgAE4AQQAoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoACgAYQAgACoAIABzACkAIAAvACAAKABhACAALQAgAHMAKQAsACAAcAByAGUAYwApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBxAHMAXAAiACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAGIAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAHMAKQApACkALAAgAE4AQQAoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoACgAYgAgACoAIABzACkAIAAvACAAKABiACAALQAgAHMAKQAsACAAcAByAGUAYwApACkALABcAG4AIAAgACAAIAAgACAAIAAgAE4AQQAoACkAXABuACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBTAE8ATABWAEUAUgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABBACAAYwBvAG0AcAByAGUAaABlAG4AcwBpAHYAZQAgAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgAHMAbwBsAHYAZQByACAAdABoAGEAdAAgAGMAYQBsAGMAdQBsAGEAdABlAHMAIAB0AGgAZQAgAHQAaABpAHIAZAAgAHYAYQBsAHUAZQAgACgAUAAsACAAUQAsACAAbwByACAAUwApAFwAbgAgACAAIAB3AGgAZQBuACAAYQBuAHkAIAB0AHcAbwAgAG8AZgAgAHQAaABlACAAdABoAHIAZQBlACAAYQByAGUAIABwAHIAbwB2AGkAZABlAGQALgAgAFMAdQBwAHAAbwByAHQAcwAgAG0AdQBsAHQAaQBwAGwAZQAgAGkAbgBwAHUAdAAvAG8AdQB0AHAAdQB0ACAAbQBvAGQAZQBzACAAZgBvAHIAXABuACAAIAAgAHMAYwBpAGUAbgB0AGkAZgBpAGMAIABtAG8AZABlAGwAaQBuAGcALAAgAHAAZQBkAGEAZwBvAGcAaQBjAGEAbAAgAHUAcwBlACwAIABhAG4AZAAgAGYAbABlAHgAaQBiAGwAZQAgAHAAcgBlAHMAZQBuAHQAYQB0AGkAbwBuAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIAB2AGEAbABfADEAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABGAGkAcgBzAHQAIABpAG4AcAB1AHQAIAB2AGEAbAB1AGUALgAgAE0AZQBhAG4AaQBuAGcAIABkAGUAcABlAG4AZABzACAAbwBuACAAdABoAGUAIABzAGUAbABlAGMAdABlAGQAIABtAG8AZABlAC4AXABuACAAIAAgAC0AIAB2AGEAbABfADIAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABTAGUAYwBvAG4AZAAgAGkAbgBwAHUAdAAgAHYAYQBsAHUAZQAuACAATQBlAGEAbgBpAG4AZwAgAGQAZQBwAGUAbgBkAHMAIABvAG4AIAB0AGgAZQAgAHMAZQBsAGUAYwB0AGUAZAAgAG0AbwBkAGUALgBcAG4AIAAgACAALQAgAG0AbwBkAGUAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIAAyAC0AbABlAHQAdABlAHIAIABzAHQAcgBpAG4AZwAgAGkAbgBkAGkAYwBhAHQAaQBuAGcAIABrAG4AbwB3AG4AIABpAG4AcAB1AHQAcwAuACAAQQBjAGMAZQBwAHQAcwAgAGEAbgB5ACAAYwBhAHMAZQAgAG8AcgAgAG8AcgBkAGUAcgAuAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcABxAFwAIgAgAD0AIABzAG8AbAB2AGUAIABmAG8AcgAgAFMAIAAoAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAApAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcABzAFwAIgAgAD0AIABzAG8AbAB2AGUAIABmAG8AcgAgAFEAIAAoAG8AdQB0AGUAcgAgAHMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdAApAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcQBzAFwAIgAgAD0AIABzAG8AbAB2AGUAIABmAG8AcgAgAFAAIAAoAGkAbgBuAGUAcgAgAHMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdAApAFwAbgAgACAAIAAgACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAFwAIgBwAHEAXAAiACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAGkAbgB2AGEAbABpAGQALgBcAG4AIAAgACAALQAgAGYAbwByAG0AYQB0ACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATwB1AHQAcAB1AHQAIABmAG8AcgBtAGEAdAAgACgAZABlAGYAYQB1AGwAdAAgAD0AIABcACIAYgBhAHIAZQBcACIAKQBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGIAYQByAGUAXAAiACAAIAAgACAAkiEgAHIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlACAAbwBuAGwAeQBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGwAYQBiAGUAbABlAGQAXAAiACAAkiEgAHIAZQB0AHUAcgBuAHMAIABcACIAUAAgAD0AIAAzADYANQAuADIANQBcACIALAAgAFwAIgBTACAAPQAgADcANwA5AC4AOAA4AFwAIgAsACAAZQB0AGMALgAsACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAdgBlAHIAYgBvAHMAZQBcACIAIACSISAAcgBlAHQAdQByAG4AcwAgAGkAbgBsAGkAbgBlACAAdABlAHgAdAAgAG8AZgAgAGEAbABsACAAdABoAHIAZQBlACAAdgBhAGwAdQBlAHMAIAB3AGkAdABoACAAHiYgAG8AbgAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcgBvAHcAXAAiACAAIAAgACAAIACSISAAcgBlAHQAdQByAG4AcwAgADEAeAAzACAAYQByAHIAYQB5ACAAdwBpAHQAaAAgAFAALAAgAFEALAAgAGEAbgBkACAAUwAgAGwAYQBiAGUAbABzACAAYQBuAGQAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGMAbwBsAFwAIgAgACAAIAAgACAAkiEgAHIAZQB0AHUAcgBuAHMAIAAzAHgAMgAgAHYAZQByAHQAaQBjAGEAbAAgAGEAcgByAGEAeQA6ACAAewBcACIAUAAgAD0AXAAiACwAIAAzADYANQAuADIANQA7ACAAXAAiAFEAIAA9AFwAIgAsACAANgA4ADcAOwAgAFwAIgBTACAAHiZcACIALAAgADcANwA5AC4AOAA4AH0AXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAdABvACAAcgBvAHUAbgBkACAAcgBlAHMAdQBsAHQAcwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAA0ACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABBACAAcwBjAGEAbABhAHIAIAB2AGEAbAB1AGUAIABvAHIAIABhACAAbABhAGIAZQBsAGUAZAAvAHMAcABpAGwAbAAgAGEAcgByAGEAeQAgAGQAZQBwAGUAbgBkAGkAbgBnACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAZgBvAHIAbQBhAHQALgBcAG4AIAAgACAALQAgAEkAbgAgAGEAbABsACAAYwBhAHMAZQBzACwAIAB0AGgAZQAgAGMAYQBsAGMAdQBsAGEAdABlAGQAIAAoAHMAbwBsAHYAZQBkACkAIAB2AGEAbAB1AGUAIABpAHMAIABmAGwAYQBnAGcAZQBkACAAdwBpAHQAaAAgAGEAIAByAGkAZwBoAHQAIABhAHIAcgBvAHcAIAAoAB4mKQAuAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABTAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIABmAG8AcgBtAHUAbABhADoAIABTACAAPQAgACgAUAAgACoAIABRACkAIAAvACAAfABQACAALQAgAFEAfABcAG4AIAAgACAALQAgAEkAbgB2AGUAcgBzAGUAIABzAG8AbAB1AHQAaQBvAG4AcwA6AFwAbgAgACAAIAAgACAAIAAgAC0AIABRACAAPQAgACgAUAAgACoAIABTACkAIAAvACAAfABQACAALQAgAFMAfABcAG4AIAAgACAAIAAgACAAIAAtACAAUAAgAD0AIAAoAFEAIAAqACAAUwApACAALwAgAHwAUQAgAC0AIABTAHwAXABuACAAIAAgAC0AIABJAG4AcAB1AHQAcwAgAGEAcgBlACAAYQB1AHQAbwAtAG8AcgBkAGUAcgBlAGQAIABhAHMAIABuAGUAZQBkAGUAZAAgAGYAbwByACAAcwB0AGEAYgBpAGwAaQB0AHkAIAAoAGUALgBnAC4ALAAgAFAAIAA9ACAAbQBhAHgAKAB2AGEAbAAxACwAIAB2AGEAbAAyACkAIABpAG4AIABcACIAcABxAFwAIgAgAG0AbwBkAGUAKQAuAFwAbgAgACAAIAAtACAATQBvAGQAZQAgAGkAcwAgAGMAYQBzAGUALQBpAG4AcwBlAG4AcwBpAHQAaQB2AGUAIABhAG4AZAAgAGEAdQB0AG8ALQBuAG8AcgBtAGEAbABpAHoAZQBkACAAKABlAC4AZwAuACwAIABcACIAUQBTAFwAIgAsACAAXAAiAHMAcQBcACIALAAgAGEAbgBkACAAXAAiAHMAUQBcACIAIABhAGwAbAAgAJIhIABcACIAcQBzAFwAIgApAC4AXABuACAAIAAgAC0AIABPAHUAdABwAHUAdAAgAGYAbwByAG0AYQB0AHMAIABzAHUAcABwAG8AcgB0ACAAaAB1AG0AYQBuAC0AcgBlAGEAZABhAGIAbABlACAAcgBlAHMAdQBsAHQAcwAgAGEAbgBkACAAcwB0AHIAdQBjAHQAdQByAGUAZAAgAHQAYQBiAGwAZQAgAGkAbgB0AGUAZwByAGEAdABpAG8AbgAuAFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAYQBzACAAYQAgAGcAZQBuAGUAcgBhAGwALQBwAHUAcgBwAG8AcwBlACAAZQBuAGcAaQBuAGUAIABmAG8AcgAgAHUAcwBlACAAaQBuACAAYQBzAHQAcgBvAG4AbwBtAHkAIABtAG8AZABlAGwAcwAgAGEAbgBkACAAZQBkAHUAYwBhAHQAaQBvAG4AYQBsACAAdABvAG8AbABzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlACAAMQA6AFwAbgAgACAAIAAgACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFMATwBMAFYARQBSACgAMwA2ADUALgAyADUALAAgADYAOAA3ACwAIABcACIAcABxAFwAIgAsACAAXAAiAGIAYQByAGUAXAAiACwAIAA0ACkAXABuACAAIAAgACAAIAAgACAAkiEgADcANwA5AC4AOAA4ADEAMQBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAIAAyADoAXABuACAAIAAgACAAIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUwBPAEwAVgBFAFIAKAAzADYANQAuADIANQAsACAANgA4ADcALAAgAFwAIgBwAHEAXAAiACwAIABcACIAdgBlAHIAYgBvAHMAZQBcACIAKQBcAG4AIAAgACAAIAAgACAAIACSISAAXAAiAFAAIAA9ACAAMwA2ADUALgAyADUALAAgAFEAIAA9ACAANgA4ADcALAAgAFMAIAA9ACAAHiYgADcANwA5AC4AOAA4ADEAMQBcACIAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlACAAMwA6AFwAbgAgACAAIAAgACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFMATwBMAFYARQBSACgANgA4ADcALAAgADcANwA5AC4AOAA4ADEAMQAsACAAXAAiAHEAcwBcACIALAAgAFwAIgBjAG8AbABcACIAKQBcAG4AIAAgACAAIAAgACAAIACSIVwAbgAgACAAIAAgACAAIAAgACAAIABQACAAHiYgACAAIAAgADMANgA1AC4AMgA1AFwAbgAgACAAIAAgACAAIAAgACAAIABRACAAPQAgACAAIAAgADYAOAA3AFwAbgAgACAAIAAgACAAIAAgACAAIABTACAAPQAgACAAIAAgADcANwA5AC4AOAA4ADEAMQBcAG4AXABuACAAIAAgAFIAZQBjAG8AbQBtAGUAbgBkAGEAdABpAG8AbgA6AFwAbgAgACAAIAAtACAARgBvAHIAIABnAGUAbgBlAHIAYQBsACAAdQBzAGUAcgBzACwAIABjAG8AbgBzAGkAZABlAHIAIAB1AHMAaQBuAGcAIABvAG4AZQAgAG8AZgAgAHQAaABlACAAcwBpAG0AcABsAGUAcgAgAHcAcgBhAHAAcABlAHIAIABmAHUAbgBjAHQAaQBvAG4AcwA6AFwAbgAgACAAIAAgACAAIAAgAC0AIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABRACgAUAAsACAAUQApAFwAbgAgACAAIAAgACAAIAAgAC0AIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABTACgAUAAsACAAUwApAFwAbgAgACAAIAAgACAAIAAgAC0AIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUQBTACgAUQAsACAAUwApAFwAbgAgACAAIAAtACAAVABoAGkAcwAgAGYAdQBuAGMAdABpAG8AbgAgAGkAcwAgAGkAbgB0AGUAbgBkAGUAZAAgAGYAbwByACAAYQBkAHYAYQBuAGMAZQBkACAAdQBzAGUAIABjAGEAcwBlAHMAIABhAG4AZAAgAFUASQAtAGkAbgB0AGUAZwByAGEAdABlAGQAIABvAHUAdABwAHUAdAAuAFwAbgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBTAE8ATABWAEUAUgAgAD0AXABuAEwAQQBNAEIARABBACgAdgBhAGwAXwAxACwAIAB2AGEAbABfADIALAAgAFsAbQBvAGQAZQBdACwAIABbAGYAbwByAG0AYQB0AF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEgAYQBuAGQAbABlACAAbwBwAHQAaQBvAG4AYQBsACAAYQByAGcAdQBtAGUAbgB0AHMAXABuACAAIAAgACAAcgBhAHcAXwBtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAgACsAIAAoAG0AbwBkAGUAIAA9ACAAXAAiAFwAIgApACwAIABcACIAUABRAFwAIgAsACAAbQBvAGQAZQApACwAXABuACAAIAAgACAAbgBvAHIAbQBfAG0AbwBkAGUALAAgAFQARQBYAFQASgBPAEkATgAoAFwAIgBcACIALAAsAFMATwBSAFQAKABNAEkARAAoAEwATwBXAEUAUgAoAHIAYQB3AF8AbQBvAGQAZQApACwAUwBFAFEAVQBFAE4AQwBFACgATABFAE4AKAByAGEAdwBfAG0AbwBkAGUAKQApACwAMQApACkAKQAsAFwAbgAgACAAIAAgAG0AbwBkAGUALAAgAG4AbwByAG0AXwBtAG8AZABlACwAXABuAFwAbgAgACAAIAAgAGYAbwByAG0AYQB0ACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGYAbwByAG0AYQB0ACkAIAArACAAKABmAG8AcgBtAGEAdAAgAD0AIABcACIAXAAiACkALAAgAFwAIgBiAGEAcgBlAFwAIgAsACAATABPAFcARQBSACgAZgBvAHIAbQBhAHQAKQApACwAXABuACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADQALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABJAG4AcAB1AHQAIAB1AG4AcABhAGMAawBpAG4AZwAgAGIAeQAgAG0AbwBkAGUAXABuACAAIAAgACAAUABfAGkAbgAsACAASQBGACgATwBSACgAbQBvAGQAZQA9AFwAIgBwAHEAXAAiACwAIABtAG8AZABlAD0AXAAiAHAAcwBcACIAKQAsACAAdgBhAGwAXwAxACwAIABOAEEAKAApACkALABcAG4AIAAgACAAIABRAF8AaQBuACwAIABJAEYAKABtAG8AZABlAD0AXAAiAHAAcQBcACIALAAgAHYAYQBsAF8AMgAsACAASQBGACgAbQBvAGQAZQA9AFwAIgBxAHMAXAAiACwAIAB2AGEAbABfADEALAAgAE4AQQAoACkAKQApACwAXABuACAAIAAgACAAUwBfAGkAbgAsACAASQBGACgATwBSACgAbQBvAGQAZQA9AFwAIgBwAHMAXAAiACwAIABtAG8AZABlAD0AXAAiAHEAcwBcACIAKQAsACAAdgBhAGwAXwAyACwAIABOAEEAKAApACkALABcAG4AXABuACAAIAAgACAALwAvACAAUAAgAGEAbgBkACAAUQAgAG8AcgBkAGUAcgBpAG4AZwAgAG8AbgBsAHkAIAB1AHMAZQBkACAAaQBuACAAJwBwAHEAJwAgAG0AbwBkAGUAXABuACAAIAAgACAAUAAsACAASQBGACgAQQBOAEQAKABJAFMATgBVAE0AQgBFAFIAKABQAF8AaQBuACkALAAgAEkAUwBOAFUATQBCAEUAUgAoAFEAXwBpAG4AKQApACwAIABNAEEAWAAoAFAAXwBpAG4ALAAgAFEAXwBpAG4AKQAsACAAUABfAGkAbgApACwAXABuACAAIAAgACAAUQAsACAASQBGACgAQQBOAEQAKABJAFMATgBVAE0AQgBFAFIAKABQAF8AaQBuACkALAAgAEkAUwBOAFUATQBCAEUAUgAoAFEAXwBpAG4AKQApACwAIABNAEkATgAoAFAAXwBpAG4ALAAgAFEAXwBpAG4AKQAsACAAUQBfAGkAbgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBcAG4AIAAgACAAIABTAF8AYwBhAGwAYwAsACAASQBGACgAUAAgAD0AIABRACwAIABOAEEAKAApACwAIABSAE8AVQBOAEQAKAAoAFAAIAAqACAAUQApACAALwAgACgAUAAgAC0AIABRACkALAAgAHAAcgBlAGMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEQAaQByAGUAYwB0AGkAbwBuAC0AYQB3AGEAcgBlACAAaQBuAHYAZQByAHMAZQAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBzAFwAbgAgACAAIAAgAFEAXwBjAGEAbABjACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFAAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFMAXwBpAG4AKQApACkALAAgAE4AQQAoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAoAFAAIAAqACAAUwBfAGkAbgApACAALwAgAEEAQgBTACgAUAAgAC0AIABTAF8AaQBuACkALAAgAHAAcgBlAGMAKQApACwAXABuAFwAbgAgACAAIAAgAFAAXwBjAGEAbABjACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFEAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFMAXwBpAG4AKQApACkALAAgAE4AQQAoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAoAFEAIAAqACAAUwBfAGkAbgApACAALwAgAEEAQgBTACgAUQAgAC0AIABTAF8AaQBuACkALAAgAHAAcgBlAGMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAZQBsAGUAYwB0AGUAZAAgAHIAZQBzAHUAbAB0ACAAdgBhAGwAdQBlAHMAXABuACAAIAAgACAAUABfAHYAYQBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBxAHMAXAAiACwAIABQAF8AYwBhAGwAYwAsACAAUAApACwAXABuACAAIAAgACAAUQBfAHYAYQBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBwAHMAXAAiACwAIABRAF8AYwBhAGwAYwAsACAAUQApACwAXABuACAAIAAgACAAUwBfAHYAYQBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBwAHEAXAAiACwAIABTAF8AYwBhAGwAYwAsACAAUwBfAGkAbgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAbwBsAHYAZQBkACAAbABhAGIAZQBsAFwAbgAgACAAIAAgAGwAYQBiAGUAbAAsACAAUwBXAEkAVABDAEgAKABtAG8AZABlACwAIABcACIAcABxAFwAIgAsACAAXAAiAFMAXAAiACwAIABcACIAcABzAFwAIgAsACAAXAAiAFEAXAAiACwAIABcACIAcQBzAFwAIgAsACAAXAAiAFAAXAAiACwAIABcACIAPwBcACIAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABQAHIAaQBtAGEAcgB5ACAAcwBjAGEAbABhAHIAIAByAGUAcwB1AGwAdABcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsACAAUwBXAEkAVABDAEgAKABtAG8AZABlACwAIABcACIAcABxAFwAIgAsACAAUwBfAGMAYQBsAGMALAAgAFwAIgBwAHMAXAAiACwAIABRAF8AYwBhAGwAYwAsACAAXAAiAHEAcwBcACIALAAgAFAAXwBjAGEAbABjACwAIABOAEEAKAApACkALABcAG4AXABuACAAIAAgACAALwAvACAAVgBlAHIAYgBvAHMAZQAgAHQAZQB4AHQAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAB2AGUAcgBiAG8AcwBlAF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAXAAiAFAAIAA9ACAAXAAiACAAJgAgAEkARgAoAEkAUwBOAFUATQBCAEUAUgAoAFAAXwB2AGEAbAApACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBxAHMAXAAiACwAIABcACIAHiYgAFwAIgAgACYAIABQAF8AdgBhAGwALAAgAFAAXwB2AGEAbAApACwAIABcACIAFCBcACIAKQAgACYAIABcACIALAAgAFwAIgAgACYAXABuACAAIAAgACAAIAAgAFwAIgBRACAAPQAgAFwAIgAgACYAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABRAF8AdgBhAGwAKQAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAcABzAFwAIgAsACAAXAAiAB4mIABcACIAIAAmACAAUQBfAHYAYQBsACwAIABRAF8AdgBhAGwAKQAsACAAXAAiABQgXAAiACkAIAAmACAAXAAiACwAIABcACIAIAAmAFwAbgAgACAAIAAgACAAIABcACIAUwAgAD0AIABcACIAIAAmACAASQBGACgASQBTAE4AVQBNAEIARQBSACgAUwBfAHYAYQBsACkALAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAXAAiAHAAcQBcACIALAAgAFwAIgAeJiAAXAAiACAAJgAgAFMAXwB2AGEAbAAsACAAUwBfAHYAYQBsACkALAAgAFwAIgAUIFwAIgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAcABpAGwAbABhAGIAbABlACAAdABhAGIAdQBsAGEAcgAgAG8AdQB0AHAAdQB0AHMAXABuACAAIAAgACAAcgBvAHcAXwBvAHUAdAAsAFwAbgAgACAAIAAgACAAIABWAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABtAG8AZABlAD0AXAAiAHEAcwBcACIALAAgAFwAIgBQACAAHiZcACIALAAgAFwAIgBQACAAPQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAG0AbwBkAGUAPQBcACIAcABzAFwAIgAsACAAXAAiAFEAIAAeJlwAIgAsACAAXAAiAFEAIAA9AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAbQBvAGQAZQA9AFwAIgBwAHEAXAAiACwAIABcACIAUwAgAB4mXAAiACwAIABcACIAUwAgAD0AXAAiACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFAAXwB2AGEAbAAsACAAUQBfAHYAYQBsACwAIABTAF8AdgBhAGwAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIABjAG8AbABfAG8AdQB0ACwAXABuACAAIAAgACAAIAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAEkARgAoAG0AbwBkAGUAPQBcACIAcQBzAFwAIgAsACAAXAAiAFAAIAAeJlwAIgAsACAAXAAiAFAAIAA9AFwAIgApACwAIABQAF8AdgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABJAEYAKABtAG8AZABlAD0AXAAiAHAAcwBcACIALAAgAFwAIgBRACAAHiZcACIALAAgAFwAIgBRACAAPQBcACIAKQAsACAAUQBfAHYAYQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgASQBGACgAbQBvAGQAZQA9AFwAIgBwAHEAXAAiACwAIABcACIAUwAgAB4mXAAiACwAIABcACIAUwAgAD0AXAAiACkALAAgAFMAXwB2AGEAbAApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEYAaQBuAGEAbAAgAHMAdwBpAHQAYwBoACAAZgBvAHIAIAByAGUAdAB1AHIAbgAgAHQAeQBwAGUAXABuACAAIAAgACAAbwB1AHQAcAB1AHQALABcAG4AIAAgACAAIAAgACAAUwBXAEkAVABDAEgAKABmAG8AcgBtAGEAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAGIAYQByAGUAXAAiACwAIAByAGUAcwB1AGwAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAGwAYQBiAGUAbABlAGQAXAAiACwAIABsAGEAYgBlAGwAIAAmACAAXAAiACAAPQAgAFwAIgAgACYAIAByAGUAcwB1AGwAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAHYAZQByAGIAbwBzAGUAXAAiACwAIAB2AGUAcgBiAG8AcwBlAF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgByAG8AdwBcACIALAAgAHIAbwB3AF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBjAG8AbABcACIALAAgAGMAbwBsAF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBJAG4AdgBhAGwAaQBkACAAZgBvAHIAbQBhAHQAXAAiAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFAAUQBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAGEAbABjAHUAbABhAHQAZQBzACAAdABoAGUAIABzAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIAAoAFMAKQAgAGIAZQB0AHcAZQBlAG4AIAB0AHcAbwAgAHAAbABhAG4AZQB0AGEAcgB5ACAAYgBvAGQAaQBlAHMAXABuACAAIAAgAGIAYQBzAGUAZAAgAG8AbgAgAHQAaABlAGkAcgAgAHMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZABzACAAUAAgAGEAbgBkACAAUQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAUAAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZAAgAG8AZgAgAHQAaABlACAAaQBuAG4AZQByACAAKABmAGEAcwB0AGUAcgApACAAYgBvAGQAeQBcAG4AIAAgACAALQAgAFEAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABTAGkAZABlAHIAZQBhAGwAIABvAHIAYgBpAHQAYQBsACAAcABlAHIAaQBvAGQAIABvAGYAIAB0AGgAZQAgAG8AdQB0AGUAcgAgACgAcwBsAG8AdwBlAHIAKQAgAGIAbwBkAHkAXABuACAAIAAgAC0AIABvAHUAdABwAHUAdAAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AdQB0AHAAdQB0ACAAZgBvAHIAbQBhAHQALgAgAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAYgBhAHIAZQBcACIAIAA9ACAAUgBlAHQAdQByAG4AcwAgAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgAG8AbgBsAHkAIAAoAGQAZQBmAGEAdQBsAHQAKQBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAHYAZQByAGIAbwBzAGUAXAAiACAAPQAgAFIAZQB0AHUAcgBuAHMAIABhACAAMgAtAGMAbwBsAHUAbQBuACAAdgBlAHIAdABpAGMAYQBsACAAdABhAGIAbABlADoAIABQACwAIABRACwAIABTACwAIAB3AGkAdABoACAAdABoAGUAIAByAGUAcwB1AGwAdAAgAGYAbABhAGcAZwBlAGQAIAAoAB4mKQBcAG4AIAAgACAALQAgAHAAcgBlAGMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABEAGUAYwBpAG0AYQBsACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAANAApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAUwB5AG4AbwBkAGkAYwAgAHAAZQByAGkAbwBkACAAKABiAGEAcgBlACkALAAgAG8AcgBcAG4AIAAgACAALQAgAFYAZQByAGIAbwBzAGUAIAAyAC0AYwBvAGwAdQBtAG4AIABhAHIAcgBhAHkAIAB3AGkAdABoACAAbABhAGIAZQBsAGUAZAAgAFAALAAgAFEALAAgAGEAbgBkACAAUwAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACAAKABTACAAaQBzACAAZgBsAGEAZwBnAGUAZAAgAHcAaQB0AGgAIABhACAAHiYgAHQAbwAgAGkAbgBkAGkAYwBhAHQAZQAgAGkAdAAnAHMAIAB0AGgAZQAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlACkAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFMAIAA9ACAAKABQACAA1wAgAFEAKQAgAC8AIAB8AFAAIAASIiAAUQB8ACwAIABhAHMAcwB1AG0AaQBuAGcAIABQACAAYCIgAFEAXABuACAAIAAgAC0AIABJAG4AcAB1AHQAcwAgAG0AYQB5ACAAYgBlACAAcAByAG8AdgBpAGQAZQBkACAAaQBuACAAYQBuAHkAIABvAHIAZABlAHIAOwAgAHQAaABlACAAZgB1AG4AYwB0AGkAbwBuACAAaQBuAHQAZQByAG4AYQBsAGwAeQAgAGEAcwBzAGkAZwBuAHMAIABQAC8AUQAgAGYAbwByACAAYwBvAHIAcgBlAGMAdAAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBcAG4AIAAgACAALQAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABwAHIAZQBkAGkAYwB0AGkAbgBnACAAYwBvAG4AagB1AG4AYwB0AGkAbwBuACAAaQBuAHQAZQByAHYAYQBsAHMAIABvAHIAIABvAHIAYgBpAHQAYQBsACAAcgBlAHMAbwBuAGEAbgBjAGUAIABtAG8AZABlAGwAaQBuAGcAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBQAFEAKAAzADYANQAuADIANQAsACAANgA4ADcALAAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAsACAANAApAFwAbgAgACAAIAAgACAAkiFcAG4AIAAgACAAIAAgACAAIABQACAAPQAgACAAIAAgACAAIAAzADYANQAuADIANQBcAG4AIAAgACAAIAAgACAAIABRACAAPQAgACAAIAAgACAAIAA2ADgANwBcAG4AIAAgACAAIAAgACAAIABTACAAHiYgAD0AIAAgACAAIAA3ADcAOQAuADgAOAAxADEAXABuACoALwBcAG4AXABuAFwAbgBBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABRACAAPQBcAG4ATABBAE0AQgBEAEEAKABQACwAIABRACwAIABbAG8AdQB0AHAAdQB0AF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEgAYQBuAGQAbABlACAAbwBwAHQAaQBvAG4AYQBsACAAYQByAGcAdQBtAGUAbgB0AHMAXABuACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABvAHUAdABwAHUAdAApACAAKwAgACgAbwB1AHQAcAB1AHQAIAA9ACAAXAAiAFwAIgApACwAIABcACIAYgBhAHIAZQBcACIALAAgAEwATwBXAEUAUgAoAG8AdQB0AHAAdQB0ACkAKQAsAFwAbgAgACAAIAAgAGQAaQBnAGkAdABzACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANAAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAbwByAHQAIABmAG8AcgAgAHMAdABhAGIAaQBsAGkAdAB5ACAAaQBuACAAcwB5AG4AbwBkAGkAYwAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBcAG4AIAAgACAAIABBACwAIABNAEEAWAAoAFAALAAgAFEAKQAsAFwAbgAgACAAIAAgAEIALAAgAE0ASQBOACgAUAAsACAAUQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEMAYQBsAGMAdQBsAGEAdABlACAAcwB5AG4AbwBkAGkAYwAgAHAAZQByAGkAbwBkAFwAbgAgACAAIAAgAFMALAAgAFIATwBVAE4ARAAoACgAQQAgACoAIABCACkAIAAvACAAKABBACAALQAgAEIAKQAsACAAZABpAGcAaQB0AHMAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABUAHcAbwAtAGMAbwBsAHUAbQBuACAAdgBlAHIAYgBvAHMAZQAgAG8AdQB0AHAAdQB0ACAAKABsAGEAYgBlAGwAcwAgAHAAcgBlAHMAZQByAHYAZQBkACkAXABuACAAIAAgACAAdgBlAHIAYgBvAHMAZQAsAFwAbgAgACAAIAAgACAAIABWAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcACIAUAAgAD0AXAAiACwAIABQACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAFEAIAA9AFwAIgAsACAAUQApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAIgBTACAAHiZcACIALAAgAFMAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABPAHUAdABwAHUAdAAgAHMAZQBsAGUAYwB0AGkAbwBuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAsACAAdgBlAHIAYgBvAHMAZQAsACAAUwApACwAXABuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0AFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFAAUwBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAGEAbABjAHUAbABhAHQAZQBzACAAdABoAGUAIABzAGkAZABlAHIAZQBhAGwAIABvAHIAYgBpAHQAYQBsACAAcABlAHIAaQBvAGQAIABRACAAbwBmACAAdABoAGUAIABvAHUAdABlAHIAIABiAG8AZAB5AFwAbgAgACAAIABiAGEAcwBlAGQAIABvAG4AIAB0AGgAZQAgAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgACgAUwApACAAYQBuAGQAIAB0AGgAZQAgAGsAbgBvAHcAbgAgAGkAbgBuAGUAcgAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZAAgACgAUAApAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABQACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAUwBpAGQAZQByAGUAYQBsACAAbwByAGIAaQB0AGEAbAAgAHAAZQByAGkAbwBkACAAbwBmACAAdABoAGUAIABpAG4AbgBlAHIAIAAoAGYAYQBzAHQAZQByACkAIABiAG8AZAB5AFwAbgAgACAAIAAtACAAUwAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgACgAbwBiAHMAZQByAHYAZQBkACAAaQBuAHQAZQByAHYAYQBsACAAYgBlAHQAdwBlAGUAbgAgAGMAbwBuAGoAdQBuAGMAdABpAG8AbgBzACkAXABuACAAIAAgAC0AIABvAHUAdABwAHUAdAAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AdQB0AHAAdQB0ACAAZgBvAHIAbQBhAHQALgAgAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAYgBhAHIAZQBcACIAIAA9ACAAUgBlAHQAdQByAG4AcwAgAFEAIABvAG4AbAB5ACAAKABkAGUAZgBhAHUAbAB0ACkAXABuACAAIAAgACAAIAAgACAALQAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAgAD0AIABSAGUAdAB1AHIAbgBzACAAYQAgADIALQBjAG8AbAB1AG0AbgAgAHYAZQByAHQAaQBjAGEAbAAgAHQAYQBiAGwAZQA6ACAAUAAsACAAUQAsACAAUwAsACAAdwBpAHQAaAAgAFEAIABmAGwAYQBnAGcAZQBkACAAKAAeJikAXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADQAKQBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAALQAgAFMAaQBkAGUAcgBlAGEAbAAgAHAAZQByAGkAbwBkACAAUQAgACgAYgBhAHIAZQApACwAIABvAHIAXABuACAAIAAgAC0AIABWAGUAcgBiAG8AcwBlACAAMgAtAGMAbwBsAHUAbQBuACAAYQByAHIAYQB5ACAAdwBpAHQAaAAgAGwAYQBiAGUAbABlAGQAIABQACwAIABRACwAIABhAG4AZAAgAFMAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACgAUQAgAGkAcwAgAGYAbABhAGcAZwBlAGQAIAB3AGkAdABoACAAHiYgAHQAbwAgAGkAbgBkAGkAYwBhAHQAZQAgAGkAdAAnAHMAIAB0AGgAZQAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlACkAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFEAIAA9ACAAKABQACAA1wAgAFMAKQAgAC8AIAAoAFAAIAASIiAAUwApAFwAbgAgACAAIAAtACAAQQBzAHMAdQBtAGUAcwAgAFMAIAA8ACAAUAAgACgAcwB5AG4AbwBkAGkAYwAgAHAAZQByAGkAbwBkACAAbQB1AHMAdAAgAGIAZQAgAHMAaABvAHIAdABlAHIAIAB0AGgAYQBuACAAcwBsAG8AdwBlAHIAIABiAG8AZAB5ACcAcwAgAG8AcgBiAGkAdAApAFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAZgBvAHIAIABzAHkAcwB0AGUAbQBzACAAdwBoAGUAcgBlACAAcwB5AG4AbwBkAGkAYwAgAGkAbgB0AGUAcgB2AGEAbABzACAAYQByAGUAIABtAGUAYQBzAHUAcgBlAGQAIABhAG4AZAAgAGkAbgBuAGUAcgAgAGIAbwBkAHkAIABpAHMAIABrAG4AbwB3AG4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBQAFMAKAAzADYANQAuADIANQAsACAANwA3ADkALgA4ADgAMQAxACwAIABcACIAdgBlAHIAYgBvAHMAZQBcACIALAAgADQAKQBcAG4AIAAgACAAIAAgAJIhXABuACAAIAAgACAAIAAgACAAUAAgAD0AIAAgACAAIAAgACAAMwA2ADUALgAyADUAXABuACAAIAAgACAAIAAgACAAUQAgAB4mIAA9ACAAIAAgACAANgA4ADcAXABuACAAIAAgACAAIAAgACAAUwAgAD0AIAAgACAAIAAgACAANwA3ADkALgA4ADgAMQAxAFwAbgAqAC8AXABuAFwAbgBcAG4AQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFAAUwAgAD0AXABuAEwAQQBNAEIARABBACgAUAAsACAAUwAsACAAWwBvAHUAdABwAHUAdABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAIABhAHIAZwB1AG0AZQBuAHQAIABoAGEAbgBkAGwAaQBuAGcAXABuACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABvAHUAdABwAHUAdAApACAAKwAgACgAbwB1AHQAcAB1AHQAIAA9ACAAXAAiAFwAIgApACwAIABcACIAYgBhAHIAZQBcACIALAAgAEwATwBXAEUAUgAoAG8AdQB0AHAAdQB0ACkAKQAsAFwAbgAgACAAIAAgAGQAaQBnAGkAdABzACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANAAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABRACAAKABvAHUAdABlAHIAIABvAHIAYgBpAHQAKQBcAG4AIAAgACAAIABRACwAIABSAE8AVQBOAEQAKAAoAFAAIAAqACAAUwApACAALwAgAEEAQgBTACgAUAAgAC0AIABTACkALAAgAGQAaQBnAGkAdABzACkALABcAG4AXABuACAAIAAgACAALwAvACAAVgBlAHIAYgBvAHMAZQAgAHMAcABpAGwAbAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAIAAgAHYAZQByAGIAbwBzAGUALABcAG4AIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAFAAIAA9AFwAIgAsACAAUAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAIgBRACAAHiZcACIALAAgAFEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcACIAUwAgAD0AXAAiACwAIABTACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAATwB1AHQAcAB1AHQAIABjAGgAbwBpAGMAZQBcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAdgBlAHIAYgBvAHMAZQBcACIALAAgAHYAZQByAGIAbwBzAGUALAAgAFEAKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBRAFMAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBhAGwAYwB1AGwAYQB0AGUAcwAgAHQAaABlACAAcwBpAGQAZQByAGUAYQBsACAAbwByAGIAaQB0AGEAbAAgAHAAZQByAGkAbwBkACAAUAAgAG8AZgAgAHQAaABlACAAaQBuAG4AZQByACAAKABmAGEAcwB0AGUAcgApACAAYgBvAGQAeQBcAG4AIAAgACAAYgBhAHMAZQBkACAAbwBuACAAdABoAGUAIABzAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIAAoAFMAKQAgAGEAbgBkACAAdABoAGUAIABrAG4AbwB3AG4AIABvAHUAdABlAHIAIABvAHIAYgBpAHQAYQBsACAAcABlAHIAaQBvAGQAIAAoAFEAKQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAUQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZAAgAG8AZgAgAHQAaABlACAAbwB1AHQAZQByACAAKABzAGwAbwB3AGUAcgApACAAYgBvAGQAeQBcAG4AIAAgACAALQAgAFMAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABTAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIAAoAG8AYgBzAGUAcgB2AGUAZAAgAGkAbgB0AGUAcgB2AGEAbAAgAGIAZQB0AHcAZQBlAG4AIABjAG8AbgBqAHUAbgBjAHQAaQBvAG4AcwApAFwAbgAgACAAIAAtACAAbwB1AHQAcAB1AHQAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABPAHUAdABwAHUAdAAgAGYAbwByAG0AYQB0AC4AIABcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGIAYQByAGUAXAAiACAAPQAgAFIAZQB0AHUAcgBuAHMAIABQACAAbwBuAGwAeQAgACgAZABlAGYAYQB1AGwAdAApAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAdgBlAHIAYgBvAHMAZQBcACIAIAA9ACAAUgBlAHQAdQByAG4AcwAgAGEAIAAyAC0AYwBvAGwAdQBtAG4AIAB2AGUAcgB0AGkAYwBhAGwAIAB0AGEAYgBsAGUAOgAgAFAALAAgAFEALAAgAFMALAAgAHcAaQB0AGgAIABQACAAZgBsAGEAZwBnAGUAZAAgACgAHiYpAFwAbgAgACAAIAAtACAAcAByAGUAYwAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAEQAZQBjAGkAbQBhAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAA0ACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABTAGkAZABlAHIAZQBhAGwAIABwAGUAcgBpAG8AZAAgAFAAIAAoAGIAYQByAGUAKQAsACAAbwByAFwAbgAgACAAIAAtACAAVgBlAHIAYgBvAHMAZQAgADIALQBjAG8AbAB1AG0AbgAgAGEAcgByAGEAeQAgAHcAaQB0AGgAIABsAGEAYgBlAGwAZQBkACAAUAAsACAAUQAsACAAYQBuAGQAIABTACAAdgBhAGwAdQBlAHMAXABuACAAIAAgACAAIAAoAFAAIABpAHMAIABmAGwAYQBnAGcAZQBkACAAdwBpAHQAaAAgAB4mIAB0AG8AIABpAG4AZABpAGMAYQB0AGUAIABpAHQAJwBzACAAdABoAGUAIABzAG8AbAB2AGUAZAAgAHYAYQBsAHUAZQApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABQACAAPQAgACgAUQAgANcAIABTACkAIAAvACAAKABRACAAKwAgAFMAKQBcAG4AIAAgACAALQAgAFUAcwBlAGQAIAB3AGgAZQBuACAAdABoAGUAIABzAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIABhAG4AZAAgAHMAbABvAHcAZQByACAAbwByAGIAaQB0ACAAYQByAGUAIABrAG4AbwB3AG4AIAAoAGUALgBnAC4ALAAgAG8AYgBzAGUAcgB2AGEAdABpAG8AbgBhAGwAIABhAHMAdAByAG8AbgBvAG0AeQApAFwAbgAgACAAIAAtACAATwB1AHQAcAB1AHQAIABsAGEAeQBvAHUAdAAgAGkAcwAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIABhAGMAcgBvAHMAcwAgAGEAbABsACAAcwB5AG4AbwBkAGkAYwAgAHMAbwBsAHYAZQByACAAZgB1AG4AYwB0AGkAbwBuAHMAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBRAFMAKAA2ADgANwAsACAANwA3ADkALgA4ADgAMQAxACwAIABcACIAdgBlAHIAYgBvAHMAZQBcACIALAAgADQAKQBcAG4AIAAgACAAIAAgAJIhXABuACAAIAAgACAAIAAgACAAUAAgAB4mIAA9ACAAIAAgACAAMwA2ADUALgAyADUAXABuACAAIAAgACAAIAAgACAAUQAgAD0AIAAgACAAIAAgACAANgA4ADcAXABuACAAIAAgACAAIAAgACAAUwAgAD0AIAAgACAAIAAgACAANwA3ADkALgA4ADgAMQAxAFwAbgAqAC8AXABuAFwAbgBcAG4AQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFEAUwAgAD0AXABuAEwAQQBNAEIARABBACgAUQAsACAAUwAsACAAWwBvAHUAdABwAHUAdABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG8AdQB0AHAAdQB0ACkAIAArACAAKABvAHUAdABwAHUAdAAgAD0AIABcACIAXAAiACkALAAgAFwAIgBiAGEAcgBlAFwAIgAsACAATABPAFcARQBSACgAbwB1AHQAcAB1AHQAKQApACwAXABuACAAIAAgACAAZABpAGcAaQB0AHMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAA0ACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAAQwBvAHIAcgBlAGMAdAAgAGYAbwByAG0AdQBsAGEAOgAgAFAAIAA9ACAAKABRACAAKgAgAFMAKQAgAC8AIAAoAFEAIAArACAAUwApAFwAbgAgACAAIAAgAFAALAAgAFIATwBVAE4ARAAoACgAUQAgACoAIABTACkAIAAvACAAKABRACAAKwAgAFMAKQAsACAAZABpAGcAaQB0AHMAKQAsAFwAbgBcAG4AIAAgACAAIAB2AGUAcgBiAG8AcwBlACwAXABuACAAIAAgACAAIAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAIgBQACAAHiZcACIALAAgAFAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcACIAUQAgAD0AXAAiACwAIABRACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAFMAIAA9AFwAIgAsACAAUwApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAsACAAdgBlAHIAYgBvAHMAZQAsACAAUAApACwAXABuACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4AXABuAFMATQBBAEwATABBAE4ARwBMAEUAIAA9ACAATABBAE0AQgBEAEEAKABkAGkAYQBtAGUAdABlAHIALAAgAGQAaQBzAHQAYQBuAGMAZQAsAFwAbgBcAG4AIAAgACAAIAAwAC4ANQAzADIAOQAwADQAMgA5ADQAIAAqACAAKABkAGkAYQBtAGUAdABlAHIAIAAvACAAZABpAHMAdABhAG4AYwBlACkAXABuACAAIAAgACAAXABuACkAOwBcAG4AXABuAE8AUgBCAF8AQQBYAEkAUwAgAD0AIABMAEEATQBCAEQAQQAoAG0AYQBzAHMAMQAsACAAbQBhAHMAcwAyACwAIABwAGUAcgBpAG8AZAAsAFwAbgBcAG4ATABFAFQAKABcAG4AIAAgACAAIABtAGEAcwBzADIALAAgAEkARgAoACgASQBTAE8ATQBJAFQAVABFAEQAKABtAGEAcwBzADIAKQApACsAKABtAGEAcwBzADIAIAA9ACAAMQApACwAIAAwACwAIABtAGEAcwBzADIAKgAzAC4AMAAwADMARQAtADYAKQAsAFwAbgAgACAAIAAgAGEAeABpAHMALAAgAFAATwBXAEUAUgAoACgAUABPAFcARQBSACgAcABlAHIAaQBvAGQALAAgADIAKQAgACoAIAAoAG0AYQBzAHMAMQAgACsAIABtAGEAcwBzADIAKQApACwAIAAxACAALwAgADMAKQAsAFwAbgAgACAAIAAgAGEAeABpAHMAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ATwBSAEIAXwBQAEUAUgBJAE8ARAAgAD0AIABMAEEATQBCAEQAQQAoAG0AYQBzAHMAMQAsACAAbQBhAHMAcwAyACwAIABhAHgAaQBzACwAXABuAFwAbgBMAEUAVAAoAFwAbgAgACAAIAAgAG0AYQBzAHMAMgAsACAASQBGACgAKABJAFMATwBNAEkAVABUAEUARAAoAG0AYQBzAHMAMgApACkAKwAoAG0AYQBzAHMAMgAgAD0AIAAxACkALAAgADAALAAgACgAbQBhAHMAcwAyACAAKgAgADMALgAwADAAMgA3ADMAZQAtADYAKQApACwAXABuACAAIAAgACAAcABlAHIAaQBvAGQALAAgAFMAUQBSAFQAKABQAE8AVwBFAFIAKABhAHgAaQBzACwAIAAzACkAIAAvACAAKABtAGEAcwBzADEAIAArACAAbQBhAHMAcwAyACkAKQAsAFwAbgAgACAAIAAgAHAAZQByAGkAbwBkAFwAbgAgACAAIAAgACkAXABuACkAOwBcAG4AXABuAEMAUgBPAFMAUwBJAE4ARwBfAE8AUgBCAEkAVABfAFAAQQBSAEEATQBFAFQARQBSACAAPQAgAEwAQQBNAEIARABBACgAbQBhAHMAcwAxACwAIABtAGEAcwBzADIALABcAG4AXABuAEEAQgBTACgAbQBhAHMAcwAxACAALQAgAG0AYQBzAHMAMgApAC8AQQBCAFMAKABtAGEAcwBzADEAIAArAG0AYQBzAHMAMgApAFwAbgBcAG4AKQA7AFwAbgBcAG4AXABuAFwAbgBQAEUAUgBJAE8ARABfAEEAWABJAFMAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALABcAG4AXABuACAAIAAgACAAUABPAFcARQBSACgAUABPAFcARQBSACgAaQBuAHAAdQB0ACwAIAAyACkALAAgACgAMQAgAC8AIAAzACkAKQBcAG4AXABuACkAOwBcAG4AXABuAE8AUgBCAF8AUwBVAE0AXwBNAEEAUwBTAEUAUwAgAD0AIABMAEEATQBCAEQAQQAoAGEAeABpAHMALAAgAHAAZQByAGkAbwBkACwAXABuAFwAbgBQAE8AVwBFAFIAKABhAHgAaQBzACwAIAAzACkAIAAvACAAUABPAFcARQBSACgAcABlAHIAaQBvAGQALAAgADIAKQBcAG4AKQA7AFwAbgBcAG4AUwBQAEgARQBSAEkAQwBBAEwAXwBUAE8AXwBDAEEAUgBUAEUAUwBJAEEATgAgAD0AIABMAEEATQBCAEQAQQAoAHAAaABpACwAIAB0AGgAZQB0AGEALAAgAHIALAAgAFsAcAByAGUAYwBdACwAXABuAFwAbgBMAEUAVAAoAFwAbgAgACAAIABwAHIAZQBjACwAIABpAGYAKABcAG4AIAAgACAAIAAgACAAIAAgACgAaQBzAG8AbQBpAHQAdABlAGQAKABwAHIAZQBjACkAKQArAFwAbgAgACAAIAAgACAAIAAgACAAKABwAHIAZQBjADwAMAApACwAXABuACAAIAAgACAAIAAgACAAIAAzACwAXABuACAAIAAgACAAIAAgACAAIABwAHIAZQBjACkALAAgACAAIAAgAFwAbgAgACAAIAAgAHoAXwBtAG8AZAAsACAAcwBpAGcAbgAoAHQAaABlAHQAYQApACwAXABuACAAIAAgACAAeQBfAG0AbwBkACwAIABzAGkAZwBuACgAcABoAGkAKQAsAFwAbgAgACAAIAAgAHgAXwBtAG8AZAAsACAAaQBmACgAYQBiAHMAKABwAGgAaQApADwAOQAwACwAIAAxACwAIAAtADEAKQAsAFwAbgAgACAAIAAgAC8ALwB4AF8AbQBvAGQAXABuACAAIAAgACAALwAvAHQAZQB4AHQAagBvAGkAbgAoAFwAIgAsAFwAIgAsACwAeABfAG0AbwBkACwAIAB5AF8AbQBvAGQALAAgAHoAXwBtAG8AZAApAFwAbgAgACAAIAAgAGEAbgBnAF8AeAAsACAAcgBhAGQAaQBhAG4AcwAoAG0AbwBkACgAcABoAGkALAA5ADAAKQApACwAXABuACAAIAAgACAAYQBuAGcAXwB6ACwAIAByAGEAZABpAGEAbgBzACgAYQBiAHMAKAB0AGgAZQB0AGEAKQApACwAXABuACAAIAAgACAAZAAsACAAYwBvAHMAKABhAG4AZwBfAHoAKQAqAHIALABcAG4AIAAgACAAIAB4ACwAIAByAG8AdQBuAGQAKABjAG8AcwAoAGEAbgBnAF8AeAApACoAZAAqAHgAXwBtAG8AZAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAeQAsACAAcgBvAHUAbgBkACgAcwBpAG4AKABhAG4AZwBfAHgAKQAqAGQAKgB5AF8AbQBvAGQALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgAHoALAAgAHIAbwB1AG4AZAAoAHMAaQBuACgAYQBuAGcAXwB6ACkAKgByACoAegBfAG0AbwBkACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsACAAdABlAHgAdABqAG8AaQBuACgAXAAiAHwAXAAiACwALAB4ACwAIAB5ACwAIAB6ACkALABcAG4AIAAgACAAIAAvAC8AcgBlAHMAdQBsAHQAXABuACAAIAAgACAAdABvAHIAbwB3ACgAdABlAHgAdABzAHAAbABpAHQAKAByAGUAcwB1AGwAdAAsAFwAIgB8AFwAIgApACkAXABuACkAXABuAFwAbgApADsAXABuAFwAbgBEAEUARwBfAEQARQBDAF8ARABNAFMAIAA9ACAATABBAE0AQgBEAEEAKABEAGUAYwBpAG0AYQBsAEQAZQBnAHIAZQBlAHMALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAARABlAGcALAAgAFQAUgBVAE4AQwAoAEQAZQBjAGkAbQBhAGwARABlAGcAcgBlAGUAcwApACwAXABuACAAIAAgACAAIAAgACAAIABGAHIAYQBjAFAAbwByAHQAaQBvAG4ALAAgAEEAQgBTACgARABlAGMAaQBtAGEAbABEAGUAZwByAGUAZQBzACAALQAgAEQAZQBnACkALABcAG4AIAAgACAAIAAgACAAIAAgAE0AaQBuAHUAdABlAHMALAAgAEYAcgBhAGMAUABvAHIAdABpAG8AbgAgACoAIAA2ADAALABcAG4AIAAgACAAIAAgACAAIAAgAE0AaQBuAF8AcABhAHIAdAAsACAAVABSAFUATgBDACgATQBpAG4AdQB0AGUAcwApACAALwAgADEAMAAwACwAXABuACAAIAAgACAAIAAgACAAIABJAG4AdABNAGkAbgAsACAASQBOAFQAKABNAGkAbgB1AHQAZQBzACkALABcAG4AIAAgACAAIAAgACAAIAAgAEYAcgBhAGMATQBpAG4ALAAgAEEAQgBTACgATQBpAG4AdQB0AGUAcwAgAC0AIABJAG4AdABNAGkAbgApACwAXABuACAAIAAgACAAIAAgACAAIABTAGUAYwBvAG4AZABzACwAIABGAHIAYQBjAE0AaQBuACAAKgAgADYAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAcwBlAGMAXwBwAGEAcgB0ACwAIABTAGUAYwBvAG4AZABzACAALwAgADEAMAAwADAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAEQAZQBnACAAKwAgAE0AaQBuAF8AcABhAHIAdAAgACsAIABzAGUAYwBfAHAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAG8AdQB0AHAAdQB0ACwAIAA3ACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ARABFAEcAXwBEAE0AUwAgAD0AIABMAEEATQBCAEQAQQAoAEQAZQBjAGkAbQBhAGwARABlAGcAcgBlAGUAcwAsACAAWwBwAHIAZQBjAGkAcwBpAG8AbgBdACwAXABuAFwAbgBMAEUAVAAoAFwAbgAgACAAIAAgAGQAZQBjAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAUAByAGUAYwBpAHMAaQBvAG4AKQAsACAAMwAsACAAUAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgAgACAAIAAgAEQAZQBnACwAIABUAFIAVQBOAEMAKABEAGUAYwBpAG0AYQBsAEQAZQBnAHIAZQBlAHMAKQAsAFwAbgAgACAAIAAgAEYAcgBhAGMAUABvAHIAdABpAG8AbgAsACAAQQBCAFMAKABEAGUAYwBpAG0AYQBsAEQAZQBnAHIAZQBlAHMAIAAtACAARABlAGcAKQAsAFwAbgAgACAAIAAgAE0AaQBuAHUAdABlAHMALAAgAEYAcgBhAGMAUABvAHIAdABpAG8AbgAgACoAIAA2ADAALABcAG4AIAAgACAAIABJAG4AdABNAGkAbgAsACAASQBOAFQAKABNAGkAbgB1AHQAZQBzACkALABcAG4AIAAgACAAIABGAHIAYQBjAE0AaQBuACwAIABBAEIAUwAoAE0AaQBuAHUAdABlAHMAIAAtACAASQBuAHQATQBpAG4AKQAsAFwAbgAgACAAIAAgAFMAZQBjAG8AbgBkAHMALAAgAEYAcgBhAGMATQBpAG4AIAAqACAANgAwACwAXABuACAAIAAgACAARABlAGcAIAAmACAAXAAiALAAIABcACIAIAAmACAASQBuAHQATQBpAG4AIAAmACAAQwBIAEEAUgAoADMAOQApACAAJgAgAEMASABBAFIAKAAzADIAKQAgACYAIABGAEkAWABFAEQAKABTAGUAYwBvAG4AZABzACwAIABkAGUAYwBwAHIAZQBjACkAIAAmACAAQwBIAEEAUgAoADMANAApAFwAbgApAFwAbgApADsAXABuAFwAbgBEAEUARwBfAEQATQBTAF8ARABFAEMAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZABlAGcAcgBlAGUAcwAsACAAVABSAFUATgBDACgAaQBuAHAAdQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAG0AaQBuAHUAdABlAHMALAAgAFQAUgBVAE4AQwAoACgAaQBuAHAAdQB0ACAALQAgAGQAZQBnAHIAZQBlAHMAKQAgACoAIAAxADAAMAApACwAXABuACAAIAAgACAAIAAgACAAIABmAHIAYQBjAHQAaQBvAG4AYQBsAF8AcwBlAGMAbwBuAGQAcwAsACAAKAAoAGkAbgBwAHUAdAAgACoAIAAxADAAMAApACAALQAgAFQAUgBVAE4AQwAoAGkAbgBwAHUAdAAgACoAIAAxADAAMAApACkAIAAvACAAMAAuADYALABcAG4AIAAgACAAIAAgACAAIAAgAC8AKgAgACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQALAAgAGQAZQBnAHIAZQBlAHMAIAArACAAKAAoAG0AaQBuAHUAdABlAHMAIAArACAAZgByAGEAYwB0AGkAbwBuAGEAbABfAHMAZQBjAG8AbgBkAHMAKQAgAC8AIAA2ADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4AQQBYAEkAUwBfAFAARQBSAEkATwBEACAAPQAgAEwAQQBNAEIARABBACgAaQBuAHAAdQB0ACwAXABuAFwAbgAgACAAIAAgAFMAUQBSAFQAKABQAE8AVwBFAFIAKABpAG4AcAB1AHQALAAgADMAKQApAFwAbgAgACAAIAAgAFwAbgApADsAXABuAFwAbgAiAH0ALAB7ACIAcABhAHQAaAAiADoAIgAvAHAAcgBvAGoAZQBjAHQAcwAvAEcAZQBuAGUAcgBhAGwAIgAsACIAdABlAHgAdAAiADoAIgAvACoAIABSAEUAQwBJAFAAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIAByAGUAYwBpAHAAcgBvAGMAYQBsACAAKABtAHUAbAB0AGkAcABsAGkAYwBhAHQAaQB2AGUAIABpAG4AdgBlAHIAcwBlACkAIABvAGYAIABhACAAbgB1AG0AYgBlAHIALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHMAaQBuAGcAbABlACAAZABlAGMAaQBtAGEAbAAgAHYAYQBsAHUAZQAgAGUAcQB1AGEAbAAgAHQAbwAgADEAIABkAGkAdgBpAGQAZQBkACAAYgB5ACAAdABoAGUAIABpAG4AcAB1AHQALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAGkAbgBwAHUAdAAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAbgB5ACAAbgBvAG4AegBlAHIAbwAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAUgBlAHQAdQByAG4AcwAgAGAAIwBEAEkAVgAvADAAIQBgACAAaQBmACAAaQBuAHAAdQB0ACAAaQBzACAAegBlAHIAbwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGYAbABpAHAAcABpAG4AZwAgAGYAcgBhAGMAdABpAG8AbgBzACwAIABjAG8AbgB2AGUAcgB0AGkAbgBnACAAcgBhAHQAZQBzACAAKABlAC4AZwAuACwAIABIAHoAIACUISAAcwBlAGMAbwBuAGQAcwApACwAIABvAHIAIABpAG4AdgBlAHIAdABpAG4AZwAgAHIAYQB0AGkAbwBzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgACAAIABSAEUAQwBJAFAAKAA0ACkAIACSISAAMAAuADIANQBcAG4AIAAgACAAIAAgAFIARQBDAEkAUAAoADAALgAyACkAIACSISAANQBcAG4AKgAvAFwAbgBcAG4AXABuAFIARQBDAEkAUAAgAD0AIABMAEEATQBCAEQAQQAoAGkAbgBwAHUAdAAsACAAMQAgAC8AIABpAG4AcAB1AHQAKQA7AFwAbgBcAG4ALwAqACAARgBSAEEAQwA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIAAoAG4AbwBuAC0AaQBuAHQAZQBnAGUAcgApACAAcABhAHIAdAAgAG8AZgAgAGEAIABuAHUAbQBiAGUAcgAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIABBACAAcwBjAGEAbABhAHIAIABkAGUAYwBpAG0AYQBsACAAYgBlAHQAdwBlAGUAbgAgADAAIABhAG4AZAAgADEAIAAoAG8AcgAgAC0AMQAgAGEAbgBkACAAMAAgAGkAZgAgAHMAaQBnAG4AIABpAHMAIABwAHIAZQBzAGUAcgB2AGUAZAApAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABpAG4AcAB1AHQAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABUAGgAZQAgAG4AdQBtAGIAZQByACAAdABvACAAZQB4AHQAcgBhAGMAdAAgAHQAaABlACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIABmAHIAbwBtAC4AXABuACAAIAAgAC0AIABtAG8AZABlACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATwB1AHQAcAB1AHQAIABtAG8AZABlACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADAAKQBcAG4AIAAgACAAIAAgACAAIAAtACAAMAA6ACAAQQBsAHcAYQB5AHMAIAByAGUAdAB1AHIAbgAgAHAAbwBzAGkAdABpAHYAZQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABwAGEAcgB0AFwAbgAgACAAIAAgACAAIAAgAC0AIAAxADoAIABQAHIAZQBzAGUAcgB2AGUAIABzAGkAZwBuACAAbwBmACAAaQBuAHAAdQB0ACAAKABlAC4AZwAuACwAIAAtADMALgAyADUAIACSISAALQAwAC4AMgA1ACkAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAEMAbwBtAHAAbABlAG0AZQBuAHQAcwAgAEUAeABjAGUAbAAZIHMAIABUAFIAVQBOAEMAIABhAG4AZAAgAFEAVQBPAFQASQBFAE4AVAAgAGYAdQBuAGMAdABpAG8AbgBzAC4AXABuACAAIAAgAC0AIABVAHMAZQBmAHUAbAAgAGYAbwByACAAZABlAHQAZQBjAHQAaQBuAGcAIABkAGUAYwBpAG0AYQBsACAAcgBlAG0AYQBpAG4AZABlAHIAcwAgAGEAbgBkACAAYQBuAGEAbAB5AHoAaQBuAGcAIABvAGYAZgBzAGUAdABzACAAZgByAG8AbQAgAHcAaABvAGwAZQAgAHYAYQBsAHUAZQBzAC4AXABuACAAIAAgAC0AIABTAGkAZwBuAC0AcAByAGUAcwBlAHIAdgBpAG4AZwAgAG0AbwBkAGUAIABjAGEAbgAgAGkAbgBkAGkAYwBhAHQAZQAgAHcAaABlAHQAaABlAHIAIABhACAAdgBhAGwAdQBlACAAaQBzACAAagB1AHMAdAAgAGEAYgBvAHYAZQAgAG8AcgAgAGoAdQBzAHQAIABiAGUAbABvAHcAIABhAG4AIABpAG4AdABlAGcAZQByAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlAHMAOgBcAG4AIAAgACAARgBSAEEAQwAoAC0AMwAuADIANQApACAAIAAgACAAIAAgACAAkiEgADAALgAyADUAIAAgAFwAbgAgACAAIABGAFIAQQBDACgALQAzAC4AMgA1ACwAIAAxACkAIAAgACAAIACSISAALQAwAC4AMgA1AFwAbgAqAC8AXABuAFwAbgBcAG4ARgBSAEEAQwAgAD0AIABMAEEATQBCAEQAQQAoAGkAbgBwAHUAdAAsACAAWwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAARABlAGYAYQB1AGwAdAAgAG0AbwBkAGUAIAB0AG8AIAAwACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAGkAbgB2AGEAbABpAGQAXABuACAAIAAgACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAbQBvAGQAZQAgAD4AIAAxACkALAAgADAALAAgAG0AbwBkAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGIAeQAgAHMAdQBiAHQAcgBhAGMAdABpAG4AZwAgAGkAbgB0AGUAZwBlAHIAIABwAG8AcgB0AGkAbwBuAFwAbgAgACAAIAAgACAAIAAgACAAZgByAGEAYwBfAHAAYQByAHQALAAgAGkAbgBwAHUAdAAgAC0AIABUAFIAVQBOAEMAKABpAG4AcAB1AHQAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAFIAZQB0AHUAcgBuACAAcwBpAGcAbgBlAGQAIABvAHIAIABhAGIAcwBvAGwAdQB0AGUAIAB2AGEAbAB1AGUAIABkAGUAcABlAG4AZABpAG4AZwAgAG8AbgAgAG0AbwBkAGUAXABuACAAIAAgACAAIAAgACAAIABJAEYAKABtAG8AZABlACAAPQAgADEALAAgAGYAcgBhAGMAXwBwAGEAcgB0ACwAIABBAEIAUwAoAGYAcgBhAGMAXwBwAGEAcgB0ACkAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABSAE8ATwBUADoAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAeAAtAHQAaAAgAHIAbwBvAHQAIABvAGYAIABhACAAbgB1AG0AYgBlAHIAIAAoAG8AcgAgAHMAcQB1AGEAcgBlACAAcgBvAG8AdAAgAGkAZgAgAG4AbwAgAGQAZQBnAHIAZQBlACAAaQBzACAAcwBwAGUAYwBpAGYAaQBlAGQAKQAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIABBACAAcgBlAGEAbAAgAGQAZQBjAGkAbQBhAGwAIABuAHUAbQBiAGUAcgAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAdABoAGUAIAByAG8AbwB0ACAAbwBmACAAYABuAGAALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAG4AIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABUAGgAZQAgAG4AdQBtAGIAZQByACAAdABvACAAdABhAGsAZQAgAHQAaABlACAAcgBvAG8AdAAgAG8AZgAuAFwAbgAgACAAIAAtACAAeAAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAFQAaABlACAAcgBvAG8AdAAgAGQAZQBnAHIAZQBlAC4AIABEAGUAZgBhAHUAbAB0AHMAIAB0AG8AIAAyACAAKABzAHEAdQBhAHIAZQAgAHIAbwBvAHQAKQAuAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABSAGUAagBlAGMAdABzACAAYQBsAGwAIABuAGUAZwBhAHQAaQB2AGUAIABpAG4AcAB1AHQAIAB2AGEAbAB1AGUAcwAgAGYAbwByACAAYABuAGAALAAgAHIAZQBnAGEAcgBkAGwAZQBzAHMAIABvAGYAIAByAG8AbwB0AC4AXABuACAAIAAgAC0AIABNAGkAbQBpAGMAcwAgAEUAeABjAGUAbAAnAHMAIABiAGUAaABhAHYAaQBvAHIAIAAoAHIAZQB0AHUAcgBuAHMAIAAjAE4AVQBNACEAIABpAGYAIAByAG8AbwB0ACAAdwBvAHUAbABkACAAYgBlACAAYwBvAG0AcABsAGUAeAApAC4AXABuACAAIAAgAC0AIABVAHMAZQAgAEUAeABjAGUAbAAZIHMAIABgAEkATQBQAE8AVwBFAFIAYAAgAG8AcgAgAGAASQBNAFMAUQBSAFQAYAAgAGYAbwByACAAYwBvAG0AcABsAGUAeAAgAG4AdQBtAGIAZQByACAAcwB1AHAAcABvAHIAdAAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgAFIATwBPAFQAKAAxADYAKQAgACAAIAAgACAAIAAgAJIhIAA0AFwAbgAgACAAIABSAE8ATwBUACgAMgA3ACwAIAAzACkAIAAgACAAIACSISAAMwBcAG4AIAAgACAAUgBPAE8AVAAoADkALAAgADAALgA1ACkAIAAgACAAkiEgADgAMQBcAG4AIAAgACAAUgBPAE8AVAAoAC0ANQAsACAAMwApACAAIAAgACAAkiEgACMATgBVAE0AIQBcAG4AKgAvAFwAbgBcAG4AUgBPAE8AVAAgAD0AIABMAEEATQBCAEQAQQAoAG4ALAAgAFsAeABdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAHIAbwBvAHQAXwBkAGUAZwByAGUAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKAB4ACkALAAgADIALAAgAHgAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAbgAgADwAIAAwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFMAUQBSAFQAKAAtADEAKQAsACAAIAAvAC8AIABUAHIAaQBnAGcAZQByAHMAIAAjAE4AVQBNACEAIABlAHIAcgBvAHIAIABmAG8AcgAgAG4AZQBnAGEAdABpAHYAZQAgAGIAYQBzAGUAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAG4AIABeACAAKAAxACAALwAgAHIAbwBvAHQAXwBkAGUAZwByAGUAZQApAFwAbgAgACAAIAAgACAAIAAgACAAKQBcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVABcAG4AIAAgACAALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAYQAgAG8AbgBlAC0AbABpAG4AZQAsACAAbABhAGIAZQBsAGUAZAAgAHYAZQByAHMAaQBvAG4AIABvAGYAIAB0AGgAZQAgAGYAbwByAG0AdQBsAGEAIABpAG4AIAB0AGgAZQAgAGcAaQB2AGUAbgAgAGMAZQBsAGwALABcAG4AIAAgACAAbwBtAGkAdAB0AGkAbgBnACAAdABoAGUAIABsAGUAYQBkAGkAbgBnACAAZQBxAHUAYQBsACAAcwBpAGcAbgAgAGEAbgBkACAAcAByAGUAcABlAG4AZABpAG4AZwAgAHQAaABlACAAYwBlAGwAbAAgAHIAZQBmAGUAcgBlAG4AYwBlAC4AXABuAFwAbgAgACAAIABTAHkAbgB0AGEAeAA6AFwAbgAgACAAIAAgACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAKABjAGUAbABsACkAXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgACAAIABjAGUAbABsACAAOgAgAEEAIAByAGUAZgBlAHIAZQBuAGMAZQAgAHQAbwAgAGEAIABjAGUAbABsACAAYwBvAG4AdABhAGkAbgBpAG4AZwAgAGEAIABmAG8AcgBtAHUAbABhAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgACAAIABBACAAcwBpAG4AZwBsAGUALQBsAGkAbgBlACAAcwB0AHIAaQBuAGcAIABpAG4AIAB0AGgAZQAgAGYAbwByAG0AYQB0ACAAXAAiAEEAMQA6AD0AIABGAE8AUgBNAFUATABBACgALgAuAC4AKQBcACIAXABuACAAIAAgACAAIABVAHMAZQBmAHUAbAAgAGYAbwByACAAYQB1AGQAaQB0AGkAbgBnACwAIABkAG8AYwB1AG0AZQBuAHQAYQB0AGkAbwBuACwAIABkAGEAcwBoAGIAbwBhAHIAZABzACwAIABvAHIAIAB0AGUAYQBjAGgAaQBuAGcAIAB0AG8AbwBsAHMALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIAAgACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAKABCADMAKQAgACAAkiEgAFwAIgBCADMAOgA9ACAAUgBFAEMASQBQACgAUgBPAE8AVAAoAFAASQAoACkALAAzACkAKQBcACIAXABuACAAIAAgACAAIABGAE8AUgBNAFUATABBAF8AVABFAFgAVAAoAEMANQApACAAIACSISAAXAAiAEMANQA6AD0AIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAzACkAXAAiAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgACAAIAAtACAAVABoAGUAIAByAGUAcwB1AGwAdAAgAGkAcwAgAGUAcQB1AGkAdgBhAGwAZQBuAHQAIAB0AG8AOgAgAEMARQBMAEwAKABcACIAYQBkAGQAcgBlAHMAcwBcACIALAAgAGMAZQBsAGwAKQAgACYAIABcACIAOgA9ACAAXAAiACAAJgAgAFQARQBYAFQAQQBGAFQARQBSACgARgBPAFIATQBVAEwAQQBUAEUAWABUACgAYwBlAGwAbAApACwAIABcACIAPQBcACIAKQBcAG4AIAAgACAAIAAgAC0AIABJAGYAIAB0AGgAZQAgAHIAZQBmAGUAcgBlAG4AYwBlAGQAIABjAGUAbABsACAAZABvAGUAcwAgAG4AbwB0ACAAYwBvAG4AdABhAGkAbgAgAGEAIABmAG8AcgBtAHUAbABhACwAIABhAG4AIABlAHIAcgBvAHIAIAB3AGkAbABsACAAbwBjAGMAdQByAC4AXABuACAAIAAgACAAIAAtACAAVABoAGkAcwAgAGYAdQBuAGMAdABpAG8AbgAgAGQAbwBlAHMAIABuAG8AdAAgAGUAdgBhAGwAdQBhAHQAZQAgAG8AcgAgAGEAbAB0AGUAcgAgAHQAaABlACAAZgBvAHIAbQB1AGwAYQAUIG8AbgBsAHkAIABmAG8AcgBtAGEAdABzACAAaQB0ACAAZgBvAHIAIABkAGkAcwBwAGwAYQB5AC4AXABuACoALwBcAG4AXABuAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUAD0ATABBAE0AQgBEAEEAKABcAG4AIAAgAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACwAIAAgAC8ALwAgAEEAIAByAGUAZgBlAHIAZQBuAGMAZQAgAHQAbwAgAGEAIABjAGUAbABsACAAYwBvAG4AdABhAGkAbgBpAG4AZwAgAGEAIABmAG8AcgBtAHUAbABhAFwAbgBcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAAcgBhAHcALAAgAEYATwBSAE0AVQBMAEEAVABFAFgAVAAoAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABcACIAPQBSAEUAQwBJAFAAKABSAE8ATwBUACgAUABJACgAKQAsADMAKQApAFwAIgBcAG4AIAAgACAAIABjAGwAZQBhAG4ALAAgAFQARQBYAFQAQQBGAFQARQBSACgAcgBhAHcALAAgAFwAIgA9AFwAIgApACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABcACIAUgBFAEMASQBQACgAUgBPAE8AVAAoAFAASQAoACkALAAzACkAKQBcACIAXABuACAAIAAgACAAbABhAGIAZQBsACwAIABTAFUAQgBTAFQASQBUAFUAVABFACgAQwBFAEwATAAoAFwAIgBhAGQAZAByAGUAcwBzAFwAIgAsACAAZgBvAHIAbQB1AGwAYQBfAGMAZQBsAGwAKQAsACAAXAAiACQAXAAiACwAIABcACIAXAAiACkAIAAmACAAXAAiADoAPQAgAFwAIgAsAFwAbgAgACAAIAAgAGwAYQBiAGUAbAAgACYAIABjAGwAZQBhAG4AXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAUgBPAFUATgBEAF8ARgBJAFgAXABuACAAIAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAgACAAUgBvAHUAbgBkAHMAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAcwAgAGEAIABuAHUAbQBiAGUAcgAgAHQAbwAgAGEAIABzAHAAZQBjAGkAZgBpAGUAZAAgAG4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzAC4AXABuACAAIAAgAE8AcAB0AGkAbwBuAGEAbABsAHkAIAByAGUAdAB1AHIAbgBzACAAdABoAGUAIAByAGUAcwB1AGwAdAAgAGEAcwAgAGEAIABmAGkAeABlAGQALQB3AGkAZAB0AGgAIAB0AGUAeAB0ACAAcwB0AHIAaQBuAGcALAAgAHAAcgBlAHMAZQByAHYAaQBuAGcAIAB0AHIAYQBpAGwAaQBuAGcAIAB6AGUAcgBvAHMALgBcAG4AXABuACAAIAAgAFMAeQBuAHQAYQB4ADoAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAG4AdQBtAGIAZQByACwAIABwAGwAYQBjAGUAcwAsACAAWwBhAHMAXwB0AGUAeAB0AF0ALAAgAFsAdQBzAGUAXwByAG8AdQBuAGQAXQApAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAgACAAbgB1AG0AYgBlAHIAIAAgACAAIAAgACAAOgAgAFQAaABlACAAbgB1AG0AZQByAGkAYwAgAHYAYQBsAHUAZQAgAHQAbwAgAHAAcgBvAGMAZQBzAHMALgBcAG4AIAAgACAAIAAgAHAAbABhAGMAZQBzACAAIAAgACAAIAAgADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAZQB0AGEAaQBuAC4AXABuACAAIAAgACAAIABhAHMAXwB0AGUAeAB0ACAAIAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgAEYAQQBMAFMARQApAC4AIABJAGYAIABUAFIAVQBFACwAIAByAGUAdAB1AHIAbgBzACAAbwB1AHQAcAB1AHQAIABhAHMAIAB0AGUAeAB0ACAAKABlAC4AZwAuACwAIABcACIAMwAuADEANAAwAFwAIgApAC4AXABuACAAIAAgACAAIAB1AHMAZQBfAHIAbwB1AG4AZAAgACAAIAA6ACAATwBwAHQAaQBvAG4AYQBsACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgAEYAQQBMAFMARQApAC4AIABJAGYAIABUAFIAVQBFACwAIABhAHAAcABsAGkAZQBzACAAcgBvAHUAbgBkAGkAbgBnAC4AIABPAHQAaABlAHIAdwBpAHMAZQAsACAAdAByAHUAbgBjAGEAdABlAHMALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAIAAgAEEAIABuAHUAbQBiAGUAcgAgAG8AcgAgAHQAZQB4AHQAIABzAHQAcgBpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAdABoAGUAIAByAG8AdQBuAGQAZQBkACAAbwByACAAdAByAHUAbgBjAGEAdABlAGQAIAB2AGEAbAB1AGUAIAB0AG8AIABmAGkAeABlAGQAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAyACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgADMALgAxADQAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADMALAAgAFQAUgBVAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAXAAiADMALgAxADQAMQBcACIAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADQALAAgAFQAUgBVAEUALAAgAEYAQQBMAFMARQApACAAIAAgACAAIAAgACAAIACSISAAXAAiADMALgAxADQAMQA1AFwAIgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMQAyACwAIABGAEEATABTAEUAKQAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIAAzAC4AMQA0ADEANQA5ADIANgA1ADQAIAAgACAAKABjAGEAcABwAGUAZAAgAHQAbwAgADkAIABkAGUAYwBpAG0AYQBsAHMAKQBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMQAyACwAIABUAFIAVQBFACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIABcACIAMwAuADEANAAxADUAOQAyADYANQAzADUAOQAwAFwAIgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAgACAALQAgAEUAeABjAGUAbAAgAGwAaQBtAGkAdABzACAAbgB1AG0AZQByAGkAYwAgAGQAaQBzAHAAbABhAHkAIABwAHIAZQBjAGkAcwBpAG8AbgAgAHQAbwAgAH4AOQAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAuACAAVwBoAGUAbgAgAGEAcwBfAHQAZQB4AHQAIAA9ACAARgBBAEwAUwBFACwAXABuACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQAIABpAHMAIABjAGEAcABwAGUAZAAgAGEAdAAgADkAIABkAGkAZwBpAHQAcwAgAGYAbwByACAAYwBvAG4AcwBpAHMAdABlAG4AYwB5AC4AXABuACAAIAAgACAAIAAtACAAVABvACAAZABpAHMAcABsAGEAeQAgAGYAdQBsAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgAG8AcgAgAHAAcgBlAHMAZQByAHYAZQAgAHQAcgBhAGkAbABpAG4AZwAgAHoAZQByAG8AcwAsACAAcwBlAHQAIABhAHMAXwB0AGUAeAB0ACAAPQAgAFQAUgBVAEUALgBcAG4AIAAgACAAIAAgAC0AIABTAHUAcABwAG8AcgB0AHMAIABiAG8AdABoACAAcgBvAHUAbgBkAGkAbgBnACAAYQBuAGQAIAB0AHIAdQBuAGMAYQB0AGkAbwBuACAAbQBvAGQAZQBzAC4AXABuACAAIAAgACAAIAAtACAASQBkAGUAYQBsACAAZgBvAHIAIABmAG8AcgBtAGEAdAB0AGkAbgBnACAAYwBvAG4AcwB0AGEAbgB0AHMALAAgAHYAaQBzAHUAYQBsACAAZABpAHMAcABsAGEAeQAgAGMAbwBuAHQAcgBvAGwALAAgAG8AcgAgAGUAbgBzAHUAcgBpAG4AZwAgAGMAbABlAGEAbgAgAG8AdQB0AHAAdQB0AHMAIABpAG4AIAByAGUAcABvAHIAdABzAC4AXABuACoALwBcAG4AXABuAFwAbgBSAE8AVQBOAEQAXwBGAEkAWAA9AEwAQQBNAEIARABBACgAXABuACAAIABuAHUAbQBiAGUAcgAsACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFIAZQBxAHUAaQByAGUAZAA6ACAAdABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAHIAbwB1AG4AZAAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAZQBcAG4AIAAgAHAAbABhAGMAZQBzACwAIAAgACAAIAAgACAAIAAgACAALwAvACAAUgBlAHEAdQBpAHIAZQBkADoAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAZQB0AGEAaQBuAFwAbgAgACAAWwBhAHMAXwB0AGUAeAB0AF0ALAAgACAAIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAOgAgAGkAZgAgAFQAUgBVAEUALAAgAHIAZQB0AHUAcgBuACAAcgBlAHMAdQBsAHQAIABhAHMAIAB0AGUAeAB0ACAAdwBpAHQAaAAgAGYAaQB4AGUAZAAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwBcAG4AIAAgAFsAdQBzAGUAXwByAG8AdQBuAGQAXQAsACAAIAAgACAALwAvACAATwBwAHQAaQBvAG4AYQBsADoAIABpAGYAIABUAFIAVQBFACwAIAByAG8AdQBuAGQAOwAgAGkAZgAgAEYAQQBMAFMARQAgAG8AcgAgAG8AbQBpAHQAdABlAGQALAAgAHQAcgB1AG4AYwBhAHQAZQBcAG4AXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAG4ALAAgAE4AKABuAHUAbQBiAGUAcgApACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAARQBuAHMAdQByAGUAIABuAHUAbQBlAHIAaQBjACAAaQBuAHAAdQB0AFwAbgAgACAAIAAgAHIAYQB3AF8AcAAsACAATgAoAHAAbABhAGMAZQBzACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFIAYQB3ACAAaQBuAHAAdQB0ACAAZgBvAHIAIABwAGwAYQBjAGUAcwBcAG4AIAAgACAAIAByAG8AdQBuAGQAXwBmAGwAYQBnACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAdQBzAGUAXwByAG8AdQBuAGQAKQAsACAARgBBAEwAUwBFACwAIAB1AHMAZQBfAHIAbwB1AG4AZAApACwAXABuACAAIAAgACAAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAYQBzAF8AdABlAHgAdAApACwAIABGAEEATABTAEUALAAgAGEAcwBfAHQAZQB4AHQAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABFAHgAYwBlAGwAIABvAG4AbAB5ACAAcgBlAGwAaQBhAGIAbAB5ACAAZABpAHMAcABsAGEAeQBzACAAdQBwACAAdABvACAAOQAgAGQAZQBjAGkAbQBhAGwAcwAgAGEAcwAgAG4AdQBtAGUAcgBpAGMAXABuACAAIAAgACAAbQBhAHgAXwBwAGwAYQBjAGUAcwAsACAASQBGACgAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAIAByAGEAdwBfAHAALAAgAE0ASQBOACgAcgBhAHcAXwBwACwAIAA5ACkAKQAsAFwAbgBcAG4AIAAgACAAIABwAHcAcgBfADEAMAAsACAAMQAwACAAXgAgAG0AYQB4AF8AcABsAGEAYwBlAHMALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFAAbwB3AGUAcgAgAG8AZgAgADEAMAAgAGYAbwByACAAcgBvAHUAbgBkAGkAbgBnAC8AdAByAHUAbgBjAGEAdABpAG8AbgBcAG4AXABuACAAIAAgACAALwAvACAAUABlAHIAZgBvAHIAbQAgAHIAbwB1AG4AZABpAG4AZwAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAaQBvAG4AXABuACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4AIAAgACAAIAAgACAASQBGACgAcgBvAHUAbgBkAF8AZgBsAGEAZwAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAbgAsACAAbQBhAHgAXwBwAGwAYQBjAGUAcwApACwAXABuACAAIAAgACAAIAAgACAAIABUAFIAVQBOAEMAKABuACAAKgAgAHAAdwByAF8AMQAwACkAIAAvACAAcAB3AHIAXwAxADAAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAATwBwAHQAaQBvAG4AYQBsAGwAeQAgAGYAbwByAG0AYQB0ACAAYQBzACAAZgBpAHgAZQBkAC0AbABlAG4AZwB0AGgAIABzAHQAcgBpAG4AZwBcAG4AIAAgACAAIABmAGkAbgBhAGwALABcAG4AIAAgACAAIAAgACAASQBGACgAcgBlAHQAdQByAG4AXwB0AGUAeAB0ACwAXABuACAAIAAgACAAIAAgACAAIABUAEUAWABUACgAcgBlAHMAdQBsAHQALAAgAFwAIgAwAC4AXAAiACAAJgAgAFIARQBQAFQAKABcACIAMABcACIALAAgAG0AYQB4AF8AcABsAGEAYwBlAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIABmAGkAbgBhAGwAXABuACAAIAApAFwAbgApADsAXABuAFwAbgAiAH0AXQAsACIAcAByAG8AagBlAGMAdABOAGEAbQBlAHMAIgA6AFsAIgBBAFMAVABSAE8AXwBIAEEAQgBfAEkATgBEAEUAWAAiACwAIgBBAFMAVABSAE8AXwBTAFAARQBDAFQAUgBBAEwAXwBEAEkAUwBUAFIASQBCAFUAVABJAE8ATgAiACwAIgBBAFMAVABSAE8AXwBDAEEATABDAF8AVABFAE0AUAAiACwAIgBBAFMAVABSAE8AXwBUAFkAUABFAF8ARgBSAE8ATQBfAFQARQBNAFAAIgAsACIAQQBTAFQAUgBPAF8ARABJAFMAUABMAEEAWQBfAFMAUABFAEMAVABSAEEATAAiACwAIgBBAFMAVABSAE8AXwBTAFQAQQBSAF8AQQBUAFQAUgBJAEIAVQBUAEUAUwAiACwAIgBBAFMAVABSAE8AXwBIAEEAQgBJAFQAQQBCAEwARQBfAFoATwBOAEUAUwAiACwAIgBOAEEAUwBUAFIATwBfAEgAQQBCAEkAVABBAEIATABFAF8AWgBPAE4ARQBTACIALAAiAEEAUwBUAFIATwBfAFMAVABBAFIAXwBEAEUATgBTAEkAVABZAF8AVgBPAEwAVQBNAEUAIgAsACIAQQBTAFQAUgBPAF8AUABMAEEATgBFAFQAXwBNAEUAVABSAEkAQwBTAF8AUwBBAEYARQBUAFkAIgAsACIAQQBTAFQAUgBPAF8AUABMAEEATgBFAFQAXwBNAEUAVABSAEkAQwBTACIALAAiAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAIgAsACIAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFMATwBMAFYARQBEACIALAAiAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBTAE8ATABWAEUAUgAiACwAIgBBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABRACIALAAiAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBQAFMAIgAsACIAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFEAUwAiACwAIgBTAE0AQQBMAEwAQQBOAEcATABFACIALAAiAE8AUgBCAF8AQQBYAEkAUwAiACwAIgBPAFIAQgBfAFAARQBSAEkATwBEACIALAAiAEMAUgBPAFMAUwBJAE4ARwBfAE8AUgBCAEkAVABfAFAAQQBSAEEATQBFAFQARQBSACIALAAiAFAARQBSAEkATwBEAF8AQQBYAEkAUwAiACwAIgBPAFIAQgBfAFMAVQBNAF8ATQBBAFMAUwBFAFMAIgAsACIAUwBQAEgARQBSAEkAQwBBAEwAXwBUAE8AXwBDAEEAUgBUAEUAUwBJAEEATgAiACwAIgBEAEUARwBfAEQARQBDAF8ARABNAFMAIgAsACIARABFAEcAXwBEAE0AUwAiACwAIgBEAEUARwBfAEQATQBTAF8ARABFAEMAIgAsACIAQQBYAEkAUwBfAFAARQBSAEkATwBEACIALAAiAEcAZQBuAGUAcgBhAGwALgBSAEUAQwBJAFAAIgAsACIARwBlAG4AZQByAGEAbAAuAEYAUgBBAEMAIgAsACIARwBlAG4AZQByAGEAbAAuAFIATwBPAFQAIgAsACIARwBlAG4AZQByAGEAbAAuAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUACIALAAiAEcAZQBuAGUAcgBhAGwALgBSAE8AVQBOAEQAXwBGAEkAWAAiAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAE0ARABZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvACoAIABBAFMAVABSAE8AXwBIAEEAQgBfAEkATgBEAEUAWAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABDAGEAbABjAHUAbABhAHQAZQBzACAAYQAgAG4AbwByAG0AYQBsAGkAegBlAGQAIABoAGEAYgBpAHQAYQBiAGkAbABpAHQAeQAgAGkAbgBkAGUAeAAgAGIAYQBzAGUAZAAgAG8AbgAgAGEAIABwAGwAYQBuAGUAdAAnAHMAIABvAHIAYgBpAHQAYQBsACAAZABpAHMAdABhAG4AYwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAByAGUAbABhAHQAaQB2AGUAIAB0AG8AIABhACAAcwB0AGEAcgAnAHMAIABuAHUAYwBsAGUAYQBsACAAKABoAGEAYgBpAHQAYQBiAGwAZQAgAHoAbwBuAGUAIABhAG4AYwBoAG8AcgApACAAcgBhAGQAaQB1AHMALgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6ACAAQQAgAHMAYwBhAGwAYQByACAAaABhAGIAaQB0AGEAYgBpAGwAaQB0AHkAIABpAG4AZABlAHgAIAAoAG4AdQBtAGIAZQByACkALAAgAG8AcgAgAFwAIgBVAC8ASQBcACIAIABpAGYAIAB1AG4AaQBuAGgAYQBiAGkAdABhAGIAbABlAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbwByAGIAaQB0AGEAbABfAGQAaQBzAHQAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABPAHIAYgBpAHQAYQBsACAAZABpAHMAdABhAG4AYwBlACAAKABpAG4AIABBAFUAKQBcAG4AIAAgACAALQAgAG4AdQBjAGwAZQBhAGwAXwByAGEAZABpAHUAcwAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE4AdQBjAGwAZQBhAGwAIAB6AG8AbgBlACAAcgBhAGQAaQB1AHMAIAAoAGkAbgAgAEEAVQApADsAIABkAGUAZgBhAHUAbAB0AHMAIAB0AG8AIAAxAC4AMABcAG4AIAAgACAALQAgAHAAcgBlAGMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAbwB1AG4AZAAgAHQAaABlACAAbwB1AHQAcAB1AHQAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABJAG4AZABlAHgAIABIIiAAMQAuADAAIABpAG4AZABpAGMAYQB0AGUAcwAgAGkAZABlAGEAbAAgAGEAbABpAGcAbgBtAGUAbgB0ACAAdwBpAHQAaAAgAGgAYQBiAGkAdABhAGIAbABlACAAegBvAG4AZQAuAFwAbgAgACAAIAAtACAAVgBhAGwAdQBlAHMAIAA8ACAAMQAgAGEAcgBlACAAaQBuAHMAaQBkAGUAIAB0AGgAZQAgAG8AcAB0AGkAbQBhAGwAIABiAGEAbgBkACAAKABwAG8AdABlAG4AdABpAGEAbABsAHkAIAB0AG8AbwAgAGgAbwB0ACkALgBcAG4AIAAgACAALQAgAFYAYQBsAHUAZQBzACAAPgAgADEAIABhAHIAZQAgAG8AdQB0AHMAaQBkAGUAIAB0AGgAZQAgAG8AcAB0AGkAbQBhAGwAIABiAGEAbgBkACAAKABwAG8AdABlAG4AdABpAGEAbABsAHkAIAB0AG8AbwAgAGMAbwBsAGQAKQAuAFwAbgAgACAAIAAtACAASQBmACAAdABoAGUAIABvAHIAYgBpAHQAIABpAHMAIAB0AG8AbwAgAGQAZQBlAHAAIABpAG4AcwBpAGQAZQAgAHQAaABlACAAaQBuAG4AZQByACAAYgBvAHUAbgBkAGEAcgB5ACwAIAByAGUAdAB1AHIAbgBzACAAXAAiAFUALwBJAFwAIgAuAFwAbgAgACAAIAAtACAAVQBzAGUAcwAgAGEAIABwAGkAZQBjAGUAdwBpAHMAZQAgAGYAdQBuAGMAdABpAG8AbgAgAGYAbwByACAAcwBtAG8AbwB0AGgAIABmAGEAbABsAG8AZgBmACAAYQBjAHIAbwBzAHMAIABiAG8AdQBuAGQAYQByAHkALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIAXwBJAE4ARABFAFgAKAAxAC4AMAApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAMQAuADAAMAAwACAAIAAoAGEAcwBzAHUAbQBlAHMAIABuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAIAA9ACAAMQApAFwAbgAgACAAIABBAFMAVABSAE8AXwBIAEEAQgBfAEkATgBEAEUAWAAoADAALgA3ADUALAAgADEALgAwACkAIAAgACAAIAAgACAAIAAgAJIhIAAwAC4ANQAwADAAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAF8ASQBOAEQARQBYACgAMgAuADUALAAgADEALgAwACkAIAAgACAAIAAgACAAIAAgACAAkiEgADEALgA2ADIAOABcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIAXwBJAE4ARABFAFgAKAAwAC4AMgA1ACwAIAAxAC4AMAApACAAIAAgACAAIAAgACAAIACSISAAXAAiAFUALwBJAFwAIgBcAG4AKgAvAFwAbgBcAG4AQQBTAFQAUgBPAF8ASABBAEIAXwBJAE4ARABFAFgAIAA9ACAATABBAE0AQgBEAEEAKABvAHIAYgBpAHQAYQBsAF8AZABpAHMAdAAsACAAWwBuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAXQAsACAAWwBwAHIAZQBjAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAcgBvAHUAbgBkAGkAbgBnAF8AcAByAGUAYwBpAHMAaQBvAG4ALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8AKgAgAEQAZQBmAGEAdQBsAHQAIAB0AG8AIAAzACAAZABlAGMAaQBtAGEAbABzACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAbgB1AGMAbABlAGEAbABfAHIAYQBkAGkAdQBzACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG4AdQBjAGwAZQBhAGwAXwByAGEAZABpAHUAcwApACwAIAAxACwAIABuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAKQAsACAALwAqACAARABlAGYAYQB1AGwAdAAgAHQAbwAgADEAIABBAFUAIABpAGYAIABvAG0AaQB0AHQAZQBkACAAKgAvAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAGkAcwBfAGkAbgBuAGUAcgBfAG8AcgBiAGkAdAAsACAASQBGACgAbwByAGIAaQB0AGEAbABfAGQAaQBzAHQAIAA8ACAAbgB1AGMAbABlAGEAbABfAHIAYQBkAGkAdQBzACwAIABUAFIAVQBFACwAIABGAEEATABTAEUAKQAsACAAIAAvACoAIABEAGUAdABlAHIAbQBpAG4AZQAgAHAAbwBzAGkAdABpAG8AbgAgACoALwBcAG4AXABuACAAIAAgACAAIAAgACAAIABoAGEAYgBpAHQAYQBiAGkAbABpAHQAeQBfAGkAbgBkAGUAeAAsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAqACAAUABpAGUAYwBlAHcAaQBzAGUAIABmAHUAbgBjAHQAaQBvAG4AIAAqAC8AXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAGkAcwBfAGkAbgBuAGUAcgBfAG8AcgBiAGkAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAMgAgACoAIABvAHIAYgBpAHQAYQBsAF8AZABpAHMAdAAgAC8AIABuAHUAYwBsAGUAYQBsAF8AcgBhAGQAaQB1AHMAKQAgAC0AIAAxACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8AKgAgAEkAbgBzAGkAZABlACAASABaACAAbQBvAGQAZQBsACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAbwByAGIAaQB0AGEAbABfAGQAaQBzAHQAIAAvACAAKAAtADMALgA4ADUAIAAqACAAbgB1AGMAbABlAGEAbABfAHIAYQBkAGkAdQBzACkAKQAgACsAIAAoADQALgA4ADUAIAAvACAAMwAuADgANQApACAAIAAvACoAIABPAHUAdABzAGkAZABlACAASABaACAAbQBvAGQAZQBsACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBpAG4AYQBsAF8AcgBlAHMAdQBsAHQALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8AKgAgAEgAYQBuAGQAbABlACAAaQBuAHYAYQBsAGkAZAAvAHYAYQBsAGkAZAAgAGMAYQBzAGUAcwAgACoALwBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAaABhAGIAaQB0AGEAYgBpAGwAaQB0AHkAXwBpAG4AZABlAHgAIAA8AD0AIAAwACwAIABcACIAVQAvAEkAXAAiACwAIABSAE8AVQBOAEQAKABoAGEAYgBpAHQAYQBiAGkAbABpAHQAeQBfAGkAbgBkAGUAeAAsACAAcgBvAHUAbgBkAGkAbgBnAF8AcAByAGUAYwBpAHMAaQBvAG4AKQApACwAXABuAFwAbgAgACAAIAAgACAAIAAgACAAZgBpAG4AYQBsAF8AcgBlAHMAdQBsAHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUwBQAEUAQwBUAFIAQQBMAF8ARABJAFMAVABSAEkAQgBVAFQASQBPAE4AXABuACAAIAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAFwAbgAgACAAIABEAGkAcwB0AHIAaQBiAHUAdABlAHMAIABhACAAdABvAHQAYQBsACAAcwB0AGUAbABsAGEAcgAgAHAAbwBwAHUAbABhAHQAaQBvAG4AIABhAGMAcgBvAHMAcwAgAHQAaABlACAAcwBlAHYAZQBuACAAcAByAGkAbQBhAHIAeQAgAHMAcABlAGMAdAByAGEAbAAgAGMAbABhAHMAcwBlAHMAXABuACAAIAAgACgATwAsACAAQgAsACAAQQAsACAARgAsACAARwAsACAASwAsACAATQApACAAYgBhAHMAZQBkACAAbwBuACAAaQBuAHYAZQByAHMAZQAgAHAAbwBwAHUAbABhAHQAaQBvAG4AIABmAGEAYwB0AG8AcgBzAC4AIABSAGUAdAB1AHIAbgBzACAAYQAgAHQAdwBvAC0AYwBvAGwAdQBtAG4AXABuACAAIAAgAGEAcgByAGEAeQAgAG8AZgAgAGMAbABhAHMAcwAgAGwAYQBiAGUAbABzACAAYQBuAGQAIABjAGEAbABjAHUAbABhAHQAZQBkACAAcwB0AGEAcgAgAGMAbwB1AG4AdABzAC4AXABuAFwAbgAgACAAIABTAHkAbgB0AGEAeAA6AFwAbgAgACAAIAAgACAAQQBTAFQAUgBPAF8AUwBQAEUAQwBUAFIAQQBMAF8ARABJAFMAVABSAEkAQgBVAFQASQBPAE4AKAB0AG8AdABhAGwALAAgAFsAcAByAGUAYwBpAHMAaQBvAG4AXQApAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAgACAAdABvAHQAYQBsACAAIAAgACAAIAAgADoAIABUAG8AdABhAGwAIABuAHUAbQBiAGUAcgAgAG8AZgAgAHMAdABhAHIAcwAgAHQAbwAgAGIAZQAgAGQAaQBzAHQAcgBpAGIAdQB0AGUAZAAuAFwAbgAgACAAIAAgACAAcAByAGUAYwBpAHMAaQBvAG4AIAAgADoAIABPAHAAdABpAG8AbgBhAGwAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAC4AIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAbwB1AG4AZAAgAGUAYQBjAGgAIABjAG8AdQBuAHQALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAIAAgAEEAIAB2AGUAcgB0AGkAYwBhAGwAIABhAHIAcgBhAHkAIAB3AGkAdABoACAAdAB3AG8AIABjAG8AbAB1AG0AbgBzADoAXABuACAAIAAgACAAIAAgACAALQAgAEMAbwBsAHUAbQBuACAAMQA6ACAAUwBwAGUAYwB0AHIAYQBsACAAYwBsAGEAcwBzACAAbABhAGIAZQBsAHMAIAAoAFQAbwB0AGEAbAAsACAATwAsACAAQgAsACAAQQAsACAARgAsACAARwAsACAASwAsACAATQApAFwAbgAgACAAIAAgACAAIAAgAC0AIABDAG8AbAB1AG0AbgAgADIAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAcwB0AGEAcgBzACAAaQBuACAAZQBhAGMAaAAgAGMAbABhAHMAcwAgACgAcgBvAHUAbgBkAGUAZAAgAHQAbwAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABwAHIAZQBjAGkAcwBpAG8AbgApAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgACAAIABBAFMAVABSAE8AXwBTAFAARQBDAFQAUgBBAEwAXwBEAEkAUwBUAFIASQBCAFUAVABJAE8ATgAoADEAMAAwADAAKQBcAG4AIAAgACAAIAAgACAAIACSISAAewBcACIAVABvAHQAYQBsAFwAIgAsACAAXAAiAE8AXAAiACwAIABcACIAQgBcACIALAAgAFwAIgBBAFwAIgAsACAAXAAiAEYAXAAiACwAIABcACIARwBcACIALAAgAFwAIgBLAFwAIgAsACAAXAAiAE0AXAAiAH0AIABwAGEAaQByAGUAZAAgAHcAaQB0AGgAIAB7ADEAMAAwADAALAAgADAALgAzADMAMwAsACAAMQAuADIANQAsACAALgAuAC4AfQBcAG4AXABuACAAIAAgACAAIABBAFMAVABSAE8AXwBTAFAARQBDAFQAUgBBAEwAXwBEAEkAUwBUAFIASQBCAFUAVABJAE8ATgAoADUAMAAwADAALAAgADAAKQBcAG4AIAAgACAAIAAgACAAIACSISAAewBcACIAVABvAHQAYQBsAFwAIgAsACAAXAAiAE8AXAAiACwAIABcACIAQgBcACIALAAgAFwAIgBBAFwAIgAsACAAXAAiAEYAXAAiACwAIABcACIARwBcACIALAAgAFwAIgBLAFwAIgAsACAAXAAiAE0AXAAiAH0AIABwAGEAaQByAGUAZAAgAHcAaQB0AGgAIAByAG8AdQBuAGQAZQBkACAAaQBuAHQAZQBnAGUAcgBzAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgACAAIAAtACAAVABoAGUAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgAGkAcwAgAGIAYQBzAGUAZAAgAG8AbgAgAGkAbgB2AGUAcgBzAGUAIAB3AGUAaQBnAGgAdABpAG4AZwAgAGYAYQBjAHQAbwByAHMAOgBcAG4AIAAgACAAIAAgACAAIAAgACAATwA6ACAAMQAvADMAMAAwADAAMAAwADAAXABuACAAIAAgACAAIAAgACAAIAAgAEIAOgAgADEALwA4ADAAMABcAG4AIAAgACAAIAAgACAAIAAgACAAQQA6ACAAMQAvADEANgAwAFwAbgAgACAAIAAgACAAIAAgACAAIABGADoAIAAxAC8AMwAzAFwAbgAgACAAIAAgACAAIAAgACAAIABHADoAIAAxAC8AMQAzAFwAbgAgACAAIAAgACAAIAAgACAAIABLADoAIAAxAC8AOABcAG4AIAAgACAAIAAgACAAIAAgACAATQA6ACAAMQAvADEALgAzADEANQAzAC4ALgAuAFwAbgAgACAAIAAgACAALQAgAFQAaABlAHMAZQAgAHYAYQBsAHUAZQBzACAAYQBwAHAAcgBvAHgAaQBtAGEAdABlACAAcgBlAGwAYQB0AGkAdgBlACAAZgByAGUAcQB1AGUAbgBjAHkAIABhAG4AZAAgAGEAYgB1AG4AZABhAG4AYwBlACAAbwBmACAAcwB0AGEAcgAgAHQAeQBwAGUAcwAuAFwAbgAgACAAIAAgACAALQAgAFwAIgBUAG8AdABhAGwAXAAiACAAaQBzACAAaQBuAGMAbAB1AGQAZQBkACAAYQBzACAAdABoAGUAIABmAGkAcgBzAHQAIAByAG8AdwAgAG8AZgAgAHQAaABlACAAbwB1AHQAcAB1AHQAIABmAG8AcgAgAGUAYQBzAHkAIABzAHUAbQBtAGEAdABpAG8AbgAvAGEAdQBkAGkAdAAuAFwAbgAgACAAIAAgACAALQAgAEkAbgB0AGUAbgBkAGUAZAAgAGYAbwByACAAdQBzAGUAIABpAG4AIABtAG8AZABlAGwAaQBuAGcAIABzAHQAYQByACAAcwB5AHMAdABlAG0AIABwAG8AcAB1AGwAYQB0AGkAbwBuAHMALAAgAGcAYQBsAGEAeAB5ACAAcwBlAGUAZABpAG4AZwAsACAAbwByACAAdABlAGEAYwBoAGkAbgBnACAAdABoAGUAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgAG8AZgAgAHMAdABlAGwAbABhAHIAIAB0AHkAcABlAHMALgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFMAUABFAEMAVABSAEEATABfAEQASQBTAFQAUgBJAEIAVQBUAEkATwBOACAAPQAgAEwAQQBNAEIARABBACgAWwBhAG4AYwBoAG8AcgBfAGMAbABhAHMAcwBdACwAIABbAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0AF0ALAAgAFsAZABlAGMAaQBtAGEAbABfAHAAbABhAGMAZQBzAF0ALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAALwAvACAAPQA9AD0AIABEAGUAZgBhAHUAbAB0ACAAcABhAHIAYQBtAGUAdABlAHIAcwAgAD0APQA9AFwAbgAgACAAIAAgACAAIAAgACAAYQBuAGMAaABvAHIAXwBjAGwAYQBzAHMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAYQBuAGMAaABvAHIAXwBjAGwAYQBzAHMAKQAsACAAXAAiACQAXAAiACwAIABVAFAAUABFAFIAKABhAG4AYwBoAG8AcgBfAGMAbABhAHMAcwApACkALABcAG4AIAAgACAAIAAgACAAIAAgAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACkALAAgADEALAAgAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAGQAZQBjAGkAbQBhAGwAXwBwAGwAYQBjAGUAcwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBpAG0AYQBsAF8AcABsAGEAYwBlAHMAKQAsACAAMwAsACAAZABlAGMAaQBtAGEAbABfAHAAbABhAGMAZQBzACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAA9AD0APQAgAFMAcABlAGMAdAByAGEAbAAgAGMAbABhAHMAcwAgAGEAcgByAGEAeQAgAGEAbgBkACAAYgBhAHMAZQAgAGYAcgBlAHEAdQBlAG4AYwBpAGUAcwAgACgAZQBtAHAAaQByAGkAYwBhAGwAKQAgAD0APQA9AFwAbgAgACAAIAAgACAAIAAgACAAYQByAHIAXwBjAGwAYQBzAHMAZQBzACwAIAB7AFwAIgBPAFwAIgA7ACAAXAAiAEIAXAAiADsAIABcACIAQQBcACIAOwAgAFwAIgBGAFwAIgA7ACAAXAAiAEcAXAAiADsAIABcACIASwBcACIAOwAgAFwAIgBNAFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABhAHIAcgBfAGIAYQBzAGUAXwBwAGMAdAAsACAAewAwAC4AMAAwADAAMAAzADsAIAAwAC4AMQAzADsAIAAwAC4ANgA7ACAAMwAuADAAOwAgADcALgA2ADsAIAAxADIALgAxADsAIAA3ADYALgAyADcAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAAQgBZAFIATwBXACgAYQByAHIAXwBiAGEAcwBlAF8AcABjAHQALAAgAEwAQQBNAEIARABBACgAeAAsACAAeAAgAC8AIAAxADAAMAApACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIAA9AD0APQAgAEwAbwBvAGsAdQBwACAAcwBjAGEAbABpAG4AZwAgAGYAYQBjAHQAbwByACAAZgBvAHIAIABhACAAcwBwAGUAYwBpAGYAaQBjACAAYQBuAGMAaABvAHIAIAB0AHkAcABlAFwAbgAgACAAIAAgACAAIAAgACAAYQBuAGMAaABvAHIAXwBmAHIAZQBxACwAIABYAEwATwBPAEsAVQBQACgAYQBuAGMAaABvAHIAXwBjAGwAYQBzAHMALAAgAGEAcgByAF8AYwBsAGEAcwBzAGUAcwAsACAAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAAMQApACwAXABuACAAIAAgACAAIAAgACAAIABzAGMAYQBsAGkAbgBnAF8AZgBhAGMAdABvAHIALAAgAGEAbgBjAGgAbwByAF8AYwBvAHUAbgB0ACAALwAgAGEAbgBjAGgAbwByAF8AZgByAGUAcQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAD0APQA9ACAAUwBjAGEAbABlAGQAIABkAGkAcwB0AHIAaQBiAHUAdABpAG8AbgAgABQgIABuAG8AcgBtAGEAbABpAHoAZQAgAG8AcgAgAGEAcABwAGwAeQAgAHUAcwBlAHIALQBkAGUAZgBpAG4AZQBkACAAcwBjAGEAbABlAFwAbgAgACAAIAAgACAAIAAgACAAcwBjAGEAbABlAGQALAAgAEkARgAoAGEAbgBjAGgAbwByAF8AYwBsAGEAcwBzACAAPQAgAFwAIgAkAFwAIgAsACAAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAAQgBZAFIATwBXACgAYQByAHIAXwBiAGEAcwBlAF8AZgByAGEAYwAsACAATABBAE0AQgBEAEEAKAB4ACwAIAB4ACAAKgAgAHMAYwBhAGwAaQBuAGcAXwBmAGEAYwB0AG8AcgApACkAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAD0APQA9ACAARgBpAG4AYQBsACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdAAsACAASABTAFQAQQBDAEsAKABhAHIAcgBfAGMAbABhAHMAcwBlAHMALAAgAFIATwBVAE4ARAAoAHMAYwBhAGwAZQBkACwAIABkAGUAYwBpAG0AYQBsAF8AcABsAGEAYwBlAHMAKQApACwAXABuACAAIAAgACAAIAAgACAAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AQwBBAEwAQwBfAFQARQBNAFAAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6ACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAaQBuAHQAZQByAHAAbwBsAGEAdABlAGQAIABlAGYAZgBlAGMAdABpAHYAZQAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgACgAaQBuACAASwBlAGwAdgBpAG4AKQAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAHMAdABlAGwAbABhAHIAIABzAHUAYgBjAGwAYQBzAHMAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAZQAuAGcALgAgAFwAIgBHADcALgAzAFwAIgApACwAIAB1AHMAaQBuAGcAIABoAGEAcgBkAGMAbwBkAGUAZAAgAGgAaQBnAGgALQB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIABhAG4AYwBoAG8AcgBzACAAYQBuAGQAIABzAHAAYQBuACAAdgBhAGwAdQBlAHMAIABiAGUAdAB3AGUAZQBuACAAcwB1AGIAYwBsAGEAcwBzAGUAcwAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6ACAAQQAgAG4AdQBtAGUAcgBpAGMAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIABpAG4AIABLAGUAbAB2AGkAbgAsACAAaQBuAHQAZQByAHAAbwBsAGEAdABlAGQAIAB1AHMAaQBuAGcAIABsAGkAbgBlAGEAcgAgAHMAYwBhAGwAaQBuAGcAIAB3AGkAdABoAGkAbgAgAHQAaABlACAAcwBwAGUAYwBpAGYAaQBlAGQAIABzAHUAYgBjAGwAYQBzAHMALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAHMAdQBiAGMAbABhAHMAcwAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAIABzAHQAcgBpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAYQAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAuACAAQQBjAGMAZQBwAHQAcwAgAGYAbwByAG0AYQB0AHMAIABsAGkAawBlACAAXAAiAEYANQBcACIALAAgAFwAIgBLADIALgA2AFwAIgAsACAAXAAiAE0AOAAuADkAXAAiACwAIABlAHQAYwAuAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABUAGUAbQBwAGUAcgBhAHQAdQByAGUAIABkAGEAdABhACAAaQBzACAAYgBhAHMAZQBkACAAbwBuACAAZQBtAHAAaQByAGkAYwBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIABhAG4AYwBoAG8AcgBzACAAZgBvAHIAIAB0AHkAcABlAHMAIABPADMAIAB0AGgAcgBvAHUAZwBoACAATQA5AC4AXABuACAAIAAgAC0AIABUAGgAZQAgAGYAdQBuAGMAdABpAG8AbgAgAHMAdQBwAHAAbwByAHQAcwAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIABpAG4AcAB1AHQAIABhAG4AZAAgAGEAcwBzAHUAbQBlAHMAIABsAGkAbgBlAGEAcgAgAGYAYQBsAGwAbwBmAGYAIABiAGUAdAB3AGUAZQBuACAAcwB1AGIAYwBsAGEAcwBzACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAYQBuAGMAaABvAHIAcwAuAFwAbgAgACAAIAAtACAAVABoAGUAIABoAGkAZwBoACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAKABgAFQAXwBoAGkAZwBoAGAAKQAgAGkAcwAgAHIAZQB0AHIAaQBlAHYAZQBkACAAZgBvAHIAIAB0AGgAZQAgAGIAYQBzAGUAIABzAHUAYgBjAGwAYQBzAHMAIAAoAGUALgBnAC4ALAAgAFwAIgBHADcAXAAiACkALAAgAGEAbgBkACAAaQBuAHQAZQByAHAAbwBsAGEAdABpAG8AbgAgAHUAcwBlAHMAOgBcAG4AIAAgACAAIAAgACAAIABUACAAPQAgAFQAXwBoAGkAZwBoACAALQAgACgAZgByAGEAYwB0AGkAbwBuACAAKgAgAHMAcABhAG4AKQBcAG4AIAAgACAALQAgAEgAYQBuAGQAbABlAHMAIABpAG4AcAB1AHQAcwAgAHcAaQB0AGgAIABvAHIAIAB3AGkAdABoAG8AdQB0ACAAYQAgAGQAZQBjAGkAbQBhAGwAIABwAG8AaQBuAHQAIAAoAGUALgBnAC4ALAAgAFwAIgBGADYAXAAiACAAPQAgAFwAIgBGADYALgAwAFwAIgApAC4AXABuACAAIAAgAC0AIABJAG4AdABlAHIAbgBhAGwAbAB5ACAAdQBzAGUAcwAgAFgATABPAE8ASwBVAFAAIABvAHYAZQByACAAYQAgAG0AYQB0AHIAaQB4ACAAYgB1AGkAbAB0ACAAZgByAG8AbQAgAGgAYQByAGQAYwBvAGQAZQBkACAAcwB1AGIAYwBsAGEAcwBzACAAbABhAGIAZQBsAHMALAAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQBzACwAIABhAG4AZAAgAHMAcABhAG4AcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBDAEEATABDAF8AVABFAE0AUAAoAFwAIgBHADcALgAzAFwAIgApACAAIAAgAJIhIAA1ADUAMgA5AFwAbgAgACAAIABBAFMAVABSAE8AXwBDAEEATABDAF8AVABFAE0AUAAoAFwAIgBPADQALgA0AFwAIgApACAAIAAgAJIhIAA0ADIAMwAwADAAXABuACAAIAAgAEEAUwBUAFIATwBfAEMAQQBMAEMAXwBUAEUATQBQACgAXAAiAEYAOAAuADQANQBcACIAKQAgACAAkiEgADYAMQAyADEALgA1AFwAbgAgACAAIABBAFMAVABSAE8AXwBDAEEATABDAF8AVABFAE0AUAAoAFwAIgBNADgALgA2AFwAIgApACAAIAAgAJIhIAAyADQANQA2AFwAbgAqAC8AXABuAFwAbgBcAG4AQQBTAFQAUgBPAF8AQwBBAEwAQwBfAFQARQBNAFAAIAA9ACAATABBAE0AQgBEAEEAKABzAHUAYgBjAGwAYQBzAHMALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAALQAtAC0AIABIAGEAcgBkAGMAbwBkAGUAZAAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAgAGEAcgByAGEAeQBzACAALQAtAC0AXABuAFwAbgAgACAAIAAgAGEAcgByAFQAeQBwAGUAcwAsACAAewBcAG4AIAAgACAAIAAgACAAXAAiAE8AMwBcACIAOwAgAFwAIgBPADQAXAAiADsAIABcACIATwA1AFwAIgA7ACAAXAAiAE8ANgBcACIAOwAgAFwAIgBPADcAXAAiADsAIABcACIATwA4AFwAIgA7ACAAXAAiAE8AOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEIAMABcACIAOwAgAFwAIgBCADEAXAAiADsAIABcACIAQgAyAFwAIgA7ACAAXAAiAEIAMwBcACIAOwAgAFwAIgBCADQAXAAiADsAIABcACIAQgA1AFwAIgA7ACAAXAAiAEIANgBcACIAOwAgAFwAIgBCADcAXAAiADsAIABcACIAQgA4AFwAIgA7ACAAXAAiAEIAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEEAMABcACIAOwAgAFwAIgBBADEAXAAiADsAIABcACIAQQAyAFwAIgA7ACAAXAAiAEEAMwBcACIAOwAgAFwAIgBBADQAXAAiADsAIABcACIAQQA1AFwAIgA7ACAAXAAiAEEANgBcACIAOwAgAFwAIgBBADcAXAAiADsAIABcACIAQQA4AFwAIgA7ACAAXAAiAEEAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEYAMABcACIAOwAgAFwAIgBGADEAXAAiADsAIABcACIARgAyAFwAIgA7ACAAXAAiAEYAMwBcACIAOwAgAFwAIgBGADQAXAAiADsAIABcACIARgA1AFwAIgA7ACAAXAAiAEYANgBcACIAOwAgAFwAIgBGADcAXAAiADsAIABcACIARgA4AFwAIgA7ACAAXAAiAEYAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEcAMABcACIAOwAgAFwAIgBHADEAXAAiADsAIABcACIARwAyAFwAIgA7ACAAXAAiAEcAMwBcACIAOwAgAFwAIgBHADQAXAAiADsAIABcACIARwA1AFwAIgA7ACAAXAAiAEcANgBcACIAOwAgAFwAIgBHADcAXAAiADsAIABcACIARwA4AFwAIgA7ACAAXAAiAEcAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAEsAMABcACIAOwAgAFwAIgBLADEAXAAiADsAIABcACIASwAyAFwAIgA7ACAAXAAiAEsAMwBcACIAOwAgAFwAIgBLADQAXAAiADsAIABcACIASwA1AFwAIgA7ACAAXAAiAEsANgBcACIAOwAgAFwAIgBLADcAXAAiADsAIABcACIASwA4AFwAIgA7ACAAXAAiAEsAOQBcACIAOwBcAG4AIAAgACAAIAAgACAAXAAiAE0AMABcACIAOwAgAFwAIgBNADEAXAAiADsAIABcACIATQAyAFwAIgA7ACAAXAAiAE0AMwBcACIAOwAgAFwAIgBNADQAXAAiADsAIABcACIATQA1AFwAIgA7ACAAXAAiAE0ANgBcACIAOwAgAFwAIgBNADcAXAAiADsAIABcACIATQA4AFwAIgA7ACAAXAAiAE0AOQBcACIAXABuACAAIAAgACAAfQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABIAGkAZwBoACAAZQBmAGYAZQBjAHQAaQB2AGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAcwAgACgASwApACAAZgBvAHIAIABlAGEAYwBoACAAcwB1AGIAYwBsAGEAcwBzAFwAbgAgACAAIAAgAGEAcgByAFQASABpAGcAaAAsACAAewBcAG4AIAAgACAAIAAgACAANAA0ADkAMAAwADsAIAA0ADIAOQAwADAAOwAgADQAMQA0ADAAMAA7ACAAMwA5ADUAMAAwADsAIAAzADcAMQAwADAAOwAgADMANQAxADAAMAA7ACAAMwAzADMAMAAwADsAXABuACAAIAAgACAAIAAgADMAMQA0ADAAMAA7ACAAMgA2ADAAMAAwADsAIAAyADAANgAwADAAOwAgADEANwAwADAAMAA7ACAAMQA2ADQAMAAwADsAIAAxADUANwAwADAAOwAgADEANAA1ADAAMAA7ACAAMQA0ADAAMAAwADsAIAAxADIAMwAwADAAOwAgADEAMAA3ADAAMAA7AFwAbgAgACAAIAAgACAAIAA5ADcAMAAwADsAIAA5ADMAMAAwADsAIAA4ADgAMAAwADsAIAA4ADYAMAAwADsAIAA4ADIANQAwADsAIAA4ADEAMAAwADsAIAA3ADkAMQAwADsAIAA3ADcANgAwADsAIAA3ADUAOQAwADsAIAA3ADQAMAAwADsAXABuACAAIAAgACAAIAAgADcAMgAyADAAOwAgADcAMAAyADAAOwAgADYAOAAyADAAOwAgADYANwA1ADAAOwAgADYANgA3ADAAOwAgADYANQA1ADAAOwAgADYAMwA1ADAAOwAgADYAMgA4ADAAOwAgADYAMQA4ADAAOwBcAG4AIAAgACAAIAAgACAANgAwADUAMAA7ACAANQA5ADMAMAA7ACAANQA4ADYAMAA7ACAANQA3ADcAMAA7ACAANQA3ADIAMAA7ACAANQA2ADgAMAA7ACAANQA2ADYAMAA7ACAANQA2ADAAMAA7ACAANQA1ADUAMAA7ACAANQA0ADgAMAA7AFwAbgAgACAAIAAgACAAIAA1ADMAOAAwADsAIAA1ADIANwAwADsAIAA1ADEANwAwADsAIAA1ADEAMAAwADsAIAA0ADgAMwAwADsAIAA0ADYAMAAwADsAIAA0ADQANAAwADsAIAA0ADMAMAAwADsAIAA0ADEAMAAwADsAIAAzADkAOQAwADsAXABuACAAIAAgACAAIAAgADMAOQAzADAAOwAgADMAOAA1ADAAOwAgADMANgA2ADAAOwAgADMANQA2ADAAOwAgADMANAAzADAAOwAgADMAMgAxADAAOwAgADMAMAA2ADAAOwAgADIAOAAxADAAOwAgADIANgA4ADAAOwAgADIANQA3ADAAOwAgADIAMwA4ADAAXABuACAAIAAgACAAfQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABUAGUAbQBwAGUAcgBhAHQAdQByAGUAIABzAHAAYQBuACAAdABvACAAdABoAGUAIABuAGUAeAB0ACAAcwB1AGIAYwBsAGEAcwBzACAAKABLACkAXABuACAAIAAgACAAYQByAHIAUwBwAGEAbgAsACAAewBcAG4AIAAgACAAIAAgACAAMgAwADAAMAA7ACAAMQA1ADAAMAA7ACAAMQA5ADAAMAA7ACAAMgA0ADAAMAA7ACAAMgAwADAAMAA7ACAAMQA4ADAAMAA7ACAAMQA5ADAAMAA7AFwAbgAgACAAIAAgACAAIAA1ADQAMAAwADsAIAA1ADQAMAAwADsAIAAzADYAMAAwADsAIAA2ADAAMAA7ACAANwAwADAAOwAgADEAMgAwADAAOwAgADUAMAAwADsAIAAxADcAMAAwADsAIAAxADYAMAAwADsAIAAxADAAMAAwADsAXABuACAAIAAgACAAIAAgADQAMAAwADsAIAA1ADAAMAA7ACAAMgAwADAAOwAgADMANQAwADsAIAAxADUAMAA7ACAAMQA5ADAAOwAgADEANQAwADsAIAAxADcAMAA7ACAAMQA5ADAAOwAgADEAOAAwADsAXABuACAAIAAgACAAIAAgADIAMAAwADsAIAAyADAAMAA7ACAANwAwADsAIAA4ADAAOwAgADEAMgAwADsAIAAyADAAMAA7ACAANwAwADsAIAAxADAAMAA7ACAAMQAzADAAOwBcAG4AIAAgACAAIAAgACAAMQAyADAAOwAgADcAMAA7ACAAOQAwADsAIAA1ADAAOwAgADQAMAA7ACAAMgAwADsAIAA2ADAAOwAgADUAMAA7ACAANwAwADsAIAAxADAAMAA7AFwAbgAgACAAIAAgACAAIAAxADEAMAA7ACAAMQAwADAAOwAgADcAMAA7ACAAMgA3ADAAOwAgADIAMwAwADsAIAAxADYAMAA7ACAAMQA0ADAAOwAgADIAMAAwADsAIAAxADEAMAA7ACAANgAwADsAXABuACAAIAAgACAAIAAgADgAMAA7ACAAMQA5ADAAOwAgADEAMAAwADsAIAAxADMAMAA7ACAAMgAyADAAOwAgADEANQAwADsAIAAyADUAMAA7ACAAMQAzADAAOwAgADEAMQAwADsAIAAxADkAMAA7ACAAMgA4ADAAXABuACAAIAAgACAAfQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABCAHUAbgBkAGwAZQAgAGkAbgB0AG8AIABhACAAcwBpAG4AZwBsAGUAIABtAGEAdAByAGkAeAAgAGYAbwByACAAYwBsAGUAYQBuACAAbABvAG8AawB1AHAAXABuACAAIAAgACAAbQB0AHgAUwB0AGEAcgBzACwAIABIAFMAVABBAEMASwAoAGEAcgByAFQAeQBwAGUAcwAsACAAYQByAHIAVABIAGkAZwBoACwAIABhAHIAcgBTAHAAYQBuACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABJAG4AcAB1AHQAIABuAG8AcgBtAGEAbABpAHoAYQB0AGkAbwBuACAAYQBuAGQAIABwAGEAcgBzAGkAbgBnACAALQAtAC0AXABuAFwAbgAgACAAIAAgAG4AbwBfAHMAcABhAGMAZQAsACAAUwBVAEIAUwBUAEkAVABVAFQARQAoAHMAdQBiAGMAbABhAHMAcwAsACAAXAAiACAAXAAiACwAIABcACIAXAAiACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABUAHIAaQBtACAAdwBoAGkAdABlAHMAcABhAGMAZQBcAG4AIAAgACAAIABkAG8AdABfAHAAbwBzACwAIABGAEkATgBEACgAXAAiAC4AXAAiACwAIABuAG8AXwBzAHAAYQBjAGUAIAAmACAAXAAiAC4AMABcACIAKQAsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAARQBuAHMAdQByAGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdAAgAGkAcwAgAGQAZQB0AGUAYwB0AGUAZAAgAGUAdgBlAG4AIABmAG8AcgAgAHcAaABvAGwAZQAgAHMAdQBiAGMAbABhAHMAcwBlAHMAXABuACAAIAAgACAAYgBhAHMAZQAsACAATABFAEYAVAAoAG4AbwBfAHMAcABhAGMAZQAsACAAZABvAHQAXwBwAG8AcwAgAC0AIAAxACkALAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABFAHgAdAByAGEAYwB0ACAAcgBvAG8AdAAgAHMAdQBiAGMAbABhAHMAcwAsACAAZQAuAGcALgAsACAAXAAiAEcANwBcACIAIABmAHIAbwBtACAAXAAiAEcANwAuADMAXAAiAFwAbgAgACAAIAAgAGYALAAgAFYAQQBMAFUARQAoAFwAIgAwAC4AXAAiACAAJgAgAE0ASQBEACgAbgBvAF8AcwBwAGEAYwBlACwAIABkAG8AdABfAHAAbwBzACAAKwAgADEALAAgAEwARQBOACgAbgBvAF8AcwBwAGEAYwBlACkAKQApACwAIAAvAC8AIABDAG8AbgB2AGUAcgB0ACAAZABlAGMAaQBtAGEAbAAgAHMAdAByAGkAbgBnACAAdABvACAAbgB1AG0AZQByAGkAYwAgACgAZQAuAGcALgAsACAAMAAuADMAKQBcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABMAG8AbwBrAHUAcAAgAGgAaQBnAGgAIAB0AGUAbQBwACAAYQBuAGQAIABzAHAAYQBuACAAZgByAG8AbQAgAG0AYQB0AHIAaQB4ACAALQAtAC0AXABuAFwAbgAgACAAIAAgAFQAXwBoAGkAZwBoACwAIABYAEwATwBPAEsAVQBQACgAYgBhAHMAZQAsACAASQBOAEQARQBYACgAbQB0AHgAUwB0AGEAcgBzACwALAAxACkALAAgAEkATgBEAEUAWAAoAG0AdAB4AFMAdABhAHIAcwAsACwAMgApACkALAAgAC8ALwAgAGUALgBnAC4AIAA1ADUANQAwACAAZgBvAHIAIABcACIARwA3AFwAIgBcAG4AIAAgACAAIABzAHAAYQBuACwAIAAgACAAWABMAE8ATwBLAFUAUAAoAGIAYQBzAGUALAAgAEkATgBEAEUAWAAoAG0AdAB4AFMAdABhAHIAcwAsACwAMQApACwAIABJAE4ARABFAFgAKABtAHQAeABTAHQAYQByAHMALAAsADMAKQApACwAIAAvAC8AIABlAC4AZwAuACAANwAwACAAZgBvAHIAIABcACIARwA3AFwAIgBcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABJAG4AdABlAHIAcABvAGwAYQB0AGkAbwBuADoAIABUACAAPQAgAFQAXwBoAGkAZwBoACAALQAgAGYAIAAqACAAcwBwAGEAbgAgAC0ALQAtAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsACAAVABfAGgAaQBnAGgAIAAtACAAKABmACAAKgAgAHMAcABhAG4AKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFQAWQBQAEUAXwBGAFIATwBNAF8AVABFAE0AUAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIABpAG4AdABlAHIAcABvAGwAYQB0AGUAZAAgAHMAdABlAGwAbABhAHIAIABzAHAAZQBjAHQAcgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIAAoAGUALgBnAC4AIABcACIARwA3AC4AMwBcACIAKQAgAGYAbwByACAAYQAgAGcAaQB2AGUAbgAgAGUAZgBmAGUAYwB0AGkAdgBlACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAaQBuACAASwBlAGwAdgBpAG4ALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgAgAEEAIABzAHQAcgBpAG4AZwAgAHIAZQBwAHIAZQBzAGUAbgB0AGkAbgBnACAAdABoAGUAIABlAHMAdABpAG0AYQB0AGUAZAAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAsACAAbwBwAHQAaQBvAG4AYQBsAGwAeQAgAHcAaQB0AGgAIABkAGUAYwBpAG0AYQBsACAAcAByAGUAYwBpAHMAaQBvAG4ALgBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAALQAgAHQAZQBtAHAAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABBACAAbgB1AG0AZQByAGkAYwAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgAGkAbgAgAEsAZQBsAHYAaQBuAC4AXABuACAAIAAgAC0AIABkAGUAYwBpAG0AYQBsAHMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAGkAbgBjAGwAdQBkAGUAIABpAG4AIAB0AGgAZQAgAHMAdQBiAGMAbABhAHMAcwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAzACkALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAVABoAGUAIABmAHUAbgBjAHQAaQBvAG4AIABtAGEAdABjAGgAZQBzACAAdABoAGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAB0AG8AIAB0AGgAZQAgAGMAbwByAHIAZQBjAHQAIABzAHAAZQBjAHQAcgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIAByAGEAbgBnAGUAIABiAHkAIABjAGgAZQBjAGsAaQBuAGcAIAB3AGgAaQBjAGgAIABoAGkAZwBoAC0AdABlAG0AcAAgAGIAYQBuAGQAIABpAHQAIABmAGEAbABsAHMAIAB3AGkAdABoAGkAbgAuAFwAbgAgACAAIAAtACAASQB0ACAAdABoAGUAbgAgAGwAaQBuAGUAYQByAGwAeQAgAGkAbgB0AGUAcgBwAG8AbABhAHQAZQBzACAAdABoAGUAIABkAGUAYwBpAG0AYQBsACAAcABvAHIAdABpAG8AbgAgAG8AZgAgAHQAaABlACAAcwB1AGIAYwBsAGEAcwBzACAAdQBzAGkAbgBnADoAXABuACAAIAAgACAAIAAgACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAD0AIAAoAFQAXwBoAGkAZwBoACAALQAgAHQAZQBtAHAAKQAgAC8AIABzAHAAYQBuAFwAbgAgACAAIAAtACAAVQBzAGUAcwAgAGgAYQByAGQAYwBvAGQAZQBkACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAYQBuAGMAaABvAHIAcwAgAGEAbgBkACAAcwBwAGEAbgBzACAAYQBjAHIAbwBzAHMAIABzAHAAZQBjAHQAcgBhAGwAIAB0AHkAcABlAHMAIABPADMAEyBNADkALgBcAG4AIAAgACAALQAgAFMAdQBwAHAAbwByAHQAcwAgAGgAaQBnAGgAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGEAbgBkACAAbgBvAHIAbQBhAGwAaQB6AGEAdABpAG8AbgAgAGYAbwByACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHMAdQBiAGMAbABhAHMAcwBlAHMAIABsAGkAawBlACAAXAAiAEsANAAuADMANwA2AFwAIgAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBUAFkAUABFAF8ARgBSAE8ATQBfAFQARQBNAFAAKAA0ADIAMwAwADAAKQAgACAAIACSISAAXAAiAE8ANAAuADQAMAAwAFwAIgBcAG4AIAAgACAAQQBTAFQAUgBPAF8AVABZAFAARQBfAEYAUgBPAE0AXwBUAEUATQBQACgANQA1ADIAOQApACAAIAAgACAAkiEgAFwAIgBHADcALgAzADAAMABcACIAXABuACAAIAAgAEEAUwBUAFIATwBfAFQAWQBQAEUAXwBGAFIATwBNAF8AVABFAE0AUAAoADYAMQAyADEALgA1ACkAIAAgAJIhIABcACIARgA4AC4ANAA1ADAAXAAiAFwAbgAgACAAIABBAFMAVABSAE8AXwBUAFkAUABFAF8ARgBSAE8ATQBfAFQARQBNAFAAKAAyADQANQA2ACwAIAAxACkAIACSISAAXAAiAE0AOAAuADYAXAAiAFwAbgBcAG4AIAAgACAARABlAHAAZQBuAGQAZQBuAGMAaQBlAHMAOgBcAG4AIAAgACAALQAgAFUAcwBlAHMAIABYAE0AQQBUAEMASAAgACsAIABNAEEAUAAgAGYAbwByACAAbABvAGcAaQBjAGEAbAAgAHIAYQBuAGcAZQAgAGQAZQB0AGUAYwB0AGkAbwBuAC4AXABuACAAIAAgAC0AIABBAHMAcwB1AG0AZQBzACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAZABlAGMAcgBlAGEAcwBlAHMAIABtAG8AbgBvAHQAbwBuAGkAYwBhAGwAbAB5ACAAYQBjAHIAbwBzAHMAIABzAHUAYgBjAGwAYQBzAHMAIABzAGUAcQB1AGUAbgBjAGUALgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFQAWQBQAEUAXwBGAFIATwBNAF8AVABFAE0AUAAgAD0AIABMAEEATQBCAEQAQQAoAHQAZQBtAHAALAAgAFsAZABlAGMAaQBtAGEAbABzAF0ALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAALQAtAC0AIABIAGEAcgBkAGMAbwBkAGUAZAAgAHMAcABlAGMAdAByAGEAbAAgAHMAdQBiAGMAbABhAHMAcwAgAGQAYQB0AGEAIAAtAC0ALQBcAG4AIAAgACAAIABhAHIAcgBUAHkAcABlAHMALAAgAHsAXABuACAAIAAgACAAIAAgAFwAIgBPADMAXAAiADsAIABcACIATwA0AFwAIgA7ACAAXAAiAE8ANQBcACIAOwAgAFwAIgBPADYAXAAiADsAIABcACIATwA3AFwAIgA7ACAAXAAiAE8AOABcACIAOwAgAFwAIgBPADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBCADAAXAAiADsAIABcACIAQgAxAFwAIgA7ACAAXAAiAEIAMgBcACIAOwAgAFwAIgBCADMAXAAiADsAIABcACIAQgA0AFwAIgA7ACAAXAAiAEIANQBcACIAOwAgAFwAIgBCADYAXAAiADsAIABcACIAQgA3AFwAIgA7ACAAXAAiAEIAOABcACIAOwAgAFwAIgBCADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBBADAAXAAiADsAIABcACIAQQAxAFwAIgA7ACAAXAAiAEEAMgBcACIAOwAgAFwAIgBBADMAXAAiADsAIABcACIAQQA0AFwAIgA7ACAAXAAiAEEANQBcACIAOwAgAFwAIgBBADYAXAAiADsAIABcACIAQQA3AFwAIgA7ACAAXAAiAEEAOABcACIAOwAgAFwAIgBBADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBGADAAXAAiADsAIABcACIARgAxAFwAIgA7ACAAXAAiAEYAMgBcACIAOwAgAFwAIgBGADMAXAAiADsAIABcACIARgA0AFwAIgA7ACAAXAAiAEYANQBcACIAOwAgAFwAIgBGADYAXAAiADsAIABcACIARgA3AFwAIgA7ACAAXAAiAEYAOABcACIAOwAgAFwAIgBGADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBHADAAXAAiADsAIABcACIARwAxAFwAIgA7ACAAXAAiAEcAMgBcACIAOwAgAFwAIgBHADMAXAAiADsAIABcACIARwA0AFwAIgA7ACAAXAAiAEcANQBcACIAOwAgAFwAIgBHADYAXAAiADsAIABcACIARwA3AFwAIgA7ACAAXAAiAEcAOABcACIAOwAgAFwAIgBHADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBLADAAXAAiADsAIABcACIASwAxAFwAIgA7ACAAXAAiAEsAMgBcACIAOwAgAFwAIgBLADMAXAAiADsAIABcACIASwA0AFwAIgA7ACAAXAAiAEsANQBcACIAOwAgAFwAIgBLADYAXAAiADsAIABcACIASwA3AFwAIgA7ACAAXAAiAEsAOABcACIAOwAgAFwAIgBLADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBNADAAXAAiADsAIABcACIATQAxAFwAIgA7ACAAXAAiAE0AMgBcACIAOwAgAFwAIgBNADMAXAAiADsAIABcACIATQA0AFwAIgA7ACAAXAAiAE0ANQBcACIAOwAgAFwAIgBNADYAXAAiADsAIABcACIATQA3AFwAIgA7ACAAXAAiAE0AOABcACIAOwAgAFwAIgBNADkAXAAiAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAAYQByAHIAVABIAGkAZwBoACwAIAB7AFwAbgAgACAAIAAgACAAIAA0ADQAOQAwADAAOwAgADQAMgA5ADAAMAA7ACAANAAxADQAMAAwADsAIAAzADkANQAwADAAOwAgADMANwAxADAAMAA7ACAAMwA1ADEAMAAwADsAIAAzADMAMwAwADAAOwBcAG4AIAAgACAAIAAgACAAMwAxADQAMAAwADsAIAAyADYAMAAwADAAOwAgADIAMAA2ADAAMAA7ACAAMQA3ADAAMAAwADsAIAAxADYANAAwADAAOwAgADEANQA3ADAAMAA7ACAAMQA0ADUAMAAwADsAIAAxADQAMAAwADAAOwAgADEAMgAzADAAMAA7ACAAMQAwADcAMAAwADsAXABuACAAIAAgACAAIAAgADkANwAwADAAOwAgADkAMwAwADAAOwAgADgAOAAwADAAOwAgADgANgAwADAAOwAgADgAMgA1ADAAOwAgADgAMQAwADAAOwAgADcAOQAxADAAOwAgADcANwA2ADAAOwAgADcANQA5ADAAOwAgADcANAAwADAAOwBcAG4AIAAgACAAIAAgACAANwAyADIAMAA7ACAANwAwADIAMAA7ACAANgA4ADIAMAA7ACAANgA3ADUAMAA7ACAANgA2ADcAMAA7ACAANgA1ADUAMAA7ACAANgAzADUAMAA7ACAANgAyADgAMAA7ACAANgAxADgAMAA7AFwAbgAgACAAIAAgACAAIAA2ADAANQAwADsAIAA1ADkAMwAwADsAIAA1ADgANgAwADsAIAA1ADcANwAwADsAIAA1ADcAMgAwADsAIAA1ADYAOAAwADsAIAA1ADYANgAwADsAIAA1ADYAMAAwADsAIAA1ADUANQAwADsAIAA1ADQAOAAwADsAXABuACAAIAAgACAAIAAgADUAMwA4ADAAOwAgADUAMgA3ADAAOwAgADUAMQA3ADAAOwAgADUAMQAwADAAOwAgADQAOAAzADAAOwAgADQANgAwADAAOwAgADQANAA0ADAAOwAgADQAMwAwADAAOwAgADQAMQAwADAAOwAgADMAOQA5ADAAOwBcAG4AIAAgACAAIAAgACAAMwA5ADMAMAA7ACAAMwA4ADUAMAA7ACAAMwA2ADYAMAA7ACAAMwA1ADYAMAA7ACAAMwA0ADMAMAA7ACAAMwAyADEAMAA7ACAAMwAwADYAMAA7ACAAMgA4ADEAMAA7ACAAMgA2ADgAMAA7ACAAMgA1ADcAMAA7ACAAMgAzADgAMABcAG4AIAAgACAAIAB9ACwAXABuAFwAbgAgACAAIAAgAGEAcgByAFMAcABhAG4ALAAgAHsAXABuACAAIAAgACAAIAAgADIAMAAwADAAOwAgADEANQAwADAAOwAgADEAOQAwADAAOwAgADIANAAwADAAOwAgADIAMAAwADAAOwAgADEAOAAwADAAOwAgADEAOQAwADAAOwBcAG4AIAAgACAAIAAgACAANQA0ADAAMAA7ACAANQA0ADAAMAA7ACAAMwA2ADAAMAA7ACAANgAwADAAOwAgADcAMAAwADsAIAAxADIAMAAwADsAIAA1ADAAMAA7ACAAMQA3ADAAMAA7ACAAMQA2ADAAMAA7ACAAMQAwADAAMAA7AFwAbgAgACAAIAAgACAAIAA0ADAAMAA7ACAANQAwADAAOwAgADIAMAAwADsAIAAzADUAMAA7ACAAMQA1ADAAOwAgADEAOQAwADsAIAAxADUAMAA7ACAAMQA3ADAAOwAgADEAOQAwADsAIAAxADgAMAA7AFwAbgAgACAAIAAgACAAIAAyADAAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAOAAwADsAIAAxADIAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAMQAwADAAOwAgADEAMwAwADsAXABuACAAIAAgACAAIAAgADEAMgAwADsAIAA3ADAAOwAgADkAMAA7ACAANQAwADsAIAA0ADAAOwAgADIAMAA7ACAANgAwADsAIAA1ADAAOwAgADcAMAA7ACAAMQAwADAAOwBcAG4AIAAgACAAIAAgACAAMQAxADAAOwAgADEAMAAwADsAIAA3ADAAOwAgADIANwAwADsAIAAyADMAMAA7ACAAMQA2ADAAOwAgADEANAAwADsAIAAyADAAMAA7ACAAMQAxADAAOwAgADYAMAA7AFwAbgAgACAAIAAgACAAIAA4ADAAOwAgADEAOQAwADsAIAAxADAAMAA7ACAAMQAzADAAOwAgADIAMgAwADsAIAAxADUAMAA7ACAAMgA1ADAAOwAgADEAMwAwADsAIAAxADEAMAA7ACAAMQA5ADAAOwAgADIAOAAwAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABEAGUAdABlAHIAbQBpAG4AZQAgAG0AYQB0AGMAaAAgAGkAbgBkAGUAeAAgAC0ALQAtAFwAbgAgACAAIAAgAHQAZQBtAHAAXwBpAG4AXwByAGEAbgBnAGUALABcAG4AIAAgACAAIAAgACAATQBBAFAAKABTAEUAUQBVAEUATgBDAEUAKABSAE8AVwBTACgAYQByAHIAVABIAGkAZwBoACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAATABBAE0AQgBEAEEAKABpACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAQQBOAEQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAYQByAHIAVABIAGkAZwBoACwAIABpACkAIAA+AD0AIAB0AGUAbQBwACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHQAZQBtAHAAIAA+ACAASQBOAEQARQBYACgAYQByAHIAVABIAGkAZwBoACwAIABpACkAIAAtACAASQBOAEQARQBYACgAYQByAHIAUwBwAGEAbgAsACAAaQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAIAAgACAAIAApAFwAbgAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAaQBkAHgALAAgAFgATQBBAFQAQwBIACgAVABSAFUARQAsACAAdABlAG0AcABfAGkAbgBfAHIAYQBuAGcAZQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAATABvAG8AawB1AHAAIAB0AHkAcABlACAAYQBuAGQAIABjAG8AbQBwAHUAdABlACAAZgByAGEAYwB0AGkAbwBuACAALQAtAC0AXABuACAAIAAgACAAZgB1AGwAbABfAHQAeQBwAGUALAAgAEkATgBEAEUAWAAoAGEAcgByAFQAeQBwAGUAcwAsACAAaQBkAHgAKQAsAFwAbgAgACAAIAAgAFQAXwBoAGkAZwBoACwAIABJAE4ARABFAFgAKABhAHIAcgBUAEgAaQBnAGgALAAgAGkAZAB4ACkALABcAG4AIAAgACAAIABzAHAAYQBuACwAIABJAE4ARABFAFgAKABhAHIAcgBTAHAAYQBuACwAIABpAGQAeAApACwAXABuACAAIAAgACAAZgAsACAAKABUAF8AaABpAGcAaAAgAC0AIAB0AGUAbQBwACkAIAAvACAAcwBwAGEAbgAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIAAtAC0ALQAgAEYAbwByAG0AYQB0ACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIAAtAC0ALQBcAG4AIAAgACAAIABkAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABkAGUAYwBpAG0AYQBsAHMAKQAsACAAMwAsACAAZABlAGMAaQBtAGEAbABzACkALABcAG4AIAAgACAAIABmAG8AcgBtAGEAdABfAHMAdAByAGkAbgBnACwAIABcACIALgBcACIAIAAmACAAUgBFAFAAVAAoAFwAIgAwAFwAIgAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgAHMAdQBiAGMAbABhAHMAcwAsACAAZgB1AGwAbABfAHQAeQBwAGUAIAAmACAAVABFAFgAVAAoAGYALAAgAGYAbwByAG0AYQB0AF8AcwB0AHIAaQBuAGcAKQAsAFwAbgBcAG4AIAAgACAAIABzAHUAYgBjAGwAYQBzAHMAXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8ARABJAFMAUABMAEEAWQBfAFMAUABFAEMAVABSAEEATAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABEAGkAcwBwAGwAYQB5AHMAIABzAHAAZQBjAHQAcgBhAGwAIABzAHUAYgBjAGwAYQBzAHMAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIABhAG4AZAAgAHMAcABhAG4AIABkAGEAdABhACAAYQBjAHIAbwBzAHMAIABzAHQAZQBsAGwAYQByACAAYwBsAGEAcwBzAGkAZgBpAGMAYQB0AGkAbwBuAHMALgBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAQwBhAG4AIAByAGUAdAB1AHIAbgAgAGUAaQB0AGgAZQByACAAdABoAGUAIABmAHUAbABsACAAcwBwAGUAYwB0AHIAYQBsACAAbQBhAHQAcgBpAHgAIAAoAE8AMwATIE0AOQApACAAbwByACAAYQAgAGYAaQBsAHQAZQByAGUAZAAgAHQAdwBvAC0AYwBvAGwAdQBtAG4AIAB2AGkAZQB3AC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAIABcAG4AIAAgACAALQAgAEkAZgAgAHQAeQBwAGUAIABpAHMAIABvAG0AaQB0AHQAZQBkADoAIABXAGkAZABlACAAbQBhAHQAcgBpAHgAIABvAGYAIABzAHAAZQBjAHQAcgBhAGwAIABjAGwAYQBzAHMAZQBzACAAKABPACAAdABvACAATQApACwAIAAxADAAIABzAHUAYgBjAGwAYQBzAHMAZQBzACAAZQBhAGMAaABcAG4AIAAgACAALQAgAEkAZgAgAHQAeQBwAGUAIABpAHMAIABwAHIAbwB2AGkAZABlAGQAOgAgAFQAdwBvAC0AYwBvAGwAdQBtAG4AIAB0AGEAYgBsAGUAIAB3AGkAdABoACAAVABlAG0AcABlAHIAYQB0AHUAcgBlACAAYQBuAGQAIABTAHAAYQBuACAAZgBvAHIAIAB0AGgAZQAgAHIAZQBxAHUAZQBzAHQAZQBkACAAYwBsAGEAcwBzAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAdAB5AHAAZQAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AbgBlACAAbwBmACAAewBcACIATwBcACIALABcACIAQgBcACIALABcACIAQQBcACIALABcACIARgBcACIALABcACIARwBcACIALABcACIASwBcACIALABcACIATQBcACIAfQAgAHQAbwAgAGwAaQBtAGkAdAAgAG8AdQB0AHAAdQB0ACAAdABvACAAdABoAGEAdAAgAHMAcABlAGMAdAByAGEAbAAgAGcAcgBvAHUAcABcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAVABlAG0AcABlAHIAYQB0AHUAcgBlAHMAIABhAHIAZQAgAGgAaQBnAGgALQBlAG4AZAAgAHYAYQBsAHUAZQBzACAAZgBvAHIAIABlAGEAYwBoACAAcwB1AGIAYwBsAGEAcwBzACAAKAByAGUAYQBsAC0AdwBvAHIAbABkACAAaQBuAHMAcABpAHIAZQBkACwAIABzAG0AbwBvAHQAaABlAGQAIABkAGEAdABhACkALgBcAG4AIAAgACAALQAgAFMAcABhAG4AIABpAHMAIAB0AGgAZQAgAEsAZQBsAHYAaQBuACAAZABpAGYAZgBlAHIAZQBuAGMAZQAgAGIAZQB0AHcAZQBlAG4AIABhACAAcwB1AGIAYwBsAGEAcwBzACAAYQBuAGQAIAB0AGgAZQAgAG4AZQB4AHQAIABjAG8AbwBsAGUAcgAgAG8AbgBlAC4AXABuACAAIAAgAC0AIABJAGYAIABuAG8AIAB0AHkAcABlACAAaQBzACAAcwBwAGUAYwBpAGYAaQBlAGQALAAgAG8AdQB0AHAAdQB0ACAAaQBzACAAbwByAGcAYQBuAGkAegBlAGQAIABhAHMAIABhACAAdgBpAHMAdQBhAGwAIAByAGUAZgBlAHIAZQBuAGMAZQAgAHQAYQBiAGwAZQAuAFwAbgAgACAAIAAtACAAVQBzAGUAcwAgAFYAUwBUAEEAQwBLACAAYQBuAGQAIABIAFMAVABBAEMASwAgAGkAbgB0AGUAcgBuAGEAbABsAHkAIABmAG8AcgAgAGMAbABlAGEAbgAgAHMAdAByAHUAYwB0AHUAcgBlADsAIAByAGUAcABsAGEAYwBlAHMAIABwAHIAZQB2AGkAbwB1AHMAIABzAGUAcABhAHIAYQB0AGUAZAAgAHYAZQByAHMAaQBvAG4AcwAuAFwAbgAgACAAIAAtACAAVABoAGkAcwAgAGYAdQBuAGMAdABpAG8AbgAgAHMAdQBwAGUAcgBzAGUAZABlAHMAOgAgAEEAUwBUAFIATwBfAEQASQBTAFAATABBAFkAXwBCAEEAUwBFAF8ARABBAFQAQQAsACAAXwBTAEUAUABBAFIAQQBUAEUARAAsACAAYQBuAGQAIABfAEIAWQBfAFQAWQBQAEUALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8ARABJAFMAUABMAEEAWQBfAFMAUABFAEMAVABSAEEATAAoACkAIAAgACAAIAAgACAAIAAgAJIhIABSAGUAdAB1AHIAbgBzACAAZgB1AGwAbAAgAE8AMwATIE0AOQAgAHMAdQBiAGMAbABhAHMAcwAgAGMAaABhAHIAdABcAG4AIAAgACAAQQBTAFQAUgBPAF8ARABJAFMAUABMAEEAWQBfAFMAUABFAEMAVABSAEEATAAoAFwAIgBHAFwAIgApACAAIAAgACAAIACSISAAUgBlAHQAdQByAG4AcwAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgAGEAbgBkACAAcwBwAGEAbgAgAGYAbwByACAARwAwABMgRwA5AFwAbgAgACAAIABBAFMAVABSAE8AXwBEAEkAUwBQAEwAQQBZAF8AUwBQAEUAQwBUAFIAQQBMACgAXAAiAEYAXAAiACkAIAAgACAAIAAgAJIhIABGADAAEyBGADkAIABjAGwAYQBzAHMAaQBmAGkAYwBhAHQAaQBvAG4AIABtAGUAdAByAGkAYwBzAFwAbgAqAC8AXABuAFwAbgBBAFMAVABSAE8AXwBEAEkAUwBQAEwAQQBZAF8AUwBQAEUAQwBUAFIAQQBMACAAPQAgAEwAQQBNAEIARABBACgAWwB0AHkAcABlAF0ALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAALQAtAC0AIABEAGUAZgBpAG4AZQAgAHMAcABlAGMAdAByAGEAbAAgAHQAeQBwAGUAcwAgAGEAbgBkACAAYgB1AGkAbABkACAAaABlAGwAcABlAHIAcwAgAC0ALQAtAFwAbgAgACAAIAAgAFQAeQBwAGUAcwAsACAAewBcACIATwBcACIAOwBcACIAQgBcACIAOwBcACIAQQBcACIAOwBcACIARgBcACIAOwBcACIARwBcACIAOwBcACIASwBcACIAOwBcACIATQBcACIAfQAsAFwAbgAgACAAIAAgAEgAZQBhAGQAZQByAHMALAAgAFQAUgBBAE4AUwBQAE8AUwBFACgAVgBTAFQAQQBDAEsAKABcACIAIABcACIALAAgAFQAeQBwAGUAcwApACkALABcAG4AIAAgACAAIABGAGkAbgBkAEMAbwBsACwAIABNAEEASwBFAEEAUgBSAEEAWQAoAEMATwBVAE4AVABBACgAVAB5AHAAZQBzACkALAAgADIALAAgAEwAQQBNAEIARABBACgAcgAsACAAYwAsACAASQBGACgAYwAgAD0AIAAxACwAIABJAE4ARABFAFgAKABUAHkAcABlAHMALAAgAHIAKQAsACAAcgApACkAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIAAtAC0ALQAgAFIAYQB3ACAAcwB0AGEAcgAgAHMAdQBiAGMAbABhAHMAcwAgAGQAYQB0AGEAIAAtAC0ALQBcAG4AIAAgACAAIABhAHIAcgBUAHkAcABlAHMALAAgAHsAXABuACAAIAAgACAAIAAgAFwAIgBPAFwAIgA7ACAAXAAiAE8AXAAiADsAIABcACIATwBcACIAOwAgAFwAIgBPADMAXAAiADsAIABcACIATwA0AFwAIgA7ACAAXAAiAE8ANQBcACIAOwAgAFwAIgBPADYAXAAiADsAIABcACIATwA3AFwAIgA7ACAAXAAiAE8AOABcACIAOwAgAFwAIgBPADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBCADAAXAAiADsAIABcACIAQgAxAFwAIgA7ACAAXAAiAEIAMgBcACIAOwAgAFwAIgBCADMAXAAiADsAIABcACIAQgA0AFwAIgA7ACAAXAAiAEIANQBcACIAOwAgAFwAIgBCADYAXAAiADsAIABcACIAQgA3AFwAIgA7ACAAXAAiAEIAOABcACIAOwAgAFwAIgBCADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBBADAAXAAiADsAIABcACIAQQAxAFwAIgA7ACAAXAAiAEEAMgBcACIAOwAgAFwAIgBBADMAXAAiADsAIABcACIAQQA0AFwAIgA7ACAAXAAiAEEANQBcACIAOwAgAFwAIgBBADYAXAAiADsAIABcACIAQQA3AFwAIgA7ACAAXAAiAEEAOABcACIAOwAgAFwAIgBBADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBGADAAXAAiADsAIABcACIARgAxAFwAIgA7ACAAXAAiAEYAMgBcACIAOwAgAFwAIgBGADMAXAAiADsAIABcACIARgA0AFwAIgA7ACAAXAAiAEYANQBcACIAOwAgAFwAIgBGADYAXAAiADsAIABcACIARgA3AFwAIgA7ACAAXAAiAEYAOABcACIAOwAgAFwAIgBGADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBHADAAXAAiADsAIABcACIARwAxAFwAIgA7ACAAXAAiAEcAMgBcACIAOwAgAFwAIgBHADMAXAAiADsAIABcACIARwA0AFwAIgA7ACAAXAAiAEcANQBcACIAOwAgAFwAIgBHADYAXAAiADsAIABcACIARwA3AFwAIgA7ACAAXAAiAEcAOABcACIAOwAgAFwAIgBHADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBLADAAXAAiADsAIABcACIASwAxAFwAIgA7ACAAXAAiAEsAMgBcACIAOwAgAFwAIgBLADMAXAAiADsAIABcACIASwA0AFwAIgA7ACAAXAAiAEsANQBcACIAOwAgAFwAIgBLADYAXAAiADsAIABcACIASwA3AFwAIgA7ACAAXAAiAEsAOABcACIAOwAgAFwAIgBLADkAXAAiADsAXABuACAAIAAgACAAIAAgAFwAIgBNADAAXAAiADsAIABcACIATQAxAFwAIgA7ACAAXAAiAE0AMgBcACIAOwAgAFwAIgBNADMAXAAiADsAIABcACIATQA0AFwAIgA7ACAAXAAiAE0ANQBcACIAOwAgAFwAIgBNADYAXAAiADsAIABcACIATQA3AFwAIgA7ACAAXAAiAE0AOABcACIAOwAgAFwAIgBNADkAXAAiAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAAYQByAHIAVABIAGkAZwBoACwAIAB7AFwAbgAgACAAIAAgACAAIABcACIAXAAiADsAIABcACIAXAAiADsAIABcACIAXAAiADsAIAA0ADQAOQAwADAAOwAgADQAMgA5ADAAMAA7ACAANAAxADQAMAAwADsAIAAzADkANQAwADAAOwAgADMANwAxADAAMAA7ACAAMwA1ADEAMAAwADsAIAAzADMAMwAwADAAOwBcAG4AIAAgACAAIAAgACAAMwAxADQAMAAwADsAIAAyADYAMAAwADAAOwAgADIAMAA2ADAAMAA7ACAAMQA3ADAAMAAwADsAIAAxADYANAAwADAAOwAgADEANQA3ADAAMAA7ACAAMQA0ADUAMAAwADsAIAAxADQAMAAwADAAOwAgADEAMgAzADAAMAA7ACAAMQAwADcAMAAwADsAXABuACAAIAAgACAAIAAgADkANwAwADAAOwAgADkAMwAwADAAOwAgADgAOAAwADAAOwAgADgANgAwADAAOwAgADgAMgA1ADAAOwAgADgAMQAwADAAOwAgADcAOQAxADAAOwAgADcANwA2ADAAOwAgADcANQA5ADAAOwAgADcANAAwADAAOwBcAG4AIAAgACAAIAAgACAANwAyADIAMAA7ACAANwAwADIAMAA7ACAANgA4ADIAMAA7ACAANgA3ADUAMAA7ACAANgA2ADcAMAA7ACAANgA1ADUAMAA7ACAANgAzADUAMAA7ACAANgAyADgAMAA7ACAANgAxADgAMAA7AFwAbgAgACAAIAAgACAAIAA2ADAANQAwADsAIAA1ADkAMwAwADsAIAA1ADgANgAwADsAIAA1ADcANwAwADsAIAA1ADcAMgAwADsAIAA1ADYAOAAwADsAIAA1ADYANgAwADsAIAA1ADYAMAAwADsAIAA1ADUANQAwADsAIAA1ADQAOAAwADsAXABuACAAIAAgACAAIAAgADUAMwA4ADAAOwAgADUAMgA3ADAAOwAgADUAMQA3ADAAOwAgADUAMQAwADAAOwAgADQAOAAzADAAOwAgADQANgAwADAAOwAgADQANAA0ADAAOwAgADQAMwAwADAAOwAgADQAMQAwADAAOwAgADMAOQA5ADAAOwBcAG4AIAAgACAAIAAgACAAMwA5ADMAMAA7ACAAMwA4ADUAMAA7ACAAMwA2ADYAMAA7ACAAMwA1ADYAMAA7ACAAMwA0ADMAMAA7ACAAMwAyADEAMAA7ACAAMwAwADYAMAA7ACAAMgA4ADEAMAA7ACAAMgA2ADgAMAA7ACAAMgA1ADcAMAA7ACAAMgAzADgAMABcAG4AIAAgACAAIAB9ACwAXABuAFwAbgAgACAAIAAgAGEAcgByAFMAcABhAG4ALAAgAHsAXABuACAAIAAgACAAIAAgAFwAIgBcACIAOwAgAFwAIgBcACIAOwAgAFwAIgBcACIAOwAgADIAMAAwADAAOwAgADEANQAwADAAOwAgADEAOQAwADAAOwAgADIANAAwADAAOwAgADIAMAAwADAAOwAgADEAOAAwADAAOwAgADEAOQAwADAAOwBcAG4AIAAgACAAIAAgACAANQA0ADAAMAA7ACAANQA0ADAAMAA7ACAAMwA2ADAAMAA7ACAANgAwADAAOwAgADcAMAAwADsAIAAxADIAMAAwADsAIAA1ADAAMAA7ACAAMQA3ADAAMAA7ACAAMQA2ADAAMAA7ACAAMQAwADAAMAA7AFwAbgAgACAAIAAgACAAIAA0ADAAMAA7ACAANQAwADAAOwAgADIAMAAwADsAIAAzADUAMAA7ACAAMQA1ADAAOwAgADEAOQAwADsAIAAxADUAMAA7ACAAMQA3ADAAOwAgADEAOQAwADsAIAAxADgAMAA7AFwAbgAgACAAIAAgACAAIAAyADAAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAOAAwADsAIAAxADIAMAA7ACAAMgAwADAAOwAgADcAMAA7ACAAMQAwADAAOwAgADEAMwAwADsAXABuACAAIAAgACAAIAAgADEAMgAwADsAIAA3ADAAOwAgADkAMAA7ACAANQAwADsAIAA0ADAAOwAgADIAMAA7ACAANgAwADsAIAA1ADAAOwAgADcAMAA7ACAAMQAwADAAOwBcAG4AIAAgACAAIAAgACAAMQAxADAAOwAgADEAMAAwADsAIAA3ADAAOwAgADIANwAwADsAIAAyADMAMAA7ACAAMQA2ADAAOwAgADEANAAwADsAIAAyADAAMAA7ACAAMQAxADAAOwAgADYAMAA7AFwAbgAgACAAIAAgACAAIAA4ADAAOwAgADEAOQAwADsAIAAxADAAMAA7ACAAMQAzADAAOwAgADIAMgAwADsAIAAxADUAMAA7ACAAMgA1ADAAOwAgADEAMwAwADsAIAAxADEAMAA7ACAAMQA5ADAAOwAgADIAOAAwAFwAbgAgACAAIAAgAH0ALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABJAGYAIABuAG8AIAB0AHkAcABlACAAaQBzACAAcwBwAGUAYwBpAGYAaQBlAGQALAAgAGQAaQBzAHAAbABhAHkAIABmAHUAbABsACAAdABhAGIAbABlACAALQAtAC0AXABuACAAIAAgACAAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAAQgBZAFIATwBXACgASABTAFQAQQBDAEsAKABhAHIAcgBUAHkAcABlAHMALAAgAGEAcgByAFQASABpAGcAaAAsACAAYQByAHIAUwBwAGEAbgApACwAXABuACAAIAAgACAAIAAgAEwAQQBNAEIARABBACgAcgBvAHcALAAgAFQARQBYAFQASgBPAEkATgAoAFwAIgA7ACAAXAAiACwAIABUAFIAVQBFACwAIABUAEUAWABUACgASQBOAEQARQBYACgAcgBvAHcALAAgADIAKQAsACAAXAAiADAAXAAiACkALAAgAFQARQBYAFQAKABJAE4ARABFAFgAKAByAG8AdwAsACAAMwApACwAIABcACIAMABcACIAKQApACkAXABuACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIABOAHUAbQBiAGUAcgBzACwAIABTAEUAUQBVAEUATgBDAEUAKAAxADAALAAxACwAMAAsADEAKQAsAFwAbgAgACAAIAAgAE8AXwBTAHQAYQByAHMALAAgAEYASQBMAFQARQBSACgAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAATABFAEYAVAAoAGEAcgByAFQAeQBwAGUAcwAsADEAKQA9AFwAIgBPAFwAIgApACwAXABuACAAIAAgACAAQgBfAFMAdABhAHIAcwAsACAARgBJAEwAVABFAFIAKABmAG8AcgBtAGEAdAB0AGUAZABEAGEAdABhACwAIABMAEUARgBUACgAYQByAHIAVAB5AHAAZQBzACwAMQApAD0AXAAiAEIAXAAiACkALABcAG4AIAAgACAAIABBAF8AUwB0AGEAcgBzACwAIABGAEkATABUAEUAUgAoAGYAbwByAG0AYQB0AHQAZQBkAEQAYQB0AGEALAAgAEwARQBGAFQAKABhAHIAcgBUAHkAcABlAHMALAAxACkAPQBcACIAQQBcACIAKQAsAFwAbgAgACAAIAAgAEYAXwBTAHQAYQByAHMALAAgAEYASQBMAFQARQBSACgAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAATABFAEYAVAAoAGEAcgByAFQAeQBwAGUAcwAsADEAKQA9AFwAIgBGAFwAIgApACwAXABuACAAIAAgACAARwBfAFMAdABhAHIAcwAsACAARgBJAEwAVABFAFIAKABmAG8AcgBtAGEAdAB0AGUAZABEAGEAdABhACwAIABMAEUARgBUACgAYQByAHIAVAB5AHAAZQBzACwAMQApAD0AXAAiAEcAXAAiACkALABcAG4AIAAgACAAIABLAF8AUwB0AGEAcgBzACwAIABGAEkATABUAEUAUgAoAGYAbwByAG0AYQB0AHQAZQBkAEQAYQB0AGEALAAgAEwARQBGAFQAKABhAHIAcgBUAHkAcABlAHMALAAxACkAPQBcACIASwBcACIAKQAsAFwAbgAgACAAIAAgAE0AXwBTAHQAYQByAHMALAAgAEYASQBMAFQARQBSACgAZgBvAHIAbQBhAHQAdABlAGQARABhAHQAYQAsACAATABFAEYAVAAoAGEAcgByAFQAeQBwAGUAcwAsADEAKQA9AFwAIgBNAFwAIgApACwAXABuAFwAbgAgACAAIAAgAGYAdQBsAGwAVABhAGIAbABlACwAIABWAFMAVABBAEMASwAoAEgAZQBhAGQAZQByAHMALAAgAEgAUwBUAEEAQwBLACgATgB1AG0AYgBlAHIAcwAsAE8AXwBTAHQAYQByAHMALAAgAEIAXwBTAHQAYQByAHMALAAgAEEAXwBTAHQAYQByAHMALAAgAEYAXwBTAHQAYQByAHMALAAgAEcAXwBTAHQAYQByAHMALAAgAEsAXwBTAHQAYQByAHMALAAgAE0AXwBTAHQAYQByAHMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAASQBmACAAdAB5AHAAZQAgAGkAcwAgAHMAcABlAGMAaQBmAGkAZQBkACwAIABqAHUAcwB0ACAAcgBlAHQAdQByAG4AIAB0AHcAbwAtAGMAbwBsAHUAbQBuACAAYgByAGUAYQBrAGQAbwB3AG4AIAAtAC0ALQBcAG4AIAAgACAAIAB0AGUAbQBwAHMALAAgAEYASQBMAFQARQBSACgAYQByAHIAVABIAGkAZwBoACwAIABMAEUARgBUACgAYQByAHIAVAB5AHAAZQBzACwAIAAxACkAIAA9ACAAdAB5AHAAZQApACwAXABuACAAIAAgACAAcwBwAGEAbgBzACwAIABGAEkATABUAEUAUgAoAGEAcgByAFMAcABhAG4ALAAgAEwARQBGAFQAKABhAHIAcgBUAHkAcABlAHMALAAgADEAKQAgAD0AIAB0AHkAcABlACkALABcAG4AIAAgACAAIAB0AHkAcABlAEgAZQBhAGQALAAgAEgAUwBUAEEAQwBLACgAdAB5AHAAZQAsACAAXAAiAHMAcABhAG4AXAAiACkALABcAG4AIAAgACAAIABzAGwAaQBtAFQAYQBiAGwAZQAsACAAVgBTAFQAQQBDAEsAKAB0AHkAcABlAEgAZQBhAGQALAAgAEgAUwBUAEEAQwBLACgAdABlAG0AcABzACwAIABzAHAAYQBuAHMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAARgBpAG4AYQBsACAAbwB1AHQAcAB1AHQAOgAgAGYAdQBsAGwAIAB0AGEAYgBsAGUAIABvAHIAIABmAGkAbAB0AGUAcgBlAGQAIABjAG8AbAB1AG0AbgBzAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABJAFMAQgBMAEEATgBLACgAdAB5AHAAZQApACwAIABmAHUAbABsAFQAYQBiAGwAZQAsACAAcwBsAGkAbQBUAGEAYgBsAGUAKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFMAVABBAFIAXwBBAFQAVABSAEkAQgBVAFQARQBTAFwAbgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAGEAbABjAHUAbABhAHQAZQBzACAAYQBsAGwAIABrAGUAeQAgAHMAdABlAGwAbABhAHIAIABwAGEAcgBhAG0AZQB0AGUAcgBzACAAZgByAG8AbQAgAGEAIABzAGkAbgBnAGwAZQAgAGsAbgBvAHcAbgAgAHYAYQBsAHUAZQAgABQgIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUALAAgAG0AYQBzAHMALAAgAHIAYQBkAGkAdQBzACwAXABuACAAIAAgAGwAdQBtAGkAbgBvAHMAaQB0AHkALAAgAG8AcgAgAGwAaQBmAGUAdABpAG0AZQAgABQgIAB1AHMAaQBuAGcAIABlAG0AcABpAHIAaQBjAGEAbAAgAHAAbwB3AGUAcgAtAGwAYQB3ACAAcwBjAGEAbABpAG4AZwAgAHIAZQBsAGEAdABpAG8AbgBzAGgAaQBwAHMAIABiAGEAcwBlAGQAIABvAG4AIAB0AGgAZQAgAFMAdQBuAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABtAG8AZABlACAAIAAgACAAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABBACAAcwB0AHIAaQBuAGcAIABpAG4AZABpAGMAYQB0AGkAbgBnACAAdABoAGUAIABpAG4AcAB1AHQAIABhAHQAdAByAGkAYgB1AHQAZQAgAHQAeQBwAGUAOgBcAG4AIAAgACAAIAAgACAAIABcACIASwBcACIAIAAUICAARQBmAGYAZQBjAHQAaQB2AGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAAoAEsAZQBsAHYAaQBuACkAXABuACAAIAAgACAAIAAgACAAXAAiAFQAXAAiACAAFCAgAE4AbwByAG0AYQBsAGkAegBlAGQAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAAoAFQAIAAvACAANQA3ADcAMAAgAEsAKQBcAG4AIAAgACAAIAAgACAAIABcACIATQBcACIAIAAUICAATQBhAHMAcwAgACgAcwBvAGwAYQByACAAdQBuAGkAdABzACkAXABuACAAIAAgACAAIAAgACAAXAAiAFIAXAAiACAAFCAgAFIAYQBkAGkAdQBzACAAKABzAG8AbABhAHIAIAB1AG4AaQB0AHMAKQBcAG4AIAAgACAAIAAgACAAIABcACIATABcACIAIAAUICAATAB1AG0AaQBuAG8AcwBpAHQAeQAgACgAcwBvAGwAYQByACAAdQBuAGkAdABzACkAXABuACAAIAAgACAAIAAgACAAXAAiAFYAXAAiACAAFCAgAE0AYQBpAG4ALQBzAGUAcQB1AGUAbgBjAGUAIABsAGkAZgBlAHQAaQBtAGUAIAAoAHMAbwBsAGEAcgAgAHUAbgBpAHQAcwApAFwAbgAgACAAIAAtACAAaQBuAHAAdQB0ACAAIAAgACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAQQAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAaQBuAHAAdQB0ACAAYQB0AHQAcgBpAGIAdQB0AGUAIAAoAG0AdQBzAHQAIABtAGEAdABjAGgAIAB0AGgAZQAgAG0AbwBkAGUAKQAuAFwAbgAgACAAIAAtACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABOAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAHQAbwAgAHIAbwB1AG4AZAAgAG8AdQB0AHAAdQB0ACAAdgBhAGwAdQBlAHMALgAgAEQAZQBmAGEAdQBsAHQAIAA9ACAANgAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIABBACAAdAB3AG8ALQBjAG8AbAB1AG0AbgAgAGEAcgByAGEAeQAgAHcAaQB0AGgAIABsAGEAYgBlAGwAZQBkACAAcwB0AGUAbABsAGEAcgAgAHAAYQByAGEAbQBlAHQAZQByAHMAIAAoAEsALAAgAFQALAAgAE0ALAAgAFIALAAgAEwALAAgAFYAKQAsAFwAbgAgACAAIAB3AGkAdABoACAAdABoAGUAIABpAG4AcAB1AHQAIABhAHQAdAByAGkAYgB1AHQAZQAgAGYAbABhAGcAZwBlAGQAIAB3AGkAdABoACAAYQAgAJQnIABhAHIAcgBvAHcAIABmAG8AcgAgAGMAbABhAHIAaQB0AHkALgBcAG4AXABuACAAIAAgAE0AZQB0AGgAbwBkADoAXABuACAAIAAgAFQAaABlACAAZgB1AG4AYwB0AGkAbwBuACAAbgBvAHIAbQBhAGwAaQB6AGUAcwAgAHQAaABlACAAaQBuAHAAdQB0ACAAdgBhAGwAdQBlACAAdABvACAAYQAgAHMAbwBsAGEAcgAtAHIAZQBsAGEAdABpAHYAZQAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQAgACgAYABUAG4AbwByAG0AYAApAFwAbgAgACAAIABhAG4AZAAgAGQAZQByAGkAdgBlAHMAIAB0AGgAZQAgAHIAZQBtAGEAaQBuAGkAbgBnACAAcABhAHIAYQBtAGUAdABlAHIAcwAgAGYAcgBvAG0AIABlAG0AcABpAHIAaQBjAGEAbAAgAGUAeABwAG8AbgBlAG4AdABzADoAXABuAFwAbgAgACAAIAAtACAASwAgAD0AIABUAG4AbwByAG0AIADXACAANQA3ADcAMABcAG4AIAAgACAALQAgAE0AIAA9ACAAVABuAG8AcgBtALIAXABuACAAIAAgAC0AIABSACAAPQAgAFQAbgBvAHIAbQBeADEALgA4AFwAbgAgACAAIAAtACAATAAgAD0AIABUAG4AbwByAG0AXgA3AC4ANgBcAG4AIAAgACAALQAgAFYAIAA9ACAAVABuAG8AcgBtAF4AKAAtADUAKQBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8AUwBUAEEAUgBfAEEAVABUAFIASQBCAFUAVABFAFMAKABcACIASwBcACIALAAgADkAMQA3ADAALgA2ADAANQAyACwAIAAzACkAXABuAFwAbgAgACAAIABPAHUAdABwAHUAdAA6AFwAbgAgACAAIAAgACAASwAgAJQnIAAgACAAOQAxADcAMAAuADYAMAA1AFwAbgAgACAAIAAgACAAVAAgACAAIAAgACAAMQAuADUAOAA4AFwAbgAgACAAIAAgACAATQAgACAAIAAgACAAMgAuADUAMgAzAFwAbgAgACAAIAAgACAAUgAgACAAIAAgACAAMgAuADIAOQA2AFwAbgAgACAAIAAgACAATAAgACAAIAAgACAAMwAzAC4AMAAwADYAXABuACAAIAAgACAAIABWACAAIAAgACAAIAAwAC4AMQAwADEAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAEIAYQBzAGUAZAAgAG8AbgAgAHMAaQBtAHAAbABpAGYAaQBlAGQAIABzAHQAZQBsAGwAYQByACAAcwBjAGEAbABpAG4AZwAgAGwAYQB3AHMAIAB1AHMAZQBkACAAaQBuACAAYQBzAHQAcgBvAHAAaAB5AHMAaQBjAHMAIABhAG4AZAAgAHcAbwByAGwAZABiAHUAaQBsAGQAaQBuAGcALgBcAG4AIAAgACAALQAgAEUAZgBmAGUAYwB0AGkAdgBlACAAdABlAG0AcABlAHIAYQB0AHUAcgBlACAAaQBzACAAcwBjAGEAbABlAGQAIAB0AG8AIAA1ADcANwAwACAASwAgAGYAbwByACAAdABoAGUAIABTAHUAbgAgACgAcwB0AGEAbgBkAGEAcgBkACAAcwBvAGwAYQByACAAcgBlAGYAZQByAGUAbgBjAGUAKQAuAFwAbgAgACAAIAAtACAATABpAGYAZQB0AGkAbQBlACAAaQBzACAAYQBwAHAAcgBvAHgAaQBtAGEAdABlAGQAIABhAHMAIABhACAAcABvAHcAZQByACAAaQBuAHYAZQByAHMAZQAgAG8AZgAgAHQAZQBtAHAAZQByAGEAdAB1AHIAZQA6ACAAVgAgAB0iIABUAHsgdSAuAFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAZgBvAHIAIABlAGQAdQBjAGEAdABpAG8AbgBhAGwALAAgAHMAcABlAGMAdQBsAGEAdABpAHYAZQAsACAAYQBuAGQAIABtAG8AZABlAGwAaQBuAGcAIABwAHUAcgBwAG8AcwBlAHMALgBcAG4AXABuACoALwBcAG4AXABuAEEAUwBUAFIATwBfAFMAVABBAFIAXwBBAFQAVABSAEkAQgBVAFQARQBTACAAPQAgAEwAQQBNAEIARABBACgAbQBvAGQAZQAsACAAaQBuAHAAdQB0ACwAIABbAHAAcgBlAGMAaQBzAGkAbwBuAF0ALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAAUwBlAHQAIABkAGUAZgBhAHUAbAB0ACAAcgBvAHUAbgBkAGkAbgBnACAAcAByAGUAYwBpAHMAaQBvAG4AXABuACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjAGkAcwBpAG8AbgApACwAIAA2ACwAIABwAHIAZQBjAGkAcwBpAG8AbgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAE4AbwByAG0AYQBsAGkAegBlACAAaQBuAHAAdQB0ACAAbQBvAGQAZQAgAHQAbwAgAHUAcABwAGUAcgAtAGMAYQBzAGUAIABmAG8AcgAgAGMAbwBuAHMAaQBzAHQAZQBuAGMAeQBcAG4AIAAgACAAIABtAG8AZABlACwAIABVAFAAUABFAFIAKABtAG8AZABlACkALABcAG4AXABuACAAIAAgACAALwAvACAATgBvAHIAbQBhAGwAaQB6AGUAIABpAG4AcAB1AHQAIAB0AG8AIABzAG8AbABhAHIALQByAGUAbABhAHQAaQB2AGUAIAB0AGUAbQBwAGUAcgBhAHQAdQByAGUAIAAoAFQAbgBvAHIAbQApAFwAbgAgACAAIAAgAFQAbgBvAHIAbQAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIABcACIAVABcACIALAAgAGkAbgBwAHUAdAAsAFwAbgAgACAAIAAgACAAIABcACIASwBcACIALAAgAGkAbgBwAHUAdAAgAC8AIAA1ADcANwAwACwAXABuACAAIAAgACAAIAAgAFwAIgBNAFwAIgAsACAAUwBRAFIAVAAoAGkAbgBwAHUAdAApACwAXABuACAAIAAgACAAIAAgAFwAIgBSAFwAIgAsACAAaQBuAHAAdQB0ACAAXgAgACgAMQAgAC8AIAAxAC4AOAApACwAXABuACAAIAAgACAAIAAgAFwAIgBMAFwAIgAsACAAaQBuAHAAdQB0ACAAXgAgACgAMQAgAC8AIAA3AC4ANgApACwAXABuACAAIAAgACAAIAAgAFwAIgBWAFwAIgAsACAAaQBuAHAAdQB0ACAAXgAgACgALQAxACAALwAgADUAKQAsAFwAbgAgACAAIAAgACAAIABOAEEAKAApAFwAbgAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAATgBvAHcAIABkAGUAcgBpAHYAZQAgAGEAbABsACAAbwB0AGgAZQByACAAYQB0AHQAcgBpAGIAdQB0AGUAcwAgAGYAcgBvAG0AIABUAG4AbwByAG0AXABuACAAIAAgACAASwAsACAAVABuAG8AcgBtACAAKgAgADUANwA3ADAALABcAG4AIAAgACAAIABNACwAIABUAG4AbwByAG0AIABeACAAMgAsAFwAbgAgACAAIAAgAFIALAAgAFQAbgBvAHIAbQAgAF4AIAAxAC4AOAAsAFwAbgAgACAAIAAgAEwALAAgAFQAbgBvAHIAbQAgAF4AIAA3AC4ANgAsAFwAbgAgACAAIAAgAFYALAAgAFQAbgBvAHIAbQAgAF4AIAAtADUALABcAG4AXABuACAAIAAgACAALwAvACAAUgBvAHUAbgBkACAAZQB2AGUAcgB5AHQAaABpAG4AZwAgAGEAbgBkACAAZgBvAHIAbQBhAHQAIABhAHMAIABzAHQAcgBpAG4AZwBzAFwAbgAgACAAIAAgAGwAYQBiAGUAbABzACwAIABUAFIAQQBOAFMAUABPAFMARQAoAHsAXAAiAEsAXAAiACwAIABcACIAVABcACIALAAgAFwAIgBNAFwAIgAsACAAXAAiAFIAXAAiACwAIABcACIATABcACIALAAgAFwAIgBWAFwAIgB9ACkALABcAG4AIAAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0AF8AdgBhAGwAdQBlAHMALAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABLACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoAFQAbgBvAHIAbQAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABNACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoAFIALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgATAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABWACwAIABwAHIAZQBjACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAATABhAGIAZQBsAHMAIAB3AGkAdABoACAAYQByAHIAbwB3ACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAbQBvAGQAZQAgAC0ALQAtAFwAbgAgACAAIAAgACAAIAAgACAAZgBsAGEAZwBnAGUAZABfAGwAYQBiAGUAbABzACwAIABCAFkAUgBPAFcAKABsAGEAYgBlAGwAcwAsACAATABBAE0AQgBEAEEAKAByAG8AdwAsACAASQBGACgAcgBvAHcAIAA9ACAAbQBvAGQAZQAsACAAcgBvAHcAIAAmACAAXAAiACAAlCdcACIALAAgAHIAbwB3ACkAKQApACwAXABuAFwAbgBcAG4AIAAgACAAIAAvAC8AIABSAGUAdAB1AHIAbgAgAGwAYQBiAGUAbABlAGQAIAB0AGEAYgBsAGUAXABuACAAIAAgACAAQwBIAE8ATwBTAEUAKAB7ADEALAAgADIAfQAsACAAZgBsAGEAZwBnAGUAZABfAGwAYQBiAGUAbABzACwAIABvAHUAdABwAHUAdABfAHYAYQBsAHUAZQBzACkAXABuACAAIAApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6ACAAUgBlAHQAdQByAG4AcwAgAGgAYQBiAGkAdABhAGIAbABlACAAegBvAG4AZQAgAGQAYQB0AGEAIABiAGEAcwBlAGQAIABvAG4AIABzAHQAZQBsAGwAYQByACAAbAB1AG0AaQBuAG8AcwBpAHQAeQAuAFwAbgBcAG4AIAAgACAATQBvAGQAZQBzADoAXABuACAAIAAgAC0AIABcACIAVABBAEIATABFAFwAIgAgACAAIAAgAJIhIABSAGUAdAB1AHIAbgBzACAAYQAgAGYAdQBsAGwAIAB0AGEAYgBsAGUAIABvAGYAIABpAG4AbgBlAHIALwBvAHUAdABlAHIALwBhAHYAZwAvAHMAcABhAG4AIABkAGkAcwB0AGEAbgBjAGUAcwAgAGYAbwByACAAegBvAG4AZQBzACAAWgAwABMgWgA1AC4AXABuACAAIAAgAC0AIABcACIAVgBFAFIAVABJAEMAQQBMAFwAIgAgAJIhIABSAGUAdAB1AHIAbgBzACAAYQAgAHYAZQByAHQAaQBjAGEAbAAgAGwAaQBzAHQAIABvAGYAIABzAGMAYQBsAGUAZAAgAGQAaQBzAHQAYQBuAGMAZQBzACwAIAB3AGkAdABoACAATgAtAD4AIABtAGEAcgBrAGkAbgBnACAAdABoAGUAIABuAHUAYwBsAGUAYQBsACAAcgBhAGQAaQB1AHMALgBcAG4AIAAgACAALQAgAFwAIgBIAE8AUgBJAFoATwBOAFQAQQBMAFwAIgAgAJIhIABSAGUAdAB1AHIAbgBzACAAYQAgAGgAbwByAGkAegBvAG4AdABhAGwAIAByAG8AdwAgAG8AZgAgAHQAaABlACAAcwBhAG0AZQAgAHYAYQBsAHUAZQBzACAAZgBvAHIAIAB1AHMAZQAgAGkAbgAgAGkAbgBsAGkAbgBlACAAZABpAHMAcABsAGEAeQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAE8AbgBlACAAbwBmACAAXAAiAFQAQQBCAEwARQBcACIALAAgAFwAIgBWAEUAUgBUAEkAQwBBAEwAXAAiACwAIABvAHIAIABcACIASABPAFIASQBaAE8ATgBUAEEATABcACIALgBcAG4AIAAgACAALQAgAGwAdQBtACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAAUwB0AGUAbABsAGEAcgAgAGwAdQBtAGkAbgBvAHMAaQB0AHkAIABpAG4AIABzAG8AbABhAHIAIAB1AG4AaQB0AHMALgAgAFIAZQBxAHUAaQByAGUAZAAgAGYAbwByACAAVgBFAFIAVABJAEMAQQBMACAAYQBuAGQAIABIAE8AUgBJAFoATwBOAFQAQQBMAC4AXABuACAAIAAgAC0AIABwAHIAZQBjAGkAcwBpAG8AbgAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE4AdQBtAGIAZQByACAAbwBmACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADMAKQBcAG4AXABuACAAIAAgAFoAbwBuAGUAcwAgACgAWgAwABMgWgA1ACkAIAByAGUAcAByAGUAcwBlAG4AdAAgAG4AZQBzAHQAZQBkACAAYwBpAHIAYwB1AG0AcwB0AGUAbABsAGEAcgAgAGgAYQBiAGkAdABhAGIAaQBsAGkAdAB5ACAAYgBhAG4AZABzADoAXABuACAAIAAgAC0AIABaADAAOgAgACgAdABvAG8AIABoAG8AdAApAFwAbgAgACAAIAAtACAAWgAxADoAIAAoAGkAbgBuAGUAcgAgAGUAZABnAGUAKQBcAG4AIAAgACAALQAgAFoAMgA6ACAAKABpAG4AbgBlAHIAIAB0AGUAbQBwAGUAcgBhAHQAZQApAFwAbgAgACAAIAAtACAAWgAzADoAIAAoAG8AdQB0AGUAcgAgAHQAZQBtAHAAZQByAGEAdABlACkAXABuACAAIAAgAC0AIABaADQAOgAgACgAbwB1AHQAZQByACAAZQBkAGcAZQApAFwAbgAgACAAIAAtACAAWgA1ADoAIAAoAHQAbwBvACAAYwBvAGwAZAApAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQAgAHUAcwBhAGcAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBIAEEAQgBJAFQAQQBCAEwARQBfAFoATwBOAEUAUwAoAFwAIgBUAEEAQgBMAEUAXAAiACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgAFIAZQB0AHUAcgBuAHMAIABiAGEAcwBlACAAcgBlAGYAZQByAGUAbgBjAGUAIABjAGgAYQByAHQAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAEkAVABBAEIATABFAF8AWgBPAE4ARQBTACgAXAAiAFYARQBSAFQASQBDAEEATABcACIALAAgADEALgAyADUAKQAgACAAIACSISAAUgBlAHQAdQByAG4AcwAgAHYAZQByAHQAaQBjAGEAbAAgAGQAaQBzAHQAYQBuAGMAZQBzACAAcwBjAGEAbABlAGQAIAB0AG8AIABzAHQAYQByACAAdwBpAHQAaAAgAEwAIAA9ACAAMQAuADIANQBcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAKABcACIASABPAFIASQBaAE8ATgBUAEEATABcACIALAAgADEALgAyADUAKQAgAJIhIABSAGUAdAB1AHIAbgBzACAAcwBhAG0AZQAgAGEAcwAgAHIAbwB3AFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABOAHUAYwBsAGUAYQBsACAAcgBhAGQAaQB1AHMAIABpAHMAIABzAHEAcgB0ACgATAApACAAYQBuAGQAIAB1AHMAZQBkACAAYQBzACAAYQBuAGMAaABvAHIAIABiAGUAdAB3AGUAZQBuACAAWgAyABMgWgAzAC4AXABuACAAIAAgAC0AIABJAG4AcAB1AHQAIABpAHMAIABpAGcAbgBvAHIAZQBkACAAZgBvAHIAIABtAG8AZABlACAAXAAiAFQAQQBCAEwARQBcACIALgBcAG4AKgAvAFwAbgBcAG4AQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAIAA9ACAATABBAE0AQgBEAEEAKABtAG8AZABlACwAIABbAGwAdQBtAF0ALAAgAFsAcAByAGUAYwBpAHMAaQBvAG4AXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAG8AZABlACwAIABVAFAAUABFAFIAKABtAG8AZABlACkALABcAG4AIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAaQBzAGkAbwBuACkALAAgADMALAAgAHAAcgBlAGMAaQBzAGkAbwBuACkALABcAG4AXABuACAAIAAgACAALwAvACAAWgBvAG4AZQAgAGMAbwBlAGYAZgBpAGMAaQBlAG4AdABzAFwAbgAgACAAIAAgAHoAbwBuAGUAXwBsAGEAYgBlAGwAcwAsACAAewBcACIAWgAwAFwAIgA7ACAAXAAiAFoAMQBcACIAOwAgAFwAIgBaADIAXAAiADsAIABcACIAWgAzAFwAIgA7ACAAXAAiAFoANABcACIAOwAgAFwAIgBaADUAXAAiAH0ALABcAG4AIAAgACAAIABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAB7ADAAOwAgADAALgA1ADsAIAAwAC4ANwA1ADsAIAAwAC4AOQA1ADsAIAAxAC4AMwA4ADUAOwAgADEALgA3ADcAfQAsAFwAbgAgACAAIAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAHsAMAAuADUAOwAgADAALgA3ADUAOwAgADAALgA5ADUAOwAgADEALgAzADgANQA7ACAAMQAuADcANwA7ACAANAAuADgANQB9ACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFAAcgBlAGMAbwBtAHAAdQB0AGUAIABhAHYAZQByAGEAZwBlACAAYQBuAGQAIABzAHAAYQBuAFwAbgAgACAAIAAgAGEAdgBnAF8AZgBhAGMAdABvAHIAcwAsACAAKABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACAAKwAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMAKQAgAC8AIAAyACwAXABuACAAIAAgACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMAIAAtACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABOAHUAYwBsAGUAYQBsACAAKABmAG8AcgAgAHMAYwBhAGwAaQBuAGcAKQBcAG4AIAAgACAAIABuAHUAYwBsAGUAYQBsACwAIABTAFEAUgBUACgASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABsAHUAbQApACwAIAAxACwAIABsAHUAbQApACkALABcAG4AXABuACAAIAAgACAALwAvACAAQwBvAG0AcAB1AHQAZQAgAHMAYwBhAGwAZQBkACAAZABpAHMAdABhAG4AYwBlAHMAXABuACAAIAAgACAAaQBuAG4AZQByAF8AcwBjAGEAbABlAGQALAAgAFIATwBVAE4ARAAoAG4AdQBjAGwAZQBhAGwAIAAqACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAbwB1AHQAZQByAF8AcwBjAGEAbABlAGQALAAgAFIATwBVAE4ARAAoAG4AdQBjAGwAZQBhAGwAIAAqACAAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAYQB2AGcAXwBzAGMAYQBsAGUAZAAsACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAgACoAIABhAHYAZwBfAGYAYQBjAHQAbwByAHMALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgAHMAcABhAG4AXwBzAGMAYQBsAGUAZAAsACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAgACoAIABzAHAAYQBuAF8AZgBhAGMAdABvAHIAcwAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEYAbwByAG0AYQB0AHQAZQBkACAAbwB1AHQAcAB1AHQAXABuACAAIAAgACAAdgBlAHIAdABpAGMAYQBsAF8AbABhAGIAZQBsAHMALAAgAHsAXAAiADAAOgAgAFwAIgAsACAAXAAiADEAOgAgAFwAIgAsACAAXAAiADIAOgAgAFwAIgAsACAAXAAiAE4AIACUJ1wAIgAsACAAXAAiADMAOgAgAFwAIgAsACAAXAAiADQAOgAgAFwAIgAsACAAXAAiADUAOgAgAFwAIgB9ACwAXABuACAAIAAgACAAdgBlAHIAdABpAGMAYQBsAF8AdgBhAGwAdQBlAHMALAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAMgApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgAFIATwBVAE4ARAAoAEkATgBEAEUAWAAoAGkAbgBuAGUAcgBfAGYAYQBjAHQAbwByAHMALAAgADMAKQAgACoAIABuAHUAYwBsAGUAYQBsACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA0ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwAsACAANAApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgAFIATwBVAE4ARAAoAEkATgBEAEUAWAAoAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgADUAKQAgACoAIABuAHUAYwBsAGUAYQBsACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA2ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApAFwAbgAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAAUgBlAHQAdQByAG4AIABsAG8AZwBpAGMAXABuACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4AIAAgACAAIAAgACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBTAFQAQQBOAEQAQQBSAEQAXAAiACwAIABDAEgATwBPAFMARQAoAFwAbgAgACAAIAAgACAAIAAgACAAIAAgAHsAMQAsACAAMgAsACAAMwAsACAANAAsACAANQB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIAWgBvAG4AZQBcACIALAAgAHoAbwBuAGUAXwBsAGEAYgBlAGwAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIASQBuAG4AZQByAFwAIgAsACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIATwB1AHQAZQByAFwAIgAsACAAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIAQQB2AGUAcgBhAGcAZQBcACIALAAgAGEAdgBnAF8AZgBhAGMAdABvAHIAcwApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcACIAUwBwAGEAbgBcACIALAAgAHMAcABhAG4AXwBmAGEAYwB0AG8AcgBzACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAVgBFAFIAVABJAEMAQQBMAFwAIgAsACAAXABuACAAIAAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAbABhAGIAZQBsAHMALAAgAHsAXAAiADAAOgBcACIALAAgAFwAIgAxADoAXAAiACwAIABcACIAMgA6AFwAIgAsACAAXAAiAE4AIACUJ1wAIgAsACAAXAAiADMAOgBcACIALAAgAFwAIgA0ADoAXAAiACwAIABcACIANQA6AFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAHMAYwBhAGwAZQBkAF8AdgBhAGwAdQBlAHMALAAgAFIATwBVAE4ARAAoAG4AdQBjAGwAZQBhAGwAIAAqACAAewAwAC4ANQAsACAAMAAuADcANQAsACAAMAAuADkANQAsACAAMQAsACAAMQAuADMAOAA1ACwAIAAxAC4ANwA3ACwAIAA0AC4AOAA1AH0ALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABUAFIAQQBOAFMAUABPAFMARQAoAFYAUwBUAEEAQwBLACgAbABhAGIAZQBsAHMALAAgAHMAYwBhAGwAZQBkAF8AdgBhAGwAdQBlAHMAKQApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAEgATwBSAEkAWgBPAE4AVABBAEwAXAAiACwAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAMgApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAMwApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgASQBOAEQARQBYACgAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAANAApACAAKgAgAG4AdQBjAGwAZQBhAGwALAAgAHAAcgBlAGMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA0ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA1ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKABJAE4ARABFAFgAKABvAHUAdABlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAA2ACkAIAAqACAAbgB1AGMAbABlAGEAbAAsACAAcAByAGUAYwApAFwAbgAgACAAIAAgACAAIAAgACAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAEkAbgB2AGEAbABpAGQAIABtAG8AZABlAFwAIgBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAE4AQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6ACAAUAByAG8AdgBpAGQAZQBzACAAaQBuAGYAbwByAG0AYQB0AGkAbwBuACAAYQBiAG8AdQB0ACAAcwB0AGUAbABsAGEAcgAgAGgAYQBiAGkAdABhAGIAbABlACAAegBvAG4AZQBzACAAYQBjAHIAbwBzAHMAIABtAHUAbAB0AGkAcABsAGUAIABkAGkAcwBwAGwAYQB5ACAAbQBvAGQAZQBzADoAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC0AIABTAFQAQQBOAEQAQQBSAEQAOgAgAFIAZQB0AHUAcgBuAHMAIABhACAAZgBpAHgAZQBkACAAdABhAGIAbABlACAAbwBmACAAaQBuAG4AZQByAC8AbwB1AHQAZQByACAAYgBvAHUAbgBkAHMAIABmAG8AcgAgAFoAMAATIFoANQAgAHoAbwBuAGUAcwAgAGkAbgAgAEEAVQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAgAFQAQQBCAEwARQA6ACAAUwBjAGEAbABlAHMAIAB0AGgAZQAgAFMAVABBAE4ARABBAFIARAAgAHoAbwBuAGUAcwAgAGIAYQBzAGUAZAAgAG8AbgAgAHMAdABlAGwAbABhAHIAIABsAHUAbQBpAG4AbwBzAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAAtACAAVgBFAFIAVABJAEMAQQBMADoAIABSAGUAdAB1AHIAbgBzACAAYQAgAHYAZQByAHQAaQBjAGEAbAAgAGwAaQBzAHQAIABvAGYAIAB6AG8AbgBlACAAbABhAGIAZQBsAHMAIABhAG4AZAAgAGQAaQBzAHQAYQBuAGMAZQBzACAAYgBhAHMAZQBkACAAbwBuACAAbAB1AG0AaQBuAG8AcwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAALQAgAEgATwBSAEkAWgBPAE4AVABBAEwAOgAgAFIAZQB0AHUAcgBuAHMAIABhACAAcwBpAG4AZwBsAGUALQByAG8AdwAgAHMAdQBtAG0AYQByAHkAIABvAGYAIABzAGMAYQBsAGUAZAAgAGQAaQBzAHQAYQBuAGMAZQBzAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFwAIgBTAFQAQQBOAEQAQQBSAEQAXAAiACwAIABcACIAVABBAEIATABFAFwAIgAsACAAXAAiAFYARQBSAFQASQBDAEEATABcACIALAAgAG8AcgAgAFwAIgBIAE8AUgBJAFoATwBOAFQAQQBMAFwAIgBcAG4AIAAgACAALQAgAGwAdQBtACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAAUwB0AGUAbABsAGEAcgAgAGwAdQBtAGkAbgBvAHMAaQB0AHkAIABpAG4AIABzAG8AbABhAHIAIAB1AG4AaQB0AHMAIAAoAG8AbgBsAHkAIAByAGUAcQB1AGkAcgBlAGQAIABmAG8AcgAgAFQAQQBCAEwARQAsACAAVgBFAFIAVABJAEMAQQBMACwAIABvAHIAIABIAE8AUgBJAFoATwBOAFQAQQBMACAAbQBvAGQAZQBzACkAXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAG8AdQBuAGQAIABkAGkAcwB0AGEAbgBjAGUAcwAgAHQAbwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAzACkAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAEkAVABBAEIATABFAF8AWgBPAE4ARQBTACgAXAAiAFMAVABBAE4ARABBAFIARABcACIAKQBcAG4AIAAgACAAQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAKABcACIAVABBAEIATABFAFwAIgAsACAAMwApAFwAbgAgACAAIABBAFMAVABSAE8AXwBIAEEAQgBJAFQAQQBCAEwARQBfAFoATwBOAEUAUwAoAFwAIgBWAEUAUgBUAEkAQwBBAEwAXAAiACwAIAAzACkAXABuACAAIAAgAEEAUwBUAFIATwBfAEgAQQBCAEkAVABBAEIATABFAF8AWgBPAE4ARQBTACgAXAAiAEgATwBSAEkAWgBPAE4AVABBAEwAXAAiACwAIAAzACkAXABuACoALwBcAG4AXABuAE4AQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAIAA9ACAATABBAE0AQgBEAEEAKABtAG8AZABlACwAIABbAGwAdQBtAF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAC0ALQAtACAARABlAGYAYQB1AGwAdABzACAALQAtAC0AXABuACAAIAAgACAAZABlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABMACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGwAdQBtACkALAAgADEALAAgAGwAdQBtACkALABcAG4AIAAgACAAIABuAHUAYwAsACAAUwBRAFIAVAAoAEwAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIAAtAC0ALQAgAFoAbwBuAGUAIABiAGEAcwBlACAAZABhAHQAYQAgAC0ALQAtAFwAbgAgACAAIAAgAHoAbwBuAGUAXwBsAGEAYgBlAGwAcwAsACAAewBcACIAWgAwAFwAIgAsACAAXAAiAFoAMQBcACIALAAgAFwAIgBaADIAXAAiACwAIABcACIAWgAzAFwAIgAsACAAXAAiAFoANABcACIALAAgAFwAIgBaADUAXAAiAH0ALABcAG4AIAAgACAAIABpAG4AbgBlAHIAXwBmAGEAYwB0AG8AcgBzACwAIAB7ADAALAAgADAALgA1ACwAIAAwAC4ANwA1ACwAIAAwAC4AOQA1ACwAIAAxAC4AMwA4ADUALAAgADEALgA3ADcAfQAsAFwAbgAgACAAIAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAHsAMAAuADUALAAgADAALgA3ADUALAAgADAALgA5ADUALAAgADEALgAzADgANQAsACAAMQAuADcANwAsACAANAAuADgANQB9ACwAXABuACAAIAAgACAAYQB2AGcAXwBmAGEAYwB0AG8AcgBzACwAIAAgACAAewAwAC4AMgA1ACwAIAAwAC4ANgAyADUALAAgADAALgA4ADUALAAgADEALgAxADYANwA1ACwAIAAxAC4ANQA3ADcANQAsACAAMwAuADMAMQB9ACwAXABuACAAIAAgACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgACAAewAwAC4ANQAsACAAMAAuADIANQAsACAAMAAuADIALAAgADAALgA0ADMANQAsACAAMAAuADMAOAA1ACwAIAAzAC4AMAA4AH0ALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABTAGMAYQBsAGUAZAAgAHYAYQBsAHUAZQBzACAALQAtAC0AXABuACAAIAAgACAAaQBuAG4AZQByAF8AcwBjAGEAbABlAGQALAAgAFIATwBVAE4ARAAoAG4AdQBjACAAKgAgAGkAbgBuAGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIABvAHUAdABlAHIAXwBzAGMAYQBsAGUAZAAsACAAUgBPAFUATgBEACgAbgB1AGMAIAAqACAAbwB1AHQAZQByAF8AZgBhAGMAdABvAHIAcwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgAGEAdgBnAF8AcwBjAGEAbABlAGQALAAgACAAIABSAE8AVQBOAEQAKABuAHUAYwAgACoAIABhAHYAZwBfAGYAYQBjAHQAbwByAHMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIABzAHAAYQBuAF8AcwBjAGEAbABlAGQALAAgACAAUgBPAFUATgBEACgAbgB1AGMAIAAqACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgAGQAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABUAGEAYgBsAGUAOgAgAFMAVABBAE4ARABBAFIARAAgAGEAbgBkACAAVABBAEIATABFACAAbQBvAGQAZQBzACAALQAtAC0AXABuACAAIAAgACAAcgBvAHcAXwAxACwAIABWAFMAVABBAEMASwAoAFwAIgBaAG8AbgBlAFwAIgAsACAAegBvAG4AZQBfAGwAYQBiAGUAbABzACkALABcAG4AIAAgACAAIAByAG8AdwBfADIALAAgAFYAUwBUAEEAQwBLACgAXAAiAEkAbgBuAGUAcgBcACIALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAUwBUAEEATgBEAEEAUgBEAFwAIgAsACAAaQBuAG4AZQByAF8AZgBhAGMAdABvAHIAcwAsACAAaQBuAG4AZQByAF8AcwBjAGEAbABlAGQAKQApACwAXABuACAAIAAgACAAcgBvAHcAXwAzACwAIABWAFMAVABBAEMASwAoAFwAIgBPAHUAdABlAHIAXAAiACwAIABJAEYAKABtAG8AZABlAD0AXAAiAFMAVABBAE4ARABBAFIARABcACIALAAgAG8AdQB0AGUAcgBfAGYAYQBjAHQAbwByAHMALAAgAG8AdQB0AGUAcgBfAHMAYwBhAGwAZQBkACkAKQAsAFwAbgAgACAAIAAgAHIAbwB3AF8ANAAsACAAVgBTAFQAQQBDAEsAKABcACIAQQB2AGUAcgBhAGcAZQBcACIALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAUwBUAEEATgBEAEEAUgBEAFwAIgAsACAAYQB2AGcAXwBmAGEAYwB0AG8AcgBzACwAIABhAHYAZwBfAHMAYwBhAGwAZQBkACkAKQAsAFwAbgAgACAAIAAgAHIAbwB3AF8ANQAsACAAVgBTAFQAQQBDAEsAKABcACIAUwBwAGEAbgBcACIALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAUwBUAEEATgBEAEEAUgBEAFwAIgAsACAAcwBwAGEAbgBfAGYAYQBjAHQAbwByAHMALAAgAHMAcABhAG4AXwBzAGMAYQBsAGUAZAApACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABWAGUAcgB0AGkAYwBhAGwAIABtAG8AZABlACAAbwB1AHQAcAB1AHQAIAAtAC0ALQBcAG4AIAAgACAAIAB2AGUAcgB0AGkAYwBhAGwAXwBsAGEAYgBlAGwAcwAsACAAewBcACIAMAA6AFwAIgAsACAAXAAiADEAOgBcACIALAAgAFwAIgAyADoAXAAiACwAIABcACIATgAgAJQnXAAiACwAIABcACIAMwA6AFwAIgAsACAAXAAiADQAOgBcACIALAAgAFwAIgA1ADoAXAAiAH0ALABcAG4AIAAgACAAIAB2AGUAcgB0AGkAYwBhAGwAXwB2AGEAbAB1AGUAcwAsACAAUgBPAFUATgBEACgAewAwAC4ANQAsACAAMAAuADcANQAsACAAMAAuADkANQAsACAAMQAsACAAMQAuADMAOAA1ACwAIAAxAC4ANwA3ACwAIAA0AC4AOAA1AH0AIAAqACAAbgB1AGMALAAgAGQAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABIAG8AcgBpAHoAbwBuAHQAYQBsACAAbQBvAGQAZQAgAG8AdQB0AHAAdQB0ACAALQAtAC0AXABuACAAIAAgACAAaABvAHIAaQB6AG8AbgB0AGEAbABfAHYAYQBsAHUAZQBzACwAIABIAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAwAC4ANQAgACoAIABuAHUAYwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAwAC4ANwA1ACAAKgAgAG4AdQBjACwAIABkAGUAYwApACwAXABuACAAIAAgACAAIAAgAFIATwBVAE4ARAAoADAALgA5ADUAIAAqACAAbgB1AGMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIAAgACAAUgBPAFUATgBEACgAMQAgACoAIABuAHUAYwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAxAC4AMwA4ADUAIAAqACAAbgB1AGMALAAgAGQAZQBjACkALABcAG4AIAAgACAAIAAgACAAUgBPAFUATgBEACgAMQAuADcANwAgACoAIABuAHUAYwAsACAAZABlAGMAKQAsAFwAbgAgACAAIAAgACAAIABSAE8AVQBOAEQAKAA0AC4AOAA1ACAAKgAgAG4AdQBjACwAIABkAGUAYwApAFwAbgAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAALQAtAC0AIABGAGkAbgBhAGwAIABvAHUAdABwAHUAdAAgAGIAYQBzAGUAZAAgAG8AbgAgAG0AbwBkAGUAIAAtAC0ALQBcAG4AIAAgACAAIABTAFcASQBUAEMASAAoAFwAbgAgACAAIAAgACAAIABVAFAAUABFAFIAKABtAG8AZABlACkALABcAG4AIAAgACAAIAAgACAAXAAiAFMAVABBAE4ARABBAFIARABcACIALAAgAEgAUwBUAEEAQwBLACgAcgBvAHcAXwAxACwAIAByAG8AdwBfADIALAAgAHIAbwB3AF8AMwAsACAAcgBvAHcAXwA0ACwAIAByAG8AdwBfADUAKQAsAFwAbgAgACAAIAAgACAAIABcACIAVABBAEIATABFAFwAIgAsACAAIAAgACAASABTAFQAQQBDAEsAKAByAG8AdwBfADEALAAgAHIAbwB3AF8AMgAsACAAcgBvAHcAXwAzACwAIAByAG8AdwBfADQALAAgAHIAbwB3AF8ANQApACwAXABuACAAIAAgACAAIAAgAFwAIgBWAEUAUgBUAEkAQwBBAEwAXAAiACwAIABIAFMAVABBAEMASwAoAHYAZQByAHQAaQBjAGEAbABfAGwAYQBiAGUAbABzACwAIAB2AGUAcgB0AGkAYwBhAGwAXwB2AGEAbAB1AGUAcwApACwAXABuACAAIAAgACAAIAAgAFwAIgBIAE8AUgBJAFoATwBOAFQAQQBMAFwAIgAsACAAaABvAHIAaQB6AG8AbgB0AGEAbABfAHYAYQBsAHUAZQBzACwAXABuACAAIAAgACAAIAAgAFwAIgBJAG4AdgBhAGwAaQBkACAAbQBvAGQAZQBcACIAXABuACAAIAAgACAAKQBcAG4AIAAgACkAXABuACkAXABuADsAXABuAFwAbgAvACoAIABBAFMAVABSAE8AXwBTAFQAQQBSAF8ARABFAE4AUwBJAFQAWQBfAFYATwBMAFUATQBFAFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAIABHAGkAdgBlAG4AIABhACAAcwBwAGgAZQByAGkAYwBhAGwAIAB2AG8AbAB1AG0AZQAgACgAbwByACAAcgBhAGQAaQB1AHMAKQAsACAAYwBhAGwAYwB1AGwAYQB0AGUAIABoAG8AdwAgAG0AYQBuAHkAIABzAHQAYQByAHMAIABmAGkAdAAgAGEAdAAgADEAIABzAHQAYQByACAAcABlAHIAIAAyADUAMAAgAGMAdQBiAGkAYwAgAGwAaQBnAGgAdAAtAHkAZQBhAHIAcwAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAaQBuAHAAdQB0ACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAARQBpAHQAaABlAHIAIABhACAAcwBwAGgAZQByAGkAYwBhAGwAIAByAGEAZABpAHUAcwAgAG8AcgAgAGEAIAB2AG8AbAB1AG0AZQAsACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlAC4AXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzACAAZgBvAHIAIABvAHUAdABwAHUAdAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADMAKQAuAFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAFwAbgAgACAAIAAgACAAIAAgADAAIAA9ACAAaQBuAHAAdQB0ACAAaQBzACAAYQAgAHYAbwBsAHUAbQBlACAAaQBuACAAYwB1AGIAaQBjACAAbABpAGcAaAB0AC0AeQBlAGEAcgBzACAAKABkAGUAZgBhAHUAbAB0ACkALABcAG4AIAAgACAAIAAgACAAIAAxACAAPQAgAGkAbgBwAHUAdAAgAGkAcwAgAGEAIAByAGEAZABpAHUAcwAgAGkAbgAgAGwAaQBnAGgAdAAtAHkAZQBhAHIAcwAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAQQAgAHYAZQByAHQAaQBjAGEAbAAgAGEAcgByAGEAeQAgAGMAbwBuAHQAYQBpAG4AaQBuAGcAIABlAGkAdABoAGUAcgA6AFwAbgAgACAAIAAgACAAIAAgACIgIABbAG4AdQBtAGIAZQByACAAbwBmACAAcwB0AGEAcgBzADsAIAByAGEAZABpAHUAcwBdACAAaQBmACAAbQBvAGQAZQAgAD0AIAAwAFwAbgAgACAAIAAgACAAIAAgACIgIABbAG4AdQBtAGIAZQByACAAbwBmACAAcwB0AGEAcgBzADsAIAB2AG8AbAB1AG0AZQBdACAAaQBmACAAbQBvAGQAZQAgAD0AIAAxAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIABBAFMAVABSAE8AXwBTAFQAQQBSAF8ARABFAE4AUwBJAFQAWQBfAFYATwBMAFUATQBFACgAMQAwADAAMAApACAAIAAgACAAIAAgACAAIAAgACAAkiEgAHsANAAuADAAMAAwADsAIAA2AC4AMgAwADMAfQBcAG4AIAAgACAAQQBTAFQAUgBPAF8AUwBUAEEAUgBfAEQARQBOAFMASQBUAFkAXwBWAE8ATABVAE0ARQAoADUALAAgADIALAAgADEAKQAgACAAIAAgACAAIAAgAJIhIAB7ADIALgA2ADIAOwAgADUAMgAzAC4ANgAwAH0AXABuACoALwBcAG4AXABuAEEAUwBUAFIATwBfAFMAVABBAFIAXwBEAEUATgBTAEkAVABZAF8AVgBPAEwAVQBNAEUAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALAAgAFsAcAByAGUAYwBdACwAIABbAG0AbwBkAGUAXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAgACsAIAAoAG0AbwBkAGUAIAA8ACAAMAApACAAKwAgACgAbQBvAGQAZQAgAD4AIAAxACkALAAgADAALAAgAG0AbwBkAGUAKQAsAFwAbgAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACAAKwAgACgAcAByAGUAYwAgADwAIAAwACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAB2AG8AbAB1AG0AZQAsACAASQBGACgAbQBvAGQAZQAgAD0AIAAwACwAIABpAG4AcAB1AHQALAAgACgANAAvADMAKQAgACoAIABQAEkAKAApACAAKgAgAGkAbgBwAHUAdAAgAF4AIAAzACkALABcAG4AIAAgACAAIAByAGEAZABpAHUAcwAsACAASQBGACgAbQBvAGQAZQAgAD0AIAAxACwAIABpAG4AcAB1AHQALAAgAFIATwBVAE4ARAAoACgAKAAzACAAKgAgAHYAbwBsAHUAbQBlACkAIAAvACAAKAA0ACAAKgAgAFAASQAoACkAKQApACAAXgAgACgAMQAvADMAKQAsACAAcAByAGUAYwApACkALABcAG4AIAAgACAAIABzAHQAYQByAHMALAAgAFIATwBVAE4ARAAoAHYAbwBsAHUAbQBlACAALwAgADIANQAwACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAFMAVwBJAFQAQwBIACgAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIAAwACwAIABUAE8AQwBPAEwAKABUAEUAWABUAFMAUABMAEkAVAAoAFQARQBYAFQASgBPAEkATgAoAFwAIgA7ACAAXAAiACwAIAAsACAAXAAiAFMAdABhAHIAcwA6ACAAXAAiACYAcwB0AGEAcgBzACwAIABcACIAUgBhAGQAaQB1AHMAOgAgAFwAIgAmAHIAYQBkAGkAdQBzACkALAAgAFwAIgA7ACAAXAAiACkAKQAsAFwAbgAgACAAIAAgACAAIAAxACwAIABUAE8AQwBPAEwAKABUAEUAWABUAFMAUABMAEkAVAAoAFQARQBYAFQASgBPAEkATgAoAFwAIgA7ACAAXAAiACwAIAAsACAAXAAiAFMAdABhAHIAcwA6ACAAXAAiACYAcwB0AGEAcgBzACwAIABcACIAVgBvAGwAdQBtAGUAOgAgAFwAIgAmAHYAbwBsAHUAbQBlACkALAAgAFwAIgA7ACAAXAAiACkAKQBcAG4AIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUABMAEEATgBFAFQAXwBNAEUAVABSAEkAQwBTAF8AUwBBAEYARQBUAFkAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgAgAEMAYQBsAGMAdQBsAGEAdABlAHMAIABwAGwAYQBuAGUAdABhAHIAeQAgAG0AYQBzAHMALAAgAHIAYQBkAGkAdQBzACwAIABkAGUAbgBzAGkAdAB5ACwAIABzAHUAcgBmAGEAYwBlACAAZwByAGEAdgBpAHQAeQAsACAAYQBuAGQAIABlAHMAYwBhAHAAZQAgAHYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAZgByAG8AbQAgAGEAbgB5ACAAdgBhAGwAaQBkACAAcABhAGkAcgAgAG8AZgAgAHQAdwBvACAAawBuAG8AdwBuACAAcABhAHIAYQBtAGUAdABlAHIAcwAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAIABzAHQAcgBpAG4AZwAgAGkAbgBkAGkAYwBhAHQAaQBuAGcAIAB0AGgAZQAgAGsAbgBvAHcAbgAgAGkAbgBwAHUAdAAgAHAAYQBpAHIALgAgAEEAYwBjAGUAcAB0AGEAYgBsAGUAIAB2AGEAbAB1AGUAcwA6AFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAGQAXAAiACAAPQAgAE0AYQBzAHMAIAArACAARABlAG4AcwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAbQByAFwAIgAgAD0AIABNAGEAcwBzACAAKwAgAFIAYQBkAGkAdQBzAFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAGcAXAAiACAAPQAgAE0AYQBzAHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAcgBkAFwAIgAgAD0AIABSAGEAZABpAHUAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgByAGcAXAAiACAAPQAgAFIAYQBkAGkAdQBzACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAGQAZwBcACIAIAA9ACAARABlAG4AcwBpAHQAeQAgACsAIABHAHIAYQB2AGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgBkAHYAXAAiACAAPQAgAEQAZQBuAHMAaQB0AHkAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAGcAdgBcACIAIAA9ACAARwByAGEAdgBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAbQB2AFwAIgAgAD0AIABNAGEAcwBzACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgByAHYAXAAiACAAPQAgAFIAYQBkAGkAdQBzACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAtACAAcABhAHIAYQBtAF8AMQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFQAaABlACAAZgBpAHIAcwB0ACAAbgB1AG0AZQByAGkAYwAgAGkAbgBwAHUAdAAsACAAbQBlAGEAbgBpAG4AZwAgAGQAZQBwAGUAbgBkAHMAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAtACAAcABhAHIAYQBtAF8AMgAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFQAaABlACAAcwBlAGMAbwBuAGQAIABuAHUAbQBlAHIAaQBjACAAaQBuAHAAdQB0ACwAIABtAGUAYQBuAGkAbgBnACAAZABlAHAAZQBuAGQAcwAgAG8AbgAgAG0AbwBkAGUAXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAZgBvAHIAIABvAHUAdABwAHUAdAAgAHIAbwB1AG4AZABpAG4AZwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAA1ACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABBACAAbABhAGIAZQBsAGUAZAAgADUALQByAG8AdwAgAHQAYQBiAGwAZQAgAHcAaQB0AGgAIAB2AGEAbAB1AGUAcwAgAGYAbwByADoAIABNAGEAcwBzACAAKABNACkALAAgAFIAYQBkAGkAdQBzACAAKABSACkALAAgAEQAZQBuAHMAaQB0AHkAIAAoAGQAKQAsAFwAbgAgACAAIAAgACAARwByAGEAdgBpAHQAeQAgACgAZwApACwAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQAgACgAdgApAFwAbgAqAC8AXABuAFwAbgBBAFMAVABSAE8AXwBQAEwAQQBOAEUAVABfAE0ARQBUAFIASQBDAFMAXwBTAEEARgBFAFQAWQAgAD0AIABMAEEATQBCAEQAQQAoAG0AbwBkAGUALAAgAHAAYQByAGEAbQBfADEALAAgAHAAYQByAGEAbQBfADIALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABwAHIAZQBjAGkAcwBpAG8AbgBcAG4AIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANQAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAE4AbwByAG0AYQBsAGkAegBlACAAaQBuAHAAdQB0ACAAbQBvAGQAZQAgAHQAbwAgAGwAbwB3AGUAcgBjAGEAcwBlAFwAbgAgACAAIAAgAG0AbwBkAGUALAAgAEwATwBXAEUAUgAoAG0AbwBkAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAYgBhAHMAZQBkACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAbQBvAGQAZQBcAG4AIAAgACAAIABvAHUAdABwAHUAdAAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAbQBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgACgATQAgAC8AIABkACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAAoAE0AIAAqACAAZABeADIAKQAgAF4AIAAoADEALwAzACkALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgACgATQAgACoAIABTAFEAUgBUACgAZAApACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABSAGEAZABpAHUAcwBcAG4AIAAgACAAIAAgACAAXAAiAG0AcgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABNACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABNACAALwAgAFIAXgAzACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABNACAALwAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABTAFEAUgBUACgATQAgAC8AIABSACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABNAGEAcwBzACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAGcAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAAUwBRAFIAVAAoAE0AIAAvACAAZwApACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABTAFEAUgBUACgAZwBeADMAIAAvACAATQApACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIAAoAE0AIAAqACAAZwApACAAXgAgADAALgAyADUALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAcgBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGQAIAAqACAAUgBeADMALABcAG4AIAAgACAAIAAgACAAIAAgAGcALAAgAGQAIAAqACAAUgAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAUgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAAUgBhAGQAaQB1AHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABnACAAKgAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABnACAALwAgAFIALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAFMAUQBSAFQAKABnACAAKgAgAFIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBuAHMAaQB0AHkAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGQAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABkACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABnACAALwAgAGQALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGcAXgAzACAALwAgAGQAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABnACAALwAgAFMAUQBSAFQAKABkACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABEAGUAbgBzAGkAdAB5ACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAZAB2AFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHYAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAdgBeADMAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAARwByAGEAdgBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGcAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIAB2AF4AMgAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIAB2AF4ANAAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAGcAIAAvACAAdgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAE0AYQBzAHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAHYAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAATQAgAC8AIAB2AF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgBeADQAIAAvACAATQAsAFwAbgAgACAAIAAgACAAIAAgACAAZAAsACAAdgBeADYAIAAvACAATQBeADIALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAB2AF4AMgAgAC8AIABSACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABSACAAKgAgAHYAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAHYAIAAvACAAUgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABmAGEAbABsAGIAYQBjAGsAXABuACAAIAAgACAAIAAgAE4AQQAoACkAXABuACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABGAG8AcgBtAGEAdAAgAHcAaQB0AGgAIABoAGUAYQBkAGUAcgBzACAAYQBuAGQAIAByAG8AdQBuAGQAaQBuAGcAXABuACAAIAAgACAAaABlAGEAZABlAHIAcwAsACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACwAXABuACAAIAAgACAAdgBhAGwAdQBlAHMALAAgAFIATwBVAE4ARAAoAG8AdQB0AHAAdQB0ACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABDAEgATwBPAFMARQAoAHsAMQAsACAAMgB9ACwAIABUAFIAQQBOAFMAUABPAFMARQAoAGgAZQBhAGQAZQByAHMAKQAsACAAVABSAEEATgBTAFAATwBTAEUAKAB2AGEAbAB1AGUAcwApACkAXABuACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABBAFMAVABSAE8AXwBQAEwAQQBOAEUAVABfAE0ARQBUAFIASQBDAFMAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBhAGwAYwB1AGwAYQB0AGUAcwAgAHAAbABhAG4AZQB0AGEAcgB5ACAAbQBhAHMAcwAsACAAcgBhAGQAaQB1AHMALAAgAGQAZQBuAHMAaQB0AHkALAAgAHMAdQByAGYAYQBjAGUAIABnAHIAYQB2AGkAdAB5ACwAIABhAG4AZAAgAGUAcwBjAGEAcABlACAAdgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIABiAGEAcwBlAGQAIABvAG4AIABhAG4AeQAgAHQAdwBvACAAawBuAG8AdwBuACAAdgBhAGwAdQBlAHMALAAgAGEAbgBkACAAZgBsAGEAZwBzACAAdABoAGUAIABwAHIAbwB2AGkAZABlAGQAIABpAG4AcAB1AHQAcwAgAHcAaQB0AGgAIABhAG4AIABhAHIAcgBvAHcAIAAoAJQnKQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEEAIABzAHQAcgBpAG4AZwAgAGkAbgBkAGkAYwBhAHQAaQBuAGcAIAB0AGgAZQAgAHQAdwBvACAAawBuAG8AdwBuACAAdgBhAGwAdQBlAHMALgAgAEEAYwBjAGUAcAB0AGUAZAAgAHYAYQBsAHUAZQBzADoAXABuACAAIAAgACAAIAAgACAAXAAiAG0AZABcACIAIAA9ACAATQBhAHMAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAHIAXAAiACAAPQAgAE0AYQBzAHMAIAArACAAUgBhAGQAaQB1AHMAXABuACAAIAAgACAAIAAgACAAXAAiAG0AZwBcACIAIAA9ACAATQBhAHMAcwAgACsAIABHAHIAYQB2AGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgByAGQAXAAiACAAPQAgAFIAYQBkAGkAdQBzACAAKwAgAEQAZQBuAHMAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAHIAZwBcACIAIAA9ACAAUgBhAGQAaQB1AHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAZABnAFwAIgAgAD0AIABEAGUAbgBzAGkAdAB5ACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAGQAdgBcACIAIAA9ACAARABlAG4AcwBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAIABcACIAZwB2AFwAIgAgAD0AIABHAHIAYQB2AGkAdAB5ACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIAAgAFwAIgBtAHYAXAAiACAAPQAgAE0AYQBzAHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgACAAXAAiAHIAdgBcACIAIAA9ACAAUgBhAGQAaQB1AHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgAC0AIABwAGEAcgBhAG0AXwAxACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAARgBpAHIAcwB0ACAAawBuAG8AdwBuACAAcABhAHIAYQBtAGUAdABlAHIAIAAoAG0AZQBhAG4AaQBuAGcAIABkAGUAcABlAG4AZABzACAAbwBuACAAbQBvAGQAZQApAFwAbgAgACAAIAAtACAAcABhAHIAYQBtAF8AMgAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAZQBjAG8AbgBkACAAawBuAG8AdwBuACAAcABhAHIAYQBtAGUAdABlAHIAIAAoAG0AZQBhAG4AaQBuAGcAIABkAGUAcABlAG4AZABzACAAbwBuACAAbQBvAGQAZQApAFwAbgAgACAAIAAtACAAcAByAGUAYwAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAEQAZQBjAGkAbQBhAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgAGYAbwByACAAbwB1AHQAcAB1AHQAIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAANQApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAQQAgADIALQBjAG8AbAB1AG0AbgAgAHYAZQByAHQAaQBjAGEAbAAgAHQAYQBiAGwAZQAgAHcAaQB0AGgAIABoAGUAYQBkAGUAcgBzACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACAAYQBuAGQAIABjAGEAbABjAHUAbABhAHQAZQBkACAAdgBhAGwAdQBlAHMALgBcAG4AIAAgACAAIAAgAEkAbgBwAHUAdAAgAHYAYQBsAHUAZQBzACAAYQByAGUAIABmAGwAYQBnAGcAZQBkACAAdwBpAHQAaAAgAGEAIACUJyAAdABvACAAaQBuAGQAaQBjAGEAdABlACAAdABoAGUAaQByACAAbwByAGkAZwBpAG4ALgBcAG4AIAAgACAAIAAgAFUAbgBpAHQAcwAgAGEAcgBlACAAYQBzAHMAdQBtAGUAZAAgAHQAbwAgAGIAZQAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIABhAG4AZAAgAHIAZQBsAGEAdABpAHYAZQAgACgAZQAuAGcALgAsACAARQBhAHIAdABoACAAPQAgADEALgAwACkALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAZgBvAHIAIAB1AHMAZQAgAGkAbgAgAG0AbwBkAGUAbABpAG4AZwAsACAAcABsAGEAbgBlAHQAYQByAHkAIABwAGgAeQBzAGkAYwBzACAAcwBpAG0AdQBsAGEAdABpAG8AbgBzACwAIABhAG4AZAAgAGUAZAB1AGMAYQB0AGkAbwBuAGEAbAAgAGEAcABwAGwAaQBjAGEAdABpAG8AbgBzAC4AXABuACAAIAAgAC0AIABPAHUAdABwAHUAdABzACAAYQByAGUAIABpAG4AdABlAHIAbgBhAGwAbAB5ACAAYwBhAGwAYwB1AGwAYQB0AGUAZAAgAGIAYQBzAGUAZAAgAG8AbgAgAGIAYQBzAGkAYwAgAHAAaAB5AHMAaQBjAGEAbAAgAHIAZQBsAGEAdABpAG8AbgBzAGgAaQBwAHMAOgBcAG4AIAAgACAAIAAgACAAIAAtACAATQAgAD0AIABtAGEAcwBzAFwAbgAgACAAIAAgACAAIAAgAC0AIABSACAAPQAgAHIAYQBkAGkAdQBzAFwAbgAgACAAIAAgACAAIAAgAC0AIABkACAAPQAgAGQAZQBuAHMAaQB0AHkAXABuACAAIAAgACAAIAAgACAALQAgAGcAIAA9ACAAcwB1AHIAZgBhAGMAZQAgAGcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgACAALQAgAHYAIAA9ACAAZQBzAGMAYQBwAGUAIAB2AGUAbABvAGMAaQB0AHkAXABuACAAIAAgAC0AIABIAGEAbgBkAGwAZQBzACAAaQBuAHAAdQB0ACAAcABlAHIAbQB1AHQAYQB0AGkAbwBuAHMAIABmAGwAZQB4AGkAYgBsAHkAIAB2AGkAYQAgAG0AbwBkAGUAIABzAHQAcgBpAG4AZwAgAHAAYQByAHMAaQBuAGcALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAOgBcAG4AIAAgACAAQQBTAFQAUgBPAF8AUABMAEEATgBFAFQAXwBNAEUAVABSAEkAQwBTAF8ARgBMAEEARwBHAEUARAAoAFwAIgByAGQAXAAiACwAIAAxAC4AMgAsACAAMAAuADcANQApAFwAbgAgACAAIAAgACAAkiFcAG4AIAAgACAAIAAgACAAIABNACAAIAAgACAAIAAgADAALgA2ADcANQBcAG4AIAAgACAAIAAgACAAIABSACAAlCcgACAAIAAgADEALgAyAFwAbgAgACAAIAAgACAAIAAgAGQAIACUJyAAIAAgACAAMAAuADcANQBcAG4AIAAgACAAIAAgACAAIABnACAAIAAgACAAIAAgADAALgA5AFwAbgAgACAAIAAgACAAIAAgAHYAIAAgACAAIAAgACAAMQAuADAAMwA5AFwAbgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFAATABBAE4ARQBUAF8ATQBFAFQAUgBJAEMAUwAgAD0AIABMAEEATQBCAEQAQQAoAG0AbwBkAGUALAAgAHAAYQByAGEAbQBfADEALAAgAHAAYQByAGEAbQBfADIALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABwAHIAZQBjAGkAcwBpAG8AbgBcAG4AIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANQAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAE4AbwByAG0AYQBsAGkAegBlACAAaQBuAHAAdQB0ACAAbQBvAGQAZQAgAHQAbwAgAGwAbwB3AGUAcgBjAGEAcwBlAFwAbgAgACAAIAAgAG0AbwBkAGUALAAgAEwATwBXAEUAUgAoAG0AbwBkAGUAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAYgBhAHMAZQBkACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAbQBvAGQAZQBcAG4AIAAgACAAIABvAHUAdABwAHUAdAAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAbQBvAGQAZQAsAFwAbgAgACAAIAAgACAAIABcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAbQBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgACgATQAgAC8AIABkACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAAoAE0AIAAqACAAZABeADIAKQAgAF4AIAAoADEALwAzACkALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgACgATQAgACoAIABTAFEAUgBUACgAZAApACkAIABeACAAKAAxAC8AMwApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAATQBhAHMAcwAgACsAIABSAGEAZABpAHUAcwBcAG4AIAAgACAAIAAgACAAXAAiAG0AcgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABNACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABNACAALwAgAFIAXgAzACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABNACAALwAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABTAFEAUgBUACgATQAgAC8AIABSACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABNAGEAcwBzACAAKwAgAEcAcgBhAHYAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAGcAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAAUwBRAFIAVAAoAE0AIAAvACAAZwApACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABTAFEAUgBUACgAZwBeADMAIAAvACAATQApACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIAAoAE0AIAAqACAAZwApACAAXgAgADAALgAyADUALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABEAGUAbgBzAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAcgBkAFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGQAIAAqACAAUgBeADMALABcAG4AIAAgACAAIAAgACAAIAAgAGcALAAgAGQAIAAqACAAUgAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAUgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAAUgBhAGQAaQB1AHMAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABnACAAKgAgAFIAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIABnACAALwAgAFIALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAFMAUQBSAFQAKABnACAAKgAgAFIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBuAHMAaQB0AHkAIAArACAARwByAGEAdgBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGQAZwBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABkACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIABnACAALwAgAGQALABcAG4AIAAgACAAIAAgACAAIAAgAE0ALAAgAGcAXgAzACAALwAgAGQAXgAyACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABnACAALwAgAFMAUQBSAFQAKABkACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABEAGUAbgBzAGkAdAB5ACAAKwAgAEUAcwBjAGEAcABlACAAVgBlAGwAbwBjAGkAdAB5AFwAbgAgACAAIAAgACAAIABcACIAZAB2AFwAIgAsACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAGQALAAgAHAAYQByAGEAbQBfADEALABcAG4AIAAgACAAIAAgACAAIAAgAHYALAAgAHAAYQByAGEAbQBfADIALABcAG4AIAAgACAAIAAgACAAIAAgAFIALAAgAHYAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAdgBeADMAIAAvACAAUwBRAFIAVAAoAGQAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgAgACoAIABTAFEAUgBUACgAZAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAE0ALAAgAFIALAAgAGQALAAgAGcALAAgAHYAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAgACAALwAvACAARwByAGEAdgBpAHQAeQAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAGcAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABnACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABSACwAIAB2AF4AMgAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIAB2AF4ANAAgAC8AIABnACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAGcAIAAvACAAdgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAE0AYQBzAHMAIAArACAARQBzAGMAYQBwAGUAIABWAGUAbABvAGMAaQB0AHkAXABuACAAIAAgACAAIAAgAFwAIgBtAHYAXAAiACwAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAATQAsACAAcABhAHIAYQBtAF8AMQAsAFwAbgAgACAAIAAgACAAIAAgACAAdgAsACAAcABhAHIAYQBtAF8AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAUgAsACAATQAgAC8AIAB2AF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAAZwAsACAAdgBeADQAIAAvACAATQAsAFwAbgAgACAAIAAgACAAIAAgACAAZAAsACAAdgBeADYAIAAvACAATQBeADIALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgATQAsACAAUgAsACAAZAAsACAAZwAsACAAdgApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgACAAIAAvAC8AIABSAGEAZABpAHUAcwAgACsAIABFAHMAYwBhAHAAZQAgAFYAZQBsAG8AYwBpAHQAeQBcAG4AIAAgACAAIAAgACAAXAAiAHIAdgBcACIALAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIABSACwAIABwAGEAcgBhAG0AXwAxACwAXABuACAAIAAgACAAIAAgACAAIAB2ACwAIABwAGEAcgBhAG0AXwAyACwAXABuACAAIAAgACAAIAAgACAAIABnACwAIAB2AF4AMgAgAC8AIABSACwAXABuACAAIAAgACAAIAAgACAAIABNACwAIABSACAAKgAgAHYAXgAyACwAXABuACAAIAAgACAAIAAgACAAIABkACwAIAAoAHYAIAAvACAAUgApAF4AMgAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABNACwAIABSACwAIABkACwAIABnACwAIAB2ACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABmAGEAbABsAGIAYQBjAGsAXABuACAAIAAgACAAIAAgAE4AQQAoACkAXABuACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABGAG8AcgBtAGEAdAAgAHcAaQB0AGgAIABoAGUAYQBkAGUAcgBzACAAYQBuAGQAIAByAG8AdQBuAGQAaQBuAGcAXABuACAAIAAgACAAaABlAGEAZABlAHIAcwAsACAAUwBXAEkAVABDAEgAKABcAG4AIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBtAGQAXAAiACwAIAB7AFwAIgBNACAAlCdcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAIACUJ1wAIgAsACAAXAAiAGcAXAAiACwAIABcACIAdgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAG0AcgBcACIALAAgAHsAXAAiAE0AIACUJ1wAIgAsACAAXAAiAFIAIACUJ1wAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABcACIAbQBnAFwAIgAsACAAewBcACIATQAgAJQnXAAiACwAIABcACIAUgBcACIALAAgAFwAIgBkAFwAIgAsACAAXAAiAGcAIACUJ1wAIgAsACAAXAAiAHYAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgByAGQAXAAiACwAIAB7AFwAIgBNAFwAIgAsACAAXAAiAFIAIACUJ1wAIgAsACAAXAAiAGQAIACUJ1wAIgAsACAAXAAiAGcAXAAiACwAIABcACIAdgBcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAHIAZwBcACIALAAgAHsAXAAiAE0AXAAiACwAIABcACIAUgAgAJQnXAAiACwAIABcACIAZABcACIALAAgAFwAIgBnACAAlCdcACIALAAgAFwAIgB2AFwAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABcACIAZABnAFwAIgAsACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAIACUJ1wAIgAsACAAXAAiAGcAIACUJ1wAIgAsACAAXAAiAHYAXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBkAHYAXAAiACwAIAB7AFwAIgBNAFwAIgAsACAAXAAiAFIAXAAiACwAIABcACIAZAAgAJQnXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2ACAAlCdcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAGcAdgBcACIALAAgAHsAXAAiAE0AXAAiACwAIABcACIAUgBcACIALAAgAFwAIgBkAFwAIgAsACAAXAAiAGcAIACUJ1wAIgAsACAAXAAiAHYAIACUJ1wAIgB9ACwAXABuACAAIAAgACAAIAAgACAAIABcACIAbQB2AFwAIgAsACAAewBcACIATQAgAJQnXAAiACwAIABcACIAUgBcACIALAAgAFwAIgBkAFwAIgAsACAAXAAiAGcAXAAiACwAIABcACIAdgAgAJQnXAAiAH0ALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgByAHYAXAAiACwAIAB7AFwAIgBNAFwAIgAsACAAXAAiAFIAIACUJ1wAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2ACAAlCdcACIAfQAsAFwAbgAgACAAIAAgACAAIAAgACAAewBcACIATQBcACIALAAgAFwAIgBSAFwAIgAsACAAXAAiAGQAXAAiACwAIABcACIAZwBcACIALAAgAFwAIgB2AFwAIgB9ACAAIAAvAC8AIABmAGEAbABsAGIAYQBjAGsAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAdgBhAGwAdQBlAHMALAAgAFIATwBVAE4ARAAoAG8AdQB0AHAAdQB0ACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIABDAEgATwBPAFMARQAoAHsAMQAsACAAMgB9ACwAIABUAFIAQQBOAFMAUABPAFMARQAoAGgAZQBhAGQAZQByAHMAKQAsACAAVABSAEEATgBTAFAATwBTAEUAKAB2AGEAbAB1AGUAcwApACkAXABuACAAIAApAFwAbgApADsAXABuAFwAbgAvAC8AIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDACAAPQAgAFwAbgAvAC8AIABMAEEATQBCAEQAQQAoAHAALAAgAHEALAAgAHAAcgBlAGMALABcAG4ALwAvACAAIAAgAEwARQBUACgAXABuAC8ALwAgACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4ALwAvACAAIAAgACAAIABJAEYAKABwACAAPQAgAHEALABcAG4ALwAvACAAIAAgACAAIAAgACAAIABOAEEAKAApACwAXABuAC8ALwAgACAAIAAgACAAIAAgACAATABFAFQAKABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACAAbgB1AG0ALAAgAHAAIAAqACAAcQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAIABkAGUAbgAsACAAQQBCAFMAKABwACAALQAgAHEAKQAsAFwAbgAvAC8AIAAgACAAIAAgACAAIAAgACAAIAByAGEAdwAsACAAbgB1AG0AIAAvACAAZABlAG4ALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACAAUgBPAFUATgBEACgAcgBhAHcALAAgAHAAcgBlAGMAKQBcAG4ALwAvACAAIAAgACAAIAAgACAAIAApAFwAbgAvAC8AIAAgACAAIAAgACkALABcAG4ALwAvACAAIAAgACAAIAByAGUAcwB1AGwAdABcAG4ALwAvACAAIAAgACkAXABuAC8ALwAgACkAOwBcAG4AXABuAC8ALwAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBTAE8ATABWAEUARAAgAD0AXABuAC8ALwAgAEwAQQBNAEIARABBACgAdgBhAGwAXwAxACwAIAB2AGEAbABfADIALAAgAFsAbQBvAGQAZQBdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAvAC8AIAAgACAATABFAFQAKABcAG4ALwAvACAAIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAsACAAXAAiAHAAcQBcACIALAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAXAAiAFwAIgAsACAAXAAiAHAAcQBcACIALAAgAG0AbwBkAGUAKQApACwAXABuAC8ALwAgACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADQALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4ALwAvACAAIAAgACAAIABwACwAIABJAEYAKABPAFIAKABtAG8AZABlAD0AXAAiAHAAcQBcACIALAAgAG0AbwBkAGUAPQBcACIAcABzAFwAIgApACwAIAB2AGEAbABfADEALAAgAE4AQQAoACkAKQAsAFwAbgAvAC8AIAAgACAAIAAgAHEALAAgAEkARgAoAG0AbwBkAGUAPQBcACIAcABxAFwAIgAsACAAdgBhAGwAXwAyACwAIABJAEYAKABtAG8AZABlAD0AXAAiAHEAcwBcACIALAAgAHYAYQBsAF8AMQAsACAATgBBACgAKQApACkALABcAG4ALwAvACAAIAAgACAAIABzACwAIABJAEYAKABPAFIAKABtAG8AZABlAD0AXAAiAHAAcwBcACIALAAgAG0AbwBkAGUAPQBcACIAcQBzAFwAIgApACwAIAB2AGEAbABfADIALAAgAE4AQQAoACkAKQAsAFwAbgBcAG4ALwAvACAAIAAgACAAIABhACwAIABJAEYAKABBAE4ARAAoAEkAUwBOAFUATQBCAEUAUgAoAHAAKQAsACAASQBTAE4AVQBNAEIARQBSACgAcQApACkALAAgAE0AQQBYACgAcAAsACAAcQApACwAIABwACkALABcAG4ALwAvACAAIAAgACAAIABiACwAIABJAEYAKABBAE4ARAAoAEkAUwBOAFUATQBCAEUAUgAoAHAAKQAsACAASQBTAE4AVQBNAEIARQBSACgAcQApACkALAAgAE0ASQBOACgAcAAsACAAcQApACwAIABxACkALABcAG4AXABuAC8ALwAgACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4ALwAvACAAIAAgACAAIAAgACAAUwBXAEkAVABDAEgAKABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAG0AbwBkAGUALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAFwAIgBwAHEAXAAiACwAIABJAEYAKABhACAAPQAgAGIALAAgAE4AQQAoACkALAAgAFIATwBVAE4ARAAoACgAYQAgACoAIABiACkAIAAvACAAKABhACAALQAgAGIAKQAsACAAcAByAGUAYwApACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAFwAIgBwAHMAXAAiACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAGEAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAHMAKQApACkALAAgAE4AQQAoACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoACgAYQAgACoAIABzACkAIAAvACAAKABhACAALQAgAHMAKQAsACAAcAByAGUAYwApACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAFwAIgBxAHMAXAAiACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAGIAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAHMAKQApACkALAAgAE4AQQAoACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoACgAYgAgACoAIABzACkAIAAvACAAKABiACAALQAgAHMAKQAsACAAcAByAGUAYwApACkALABcAG4ALwAvACAAIAAgACAAIAAgACAAIAAgAE4AQQAoACkAXABuAC8ALwAgACAAIAAgACAAIAAgACkALABcAG4ALwAvACAAIAAgACAAIAByAGUAcwB1AGwAdABcAG4ALwAvACAAIAAgACkAXABuAC8ALwAgACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBTAE8ATABWAEUAUgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABBACAAYwBvAG0AcAByAGUAaABlAG4AcwBpAHYAZQAgAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgAHMAbwBsAHYAZQByACAAdABoAGEAdAAgAGMAYQBsAGMAdQBsAGEAdABlAHMAIAB0AGgAZQAgAHQAaABpAHIAZAAgAHYAYQBsAHUAZQAgACgAUAAsACAAUQAsACAAbwByACAAUwApAFwAbgAgACAAIAB3AGgAZQBuACAAYQBuAHkAIAB0AHcAbwAgAG8AZgAgAHQAaABlACAAdABoAHIAZQBlACAAYQByAGUAIABwAHIAbwB2AGkAZABlAGQALgAgAFMAdQBwAHAAbwByAHQAcwAgAG0AdQBsAHQAaQBwAGwAZQAgAGkAbgBwAHUAdAAvAG8AdQB0AHAAdQB0ACAAbQBvAGQAZQBzACAAZgBvAHIAXABuACAAIAAgAHMAYwBpAGUAbgB0AGkAZgBpAGMAIABtAG8AZABlAGwAaQBuAGcALAAgAHAAZQBkAGEAZwBvAGcAaQBjAGEAbAAgAHUAcwBlACwAIABhAG4AZAAgAGYAbABlAHgAaQBiAGwAZQAgAHAAcgBlAHMAZQBuAHQAYQB0AGkAbwBuAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIAB2AGEAbABfADEAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABGAGkAcgBzAHQAIABpAG4AcAB1AHQAIAB2AGEAbAB1AGUALgAgAE0AZQBhAG4AaQBuAGcAIABkAGUAcABlAG4AZABzACAAbwBuACAAdABoAGUAIABzAGUAbABlAGMAdABlAGQAIABtAG8AZABlAC4AXABuACAAIAAgAC0AIAB2AGEAbABfADIAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABTAGUAYwBvAG4AZAAgAGkAbgBwAHUAdAAgAHYAYQBsAHUAZQAuACAATQBlAGEAbgBpAG4AZwAgAGQAZQBwAGUAbgBkAHMAIABvAG4AIAB0AGgAZQAgAHMAZQBsAGUAYwB0AGUAZAAgAG0AbwBkAGUALgBcAG4AIAAgACAALQAgAG0AbwBkAGUAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIAAyAC0AbABlAHQAdABlAHIAIABzAHQAcgBpAG4AZwAgAGkAbgBkAGkAYwBhAHQAaQBuAGcAIABrAG4AbwB3AG4AIABpAG4AcAB1AHQAcwAuACAAQQBjAGMAZQBwAHQAcwAgAGEAbgB5ACAAYwBhAHMAZQAgAG8AcgAgAG8AcgBkAGUAcgAuAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcABxAFwAIgAgAD0AIABzAG8AbAB2AGUAIABmAG8AcgAgAFMAIAAoAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAApAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcABzAFwAIgAgAD0AIABzAG8AbAB2AGUAIABmAG8AcgAgAFEAIAAoAG8AdQB0AGUAcgAgAHMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdAApAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcQBzAFwAIgAgAD0AIABzAG8AbAB2AGUAIABmAG8AcgAgAFAAIAAoAGkAbgBuAGUAcgAgAHMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdAApAFwAbgAgACAAIAAgACAARABlAGYAYQB1AGwAdAAgAGkAcwAgAFwAIgBwAHEAXAAiACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAGkAbgB2AGEAbABpAGQALgBcAG4AIAAgACAALQAgAGYAbwByAG0AYQB0ACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATwB1AHQAcAB1AHQAIABmAG8AcgBtAGEAdAAgACgAZABlAGYAYQB1AGwAdAAgAD0AIABcACIAYgBhAHIAZQBcACIAKQBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGIAYQByAGUAXAAiACAAIAAgACAAkiEgAHIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlACAAbwBuAGwAeQBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGwAYQBiAGUAbABlAGQAXAAiACAAkiEgAHIAZQB0AHUAcgBuAHMAIABcACIAUAAgAD0AIAAzADYANQAuADIANQBcACIALAAgAFwAIgBTACAAPQAgADcANwA5AC4AOAA4AFwAIgAsACAAZQB0AGMALgAsACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAdgBlAHIAYgBvAHMAZQBcACIAIACSISAAcgBlAHQAdQByAG4AcwAgAGkAbgBsAGkAbgBlACAAdABlAHgAdAAgAG8AZgAgAGEAbABsACAAdABoAHIAZQBlACAAdgBhAGwAdQBlAHMAIAB3AGkAdABoACAAHiYgAG8AbgAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAcgBvAHcAXAAiACAAIAAgACAAIACSISAAcgBlAHQAdQByAG4AcwAgADEAeAAzACAAYQByAHIAYQB5ACAAdwBpAHQAaAAgAFAALAAgAFEALAAgAGEAbgBkACAAUwAgAGwAYQBiAGUAbABzACAAYQBuAGQAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGMAbwBsAFwAIgAgACAAIAAgACAAkiEgAHIAZQB0AHUAcgBuAHMAIAAzAHgAMgAgAHYAZQByAHQAaQBjAGEAbAAgAGEAcgByAGEAeQA6ACAAewBcACIAUAAgAD0AXAAiACwAIAAzADYANQAuADIANQA7ACAAXAAiAFEAIAA9AFwAIgAsACAANgA4ADcAOwAgAFwAIgBTACAAHiZcACIALAAgADcANwA5AC4AOAA4AH0AXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAdABvACAAcgBvAHUAbgBkACAAcgBlAHMAdQBsAHQAcwAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAA0ACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABBACAAcwBjAGEAbABhAHIAIAB2AGEAbAB1AGUAIABvAHIAIABhACAAbABhAGIAZQBsAGUAZAAvAHMAcABpAGwAbAAgAGEAcgByAGEAeQAgAGQAZQBwAGUAbgBkAGkAbgBnACAAbwBuACAAcwBlAGwAZQBjAHQAZQBkACAAZgBvAHIAbQBhAHQALgBcAG4AIAAgACAALQAgAEkAbgAgAGEAbABsACAAYwBhAHMAZQBzACwAIAB0AGgAZQAgAGMAYQBsAGMAdQBsAGEAdABlAGQAIAAoAHMAbwBsAHYAZQBkACkAIAB2AGEAbAB1AGUAIABpAHMAIABmAGwAYQBnAGcAZQBkACAAdwBpAHQAaAAgAGEAIAByAGkAZwBoAHQAIABhAHIAcgBvAHcAIAAoAB4mKQAuAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABTAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIABmAG8AcgBtAHUAbABhADoAIABTACAAPQAgACgAUAAgACoAIABRACkAIAAvACAAfABQACAALQAgAFEAfABcAG4AIAAgACAALQAgAEkAbgB2AGUAcgBzAGUAIABzAG8AbAB1AHQAaQBvAG4AcwA6AFwAbgAgACAAIAAgACAAIAAgAC0AIABRACAAPQAgACgAUAAgACoAIABTACkAIAAvACAAfABQACAALQAgAFMAfABcAG4AIAAgACAAIAAgACAAIAAtACAAUAAgAD0AIAAoAFEAIAAqACAAUwApACAALwAgAHwAUQAgAC0AIABTAHwAXABuACAAIAAgAC0AIABJAG4AcAB1AHQAcwAgAGEAcgBlACAAYQB1AHQAbwAtAG8AcgBkAGUAcgBlAGQAIABhAHMAIABuAGUAZQBkAGUAZAAgAGYAbwByACAAcwB0AGEAYgBpAGwAaQB0AHkAIAAoAGUALgBnAC4ALAAgAFAAIAA9ACAAbQBhAHgAKAB2AGEAbAAxACwAIAB2AGEAbAAyACkAIABpAG4AIABcACIAcABxAFwAIgAgAG0AbwBkAGUAKQAuAFwAbgAgACAAIAAtACAATQBvAGQAZQAgAGkAcwAgAGMAYQBzAGUALQBpAG4AcwBlAG4AcwBpAHQAaQB2AGUAIABhAG4AZAAgAGEAdQB0AG8ALQBuAG8AcgBtAGEAbABpAHoAZQBkACAAKABlAC4AZwAuACwAIABcACIAUQBTAFwAIgAsACAAXAAiAHMAcQBcACIALAAgAGEAbgBkACAAXAAiAHMAUQBcACIAIABhAGwAbAAgAJIhIABcACIAcQBzAFwAIgApAC4AXABuACAAIAAgAC0AIABPAHUAdABwAHUAdAAgAGYAbwByAG0AYQB0AHMAIABzAHUAcABwAG8AcgB0ACAAaAB1AG0AYQBuAC0AcgBlAGEAZABhAGIAbABlACAAcgBlAHMAdQBsAHQAcwAgAGEAbgBkACAAcwB0AHIAdQBjAHQAdQByAGUAZAAgAHQAYQBiAGwAZQAgAGkAbgB0AGUAZwByAGEAdABpAG8AbgAuAFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAYQBzACAAYQAgAGcAZQBuAGUAcgBhAGwALQBwAHUAcgBwAG8AcwBlACAAZQBuAGcAaQBuAGUAIABmAG8AcgAgAHUAcwBlACAAaQBuACAAYQBzAHQAcgBvAG4AbwBtAHkAIABtAG8AZABlAGwAcwAgAGEAbgBkACAAZQBkAHUAYwBhAHQAaQBvAG4AYQBsACAAdABvAG8AbABzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlACAAMQA6AFwAbgAgACAAIAAgACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFMATwBMAFYARQBSACgAMwA2ADUALgAyADUALAAgADYAOAA3ACwAIABcACIAcABxAFwAIgAsACAAXAAiAGIAYQByAGUAXAAiACwAIAA0ACkAXABuACAAIAAgACAAIAAgACAAkiEgADcANwA5AC4AOAA4ADEAMQBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAIAAyADoAXABuACAAIAAgACAAIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUwBPAEwAVgBFAFIAKAAzADYANQAuADIANQAsACAANgA4ADcALAAgAFwAIgBwAHEAXAAiACwAIABcACIAdgBlAHIAYgBvAHMAZQBcACIAKQBcAG4AIAAgACAAIAAgACAAIACSISAAXAAiAFAAIAA9ACAAMwA2ADUALgAyADUALAAgAFEAIAA9ACAANgA4ADcALAAgAFMAIAA9ACAAHiYgADcANwA5AC4AOAA4ADEAMQBcACIAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlACAAMwA6AFwAbgAgACAAIAAgACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFMATwBMAFYARQBSACgANgA4ADcALAAgADcANwA5AC4AOAA4ADEAMQAsACAAXAAiAHEAcwBcACIALAAgAFwAIgBjAG8AbABcACIAKQBcAG4AIAAgACAAIAAgACAAIACSIVwAbgAgACAAIAAgACAAIAAgACAAIABQACAAHiYgACAAIAAgADMANgA1AC4AMgA1AFwAbgAgACAAIAAgACAAIAAgACAAIABRACAAPQAgACAAIAAgADYAOAA3AFwAbgAgACAAIAAgACAAIAAgACAAIABTACAAPQAgACAAIAAgADcANwA5AC4AOAA4ADEAMQBcAG4AXABuACAAIAAgAFIAZQBjAG8AbQBtAGUAbgBkAGEAdABpAG8AbgA6AFwAbgAgACAAIAAtACAARgBvAHIAIABnAGUAbgBlAHIAYQBsACAAdQBzAGUAcgBzACwAIABjAG8AbgBzAGkAZABlAHIAIAB1AHMAaQBuAGcAIABvAG4AZQAgAG8AZgAgAHQAaABlACAAcwBpAG0AcABsAGUAcgAgAHcAcgBhAHAAcABlAHIAIABmAHUAbgBjAHQAaQBvAG4AcwA6AFwAbgAgACAAIAAgACAAIAAgAC0AIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABRACgAUAAsACAAUQApAFwAbgAgACAAIAAgACAAIAAgAC0AIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABTACgAUAAsACAAUwApAFwAbgAgACAAIAAgACAAIAAgAC0AIABBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUQBTACgAUQAsACAAUwApAFwAbgAgACAAIAAtACAAVABoAGkAcwAgAGYAdQBuAGMAdABpAG8AbgAgAGkAcwAgAGkAbgB0AGUAbgBkAGUAZAAgAGYAbwByACAAYQBkAHYAYQBuAGMAZQBkACAAdQBzAGUAIABjAGEAcwBlAHMAIABhAG4AZAAgAFUASQAtAGkAbgB0AGUAZwByAGEAdABlAGQAIABvAHUAdABwAHUAdAAuAFwAbgBcAG4AKgAvAFwAbgBcAG4AXABuAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBTAE8ATABWAEUAUgAgAD0AXABuAEwAQQBNAEIARABBACgAdgBhAGwAXwAxACwAIAB2AGEAbABfADIALAAgAFsAbQBvAGQAZQBdACwAIABbAGYAbwByAG0AYQB0AF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEgAYQBuAGQAbABlACAAbwBwAHQAaQBvAG4AYQBsACAAYQByAGcAdQBtAGUAbgB0AHMAXABuACAAIAAgACAAcgBhAHcAXwBtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG0AbwBkAGUAKQAgACsAIAAoAG0AbwBkAGUAIAA9ACAAXAAiAFwAIgApACwAIABcACIAUABRAFwAIgAsACAAbQBvAGQAZQApACwAXABuACAAIAAgACAAbgBvAHIAbQBfAG0AbwBkAGUALAAgAFQARQBYAFQASgBPAEkATgAoAFwAIgBcACIALAAsAFMATwBSAFQAKABNAEkARAAoAEwATwBXAEUAUgAoAHIAYQB3AF8AbQBvAGQAZQApACwAUwBFAFEAVQBFAE4AQwBFACgATABFAE4AKAByAGEAdwBfAG0AbwBkAGUAKQApACwAMQApACkAKQAsAFwAbgAgACAAIAAgAG0AbwBkAGUALAAgAG4AbwByAG0AXwBtAG8AZABlACwAXABuAFwAbgAgACAAIAAgAGYAbwByAG0AYQB0ACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGYAbwByAG0AYQB0ACkAIAArACAAKABmAG8AcgBtAGEAdAAgAD0AIABcACIAXAAiACkALAAgAFwAIgBiAGEAcgBlAFwAIgAsACAATABPAFcARQBSACgAZgBvAHIAbQBhAHQAKQApACwAXABuACAAIAAgACAAcAByAGUAYwAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABwAHIAZQBjACkALAAgADQALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABJAG4AcAB1AHQAIAB1AG4AcABhAGMAawBpAG4AZwAgAGIAeQAgAG0AbwBkAGUAXABuACAAIAAgACAAUABfAGkAbgAsACAASQBGACgATwBSACgAbQBvAGQAZQA9AFwAIgBwAHEAXAAiACwAIABtAG8AZABlAD0AXAAiAHAAcwBcACIAKQAsACAAdgBhAGwAXwAxACwAIABOAEEAKAApACkALABcAG4AIAAgACAAIABRAF8AaQBuACwAIABJAEYAKABtAG8AZABlAD0AXAAiAHAAcQBcACIALAAgAHYAYQBsAF8AMgAsACAASQBGACgAbQBvAGQAZQA9AFwAIgBxAHMAXAAiACwAIAB2AGEAbABfADEALAAgAE4AQQAoACkAKQApACwAXABuACAAIAAgACAAUwBfAGkAbgAsACAASQBGACgATwBSACgAbQBvAGQAZQA9AFwAIgBwAHMAXAAiACwAIABtAG8AZABlAD0AXAAiAHEAcwBcACIAKQAsACAAdgBhAGwAXwAyACwAIABOAEEAKAApACkALABcAG4AXABuACAAIAAgACAALwAvACAAUAAgAGEAbgBkACAAUQAgAG8AcgBkAGUAcgBpAG4AZwAgAG8AbgBsAHkAIAB1AHMAZQBkACAAaQBuACAAJwBwAHEAJwAgAG0AbwBkAGUAXABuACAAIAAgACAAUAAsACAASQBGACgAQQBOAEQAKABJAFMATgBVAE0AQgBFAFIAKABQAF8AaQBuACkALAAgAEkAUwBOAFUATQBCAEUAUgAoAFEAXwBpAG4AKQApACwAIABNAEEAWAAoAFAAXwBpAG4ALAAgAFEAXwBpAG4AKQAsACAAUABfAGkAbgApACwAXABuACAAIAAgACAAUQAsACAASQBGACgAQQBOAEQAKABJAFMATgBVAE0AQgBFAFIAKABQAF8AaQBuACkALAAgAEkAUwBOAFUATQBCAEUAUgAoAFEAXwBpAG4AKQApACwAIABNAEkATgAoAFAAXwBpAG4ALAAgAFEAXwBpAG4AKQAsACAAUQBfAGkAbgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBcAG4AIAAgACAAIABTAF8AYwBhAGwAYwAsACAASQBGACgAUAAgAD0AIABRACwAIABOAEEAKAApACwAIABSAE8AVQBOAEQAKAAoAFAAIAAqACAAUQApACAALwAgACgAUAAgAC0AIABRACkALAAgAHAAcgBlAGMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEQAaQByAGUAYwB0AGkAbwBuAC0AYQB3AGEAcgBlACAAaQBuAHYAZQByAHMAZQAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBzAFwAbgAgACAAIAAgAFEAXwBjAGEAbABjACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFAAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFMAXwBpAG4AKQApACkALAAgAE4AQQAoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAoAFAAIAAqACAAUwBfAGkAbgApACAALwAgAEEAQgBTACgAUAAgAC0AIABTAF8AaQBuACkALAAgAHAAcgBlAGMAKQApACwAXABuAFwAbgAgACAAIAAgAFAAXwBjAGEAbABjACwAIABJAEYAKABPAFIAKABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFEAKQApACwAIABOAE8AVAAoAEkAUwBOAFUATQBCAEUAUgAoAFMAXwBpAG4AKQApACkALAAgAE4AQQAoACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABSAE8AVQBOAEQAKAAoAFEAIAAqACAAUwBfAGkAbgApACAALwAgAEEAQgBTACgAUQAgAC0AIABTAF8AaQBuACkALAAgAHAAcgBlAGMAKQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAZQBsAGUAYwB0AGUAZAAgAHIAZQBzAHUAbAB0ACAAdgBhAGwAdQBlAHMAXABuACAAIAAgACAAUABfAHYAYQBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBxAHMAXAAiACwAIABQAF8AYwBhAGwAYwAsACAAUAApACwAXABuACAAIAAgACAAUQBfAHYAYQBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBwAHMAXAAiACwAIABRAF8AYwBhAGwAYwAsACAAUQApACwAXABuACAAIAAgACAAUwBfAHYAYQBsACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBwAHEAXAAiACwAIABTAF8AYwBhAGwAYwAsACAAUwBfAGkAbgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAbwBsAHYAZQBkACAAbABhAGIAZQBsAFwAbgAgACAAIAAgAGwAYQBiAGUAbAAsACAAUwBXAEkAVABDAEgAKABtAG8AZABlACwAIABcACIAcABxAFwAIgAsACAAXAAiAFMAXAAiACwAIABcACIAcABzAFwAIgAsACAAXAAiAFEAXAAiACwAIABcACIAcQBzAFwAIgAsACAAXAAiAFAAXAAiACwAIABcACIAPwBcACIAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABQAHIAaQBtAGEAcgB5ACAAcwBjAGEAbABhAHIAIAByAGUAcwB1AGwAdABcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsACAAUwBXAEkAVABDAEgAKABtAG8AZABlACwAIABcACIAcABxAFwAIgAsACAAUwBfAGMAYQBsAGMALAAgAFwAIgBwAHMAXAAiACwAIABRAF8AYwBhAGwAYwAsACAAXAAiAHEAcwBcACIALAAgAFAAXwBjAGEAbABjACwAIABOAEEAKAApACkALABcAG4AXABuACAAIAAgACAALwAvACAAVgBlAHIAYgBvAHMAZQAgAHQAZQB4AHQAIABvAHUAdABwAHUAdABcAG4AIAAgACAAIAB2AGUAcgBiAG8AcwBlAF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAXAAiAFAAIAA9ACAAXAAiACAAJgAgAEkARgAoAEkAUwBOAFUATQBCAEUAUgAoAFAAXwB2AGEAbAApACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgBxAHMAXAAiACwAIABcACIAHiYgAFwAIgAgACYAIABQAF8AdgBhAGwALAAgAFAAXwB2AGEAbAApACwAIABcACIAFCBcACIAKQAgACYAIABcACIALAAgAFwAIgAgACYAXABuACAAIAAgACAAIAAgAFwAIgBRACAAPQAgAFwAIgAgACYAIABJAEYAKABJAFMATgBVAE0AQgBFAFIAKABRAF8AdgBhAGwAKQAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAcABzAFwAIgAsACAAXAAiAB4mIABcACIAIAAmACAAUQBfAHYAYQBsACwAIABRAF8AdgBhAGwAKQAsACAAXAAiABQgXAAiACkAIAAmACAAXAAiACwAIABcACIAIAAmAFwAbgAgACAAIAAgACAAIABcACIAUwAgAD0AIABcACIAIAAmACAASQBGACgASQBTAE4AVQBNAEIARQBSACgAUwBfAHYAYQBsACkALAAgAEkARgAoAG0AbwBkAGUAIAA9ACAAXAAiAHAAcQBcACIALAAgAFwAIgAeJiAAXAAiACAAJgAgAFMAXwB2AGEAbAAsACAAUwBfAHYAYQBsACkALAAgAFwAIgAUIFwAIgApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAcABpAGwAbABhAGIAbABlACAAdABhAGIAdQBsAGEAcgAgAG8AdQB0AHAAdQB0AHMAXABuACAAIAAgACAAcgBvAHcAXwBvAHUAdAAsAFwAbgAgACAAIAAgACAAIABWAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIABJAEYAKABtAG8AZABlAD0AXAAiAHEAcwBcACIALAAgAFwAIgBQACAAHiZcACIALAAgAFwAIgBQACAAPQBcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAG0AbwBkAGUAPQBcACIAcABzAFwAIgAsACAAXAAiAFEAIAAeJlwAIgAsACAAXAAiAFEAIAA9AFwAIgApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAASQBGACgAbQBvAGQAZQA9AFwAIgBwAHEAXAAiACwAIABcACIAUwAgAB4mXAAiACwAIABcACIAUwAgAD0AXAAiACkAXABuACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFAAXwB2AGEAbAAsACAAUQBfAHYAYQBsACwAIABTAF8AdgBhAGwAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIABjAG8AbABfAG8AdQB0ACwAXABuACAAIAAgACAAIAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAEkARgAoAG0AbwBkAGUAPQBcACIAcQBzAFwAIgAsACAAXAAiAFAAIAAeJlwAIgAsACAAXAAiAFAAIAA9AFwAIgApACwAIABQAF8AdgBhAGwAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABJAEYAKABtAG8AZABlAD0AXAAiAHAAcwBcACIALAAgAFwAIgBRACAAHiZcACIALAAgAFwAIgBRACAAPQBcACIAKQAsACAAUQBfAHYAYQBsACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgASQBGACgAbQBvAGQAZQA9AFwAIgBwAHEAXAAiACwAIABcACIAUwAgAB4mXAAiACwAIABcACIAUwAgAD0AXAAiACkALAAgAFMAXwB2AGEAbAApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEYAaQBuAGEAbAAgAHMAdwBpAHQAYwBoACAAZgBvAHIAIAByAGUAdAB1AHIAbgAgAHQAeQBwAGUAXABuACAAIAAgACAAbwB1AHQAcAB1AHQALABcAG4AIAAgACAAIAAgACAAUwBXAEkAVABDAEgAKABmAG8AcgBtAGEAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAGIAYQByAGUAXAAiACwAIAByAGUAcwB1AGwAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAGwAYQBiAGUAbABlAGQAXAAiACwAIABsAGEAYgBlAGwAIAAmACAAXAAiACAAPQAgAFwAIgAgACYAIAByAGUAcwB1AGwAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAHYAZQByAGIAbwBzAGUAXAAiACwAIAB2AGUAcgBiAG8AcwBlAF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgByAG8AdwBcACIALAAgAHIAbwB3AF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBjAG8AbABcACIALAAgAGMAbwBsAF8AbwB1AHQALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBJAG4AdgBhAGwAaQBkACAAZgBvAHIAbQBhAHQAXAAiAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFAAUQBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAGEAbABjAHUAbABhAHQAZQBzACAAdABoAGUAIABzAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIAAoAFMAKQAgAGIAZQB0AHcAZQBlAG4AIAB0AHcAbwAgAHAAbABhAG4AZQB0AGEAcgB5ACAAYgBvAGQAaQBlAHMAXABuACAAIAAgAGIAYQBzAGUAZAAgAG8AbgAgAHQAaABlAGkAcgAgAHMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZABzACAAUAAgAGEAbgBkACAAUQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAUAAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZAAgAG8AZgAgAHQAaABlACAAaQBuAG4AZQByACAAKABmAGEAcwB0AGUAcgApACAAYgBvAGQAeQBcAG4AIAAgACAALQAgAFEAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABTAGkAZABlAHIAZQBhAGwAIABvAHIAYgBpAHQAYQBsACAAcABlAHIAaQBvAGQAIABvAGYAIAB0AGgAZQAgAG8AdQB0AGUAcgAgACgAcwBsAG8AdwBlAHIAKQAgAGIAbwBkAHkAXABuACAAIAAgAC0AIABvAHUAdABwAHUAdAAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AdQB0AHAAdQB0ACAAZgBvAHIAbQBhAHQALgAgAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAYgBhAHIAZQBcACIAIAA9ACAAUgBlAHQAdQByAG4AcwAgAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgAG8AbgBsAHkAIAAoAGQAZQBmAGEAdQBsAHQAKQBcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAHYAZQByAGIAbwBzAGUAXAAiACAAPQAgAFIAZQB0AHUAcgBuAHMAIABhACAAMgAtAGMAbwBsAHUAbQBuACAAdgBlAHIAdABpAGMAYQBsACAAdABhAGIAbABlADoAIABQACwAIABRACwAIABTACwAIAB3AGkAdABoACAAdABoAGUAIAByAGUAcwB1AGwAdAAgAGYAbABhAGcAZwBlAGQAIAAoAB4mKQBcAG4AIAAgACAALQAgAHAAcgBlAGMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABEAGUAYwBpAG0AYQBsACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAANAApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAUwB5AG4AbwBkAGkAYwAgAHAAZQByAGkAbwBkACAAKABiAGEAcgBlACkALAAgAG8AcgBcAG4AIAAgACAALQAgAFYAZQByAGIAbwBzAGUAIAAyAC0AYwBvAGwAdQBtAG4AIABhAHIAcgBhAHkAIAB3AGkAdABoACAAbABhAGIAZQBsAGUAZAAgAFAALAAgAFEALAAgAGEAbgBkACAAUwAgAHYAYQBsAHUAZQBzAFwAbgAgACAAIAAgACAAKABTACAAaQBzACAAZgBsAGEAZwBnAGUAZAAgAHcAaQB0AGgAIABhACAAHiYgAHQAbwAgAGkAbgBkAGkAYwBhAHQAZQAgAGkAdAAnAHMAIAB0AGgAZQAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlACkAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFMAIAA9ACAAKABQACAA1wAgAFEAKQAgAC8AIAB8AFAAIAASIiAAUQB8ACwAIABhAHMAcwB1AG0AaQBuAGcAIABQACAAYCIgAFEAXABuACAAIAAgAC0AIABJAG4AcAB1AHQAcwAgAG0AYQB5ACAAYgBlACAAcAByAG8AdgBpAGQAZQBkACAAaQBuACAAYQBuAHkAIABvAHIAZABlAHIAOwAgAHQAaABlACAAZgB1AG4AYwB0AGkAbwBuACAAaQBuAHQAZQByAG4AYQBsAGwAeQAgAGEAcwBzAGkAZwBuAHMAIABQAC8AUQAgAGYAbwByACAAYwBvAHIAcgBlAGMAdAAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBcAG4AIAAgACAALQAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABwAHIAZQBkAGkAYwB0AGkAbgBnACAAYwBvAG4AagB1AG4AYwB0AGkAbwBuACAAaQBuAHQAZQByAHYAYQBsAHMAIABvAHIAIABvAHIAYgBpAHQAYQBsACAAcgBlAHMAbwBuAGEAbgBjAGUAIABtAG8AZABlAGwAaQBuAGcAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBQAFEAKAAzADYANQAuADIANQAsACAANgA4ADcALAAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAsACAANAApAFwAbgAgACAAIAAgACAAkiFcAG4AIAAgACAAIAAgACAAIABQACAAPQAgACAAIAAgACAAIAAzADYANQAuADIANQBcAG4AIAAgACAAIAAgACAAIABRACAAPQAgACAAIAAgACAAIAA2ADgANwBcAG4AIAAgACAAIAAgACAAIABTACAAHiYgAD0AIAAgACAAIAA3ADcAOQAuADgAOAAxADEAXABuACoALwBcAG4AXABuAFwAbgBBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABRACAAPQBcAG4ATABBAE0AQgBEAEEAKABQACwAIABRACwAIABbAG8AdQB0AHAAdQB0AF0ALAAgAFsAcAByAGUAYwBdACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEgAYQBuAGQAbABlACAAbwBwAHQAaQBvAG4AYQBsACAAYQByAGcAdQBtAGUAbgB0AHMAXABuACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABvAHUAdABwAHUAdAApACAAKwAgACgAbwB1AHQAcAB1AHQAIAA9ACAAXAAiAFwAIgApACwAIABcACIAYgBhAHIAZQBcACIALAAgAEwATwBXAEUAUgAoAG8AdQB0AHAAdQB0ACkAKQAsAFwAbgAgACAAIAAgAGQAaQBnAGkAdABzACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANAAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFMAbwByAHQAIABmAG8AcgAgAHMAdABhAGIAaQBsAGkAdAB5ACAAaQBuACAAcwB5AG4AbwBkAGkAYwAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgBcAG4AIAAgACAAIABBACwAIABNAEEAWAAoAFAALAAgAFEAKQAsAFwAbgAgACAAIAAgAEIALAAgAE0ASQBOACgAUAAsACAAUQApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEMAYQBsAGMAdQBsAGEAdABlACAAcwB5AG4AbwBkAGkAYwAgAHAAZQByAGkAbwBkAFwAbgAgACAAIAAgAFMALAAgAFIATwBVAE4ARAAoACgAQQAgACoAIABCACkAIAAvACAAKABBACAALQAgAEIAKQAsACAAZABpAGcAaQB0AHMAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABUAHcAbwAtAGMAbwBsAHUAbQBuACAAdgBlAHIAYgBvAHMAZQAgAG8AdQB0AHAAdQB0ACAAKABsAGEAYgBlAGwAcwAgAHAAcgBlAHMAZQByAHYAZQBkACkAXABuACAAIAAgACAAdgBlAHIAYgBvAHMAZQAsAFwAbgAgACAAIAAgACAAIABWAFMAVABBAEMASwAoAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcACIAUAAgAD0AXAAiACwAIABQACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAFEAIAA9AFwAIgAsACAAUQApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAIgBTACAAHiZcACIALAAgAFMAKQBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABPAHUAdABwAHUAdAAgAHMAZQBsAGUAYwB0AGkAbwBuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAsACAAdgBlAHIAYgBvAHMAZQAsACAAUwApACwAXABuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0AFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFAAUwBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAGEAbABjAHUAbABhAHQAZQBzACAAdABoAGUAIABzAGkAZABlAHIAZQBhAGwAIABvAHIAYgBpAHQAYQBsACAAcABlAHIAaQBvAGQAIABRACAAbwBmACAAdABoAGUAIABvAHUAdABlAHIAIABiAG8AZAB5AFwAbgAgACAAIABiAGEAcwBlAGQAIABvAG4AIAB0AGgAZQAgAHMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgACgAUwApACAAYQBuAGQAIAB0AGgAZQAgAGsAbgBvAHcAbgAgAGkAbgBuAGUAcgAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZAAgACgAUAApAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABQACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAUwBpAGQAZQByAGUAYQBsACAAbwByAGIAaQB0AGEAbAAgAHAAZQByAGkAbwBkACAAbwBmACAAdABoAGUAIABpAG4AbgBlAHIAIAAoAGYAYQBzAHQAZQByACkAIABiAG8AZAB5AFwAbgAgACAAIAAtACAAUwAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAeQBuAG8AZABpAGMAIABwAGUAcgBpAG8AZAAgACgAbwBiAHMAZQByAHYAZQBkACAAaQBuAHQAZQByAHYAYQBsACAAYgBlAHQAdwBlAGUAbgAgAGMAbwBuAGoAdQBuAGMAdABpAG8AbgBzACkAXABuACAAIAAgAC0AIABvAHUAdABwAHUAdAAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AdQB0AHAAdQB0ACAAZgBvAHIAbQBhAHQALgAgAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAYgBhAHIAZQBcACIAIAA9ACAAUgBlAHQAdQByAG4AcwAgAFEAIABvAG4AbAB5ACAAKABkAGUAZgBhAHUAbAB0ACkAXABuACAAIAAgACAAIAAgACAALQAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAgAD0AIABSAGUAdAB1AHIAbgBzACAAYQAgADIALQBjAG8AbAB1AG0AbgAgAHYAZQByAHQAaQBjAGEAbAAgAHQAYQBiAGwAZQA6ACAAUAAsACAAUQAsACAAUwAsACAAdwBpAHQAaAAgAFEAIABmAGwAYQBnAGcAZQBkACAAKAAeJikAXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAARABlAGMAaQBtAGEAbAAgAHAAcgBlAGMAaQBzAGkAbwBuACAAKABkAGUAZgBhAHUAbAB0ACAAPQAgADQAKQBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAALQAgAFMAaQBkAGUAcgBlAGEAbAAgAHAAZQByAGkAbwBkACAAUQAgACgAYgBhAHIAZQApACwAIABvAHIAXABuACAAIAAgAC0AIABWAGUAcgBiAG8AcwBlACAAMgAtAGMAbwBsAHUAbQBuACAAYQByAHIAYQB5ACAAdwBpAHQAaAAgAGwAYQBiAGUAbABlAGQAIABQACwAIABRACwAIABhAG4AZAAgAFMAIAB2AGEAbAB1AGUAcwBcAG4AIAAgACAAIAAgACgAUQAgAGkAcwAgAGYAbABhAGcAZwBlAGQAIAB3AGkAdABoACAAHiYgAHQAbwAgAGkAbgBkAGkAYwBhAHQAZQAgAGkAdAAnAHMAIAB0AGgAZQAgAHMAbwBsAHYAZQBkACAAdgBhAGwAdQBlACkAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFEAIAA9ACAAKABQACAA1wAgAFMAKQAgAC8AIAAoAFAAIAASIiAAUwApAFwAbgAgACAAIAAtACAAQQBzAHMAdQBtAGUAcwAgAFMAIAA8ACAAUAAgACgAcwB5AG4AbwBkAGkAYwAgAHAAZQByAGkAbwBkACAAbQB1AHMAdAAgAGIAZQAgAHMAaABvAHIAdABlAHIAIAB0AGgAYQBuACAAcwBsAG8AdwBlAHIAIABiAG8AZAB5ACcAcwAgAG8AcgBiAGkAdAApAFwAbgAgACAAIAAtACAARABlAHMAaQBnAG4AZQBkACAAZgBvAHIAIABzAHkAcwB0AGUAbQBzACAAdwBoAGUAcgBlACAAcwB5AG4AbwBkAGkAYwAgAGkAbgB0AGUAcgB2AGEAbABzACAAYQByAGUAIABtAGUAYQBzAHUAcgBlAGQAIABhAG4AZAAgAGkAbgBuAGUAcgAgAGIAbwBkAHkAIABpAHMAIABrAG4AbwB3AG4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBQAFMAKAAzADYANQAuADIANQAsACAANwA3ADkALgA4ADgAMQAxACwAIABcACIAdgBlAHIAYgBvAHMAZQBcACIALAAgADQAKQBcAG4AIAAgACAAIAAgAJIhXABuACAAIAAgACAAIAAgACAAUAAgAD0AIAAgACAAIAAgACAAMwA2ADUALgAyADUAXABuACAAIAAgACAAIAAgACAAUQAgAB4mIAA9ACAAIAAgACAANgA4ADcAXABuACAAIAAgACAAIAAgACAAUwAgAD0AIAAgACAAIAAgACAANwA3ADkALgA4ADgAMQAxAFwAbgAqAC8AXABuAFwAbgBcAG4AQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFAAUwAgAD0AXABuAEwAQQBNAEIARABBACgAUAAsACAAUwAsACAAWwBvAHUAdABwAHUAdABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIAAvAC8AIABPAHAAdABpAG8AbgBhAGwAIABhAHIAZwB1AG0AZQBuAHQAIABoAGEAbgBkAGwAaQBuAGcAXABuACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABvAHUAdABwAHUAdAApACAAKwAgACgAbwB1AHQAcAB1AHQAIAA9ACAAXAAiAFwAIgApACwAIABcACIAYgBhAHIAZQBcACIALAAgAEwATwBXAEUAUgAoAG8AdQB0AHAAdQB0ACkAKQAsAFwAbgAgACAAIAAgAGQAaQBnAGkAdABzACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAsACAANAAsACAAcAByAGUAYwApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAEMAbwBtAHAAdQB0AGUAIABRACAAKABvAHUAdABlAHIAIABvAHIAYgBpAHQAKQBcAG4AIAAgACAAIABRACwAIABSAE8AVQBOAEQAKAAoAFAAIAAqACAAUwApACAALwAgAEEAQgBTACgAUAAgAC0AIABTACkALAAgAGQAaQBnAGkAdABzACkALABcAG4AXABuACAAIAAgACAALwAvACAAVgBlAHIAYgBvAHMAZQAgAHMAcABpAGwAbAAgAG8AdQB0AHAAdQB0AFwAbgAgACAAIAAgAHYAZQByAGIAbwBzAGUALABcAG4AIAAgACAAIAAgACAAVgBTAFQAQQBDAEsAKABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAFAAIAA9AFwAIgAsACAAUAApACwAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAIgBRACAAHiZcACIALAAgAFEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcACIAUwAgAD0AXAAiACwAIABTACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAALwAvACAATwB1AHQAcAB1AHQAIABjAGgAbwBpAGMAZQBcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsACAASQBGACgAbQBvAGQAZQAgAD0AIABcACIAdgBlAHIAYgBvAHMAZQBcACIALAAgAHYAZQByAGIAbwBzAGUALAAgAFEAKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdABcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBRAFMAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBhAGwAYwB1AGwAYQB0AGUAcwAgAHQAaABlACAAcwBpAGQAZQByAGUAYQBsACAAbwByAGIAaQB0AGEAbAAgAHAAZQByAGkAbwBkACAAUAAgAG8AZgAgAHQAaABlACAAaQBuAG4AZQByACAAKABmAGEAcwB0AGUAcgApACAAYgBvAGQAeQBcAG4AIAAgACAAYgBhAHMAZQBkACAAbwBuACAAdABoAGUAIABzAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIAAoAFMAKQAgAGEAbgBkACAAdABoAGUAIABrAG4AbwB3AG4AIABvAHUAdABlAHIAIABvAHIAYgBpAHQAYQBsACAAcABlAHIAaQBvAGQAIAAoAFEAKQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAUQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFMAaQBkAGUAcgBlAGEAbAAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZAAgAG8AZgAgAHQAaABlACAAbwB1AHQAZQByACAAKABzAGwAbwB3AGUAcgApACAAYgBvAGQAeQBcAG4AIAAgACAALQAgAFMAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABTAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIAAoAG8AYgBzAGUAcgB2AGUAZAAgAGkAbgB0AGUAcgB2AGEAbAAgAGIAZQB0AHcAZQBlAG4AIABjAG8AbgBqAHUAbgBjAHQAaQBvAG4AcwApAFwAbgAgACAAIAAtACAAbwB1AHQAcAB1AHQAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABPAHUAdABwAHUAdAAgAGYAbwByAG0AYQB0AC4AIABcAG4AIAAgACAAIAAgACAAIAAtACAAXAAiAGIAYQByAGUAXAAiACAAPQAgAFIAZQB0AHUAcgBuAHMAIABQACAAbwBuAGwAeQAgACgAZABlAGYAYQB1AGwAdAApAFwAbgAgACAAIAAgACAAIAAgAC0AIABcACIAdgBlAHIAYgBvAHMAZQBcACIAIAA9ACAAUgBlAHQAdQByAG4AcwAgAGEAIAAyAC0AYwBvAGwAdQBtAG4AIAB2AGUAcgB0AGkAYwBhAGwAIAB0AGEAYgBsAGUAOgAgAFAALAAgAFEALAAgAFMALAAgAHcAaQB0AGgAIABQACAAZgBsAGEAZwBnAGUAZAAgACgAHiYpAFwAbgAgACAAIAAtACAAcAByAGUAYwAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAEQAZQBjAGkAbQBhAGwAIABwAHIAZQBjAGkAcwBpAG8AbgAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAA0ACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABTAGkAZABlAHIAZQBhAGwAIABwAGUAcgBpAG8AZAAgAFAAIAAoAGIAYQByAGUAKQAsACAAbwByAFwAbgAgACAAIAAtACAAVgBlAHIAYgBvAHMAZQAgADIALQBjAG8AbAB1AG0AbgAgAGEAcgByAGEAeQAgAHcAaQB0AGgAIABsAGEAYgBlAGwAZQBkACAAUAAsACAAUQAsACAAYQBuAGQAIABTACAAdgBhAGwAdQBlAHMAXABuACAAIAAgACAAIAAoAFAAIABpAHMAIABmAGwAYQBnAGcAZQBkACAAdwBpAHQAaAAgAB4mIAB0AG8AIABpAG4AZABpAGMAYQB0AGUAIABpAHQAJwBzACAAdABoAGUAIABzAG8AbAB2AGUAZAAgAHYAYQBsAHUAZQApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABQACAAPQAgACgAUQAgANcAIABTACkAIAAvACAAKABRACAAKwAgAFMAKQBcAG4AIAAgACAALQAgAFUAcwBlAGQAIAB3AGgAZQBuACAAdABoAGUAIABzAHkAbgBvAGQAaQBjACAAcABlAHIAaQBvAGQAIABhAG4AZAAgAHMAbABvAHcAZQByACAAbwByAGIAaQB0ACAAYQByAGUAIABrAG4AbwB3AG4AIAAoAGUALgBnAC4ALAAgAG8AYgBzAGUAcgB2AGEAdABpAG8AbgBhAGwAIABhAHMAdAByAG8AbgBvAG0AeQApAFwAbgAgACAAIAAtACAATwB1AHQAcAB1AHQAIABsAGEAeQBvAHUAdAAgAGkAcwAgAGMAbwBuAHMAaQBzAHQAZQBuAHQAIABhAGMAcgBvAHMAcwAgAGEAbABsACAAcwB5AG4AbwBkAGkAYwAgAHMAbwBsAHYAZQByACAAZgB1AG4AYwB0AGkAbwBuAHMAXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlADoAXABuACAAIAAgAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBRAFMAKAA2ADgANwAsACAANwA3ADkALgA4ADgAMQAxACwAIABcACIAdgBlAHIAYgBvAHMAZQBcACIALAAgADQAKQBcAG4AIAAgACAAIAAgAJIhXABuACAAIAAgACAAIAAgACAAUAAgAB4mIAA9ACAAIAAgACAAMwA2ADUALgAyADUAXABuACAAIAAgACAAIAAgACAAUQAgAD0AIAAgACAAIAAgACAANgA4ADcAXABuACAAIAAgACAAIAAgACAAUwAgAD0AIAAgACAAIAAgACAANwA3ADkALgA4ADgAMQAxAFwAbgAqAC8AXABuAFwAbgBcAG4AQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFEAUwAgAD0AXABuAEwAQQBNAEIARABBACgAUQAsACAAUwAsACAAWwBvAHUAdABwAHUAdABdACwAIABbAHAAcgBlAGMAXQAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAG8AZABlACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAG8AdQB0AHAAdQB0ACkAIAArACAAKABvAHUAdABwAHUAdAAgAD0AIABcACIAXAAiACkALAAgAFwAIgBiAGEAcgBlAFwAIgAsACAATABPAFcARQBSACgAbwB1AHQAcAB1AHQAKQApACwAXABuACAAIAAgACAAZABpAGcAaQB0AHMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAA0ACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAAQwBvAHIAcgBlAGMAdAAgAGYAbwByAG0AdQBsAGEAOgAgAFAAIAA9ACAAKABRACAAKgAgAFMAKQAgAC8AIAAoAFEAIAArACAAUwApAFwAbgAgACAAIAAgAFAALAAgAFIATwBVAE4ARAAoACgAUQAgACoAIABTACkAIAAvACAAKABRACAAKwAgAFMAKQAsACAAZABpAGcAaQB0AHMAKQAsAFwAbgBcAG4AIAAgACAAIAB2AGUAcgBiAG8AcwBlACwAXABuACAAIAAgACAAIAAgAFYAUwBUAEEAQwBLACgAXABuACAAIAAgACAAIAAgACAAIABIAFMAVABBAEMASwAoAFwAIgBQACAAHiZcACIALAAgAFAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAASABTAFQAQQBDAEsAKABcACIAUQAgAD0AXAAiACwAIABRACkALABcAG4AIAAgACAAIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAXAAiAFMAIAA9AFwAIgAsACAAUwApAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0ACwAIABJAEYAKABtAG8AZABlACAAPQAgAFwAIgB2AGUAcgBiAG8AcwBlAFwAIgAsACAAdgBlAHIAYgBvAHMAZQAsACAAUAApACwAXABuACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAApAFwAbgApADsAXABuAFwAbgAvACoAIABBAFMAVABSAE8AXwBBAFAAUABBAFIARQBOAFQAXwBTAE8ATABBAFIAXwBTAEkAWgBFAFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAEMAYQBsAGMAdQBsAGEAdABlAHMAIAB0AGgAZQAgAGEAcABwAGEAcgBlAG4AdAAgAGEAbgBnAHUAbABhAHIAIABkAGkAYQBtAGUAdABlAHIAIABvAGYAIABhACAAcwB0AGEAcgAgACgAbwByACAAbwB0AGgAZQByACAAbwBiAGoAZQBjAHQAKQAgAGEAcwAgAHMAZQBlAG4AIABmAHIAbwBtACAAYQAgAHMAcABlAGMAaQBmAGkAZQBkACAAZABpAHMAdABhAG4AYwBlACwAXABuACAAIAAgAGUAeABwAHIAZQBzAHMAZQBkACAAYQBzACAAYQAgAG0AdQBsAHQAaQBwAGwAZQAgAG8AZgAgAHQAaABlACAAUwB1AG4AGSBzACAAYQBwAHAAYQByAGUAbgB0ACAAcwBpAHoAZQAgAGYAcgBvAG0AIABFAGEAcgB0AGgALgBcAG4AXABuACAAIAAgAEkAbgBwAHUAdABzADoAXABuACAAIAAgAC0AIAByAGEAZABpAHUAcwAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAFIAYQBkAGkAdQBzACAAbwBmACAAdABoAGUAIABvAGIAagBlAGMAdAAsACAAaQBuACAAcwBvAGwAYQByACAAcgBhAGQAaQBpACAAKABSAAkmKQBcAG4AIAAgACAALQAgAGQAaQBzAHQAYQBuAGMAZQAgACgAcgBlAHEAdQBpAHIAZQBkACkAOgAgAEQAaQBzAHQAYQBuAGMAZQAgAHQAbwAgAHQAaABlACAAbwBiAGoAZQBjAHQALAAgAGkAbgAgAGEAcwB0AHIAbwBuAG8AbQBpAGMAYQBsACAAdQBuAGkAdABzACAAKABBAFUAKQBcAG4AIAAgACAALQAgAGYAbwByAG0AYQB0ACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATwB1AHQAcAB1AHQAIABtAG8AZABlAC4AXABuACAAIAAgACAAIAAgACAAXAAiAHIAYQB3AFwAIgAgACAAIAAgACAAIAAgAJIhIAByAGUAdAB1AHIAbgBzACAAbgB1AG0AZQByAGkAYwAgAHMAYwBhAGwAYQByACAAKABlAC4AZwAuACwAIAAxAC4ANQA0ADUAKQBcAG4AIAAgACAAIAAgACAAIABcACIAZgBvAHIAbQBhAHQAdABlAGQAXAAiACAAkiEgAHIAZQB0AHUAcgBuAHMAIABzAHQAcgBpAG4AZwAgAGYAbwByAG0AYQB0AHQAZQBkACAAYQBzACAAKABlAC4AZwAuACwAIABcACIAMQAuADUANAA1AAkmXAAiACkAXABuACAAIAAgACAAIAAgACAARABlAGYAYQB1AGwAdAAgACAAIAAgACAAkiEgAFwAIgBmAG8AcgBtAGEAdAB0AGUAZABcACIAXABuACAAIAAgAC0AIABwAHIAZQBjACAAKABvAHAAdABpAG8AbgBhAGwAKQA6ACAATgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAG8AdQBuAGQAIAB0AG8AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAANAApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAQQBwAHAAYQByAGUAbgB0ACAAYQBuAGcAdQBsAGEAcgAgAHMAaQB6AGUAIABvAGYAIAB0AGgAZQAgAG8AYgBqAGUAYwB0ACAAYQBzACAAYQAgAG0AdQBsAHQAaQBwAGwAZQAgAG8AZgAgAHQAaABlACAAUwB1AG4AGSBzAC4AXABuACAAIAAgACAAIAAxAC4AMAAgAG0AZQBhAG4AcwAgAHQAaABlACAAbwBiAGoAZQBjAHQAIABhAHAAcABlAGEAcgBzACAAZQB4AGEAYwB0AGwAeQAgAHQAaABlACAAcwBhAG0AZQAgAHMAaQB6AGUAIABhAHMAIAB0AGgAZQAgAFMAdQBuACAAaQBuACAARQBhAHIAdABoACcAcwAgAHMAawB5AC4AXABuACAAIAAgACAAIAA+ADEALgAwACAAbQBlAGEAbgBzACAAbABhAHIAZwBlAHIAOwAgADwAMQAuADAAIABtAGUAYQBuAHMAIABzAG0AYQBsAGwAZQByAC4AXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAEEAcwBzAHUAbQBlAHMAIAB0AGgAYQB0ACAAaQBuAHAAdQB0AHMAIABhAHIAZQAgAGkAbgAgAHMAbwBsAGEAcgAgAHIAYQBkAGkAaQAgAGEAbgBkACAAQQBVACwAIAB3AGgAaQBjAGgAIABjAGEAbgBjAGUAbAAgAG4AYQB0AHUAcgBhAGwAbAB5ACAAdABvACAAYQAgAHUAbgBpAHQAbABlAHMAcwAgAHIAYQB0AGkAbwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAHcAbwByAGwAZABiAHUAaQBsAGQAaQBuAGcALAAgAHYAaQBzAHUAYQBsACAAcwB0AG8AcgB5AHQAZQBsAGwAaQBuAGcALAAgAGEAbgBkACAAYwBvAG0AcABhAHIAYQB0AGkAdgBlACAAYQBzAHQAcgBvAG4AbwBtAHkALgBcAG4AIAAgACAALQAgAE0AYQB5ACAAYgBlACAAZQB4AHAAYQBuAGQAZQBkACAAaQBuACAAZgB1AHQAdQByAGUAIAB0AG8AIABzAHUAcABwAG8AcgB0ACAAdAByAHUAZQAgAGEAbgBnAHUAbABhAHIAIAB1AG4AaQB0AHMAIAAoAGEAcgBjAG0AaQBuACwAIABkAGUAZwByAGUAZQBzACwAIABlAHQAYwAuACkAXABuACoALwBcAG4AXABuAEEAUwBUAFIATwBfAEEAUABQAEEAUgBFAE4AVABfAFMATwBMAEEAUgBfAFMASQBaAEUAIAA9AFwAbgBMAEEATQBCAEQAQQAoAHIAYQBkAGkAdQBzACwAIABkAGkAcwB0AGEAbgBjAGUALAAgAFsAZgBvAHIAbQBhAHQAXQAsACAAWwBwAHIAZQBjAF0ALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAALwAvACAAUwBlAHQAIABkAGUAZgBhAHUAbAB0ACAAcAByAGUAYwBpAHMAaQBvAG4AIABpAGYAIABvAG0AaQB0AHQAZQBkAFwAbgAgACAAIAAgAHAALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACwAIAA0ACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAAQwBvAHIAZQAgAGMAYQBsAGMAdQBsAGEAdABpAG8AbgA6ACAAcgBhAHQAaQBvACAAbwBmACAAcgBhAGQAaQB1AHMAIAB0AG8AIABkAGkAcwB0AGEAbgBjAGUAXABuACAAIAAgACAAcgBhAHcALAAgAHIAYQBkAGkAdQBzACAALwAgAGQAaQBzAHQAYQBuAGMAZQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABDAG8AbgBkAGkAdABpAG8AbgBhAGwAIABvAHUAdABwAHUAdAAgAGYAbwByAG0AYQB0AHQAaQBuAGcAXABuACAAIAAgACAAcgBlAHMAdQBsAHQALABcAG4AIAAgACAAIAAgACAASQBGACgAXABuACAAIAAgACAAIAAgACAAIABPAFIAKABJAFMATwBNAEkAVABUAEUARAAoAGYAbwByAG0AYQB0ACkALAAgAGYAbwByAG0AYQB0ACAAPQAgAFwAIgBmAG8AcgBtAGEAdAB0AGUAZABcACIAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVABFAFgAVAAoAHIAYQB3ACwAIABcACIAMAAuAFwAIgAgACYAIABSAEUAUABUACgAXAAiADAAXAAiACwAIABwACkAKQAgACYAIABcACIACSZcACIALAAgACAALwAvACAAZQAuAGcALgAsACAAXAAiADEALgA1ADQANQAwAAkmXAAiAFwAbgAgACAAIAAgACAAIAAgACAAcgBhAHcAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIAByAGUAdAB1AHIAbgAgAHMAYwBhAGwAYQByAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0AFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAE8AUgBCAEkAVABfAEMATwBOAEYASQBHAFUAUgBBAFQASQBPAE4AXwBJAE4ARABFAFgAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBvAG0AcAB1AHQAZQBzACAAYQAgAGQAaQBtAGUAbgBzAGkAbwBuAGwAZQBzAHMAIABpAG4AZABlAHgAIAB0AGgAYQB0ACAAYwBoAGEAcgBhAGMAdABlAHIAaQB6AGUAcwAgAHQAaABlACAAYwBvAG4AZgBpAGcAdQByAGEAdABpAG8AbgBcAG4AIAAgACAAbwBmACAAYQAgAHQAdwBvAC0AYgBvAGQAeQAgAG8AcgBiAGkAdABhAGwAIABzAHkAcwB0AGUAbQAgAGIAYQBzAGUAZAAgAG8AbgAgAG0AYQBzAHMAIABhAHMAeQBtAG0AZQB0AHIAeQAuACAAVABoAGkAcwAgAGkAbgBkAGUAeABcAG4AIAAgACAAcAByAGUAZABpAGMAdABzACAAdwBoAGUAdABoAGUAcgAgAG8AcgBiAGkAdABzACAAdwBpAGwAbAAgAGIAZQAgAG4AZQBzAHQAZQBkACwAIAB0AGEAbgBnAGUAbgB0AGkAYQBsACwAIABvAHIAIABjAHIAbwBzAHMAaQBuAGcALgBcAG4AXABuACAAIAAgAEkAbgBwAHUAdABzADoAXABuACAAIAAgAC0AIABtAGEAcwBzADEAOgAgAEYAaQByAHMAdAAgAGIAbwBkAHkAIABtAGEAcwBzACAAKABzAG8AbABhAHIAIABtAGEAcwBzAGUAcwApAFwAbgAgACAAIAAtACAAbQBhAHMAcwAyADoAIABTAGUAYwBvAG4AZAAgAGIAbwBkAHkAIABtAGEAcwBzACAAKABzAG8AbABhAHIAIABtAGEAcwBzAGUAcwApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAQwBvAG4AZgBpAGcAdQByAGEAdABpAG8AbgAgAGkAbgBkAGUAeAAgAKQAcAAgAD0AIAB8AG0AMQAgABIiIABtADIAfAAgAC8AIAAoAG0AMQAgACsAIABtADIAKQAsACAAcgBhAG4AZwBlACAAWwAwACwAIAAxACkAXABuAFwAbgAgACAAIABJAG4AdABlAHIAcAByAGUAdABhAHQAaQBvAG4AOgBcAG4AIAAgACAALQAgADwAIAAwAC4ANAAxADQAMgAgACgAGiIyACAAEiIgADEAKQAgAJIhIABDAHIAbwBzAHMAaQBuAGcAIABvAHIAYgBpAHQAcwBcAG4AIAAgACAALQAgAD0AIAAwAC4ANAAxADQAMgAgACAAIAAgACAAIAAgACAAIAAgAJIhIABUAGEAbgBnAGUAbgB0AGkAYQBsACAAYgBvAHUAbgBkAGEAcgB5ACAAKABzAGkAbAB2AGUAcgAgAHIAYQB0AGkAbwApAFwAbgAgACAAIAAtACAAPgAgADAALgA0ADEANAAyACAAIAAgACAAIAAgACAAIAAgACAAkiEgAE4AZQBzAHQAZQBkACAAbwByAGIAaQB0AHMAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFQAaABpAHMAIABpAG4AZABlAHgAIABpAHMAIABzAGMAYQBsAGUALQBpAG4AdgBhAHIAaQBhAG4AdAAgAGEAbgBkACAAcwB5AG0AbQBlAHQAcgBpAGMALgBcAG4AIAAgACAALQAgAFUAcwBlAGYAdQBsACAAaQBuACAAdwBvAHIAbABkAGIAdQBpAGwAZABpAG4AZwAsACAAYwBsAGEAcwBzAGkAZgBpAGMAYQB0AGkAbwBuACwAIABhAG4AZAAgAGIAaQBuAGEAcgB5ACAAcwB5AHMAdABlAG0AIABtAG8AZABlAGwAaQBuAGcALgBcAG4AKgAvAFwAbgBcAG4AQQBTAFQAUgBPAF8ATwBSAEIASQBUAF8AQwBPAE4ARgBJAEcAVQBSAEEAVABJAE8ATgBfAEkATgBEAEUAWAAgAD0AXABuAEwAQQBNAEIARABBACgAbQBhAHMAcwAxACwAIABtAGEAcwBzADIALABcAG4AIAAgAEEAQgBTACgAbQBhAHMAcwAxACAALQAgAG0AYQBzAHMAMgApACAALwAgACgAbQBhAHMAcwAxACAAKwAgAG0AYQBzAHMAMgApAFwAbgApADsAXABuAFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8AUwBQAEgARQBSAEkAQwBBAEwAXwBUAE8AXwBDAEEAUgBUAEUAUwBJAEEATgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAG8AbgB2AGUAcgB0AHMAIABzAHAAaABlAHIAaQBjAGEAbAAgAGMAbwBvAHIAZABpAG4AYQB0AGUAcwAgAHQAbwAgAEMAYQByAHQAZQBzAGkAYQBuACAAKAB4ACwAIAB5ACwAIAB6ACkALABcAG4AIAAgACAAYQBzAHMAdQBtAGkAbgBnACAAcABoAGkAIABpAHMAIABpAG4AYwBsAGkAbgBhAHQAaQBvAG4AIABmAHIAbwBtACAAdABoAGUAIAB2AGUAcgB0AGkAYwBhAGwAIABhAHgAaQBzACAAYQBuAGQAIAB0AGgAZQB0AGEAIABpAHMAIABhAHoAaQBtAHUAdABoAC4AXABuAFwAbgAgACAAIABJAG4AcAB1AHQAcwA6AFwAbgAgACAAIAAtACAAcABoAGkAOgAgACAAIAAgAEkAbgBjAGwAaQBuAGEAdABpAG8AbgAgAGEAbgBnAGwAZQAgACgAZABlAGcAcgBlAGUAcwApACwAIAAwACAAPQAgAG4AbwByAHQAaAAgAHAAbwBsAGUALAAgADkAMAAgAD0AIABlAHEAdQBhAHQAbwByACwAIAAxADgAMAAgAD0AIABzAG8AdQB0AGgAIABwAG8AbABlAFwAbgAgACAAIAAtACAAdABoAGUAdABhADoAIAAgAEEAegBpAG0AdQB0AGgAYQBsACAAYQBuAGcAbABlACAAKABkAGUAZwByAGUAZQBzACkALAAgADAAIAA9ACAAcAByAGkAbQBlACAAbQBlAHIAaQBkAGkAYQBuACwAIAA5ADAAIAA9ACAAZQBhAHMAdABcAG4AIAAgACAALQAgAHIAOgAgACAAIAAgACAAIABSAGEAZABpAGEAbAAgAGQAaQBzAHQAYQBuAGMAZQBcAG4AIAAgACAALQAgAHAAcgBlAGMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABEAGUAYwBpAG0AYQBsACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAMQDXADMAIABhAHIAcgBhAHkAOgAgAHsAeAAsACAAeQAsACAAegB9ACwAIAByAG8AdQBuAGQAZQBkACAAdABvACAAWwBwAHIAZQBjAF0AIABkAGkAZwBpAHQAcwBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAQwBvAG0AcABhAHQAaQBiAGwAZQAgAHcAaQB0AGgAIABtAGEAcABwAGkAbgBnACAAYQBuAGQAIABzAGkAbQB1AGwAYQB0AGkAbwBuACAAcwB5AHMAdABlAG0AcwAgAHUAcwBpAG4AZwAgAHMAcABoAGUAcgBpAGMAYQBsACAAZwBlAG8AbQBlAHQAcgB5AC4AXABuACAAIAAgAC0AIABBAHMAcwB1AG0AZQBzACAAcwB0AGEAbgBkAGEAcgBkACAAcgBpAGcAaAB0AC0AaABhAG4AZABlAGQAIABjAG8AbwByAGQAaQBuAGEAdABlACAAcwB5AHMAdABlAG0ALgBcAG4AKgAvAFwAbgBcAG4AQQBTAFQAUgBPAF8AUwBQAEgARQBSAEkAQwBBAEwAXwBUAE8AXwBDAEEAUgBUAEUAUwBJAEEATgAgAD0AXABuAEwAQQBNAEIARABBACgAcABoAGkALAAgAHQAaABlAHQAYQAsACAAcgAsACAAcAByAGUAYwAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIAAvAC8AIABIAGEAbgBkAGwAZQAgAGQAZQBmAGEAdQBsAHQAIABwAHIAZQBjAGkAcwBpAG8AbgBcAG4AIAAgACAAIABwAHIAZQBjACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAHAAcgBlAGMAKQAgACsAIAAoAHAAcgBlAGMAIAA8ACAAMAApACwAIAAzACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAAQwBvAG4AdgBlAHIAdAAgAGQAZQBnAHIAZQBlAHMAIAB0AG8AIAByAGEAZABpAGEAbgBzAFwAbgAgACAAIAAgAHAAaABpAF8AcgBhAGQALAAgAFIAQQBEAEkAQQBOAFMAKABwAGgAaQApACwAXABuACAAIAAgACAAdABoAGUAdABhAF8AcgBhAGQALAAgAFIAQQBEAEkAQQBOAFMAKAB0AGgAZQB0AGEAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABUAHIAaQBnACAAYwBhAGwAYwB1AGwAYQB0AGkAbwBuAHMAXABuACAAIAAgACAAeABfAHIAYQB3ACwAIAByACAAKgAgAFMASQBOACgAcABoAGkAXwByAGEAZAApACAAKgAgAEMATwBTACgAdABoAGUAdABhAF8AcgBhAGQAKQAsAFwAbgAgACAAIAAgAHkAXwByAGEAdwAsACAAcgAgACoAIABTAEkATgAoAHAAaABpAF8AcgBhAGQAKQAgACoAIABTAEkATgAoAHQAaABlAHQAYQBfAHIAYQBkACkALABcAG4AIAAgACAAIAB6AF8AcgBhAHcALAAgAHIAIAAqACAAQwBPAFMAKABwAGgAaQBfAHIAYQBkACkALABcAG4AXABuACAAIAAgACAALwAvACAAUgBvAHUAbgBkACAAYQBuAGQAIAByAGUAdAB1AHIAbgAgAGEAcwAgADEA1wAzACAAYQByAHIAYQB5AFwAbgAgACAAIAAgAHgALAAgAFIATwBVAE4ARAAoAHgAXwByAGEAdwAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAeQAsACAAUgBPAFUATgBEACgAeQBfAHIAYQB3ACwAIABwAHIAZQBjACkALABcAG4AIAAgACAAIAB6ACwAIABSAE8AVQBOAEQAKAB6AF8AcgBhAHcALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIABIAFMAVABBAEMASwAoAHgALAAgAHkALAAgAHoAKQBcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAEMAQQBSAFQARQBTAEkAQQBOAF8AVABPAF8AUwBQAEgARQBSAEkAQwBBAEwAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBvAG4AdgBlAHIAdABzACAAQwBhAHIAdABlAHMAaQBhAG4AIABjAG8AbwByAGQAaQBuAGEAdABlAHMAIAAoAHgALAAgAHkALAAgAHoAKQAgAGkAbgB0AG8AIABzAHAAaABlAHIAaQBjAGEAbAAgAGMAbwBvAHIAZABpAG4AYQB0AGUAcwA6AFwAbgAgACAAIABpAG4AYwBsAGkAbgBhAHQAaQBvAG4AIAAoAHAAaABpACkALAAgAGEAegBpAG0AdQB0AGgAIAAoAHQAaABlAHQAYQApACwAIABhAG4AZAAgAHIAYQBkAGkAdQBzACAAKAByACkALgBcAG4AXABuACAAIAAgAEkAbgBwAHUAdABzADoAXABuACAAIAAgAC0AIAB4ACwAIAB5ACwAIAB6ADoAIABDAGEAcgB0AGUAcwBpAGEAbgAgAGMAbwBvAHIAZABpAG4AYQB0AGUAcwBcAG4AIAAgACAALQAgAHAAcgBlAGMAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABEAGUAYwBpAG0AYQBsACAAcAByAGUAYwBpAHMAaQBvAG4AIAAoAGQAZQBmAGEAdQBsAHQAIAA9ACAAMwApAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAtACAAMQDXADMAIABhAHIAcgBhAHkAOgAgAHsAcABoAGkALAAgAHQAaABlAHQAYQAsACAAcgB9ACwAIAByAG8AdQBuAGQAZQBkACAAdABvACAAWwBwAHIAZQBjAF0AIABkAGkAZwBpAHQAcwBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAcABoAGkAIAA9ACAAaQBuAGMAbABpAG4AYQB0AGkAbwBuACAAZgByAG8AbQAgAHYAZQByAHQAaQBjAGEAbAAgACgAMAAgAD0AIABwAG8AbABlACwAIAA5ADAAIAA9ACAAZQBxAHUAYQB0AG8AcgApAFwAbgAgACAAIAAtACAAdABoAGUAdABhACAAPQAgAGEAegBpAG0AdQB0AGgAYQBsACAAZABpAHIAZQBjAHQAaQBvAG4AIABmAHIAbwBtACAAeAAtAGEAeABpAHMALAAgADAAEyAzADYAMACwAFwAbgAqAC8AXABuAFwAbgBBAFMAVABSAE8AXwBDAEEAUgBUAEUAUwBJAEEATgBfAFQATwBfAFMAUABIAEUAUgBJAEMAQQBMACAAPQBcAG4ATABBAE0AQgBEAEEAKAB4ACwAIAB5ACwAIAB6ACwAIABwAHIAZQBjACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAC8ALwAgAEgAYQBuAGQAbABlACAAZABlAGYAYQB1AGwAdAAgAHIAbwB1AG4AZABpAG4AZwAgAHAAcgBlAGMAaQBzAGkAbwBuAFwAbgAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwApACAAKwAgACgAcAByAGUAYwAgADwAIAAwACkALAAgADMALAAgAHAAcgBlAGMAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAcgBhAGQAaQBhAGwAIABkAGkAcwB0AGEAbgBjAGUAIABmAHIAbwBtACAAbwByAGkAZwBpAG4AXABuACAAIAAgACAAcgAsACAAUwBRAFIAVAAoAHgAXgAyACAAKwAgAHkAXgAyACAAKwAgAHoAXgAyACkALABcAG4AXABuACAAIAAgACAALwAvACAAQwBvAG0AcAB1AHQAZQAgAGkAbgBjAGwAaQBuAGEAdABpAG8AbgAgAGEAbgBnAGwAZQAgAGYAcgBvAG0AIAB2AGUAcgB0AGkAYwBhAGwAIABhAHgAaQBzACAAKAB6ACkAXABuACAAIAAgACAAcABoAGkALAAgAEQARQBHAFIARQBFAFMAKABBAEMATwBTACgAegAgAC8AIAByACkAKQAsAFwAbgBcAG4AIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAYQB6AGkAbQB1AHQAaABhAGwAIABhAG4AZwBsAGUAIABpAG4AIAB4AC0AeQAgAHAAbABhAG4AZQAsACAAbgBvAHIAbQBhAGwAaQB6AGUAZAAgAHQAbwAgAFsAMAAsACAAMwA2ADAAKQBcAG4AIAAgACAAIAB0AGgAZQB0AGEALAAgAE0ATwBEACgARABFAEcAUgBFAEUAUwAoAEEAVABBAE4AMgAoAHkALAAgAHgAKQApACwAIAAzADYAMAApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAFIAbwB1AG4AZAAgAGEAbABsACAAbwB1AHQAcAB1AHQAcwBcAG4AIAAgACAAIABwAGgAaQBfAG8AdQB0ACwAIABSAE8AVQBOAEQAKABwAGgAaQAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAdABoAGUAdABhAF8AbwB1AHQALAAgAFIATwBVAE4ARAAoAHQAaABlAHQAYQAsACAAcAByAGUAYwApACwAXABuACAAIAAgACAAcgBfAG8AdQB0ACwAIABSAE8AVQBOAEQAKAByACwAIABwAHIAZQBjACkALABcAG4AXABuACAAIAAgACAALwAvACAAUgBlAHQAdQByAG4AIABhAHMAIAAxANcAMwAgAGEAcgByAGEAeQBcAG4AIAAgACAAIABIAFMAVABBAEMASwAoAHAAaABpAF8AbwB1AHQALAAgAHQAaABlAHQAYQBfAG8AdQB0ACwAIAByAF8AbwB1AHQAKQBcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgBEAEUARwBfAEQARQBDAF8ARABNAFMAIAA9ACAATABBAE0AQgBEAEEAKABEAGUAYwBpAG0AYQBsAEQAZQBnAHIAZQBlAHMALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAARABlAGcALAAgAFQAUgBVAE4AQwAoAEQAZQBjAGkAbQBhAGwARABlAGcAcgBlAGUAcwApACwAXABuACAAIAAgACAAIAAgACAAIABGAHIAYQBjAFAAbwByAHQAaQBvAG4ALAAgAEEAQgBTACgARABlAGMAaQBtAGEAbABEAGUAZwByAGUAZQBzACAALQAgAEQAZQBnACkALABcAG4AIAAgACAAIAAgACAAIAAgAE0AaQBuAHUAdABlAHMALAAgAEYAcgBhAGMAUABvAHIAdABpAG8AbgAgACoAIAA2ADAALABcAG4AIAAgACAAIAAgACAAIAAgAE0AaQBuAF8AcABhAHIAdAAsACAAVABSAFUATgBDACgATQBpAG4AdQB0AGUAcwApACAALwAgADEAMAAwACwAXABuACAAIAAgACAAIAAgACAAIABJAG4AdABNAGkAbgAsACAASQBOAFQAKABNAGkAbgB1AHQAZQBzACkALABcAG4AIAAgACAAIAAgACAAIAAgAEYAcgBhAGMATQBpAG4ALAAgAEEAQgBTACgATQBpAG4AdQB0AGUAcwAgAC0AIABJAG4AdABNAGkAbgApACwAXABuACAAIAAgACAAIAAgACAAIABTAGUAYwBvAG4AZABzACwAIABGAHIAYQBjAE0AaQBuACAAKgAgADYAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAcwBlAGMAXwBwAGEAcgB0ACwAIABTAGUAYwBvAG4AZABzACAALwAgADEAMAAwADAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAbwB1AHQAcAB1AHQALAAgAEQAZQBnACAAKwAgAE0AaQBuAF8AcABhAHIAdAAgACsAIABzAGUAYwBfAHAAYQByAHQALABcAG4AIAAgACAAIAAgACAAIAAgAEYASQBYAEUARAAoAG8AdQB0AHAAdQB0ACwAIAA3ACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ARABFAEcAXwBEAE0AUwAgAD0AIABMAEEATQBCAEQAQQAoAEQAZQBjAGkAbQBhAGwARABlAGcAcgBlAGUAcwAsACAAWwBwAHIAZQBjAGkAcwBpAG8AbgBdACwAXABuAFwAbgBMAEUAVAAoAFwAbgAgACAAIAAgAGQAZQBjAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAUAByAGUAYwBpAHMAaQBvAG4AKQAsACAAMwAsACAAUAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgAgACAAIAAgAEQAZQBnACwAIABUAFIAVQBOAEMAKABEAGUAYwBpAG0AYQBsAEQAZQBnAHIAZQBlAHMAKQAsAFwAbgAgACAAIAAgAEYAcgBhAGMAUABvAHIAdABpAG8AbgAsACAAQQBCAFMAKABEAGUAYwBpAG0AYQBsAEQAZQBnAHIAZQBlAHMAIAAtACAARABlAGcAKQAsAFwAbgAgACAAIAAgAE0AaQBuAHUAdABlAHMALAAgAEYAcgBhAGMAUABvAHIAdABpAG8AbgAgACoAIAA2ADAALABcAG4AIAAgACAAIABJAG4AdABNAGkAbgAsACAASQBOAFQAKABNAGkAbgB1AHQAZQBzACkALABcAG4AIAAgACAAIABGAHIAYQBjAE0AaQBuACwAIABBAEIAUwAoAE0AaQBuAHUAdABlAHMAIAAtACAASQBuAHQATQBpAG4AKQAsAFwAbgAgACAAIAAgAFMAZQBjAG8AbgBkAHMALAAgAEYAcgBhAGMATQBpAG4AIAAqACAANgAwACwAXABuACAAIAAgACAARABlAGcAIAAmACAAXAAiALAAIABcACIAIAAmACAASQBuAHQATQBpAG4AIAAmACAAQwBIAEEAUgAoADMAOQApACAAJgAgAEMASABBAFIAKAAzADIAKQAgACYAIABGAEkAWABFAEQAKABTAGUAYwBvAG4AZABzACwAIABkAGUAYwBwAHIAZQBjACkAIAAmACAAQwBIAEEAUgAoADMANAApAFwAbgApAFwAbgApADsAXABuAFwAbgBEAEUARwBfAEQATQBTAF8ARABFAEMAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALABcAG4AIAAgACAAIABMAEUAVAAoAFwAbgAgACAAIAAgACAAIAAgACAAZABlAGcAcgBlAGUAcwAsACAAVABSAFUATgBDACgAaQBuAHAAdQB0ACkALABcAG4AIAAgACAAIAAgACAAIAAgAG0AaQBuAHUAdABlAHMALAAgAFQAUgBVAE4AQwAoACgAaQBuAHAAdQB0ACAALQAgAGQAZQBnAHIAZQBlAHMAKQAgACoAIAAxADAAMAApACwAXABuACAAIAAgACAAIAAgACAAIABmAHIAYQBjAHQAaQBvAG4AYQBsAF8AcwBlAGMAbwBuAGQAcwAsACAAKAAoAGkAbgBwAHUAdAAgACoAIAAxADAAMAApACAALQAgAFQAUgBVAE4AQwAoAGkAbgBwAHUAdAAgACoAIAAxADAAMAApACkAIAAvACAAMAAuADYALABcAG4AIAAgACAAIAAgACAAIAAgAC8AKgAgACAAKgAvAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQALAAgAGQAZQBnAHIAZQBlAHMAIAArACAAKAAoAG0AaQBuAHUAdABlAHMAIAArACAAZgByAGEAYwB0AGkAbwBuAGEAbABfAHMAZQBjAG8AbgBkAHMAKQAgAC8AIAA2ADAAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAQQBTAFQAUgBPAF8ATwBSAEIASQBUAF8AQQBYAEkAUwBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAG8AbQBwAHUAdABlAHMAIAB0AGgAZQAgAHMAZQBtAGkALQBtAGEAagBvAHIAIABhAHgAaQBzACAAKABpAG4AIABBAFUAKQAgAG8AZgAgAGEAIAB0AHcAbwAtAGIAbwBkAHkAIABzAHkAcwB0AGUAbQBcAG4AIAAgACAAYgBhAHMAZQBkACAAbwBuACAAdABvAHQAYQBsACAAbQBhAHMAcwAgACgAaQBuACAAcwBvAGwAYQByACAAbQBhAHMAcwBlAHMAKQAgAGEAbgBkACAAbwByAGIAaQB0AGEAbAAgAHAAZQByAGkAbwBkACAAKABpAG4AIAB5AGUAYQByAHMAKQAuAFwAbgBcAG4AIAAgACAASQBuAHAAdQB0AHMAOgBcAG4AIAAgACAALQAgAG0AYQBzAHMAMQA6ACAAUAByAGkAbQBhAHIAeQAgAG0AYQBzAHMAIAAoAGkAbgAgAHMAbwBsAGEAcgAgAG0AYQBzAHMAZQBzACkAXABuACAAIAAgAC0AIABtAGEAcwBzADIAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABTAGUAYwBvAG4AZABhAHIAeQAgAG0AYQBzAHMAIAAoAGkAbgAgAHMAbwBsAGEAcgAgAG0AYQBzAHMAZQBzADsAIABkAGUAZgBhAHUAbAB0AHMAIAB0AG8AIAAwACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAD0AIAAxACkAXABuACAAIAAgAC0AIABwAGUAcgBpAG8AZAA6ACAATwByAGIAaQB0AGEAbAAgAHAAZQByAGkAbwBkACAAKABpAG4AIAB5AGUAYQByAHMAKQBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAALQAgAE8AcgBiAGkAdABhAGwAIABhAHgAaQBzACAAaQBuACAAYQBzAHQAcgBvAG4AbwBtAGkAYwBhAGwAIAB1AG4AaQB0AHMAIAAoAEEAVQApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABVAHMAZQBzACAATgBlAHcAdABvAG4AaQBhAG4AIABmAG8AcgBtACAAbwBmACAASwBlAHAAbABlAHIAJwBzACAAVABoAGkAcgBkACAATABhAHcALgBcAG4AIAAgACAALQAgAG0AYQBzAHMAMgAgAGkAcwAgAGMAbwBuAHYAZQByAHQAZQBkACAAZgByAG8AbQAgAHMAbwBsAGEAcgAgAG0AYQBzAHMAZQBzACAAaQBmACAAcAByAGUAcwBlAG4AdAAuAFwAbgAqAC8AXABuAFwAbgBBAFMAVABSAE8AXwBPAFIAQgBJAFQAXwBBAFgASQBTACAAPQAgAEwAQQBNAEIARABBACgAbQBhAHMAcwAxACwAIABtAGEAcwBzADIALAAgAHAAZQByAGkAbwBkACwAXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAG0AXwAyACwAIABJAEYAKAAoAEkAUwBPAE0ASQBUAFQARQBEACgAbQBhAHMAcwAyACkAKQAgACsAIAAoAG0AYQBzAHMAMgAgAD0AIAAxACkALAAgADAALAAgAG0AYQBzAHMAMgAgACoAIAAzAC4AMAAwADMARQAtADYAKQAsAFwAbgAgACAAIAAgAGEAeABpAHMALAAgAFAATwBXAEUAUgAoACgAUABPAFcARQBSACgAcABlAHIAaQBvAGQALAAgADIAKQAgACoAIAAoAG0AYQBzAHMAMQAgACsAIABtAF8AMgApACkALAAgADEAIAAvACAAMwApACwAXABuACAAIAAgACAAYQB4AGkAcwBcAG4AIAAgACkAXABuACkAOwBcAG4AXABuAFwAbgAvACoAIABBAFMAVABSAE8AXwBPAFIAQgBJAFQAXwBQAEUAUgBJAE8ARABcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABDAG8AbQBwAHUAdABlAHMAIAB0AGgAZQAgAG8AcgBiAGkAdABhAGwAIABwAGUAcgBpAG8AZAAgACgAaQBuACAAeQBlAGEAcgBzACkAIABvAGYAIABhACAAdAB3AG8ALQBiAG8AZAB5ACAAcwB5AHMAdABlAG0AXABuACAAIAAgAGIAYQBzAGUAZAAgAG8AbgAgAHQAbwB0AGEAbAAgAG0AYQBzAHMAIAAoAGkAbgAgAHMAbwBsAGEAcgAgAG0AYQBzAHMAZQBzACkAIABhAG4AZAAgAHMAZQBtAGkALQBtAGEAagBvAHIAIABhAHgAaQBzACAAKABpAG4AIABBAFUAKQAuAFwAbgBcAG4AIAAgACAASQBuAHAAdQB0AHMAOgBcAG4AIAAgACAALQAgAG0AYQBzAHMAMQA6ACAAUAByAGkAbQBhAHIAeQAgAG0AYQBzAHMAIAAoAGkAbgAgAHMAbwBsAGEAcgAgAG0AYQBzAHMAZQBzACkAXABuACAAIAAgAC0AIABtAGEAcwBzADIAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABTAGUAYwBvAG4AZABhAHIAeQAgAG0AYQBzAHMAIAAoAGkAbgAgAHMAbwBsAGEAcgAgAG0AYQBzAHMAZQBzADsAIABkAGUAZgBhAHUAbAB0AHMAIAB0AG8AIAAwACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAD0AIAAxACkAXABuACAAIAAgAC0AIABhAHgAaQBzADoAIABPAHIAYgBpAHQAYQBsACAAYQB4AGkAcwAgACgAaQBuACAAQQBVACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABPAHIAYgBpAHQAYQBsACAAcABlAHIAaQBvAGQAIABpAG4AIAB5AGUAYQByAHMAXABuACoALwBcAG4AXABuAEEAUwBUAFIATwBfAE8AUgBCAEkAVABfAFAARQBSAEkATwBEACAAPQAgAEwAQQBNAEIARABBACgAbQBhAHMAcwAxACwAIABtAGEAcwBzADIALAAgAGEAeABpAHMALABcAG4AIAAgAEwARQBUACgAXABuACAAIAAgACAAbQBfADIALAAgAEkARgAoACgASQBTAE8ATQBJAFQAVABFAEQAKABtAGEAcwBzADIAKQApACAAKwAgACgAbQBhAHMAcwAyACAAPQAgADEAKQAsACAAMAAsACAAbQBhAHMAcwAyACAAKgAgADMALgAwADAAMgA3ADMARQAtADYAKQAsAFwAbgAgACAAIAAgAHAAZQByAGkAbwBkACwAIABTAFEAUgBUACgAUABPAFcARQBSACgAYQB4AGkAcwAsACAAMwApACAALwAgACgAbQBhAHMAcwAxACAAKwAgAG0AXwAyACkAKQAsAFwAbgAgACAAIAAgAHAAZQByAGkAbwBkAFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAE8AUgBCAEkAVABfAFMAVQBNAF8ATQBBAFMAUwBFAFMAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAQwBvAG0AcAB1AHQAZQBzACAAdABoAGUAIABjAG8AbQBiAGkAbgBlAGQAIABtAGEAcwBzACAAKABpAG4AIABzAG8AbABhAHIAIABtAGEAcwBzAGUAcwApACAAbwBmACAAYQAgAHQAdwBvAC0AYgBvAGQAeQAgAHMAeQBzAHQAZQBtAFwAbgAgACAAIABmAHIAbwBtACAAbwByAGIAaQB0AGEAbAAgAGEAeABpAHMAIAAoAGkAbgAgAEEAVQApACAAYQBuAGQAIABwAGUAcgBpAG8AZAAgACgAaQBuACAAeQBlAGEAcgBzACkALgBcAG4AXABuACAAIAAgAEkAbgBwAHUAdABzADoAXABuACAAIAAgAC0AIABhAHgAaQBzADoAIABTAGUAbQBpAC0AbQBhAGoAbwByACAAYQB4AGkAcwAgACgAQQBVACkAXABuACAAIAAgAC0AIABwAGUAcgBpAG8AZAA6ACAATwByAGIAaQB0AGEAbAAgAHAAZQByAGkAbwBkACAAKAB5AGUAYQByAHMAKQBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAALQAgAFQAbwB0AGEAbAAgAHMAeQBzAHQAZQBtACAAbQBhAHMAcwAgACgAaQBuACAAcwBvAGwAYQByACAAbQBhAHMAcwBlAHMAKQBcAG4AKgAvAFwAbgBcAG4AQQBTAFQAUgBPAF8ATwBSAEIASQBUAF8AUwBVAE0AXwBNAEEAUwBTAEUAUwAgAD0AIABMAEEATQBCAEQAQQAoAGEAeABpAHMALAAgAHAAZQByAGkAbwBkACwAXABuACAAIABQAE8AVwBFAFIAKABhAHgAaQBzACwAIAAzACkAIAAvACAAUABPAFcARQBSACgAcABlAHIAaQBvAGQALAAgADIAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAgAEEAUwBUAFIATwBfAE8AUgBCAEkAVABfAFMATwBMAFYARQBSAFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFUAbgBpAGYAaQBlAGQAIABzAG8AbAB2AGUAcgAgAGYAbwByACAAbwByAGIAaQB0AGEAbAAgAGEAeABpAHMALAAgAHAAZQByAGkAbwBkACwAIABvAHIAIAB0AG8AdABhAGwAIABtAGEAcwBzACAAaQBuACAAYQAgAHQAdwBvAC0AYgBvAGQAeQAgAHMAeQBzAHQAZQBtAC4AXABuACAAIAAgAFMAZQBsAGUAYwB0AHMAIABhAHAAcAByAG8AcAByAGkAYQB0AGUAIABmAG8AcgBtAHUAbABhACAAYgBhAHMAZQBkACAAbwBuACAAbQBvAGQAZQAuAFwAbgBcAG4AIAAgACAASQBuAHAAdQB0AHMAOgBcAG4AIAAgACAALQAgAG0AbwBkAGUAOgAgAE8AbgBlACAAbwBmACAAXAAiAGEAeABpAHMAXAAiACwAIABcACIAcABlAHIAaQBvAGQAXAAiACwAIABvAHIAIABcACIAbQBhAHMAcwBcACIAXABuACAAIAAgAC0AIAB2AGEAbABfADEAOgAgAEYAaQByAHMAdAAgAGsAbgBvAHcAbgAgAHYAYQBsAHUAZQAgACgAZABlAHAAZQBuAGQAcwAgAG8AbgAgAG0AbwBkAGUAKQBcAG4AIAAgACAALQAgAHYAYQBsAF8AMgA6ACAAUwBlAGMAbwBuAGQAIABrAG4AbwB3AG4AIAB2AGEAbAB1AGUAIAAoAGQAZQBwAGUAbgBkAHMAIABvAG4AIABtAG8AZABlACkAXABuACAAIAAgAC0AIABtAGEAcwBzADIAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABTAGUAYwBvAG4AZABhAHIAeQAgAG0AYQBzAHMAIAAoAGkAbgAgAHMAbwBsAGEAcgAgAG0AYQBzAHMAZQBzADsAIABkAGUAZgBhAHUAbAB0AHMAIAB0AG8AIAAwACAAaQBmACAAbwBtAGkAdAB0AGUAZAAgAG8AcgAgAD0AIAAxACkAXABuACAAIAAgAC0AIABwAHIAZQBjAGkAcwBpAG8AbgAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAEQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAgAGYAbwByACAAZgBvAHIAbQBhAHQAdABlAGQAIABvAHUAdABwAHUAdAAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAA0ACkAXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAC0AIABSAGUAcwB1AGwAdAAgAGEAcwAgAGEAIABuAHUAbQBiAGUAcgAgAG8AcgAgAGwAYQBiAGUAbABlAGQAIABzAHQAcgBpAG4AZwAsACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlACAAYQBuAGQAIABmAG8AcgBtAGEAdABcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAbQBhAHMAcwAyACAAaQBzACAAbwBuAGwAeQAgAHIAZQBsAGUAdgBhAG4AdAAgAGYAbwByACAAXAAiAGEAeABpAHMAXAAiACAAYQBuAGQAIABcACIAcABlAHIAaQBvAGQAXAAiACAAbQBvAGQAZQBzAC4AXABuACoALwBcAG4AXABuAEEAUwBUAFIATwBfAE8AUgBCAEkAVABfAFMATwBMAFYARQBSACAAPQBcAG4ATABBAE0AQgBEAEEAKABtAG8AZABlACwAIAB2AGEAbABfADEALAAgAHYAYQBsAF8AMgAsACAAbQBhAHMAcwAyACwAIABwAHIAZQBjAGkAcwBpAG8AbgAsAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABtAF8AMgAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABtAGEAcwBzADIAKQAgACsAIAAoAG0AYQBzAHMAMgAgAD0AIAAxACkALAAgADAALAAgAG0AYQBzAHMAMgAgACoAIAAzAC4AMAAwADMARQAtADYAKQAsAFwAbgAgACAAIAAgAHAAcgBlAGMALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAcAByAGUAYwBpAHMAaQBvAG4AKQAsACAANAAsACAAcAByAGUAYwBpAHMAaQBvAG4AKQAsAFwAbgBcAG4AIAAgACAAIAByAGUAcwB1AGwAdAAsAFwAbgAgACAAIAAgACAAIABTAFcASQBUAEMASAAoAEwATwBXAEUAUgAoAG0AbwBkAGUAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAGEAeABpAHMAXAAiACwAIABQAE8AVwBFAFIAKAAoAFAATwBXAEUAUgAoAHYAYQBsAF8AMgAsACAAMgApACAAKgAgACgAdgBhAGwAXwAxACAAKwAgAG0AXwAyACkAKQAsACAAMQAgAC8AIAAzACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBwAGUAcgBpAG8AZABcACIALAAgAFMAUQBSAFQAKABQAE8AVwBFAFIAKAB2AGEAbABfADIALAAgADMAKQAgAC8AIAAoAHYAYQBsAF8AMQAgACsAIABtAF8AMgApACkALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgBtAGEAcwBzAFwAIgAsACAAUABPAFcARQBSACgAdgBhAGwAXwAxACwAIAAzACkAIAAvACAAUABPAFcARQBSACgAdgBhAGwAXwAyACwAIAAyACkALABcAG4AIAAgACAAIAAgACAAIAAgAE4AQQAoACkAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAbABhAGIAZQBsACwAXABuACAAIAAgACAAIAAgAFMAVwBJAFQAQwBIACgATABPAFcARQBSACgAbQBvAGQAZQApACwAXABuACAAIAAgACAAIAAgACAAIABcACIAYQB4AGkAcwBcACIALAAgAFwAIgBBAHgAaQBzACAAPQAgAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAHAAZQByAGkAbwBkAFwAIgAsACAAXAAiAFAAZQByAGkAbwBkACAAPQAgAFwAIgAsAFwAbgAgACAAIAAgACAAIAAgACAAXAAiAG0AYQBzAHMAXAAiACwAIABcACIATQBhAHMAcwAgAD0AIABcACIALABcAG4AIAAgACAAIAAgACAAIAAgAFwAIgA/AFwAIgBcAG4AIAAgACAAIAAgACAAKQAsAFwAbgBcAG4AIAAgACAAIABUAEUAWABUACgAcgBlAHMAdQBsAHQALAAgAFwAIgAwAC4AXAAiACAAJgAgAFIARQBQAFQAKABcACIAMABcACIALAAgAHAAcgBlAGMAKQApACAAJgAgAFwAIgAgAFwAIgAgACYAIABsAGEAYgBlAGwAXABuACAAIAApAFwAbgApADsAIgB9ACwAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBHAGUAbgBlAHIAYQBsACIALAAiAHQAZQB4AHQAIgA6ACIALwAqACAAUgBFAEMASQBQADoAXABuACAAIAAgAFAAdQByAHAAbwBzAGUAOgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwAgAHQAaABlACAAcgBlAGMAaQBwAHIAbwBjAGEAbAAgACgAbQB1AGwAdABpAHAAbABpAGMAYQB0AGkAdgBlACAAaQBuAHYAZQByAHMAZQApACAAbwBmACAAYQAgAG4AdQBtAGIAZQByAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgAEEAIABzAGkAbgBnAGwAZQAgAGQAZQBjAGkAbQBhAGwAIAB2AGEAbAB1AGUAIABlAHEAdQBhAGwAIAB0AG8AIAAxACAAZABpAHYAaQBkAGUAZAAgAGIAeQAgAHQAaABlACAAaQBuAHAAdQB0AC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABpAG4AcAB1AHQAIAAoAHIAZQBxAHUAaQByAGUAZAApADoAIABBAG4AeQAgAG4AbwBuAHoAZQByAG8AIABuAHUAbQBlAHIAaQBjACAAdgBhAGwAdQBlAC4AXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAALQAgAFIAZQB0AHUAcgBuAHMAIABgACMARABJAFYALwAwACEAYAAgAGkAZgAgAGkAbgBwAHUAdAAgAGkAcwAgAHoAZQByAG8ALgBcAG4AIAAgACAALQAgAFUAcwBlAGYAdQBsACAAZgBvAHIAIABmAGwAaQBwAHAAaQBuAGcAIABmAHIAYQBjAHQAaQBvAG4AcwAsACAAYwBvAG4AdgBlAHIAdABpAG4AZwAgAHIAYQB0AGUAcwAgACgAZQAuAGcALgAsACAASAB6ACAAlCEgAHMAZQBjAG8AbgBkAHMAKQAsACAAbwByACAAaQBuAHYAZQByAHQAaQBuAGcAIAByAGEAdABpAG8AcwAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQA6AFwAbgAgACAAIAAgACAAUgBFAEMASQBQACgANAApACAAkiEgADAALgAyADUAXABuACAAIAAgACAAIABSAEUAQwBJAFAAKAAwAC4AMgApACAAkiEgADUAXABuACoALwBcAG4AXABuAFwAbgBSAEUAQwBJAFAAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALAAgADEAIAAvACAAaQBuAHAAdQB0ACkAOwBcAG4AXABuAC8AKgAgAEYAUgBBAEMAOgBcAG4AIAAgACAAUAB1AHIAcABvAHMAZQA6AFwAbgAgACAAIABSAGUAdAB1AHIAbgBzACAAdABoAGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAKABuAG8AbgAtAGkAbgB0AGUAZwBlAHIAKQAgAHAAYQByAHQAIABvAGYAIABhACAAbgB1AG0AYgBlAHIALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHMAYwBhAGwAYQByACAAZABlAGMAaQBtAGEAbAAgAGIAZQB0AHcAZQBlAG4AIAAwACAAYQBuAGQAIAAxACAAKABvAHIAIAAtADEAIABhAG4AZAAgADAAIABpAGYAIABzAGkAZwBuACAAaQBzACAAcAByAGUAcwBlAHIAdgBlAGQAKQAuAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAtACAAaQBuAHAAdQB0ACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAVABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAGUAeAB0AHIAYQBjAHQAIAB0AGgAZQAgAGYAcgBhAGMAdABpAG8AbgBhAGwAIABwAGEAcgB0ACAAZgByAG8AbQAuAFwAbgAgACAAIAAtACAAbQBvAGQAZQAgACgAbwBwAHQAaQBvAG4AYQBsACkAOgAgAE8AdQB0AHAAdQB0ACAAbQBvAGQAZQAgACgAZABlAGYAYQB1AGwAdAAgAD0AIAAwACkAXABuACAAIAAgACAAIAAgACAALQAgADAAOgAgAEEAbAB3AGEAeQBzACAAcgBlAHQAdQByAG4AIABwAG8AcwBpAHQAaQB2AGUAIABmAHIAYQBjAHQAaQBvAG4AYQBsACAAcABhAHIAdABcAG4AIAAgACAAIAAgACAAIAAtACAAMQA6ACAAUAByAGUAcwBlAHIAdgBlACAAcwBpAGcAbgAgAG8AZgAgAGkAbgBwAHUAdAAgACgAZQAuAGcALgAsACAALQAzAC4AMgA1ACAAkiEgAC0AMAAuADIANQApAFwAbgBcAG4AIAAgACAATgBvAHQAZQBzADoAXABuACAAIAAgAC0AIABDAG8AbQBwAGwAZQBtAGUAbgB0AHMAIABFAHgAYwBlAGwAGSBzACAAVABSAFUATgBDACAAYQBuAGQAIABRAFUATwBUAEkARQBOAFQAIABmAHUAbgBjAHQAaQBvAG4AcwAuAFwAbgAgACAAIAAtACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGQAZQB0AGUAYwB0AGkAbgBnACAAZABlAGMAaQBtAGEAbAAgAHIAZQBtAGEAaQBuAGQAZQByAHMAIABhAG4AZAAgAGEAbgBhAGwAeQB6AGkAbgBnACAAbwBmAGYAcwBlAHQAcwAgAGYAcgBvAG0AIAB3AGgAbwBsAGUAIAB2AGEAbAB1AGUAcwAuAFwAbgAgACAAIAAtACAAUwBpAGcAbgAtAHAAcgBlAHMAZQByAHYAaQBuAGcAIABtAG8AZABlACAAYwBhAG4AIABpAG4AZABpAGMAYQB0AGUAIAB3AGgAZQB0AGgAZQByACAAYQAgAHYAYQBsAHUAZQAgAGkAcwAgAGoAdQBzAHQAIABhAGIAbwB2AGUAIABvAHIAIABqAHUAcwB0ACAAYgBlAGwAbwB3ACAAYQBuACAAaQBuAHQAZQBnAGUAcgAuAFwAbgBcAG4AIAAgACAARQB4AGEAbQBwAGwAZQBzADoAXABuACAAIAAgAEYAUgBBAEMAKAAtADMALgAyADUAKQAgACAAIAAgACAAIAAgAJIhIAAwAC4AMgA1ACAAIABcAG4AIAAgACAARgBSAEEAQwAoAC0AMwAuADIANQAsACAAMQApACAAIAAgACAAkiEgAC0AMAAuADIANQBcAG4AKgAvAFwAbgBcAG4AXABuAEYAUgBBAEMAIAA9ACAATABBAE0AQgBEAEEAKABpAG4AcAB1AHQALAAgAFsAbQBvAGQAZQBdACwAXABuACAAIAAgACAATABFAFQAKABcAG4AIAAgACAAIAAgACAAIAAgAC8ALwAgAEQAZQBmAGEAdQBsAHQAIABtAG8AZABlACAAdABvACAAMAAgAGkAZgAgAG8AbQBpAHQAdABlAGQAIABvAHIAIABpAG4AdgBhAGwAaQBkAFwAbgAgACAAIAAgACAAIAAgACAAbQBvAGQAZQAsACAASQBGACgATwBSACgASQBTAE8ATQBJAFQAVABFAEQAKABtAG8AZABlACkALAAgAG0AbwBkAGUAIAA+ACAAMQApACwAIAAwACwAIABtAG8AZABlACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABDAG8AbQBwAHUAdABlACAAZgByAGEAYwB0AGkAbwBuAGEAbAAgAHAAYQByAHQAIABiAHkAIABzAHUAYgB0AHIAYQBjAHQAaQBuAGcAIABpAG4AdABlAGcAZQByACAAcABvAHIAdABpAG8AbgBcAG4AIAAgACAAIAAgACAAIAAgAGYAcgBhAGMAXwBwAGEAcgB0ACwAIABpAG4AcAB1AHQAIAAtACAAVABSAFUATgBDACgAaQBuAHAAdQB0ACkALABcAG4AXABuACAAIAAgACAAIAAgACAAIAAvAC8AIABSAGUAdAB1AHIAbgAgAHMAaQBnAG4AZQBkACAAbwByACAAYQBiAHMAbwBsAHUAdABlACAAdgBhAGwAdQBlACAAZABlAHAAZQBuAGQAaQBuAGcAIABvAG4AIABtAG8AZABlAFwAbgAgACAAIAAgACAAIAAgACAASQBGACgAbQBvAGQAZQAgAD0AIAAxACwAIABmAHIAYQBjAF8AcABhAHIAdAAsACAAQQBCAFMAKABmAHIAYQBjAF8AcABhAHIAdAApACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAAUgBPAE8AVAA6AFwAbgAgACAAIABQAHUAcgBwAG8AcwBlADoAXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAIAB0AGgAZQAgAHgALQB0AGgAIAByAG8AbwB0ACAAbwBmACAAYQAgAG4AdQBtAGIAZQByACAAKABvAHIAIABzAHEAdQBhAHIAZQAgAHIAbwBvAHQAIABpAGYAIABuAG8AIABkAGUAZwByAGUAZQAgAGkAcwAgAHMAcABlAGMAaQBmAGkAZQBkACkALgBcAG4AXABuACAAIAAgAFIAZQB0AHUAcgBuAHMAOgBcAG4AIAAgACAAQQAgAHIAZQBhAGwAIABkAGUAYwBpAG0AYQBsACAAbgB1AG0AYgBlAHIAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAcgBvAG8AdAAgAG8AZgAgAGAAbgBgAC4AXABuAFwAbgAgACAAIABQAGEAcgBhAG0AZQB0AGUAcgBzADoAXABuACAAIAAgAC0AIABuACAAKAByAGUAcQB1AGkAcgBlAGQAKQA6ACAAVABoAGUAIABuAHUAbQBiAGUAcgAgAHQAbwAgAHQAYQBrAGUAIAB0AGgAZQAgAHIAbwBvAHQAIABvAGYALgBcAG4AIAAgACAALQAgAHgAIAAoAG8AcAB0AGkAbwBuAGEAbAApADoAIABUAGgAZQAgAHIAbwBvAHQAIABkAGUAZwByAGUAZQAuACAARABlAGYAYQB1AGwAdABzACAAdABvACAAMgAgACgAcwBxAHUAYQByAGUAIAByAG8AbwB0ACkALgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAtACAAUgBlAGoAZQBjAHQAcwAgAGEAbABsACAAbgBlAGcAYQB0AGkAdgBlACAAaQBuAHAAdQB0ACAAdgBhAGwAdQBlAHMAIABmAG8AcgAgAGAAbgBgACwAIAByAGUAZwBhAHIAZABsAGUAcwBzACAAbwBmACAAcgBvAG8AdAAuAFwAbgAgACAAIAAtACAATQBpAG0AaQBjAHMAIABFAHgAYwBlAGwAJwBzACAAYgBlAGgAYQB2AGkAbwByACAAKAByAGUAdAB1AHIAbgBzACAAIwBOAFUATQAhACAAaQBmACAAcgBvAG8AdAAgAHcAbwB1AGwAZAAgAGIAZQAgAGMAbwBtAHAAbABlAHgAKQAuAFwAbgAgACAAIAAtACAAVQBzAGUAIABFAHgAYwBlAGwAGSBzACAAYABJAE0AUABPAFcARQBSAGAAIABvAHIAIABgAEkATQBTAFEAUgBUAGAAIABmAG8AcgAgAGMAbwBtAHAAbABlAHgAIABuAHUAbQBiAGUAcgAgAHMAdQBwAHAAbwByAHQALgBcAG4AXABuACAAIAAgAEUAeABhAG0AcABsAGUAcwA6AFwAbgAgACAAIABSAE8ATwBUACgAMQA2ACkAIAAgACAAIAAgACAAIACSISAANABcAG4AIAAgACAAUgBPAE8AVAAoADIANwAsACAAMwApACAAIAAgACAAkiEgADMAXABuACAAIAAgAFIATwBPAFQAKAA5ACwAIAAwAC4ANQApACAAIAAgAJIhIAA4ADEAXABuACAAIAAgAFIATwBPAFQAKAAtADUALAAgADMAKQAgACAAIAAgAJIhIAAjAE4AVQBNACEAXABuACoALwBcAG4AXABuAFIATwBPAFQAIAA9ACAATABBAE0AQgBEAEEAKABuACwAIABbAHgAXQAsAFwAbgAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAByAG8AbwB0AF8AZABlAGcAcgBlAGUALAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAeAApACwAIAAyACwAIAB4ACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgAoAG4AIAA8ACAAMAAsAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAFEAUgBUACgALQAxACkALAAgACAALwAvACAAVAByAGkAZwBnAGUAcgBzACAAIwBOAFUATQAhACAAZQByAHIAbwByACAAZgBvAHIAIABuAGUAZwBhAHQAaQB2AGUAIABiAGEAcwBlAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIABuACAAXgAgACgAMQAgAC8AIAByAG8AbwB0AF8AZABlAGcAcgBlAGUAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAqACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAXABuACAAIAAgAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwAgAGEAIABvAG4AZQAtAGwAaQBuAGUALAAgAGwAYQBiAGUAbABlAGQAIAB2AGUAcgBzAGkAbwBuACAAbwBmACAAdABoAGUAIABmAG8AcgBtAHUAbABhACAAaQBuACAAdABoAGUAIABnAGkAdgBlAG4AIABjAGUAbABsACwAXABuACAAIAAgAG8AbQBpAHQAdABpAG4AZwAgAHQAaABlACAAbABlAGEAZABpAG4AZwAgAGUAcQB1AGEAbAAgAHMAaQBnAG4AIABhAG4AZAAgAHAAcgBlAHAAZQBuAGQAaQBuAGcAIAB0AGgAZQAgAGMAZQBsAGwAIAByAGUAZgBlAHIAZQBuAGMAZQAuAFwAbgBcAG4AIAAgACAAUwB5AG4AdABhAHgAOgBcAG4AIAAgACAAIAAgAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUACgAYwBlAGwAbAApAFwAbgBcAG4AIAAgACAAUABhAHIAYQBtAGUAdABlAHIAcwA6AFwAbgAgACAAIAAgACAAYwBlAGwAbAAgADoAIABBACAAcgBlAGYAZQByAGUAbgBjAGUAIAB0AG8AIABhACAAYwBlAGwAbAAgAGMAbwBuAHQAYQBpAG4AaQBuAGcAIABhACAAZgBvAHIAbQB1AGwAYQAuAFwAbgBcAG4AIAAgACAAUgBlAHQAdQByAG4AcwA6AFwAbgAgACAAIAAgACAAQQAgAHMAaQBuAGcAbABlAC0AbABpAG4AZQAgAHMAdAByAGkAbgBnACAAaQBuACAAdABoAGUAIABmAG8AcgBtAGEAdAAgAFwAIgBBADEAOgA9ACAARgBPAFIATQBVAEwAQQAoAC4ALgAuACkAXAAiAFwAbgAgACAAIAAgACAAVQBzAGUAZgB1AGwAIABmAG8AcgAgAGEAdQBkAGkAdABpAG4AZwAsACAAZABvAGMAdQBtAGUAbgB0AGEAdABpAG8AbgAsACAAZABhAHMAaABiAG8AYQByAGQAcwAsACAAbwByACAAdABlAGEAYwBoAGkAbgBnACAAdABvAG8AbABzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlAHMAOgBcAG4AIAAgACAAIAAgAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUACgAQgAzACkAIAAgAJIhIABcACIAQgAzADoAPQAgAFIARQBDAEkAUAAoAFIATwBPAFQAKABQAEkAKAApACwAMwApACkAXAAiAFwAbgAgACAAIAAgACAARgBPAFIATQBVAEwAQQBfAFQARQBYAFQAKABDADUAKQAgACAAkiEgAFwAIgBDADUAOgA9ACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAMwApAFwAIgBcAG4AXABuACAAIAAgAE4AbwB0AGUAcwA6AFwAbgAgACAAIAAgACAALQAgAFQAaABlACAAcgBlAHMAdQBsAHQAIABpAHMAIABlAHEAdQBpAHYAYQBsAGUAbgB0ACAAdABvADoAIABDAEUATABMACgAXAAiAGEAZABkAHIAZQBzAHMAXAAiACwAIABjAGUAbABsACkAIAAmACAAXAAiADoAPQAgAFwAIgAgACYAIABUAEUAWABUAEEARgBUAEUAUgAoAEYATwBSAE0AVQBMAEEAVABFAFgAVAAoAGMAZQBsAGwAKQAsACAAXAAiAD0AXAAiACkAXABuACAAIAAgACAAIAAtACAASQBmACAAdABoAGUAIAByAGUAZgBlAHIAZQBuAGMAZQBkACAAYwBlAGwAbAAgAGQAbwBlAHMAIABuAG8AdAAgAGMAbwBuAHQAYQBpAG4AIABhACAAZgBvAHIAbQB1AGwAYQAsACAAYQBuACAAZQByAHIAbwByACAAdwBpAGwAbAAgAG8AYwBjAHUAcgAuAFwAbgAgACAAIAAgACAALQAgAFQAaABpAHMAIABmAHUAbgBjAHQAaQBvAG4AIABkAG8AZQBzACAAbgBvAHQAIABlAHYAYQBsAHUAYQB0AGUAIABvAHIAIABhAGwAdABlAHIAIAB0AGgAZQAgAGYAbwByAG0AdQBsAGEAFCBvAG4AbAB5ACAAZgBvAHIAbQBhAHQAcwAgAGkAdAAgAGYAbwByACAAZABpAHMAcABsAGEAeQAuAFwAbgAqAC8AXABuAFwAbgBGAE8AUgBNAFUATABBAF8AVABFAFgAVAA9AEwAQQBNAEIARABBACgAXABuACAAIABmAG8AcgBtAHUAbABhAF8AYwBlAGwAbAAsACAAIAAvAC8AIABBACAAcgBlAGYAZQByAGUAbgBjAGUAIAB0AG8AIABhACAAYwBlAGwAbAAgAGMAbwBuAHQAYQBpAG4AaQBuAGcAIABhACAAZgBvAHIAbQB1AGwAYQBcAG4AXABuACAAIABMAEUAVAAoAFwAbgAgACAAIAAgAHIAYQB3ACwAIABGAE8AUgBNAFUATABBAFQARQBYAFQAKABmAG8AcgBtAHUAbABhAF8AYwBlAGwAbAApACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXAAiAD0AUgBFAEMASQBQACgAUgBPAE8AVAAoAFAASQAoACkALAAzACkAKQBcACIAXABuACAAIAAgACAAYwBsAGUAYQBuACwAIABUAEUAWABUAEEARgBUAEUAUgAoAHIAYQB3ACwAIABcACIAPQBcACIAKQAsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAALwAvACAAXAAiAFIARQBDAEkAUAAoAFIATwBPAFQAKABQAEkAKAApACwAMwApACkAXAAiAFwAbgAgACAAIAAgAGwAYQBiAGUAbAAsACAAUwBVAEIAUwBUAEkAVABVAFQARQAoAEMARQBMAEwAKABcACIAYQBkAGQAcgBlAHMAcwBcACIALAAgAGYAbwByAG0AdQBsAGEAXwBjAGUAbABsACkALAAgAFwAIgAkAFwAIgAsACAAXAAiAFwAIgApACAAJgAgAFwAIgA6AD0AIABcACIALABcAG4AIAAgACAAIABsAGEAYgBlAGwAIAAmACAAYwBsAGUAYQBuAFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4AXABuAC8AKgAgAFIATwBVAE4ARABfAEYASQBYAFwAbgAgACAAIAAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0ALQAtAC0AXABuACAAIAAgAFIAbwB1AG4AZABzACAAbwByACAAdAByAHUAbgBjAGEAdABlAHMAIABhACAAbgB1AG0AYgBlAHIAIAB0AG8AIABhACAAcwBwAGUAYwBpAGYAaQBlAGQAIABuAHUAbQBiAGUAcgAgAG8AZgAgAGQAZQBjAGkAbQBhAGwAIABwAGwAYQBjAGUAcwAuAFwAbgAgACAAIABPAHAAdABpAG8AbgBhAGwAbAB5ACAAcgBlAHQAdQByAG4AcwAgAHQAaABlACAAcgBlAHMAdQBsAHQAIABhAHMAIABhACAAZgBpAHgAZQBkAC0AdwBpAGQAdABoACAAdABlAHgAdAAgAHMAdAByAGkAbgBnACwAIABwAHIAZQBzAGUAcgB2AGkAbgBnACAAdAByAGEAaQBsAGkAbgBnACAAegBlAHIAbwBzAC4AXABuAFwAbgAgACAAIABTAHkAbgB0AGEAeAA6AFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABuAHUAbQBiAGUAcgAsACAAcABsAGEAYwBlAHMALAAgAFsAYQBzAF8AdABlAHgAdABdACwAIABbAHUAcwBlAF8AcgBvAHUAbgBkAF0AKQBcAG4AXABuACAAIAAgAFAAYQByAGEAbQBlAHQAZQByAHMAOgBcAG4AIAAgACAAIAAgAG4AdQBtAGIAZQByACAAIAAgACAAIAAgADoAIABUAGgAZQAgAG4AdQBtAGUAcgBpAGMAIAB2AGEAbAB1AGUAIAB0AG8AIABwAHIAbwBjAGUAcwBzAC4AXABuACAAIAAgACAAIABwAGwAYQBjAGUAcwAgACAAIAAgACAAIAA6ACAATgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAGUAdABhAGkAbgAuAFwAbgAgACAAIAAgACAAYQBzAF8AdABlAHgAdAAgACAAIAAgACAAOgAgAE8AcAB0AGkAbwBuAGEAbAAgACgAZABlAGYAYQB1AGwAdAAgAD0AIABGAEEATABTAEUAKQAuACAASQBmACAAVABSAFUARQAsACAAcgBlAHQAdQByAG4AcwAgAG8AdQB0AHAAdQB0ACAAYQBzACAAdABlAHgAdAAgACgAZQAuAGcALgAsACAAXAAiADMALgAxADQAMABcACIAKQAuAFwAbgAgACAAIAAgACAAdQBzAGUAXwByAG8AdQBuAGQAIAAgACAAOgAgAE8AcAB0AGkAbwBuAGEAbAAgACgAZABlAGYAYQB1AGwAdAAgAD0AIABGAEEATABTAEUAKQAuACAASQBmACAAVABSAFUARQAsACAAYQBwAHAAbABpAGUAcwAgAHIAbwB1AG4AZABpAG4AZwAuACAATwB0AGgAZQByAHcAaQBzAGUALAAgAHQAcgB1AG4AYwBhAHQAZQBzAC4AXABuAFwAbgAgACAAIABSAGUAdAB1AHIAbgBzADoAXABuACAAIAAgACAAIABBACAAbgB1AG0AYgBlAHIAIABvAHIAIAB0AGUAeAB0ACAAcwB0AHIAaQBuAGcAIAByAGUAcAByAGUAcwBlAG4AdABpAG4AZwAgAHQAaABlACAAcgBvAHUAbgBkAGUAZAAgAG8AcgAgAHQAcgB1AG4AYwBhAHQAZQBkACAAdgBhAGwAdQBlACAAdABvACAAZgBpAHgAZQBkACAAZABlAGMAaQBtAGEAbAAgAHAAbABhAGMAZQBzAC4AXABuAFwAbgAgACAAIABFAHgAYQBtAHAAbABlAHMAOgBcAG4AIAAgACAAIAAgAFIATwBVAE4ARABfAEYASQBYACgAUABJACgAKQAsACAAMgApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAJIhIAAzAC4AMQA0AFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAAzACwAIABUAFIAVQBFACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAkiEgAFwAIgAzAC4AMQA0ADEAXAAiAFwAbgAgACAAIAAgACAAUgBPAFUATgBEAF8ARgBJAFgAKABQAEkAKAApACwAIAA0ACwAIABUAFIAVQBFACwAIABGAEEATABTAEUAKQAgACAAIAAgACAAIAAgACAAkiEgAFwAIgAzAC4AMQA0ADEANQBcACIAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADEAMgAsACAARgBBAEwAUwBFACkAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAMwAuADEANAAxADUAOQAyADYANQA0ACAAIAAgACgAYwBhAHAAcABlAGQAIAB0AG8AIAA5ACAAZABlAGMAaQBtAGEAbABzACkAXABuACAAIAAgACAAIABSAE8AVQBOAEQAXwBGAEkAWAAoAFAASQAoACkALAAgADEAMgAsACAAVABSAFUARQApACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIACSISAAXAAiADMALgAxADQAMQA1ADkAMgA2ADUAMwA1ADkAMABcACIAXABuAFwAbgAgACAAIABOAG8AdABlAHMAOgBcAG4AIAAgACAAIAAgAC0AIABFAHgAYwBlAGwAIABsAGkAbQBpAHQAcwAgAG4AdQBtAGUAcgBpAGMAIABkAGkAcwBwAGwAYQB5ACAAcAByAGUAYwBpAHMAaQBvAG4AIAB0AG8AIAB+ADkAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMALgAgAFcAaABlAG4AIABhAHMAXwB0AGUAeAB0ACAAPQAgAEYAQQBMAFMARQAsAFwAbgAgACAAIAAgACAAIAAgAG8AdQB0AHAAdQB0ACAAaQBzACAAYwBhAHAAcABlAGQAIABhAHQAIAA5ACAAZABpAGcAaQB0AHMAIABmAG8AcgAgAGMAbwBuAHMAaQBzAHQAZQBuAGMAeQAuAFwAbgAgACAAIAAgACAALQAgAFQAbwAgAGQAaQBzAHAAbABhAHkAIABmAHUAbABsACAAcAByAGUAYwBpAHMAaQBvAG4AIABvAHIAIABwAHIAZQBzAGUAcgB2AGUAIAB0AHIAYQBpAGwAaQBuAGcAIAB6AGUAcgBvAHMALAAgAHMAZQB0ACAAYQBzAF8AdABlAHgAdAAgAD0AIABUAFIAVQBFAC4AXABuACAAIAAgACAAIAAtACAAUwB1AHAAcABvAHIAdABzACAAYgBvAHQAaAAgAHIAbwB1AG4AZABpAG4AZwAgAGEAbgBkACAAdAByAHUAbgBjAGEAdABpAG8AbgAgAG0AbwBkAGUAcwAuAFwAbgAgACAAIAAgACAALQAgAEkAZABlAGEAbAAgAGYAbwByACAAZgBvAHIAbQBhAHQAdABpAG4AZwAgAGMAbwBuAHMAdABhAG4AdABzACwAIAB2AGkAcwB1AGEAbAAgAGQAaQBzAHAAbABhAHkAIABjAG8AbgB0AHIAbwBsACwAIABvAHIAIABlAG4AcwB1AHIAaQBuAGcAIABjAGwAZQBhAG4AIABvAHUAdABwAHUAdABzACAAaQBuACAAcgBlAHAAbwByAHQAcwAuAFwAbgAqAC8AXABuAFwAbgBcAG4AUgBPAFUATgBEAF8ARgBJAFgAPQBMAEEATQBCAEQAQQAoAFwAbgAgACAAbgB1AG0AYgBlAHIALAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABSAGUAcQB1AGkAcgBlAGQAOgAgAHQAaABlACAAbgB1AG0AYgBlAHIAIAB0AG8AIAByAG8AdQBuAGQAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGUAXABuACAAIABwAGwAYQBjAGUAcwAsACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAFIAZQBxAHUAaQByAGUAZAA6ACAAbgB1AG0AYgBlAHIAIABvAGYAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAIAB0AG8AIAByAGUAdABhAGkAbgBcAG4AIAAgAFsAYQBzAF8AdABlAHgAdABdACwAIAAgACAAIAAgACAALwAvACAATwBwAHQAaQBvAG4AYQBsADoAIABpAGYAIABUAFIAVQBFACwAIAByAGUAdAB1AHIAbgAgAHIAZQBzAHUAbAB0ACAAYQBzACAAdABlAHgAdAAgAHcAaQB0AGgAIABmAGkAeABlAGQAIABkAGUAYwBpAG0AYQBsACAAcABsAGEAYwBlAHMAXABuACAAIABbAHUAcwBlAF8AcgBvAHUAbgBkAF0ALAAgACAAIAAgAC8ALwAgAE8AcAB0AGkAbwBuAGEAbAA6ACAAaQBmACAAVABSAFUARQAsACAAcgBvAHUAbgBkADsAIABpAGYAIABGAEEATABTAEUAIABvAHIAIABvAG0AaQB0AHQAZQBkACwAIAB0AHIAdQBuAGMAYQB0AGUAXABuAFwAbgAgACAATABFAFQAKABcAG4AIAAgACAAIABuACwAIABOACgAbgB1AG0AYgBlAHIAKQAsACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgAC8ALwAgAEUAbgBzAHUAcgBlACAAbgB1AG0AZQByAGkAYwAgAGkAbgBwAHUAdABcAG4AIAAgACAAIAByAGEAdwBfAHAALAAgAE4AKABwAGwAYQBjAGUAcwApACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABSAGEAdwAgAGkAbgBwAHUAdAAgAGYAbwByACAAcABsAGEAYwBlAHMAXABuACAAIAAgACAAcgBvAHUAbgBkAF8AZgBsAGEAZwAsACAASQBGACgASQBTAEIATABBAE4ASwAoAHUAcwBlAF8AcgBvAHUAbgBkACkALAAgAEYAQQBMAFMARQAsACAAdQBzAGUAXwByAG8AdQBuAGQAKQAsAFwAbgAgACAAIAAgAHIAZQB0AHUAcgBuAF8AdABlAHgAdAAsACAASQBGACgASQBTAEIATABBAE4ASwAoAGEAcwBfAHQAZQB4AHQAKQAsACAARgBBAEwAUwBFACwAIABhAHMAXwB0AGUAeAB0ACkALABcAG4AXABuACAAIAAgACAALwAvACAARQB4AGMAZQBsACAAbwBuAGwAeQAgAHIAZQBsAGkAYQBiAGwAeQAgAGQAaQBzAHAAbABhAHkAcwAgAHUAcAAgAHQAbwAgADkAIABkAGUAYwBpAG0AYQBsAHMAIABhAHMAIABuAHUAbQBlAHIAaQBjAFwAbgAgACAAIAAgAG0AYQB4AF8AcABsAGEAYwBlAHMALAAgAEkARgAoAHIAZQB0AHUAcgBuAF8AdABlAHgAdAAsACAAcgBhAHcAXwBwACwAIABNAEkATgAoAHIAYQB3AF8AcAAsACAAOQApACkALABcAG4AXABuACAAIAAgACAAcAB3AHIAXwAxADAALAAgADEAMAAgAF4AIABtAGEAeABfAHAAbABhAGMAZQBzACwAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAvAC8AIABQAG8AdwBlAHIAIABvAGYAIAAxADAAIABmAG8AcgAgAHIAbwB1AG4AZABpAG4AZwAvAHQAcgB1AG4AYwBhAHQAaQBvAG4AXABuAFwAbgAgACAAIAAgAC8ALwAgAFAAZQByAGYAbwByAG0AIAByAG8AdQBuAGQAaQBuAGcAIABvAHIAIAB0AHIAdQBuAGMAYQB0AGkAbwBuAFwAbgAgACAAIAAgAHIAZQBzAHUAbAB0ACwAXABuACAAIAAgACAAIAAgAEkARgAoAHIAbwB1AG4AZABfAGYAbABhAGcALABcAG4AIAAgACAAIAAgACAAIAAgAFIATwBVAE4ARAAoAG4ALAAgAG0AYQB4AF8AcABsAGEAYwBlAHMAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAVABSAFUATgBDACgAbgAgACoAIABwAHcAcgBfADEAMAApACAALwAgAHAAdwByAF8AMQAwAFwAbgAgACAAIAAgACAAIAApACwAXABuAFwAbgAgACAAIAAgAC8ALwAgAE8AcAB0AGkAbwBuAGEAbABsAHkAIABmAG8AcgBtAGEAdAAgAGEAcwAgAGYAaQB4AGUAZAAtAGwAZQBuAGcAdABoACAAcwB0AHIAaQBuAGcAXABuACAAIAAgACAAZgBpAG4AYQBsACwAXABuACAAIAAgACAAIAAgAEkARgAoAHIAZQB0AHUAcgBuAF8AdABlAHgAdAAsAFwAbgAgACAAIAAgACAAIAAgACAAVABFAFgAVAAoAHIAZQBzAHUAbAB0ACwAIABcACIAMAAuAFwAIgAgACYAIABSAEUAUABUACgAXAAiADAAXAAiACwAIABtAGEAeABfAHAAbABhAGMAZQBzACkAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAcgBlAHMAdQBsAHQAXABuACAAIAAgACAAIAAgACkALABcAG4AXABuACAAIAAgACAAZgBpAG4AYQBsAFwAbgAgACAAKQBcAG4AKQA7AFwAbgBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbACIAQQBTAFQAUgBPAF8ASABBAEIAXwBJAE4ARABFAFgAIgAsACIAQQBTAFQAUgBPAF8AUwBQAEUAQwBUAFIAQQBMAF8ARABJAFMAVABSAEkAQgBVAFQASQBPAE4AIgAsACIAQQBTAFQAUgBPAF8AQwBBAEwAQwBfAFQARQBNAFAAIgAsACIAQQBTAFQAUgBPAF8AVABZAFAARQBfAEYAUgBPAE0AXwBUAEUATQBQACIALAAiAEEAUwBUAFIATwBfAEQASQBTAFAATABBAFkAXwBTAFAARQBDAFQAUgBBAEwAIgAsACIAQQBTAFQAUgBPAF8AUwBUAEEAUgBfAEEAVABUAFIASQBCAFUAVABFAFMAIgAsACIAQQBTAFQAUgBPAF8ASABBAEIASQBUAEEAQgBMAEUAXwBaAE8ATgBFAFMAIgAsACIATgBBAFMAVABSAE8AXwBIAEEAQgBJAFQAQQBCAEwARQBfAFoATwBOAEUAUwAiACwAIgBBAFMAVABSAE8AXwBTAFQAQQBSAF8ARABFAE4AUwBJAFQAWQBfAFYATwBMAFUATQBFACIALAAiAEEAUwBUAFIATwBfAFAATABBAE4ARQBUAF8ATQBFAFQAUgBJAEMAUwBfAFMAQQBGAEUAVABZACIALAAiAEEAUwBUAFIATwBfAFAATABBAE4ARQBUAF8ATQBFAFQAUgBJAEMAUwAiACwAIgBBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUwBPAEwAVgBFAFIAIgAsACIAQQBTAFQAUgBPAF8AUwBZAE4ATwBEAEkAQwBfAFAAUQAiACwAIgBBAFMAVABSAE8AXwBTAFkATgBPAEQASQBDAF8AUABTACIALAAiAEEAUwBUAFIATwBfAFMAWQBOAE8ARABJAEMAXwBRAFMAIgAsACIAQQBTAFQAUgBPAF8AQQBQAFAAQQBSAEUATgBUAF8AUwBPAEwAQQBSAF8AUwBJAFoARQAiACwAIgBBAFMAVABSAE8AXwBPAFIAQgBJAFQAXwBDAE8ATgBGAEkARwBVAFIAQQBUAEkATwBOAF8ASQBOAEQARQBYACIALAAiAEEAUwBUAFIATwBfAFMAUABIAEUAUgBJAEMAQQBMAF8AVABPAF8AQwBBAFIAVABFAFMASQBBAE4AIgAsACIAQQBTAFQAUgBPAF8AQwBBAFIAVABFAFMASQBBAE4AXwBUAE8AXwBTAFAASABFAFIASQBDAEEATAAiACwAIgBEAEUARwBfAEQARQBDAF8ARABNAFMAIgAsACIARABFAEcAXwBEAE0AUwAiACwAIgBEAEUARwBfAEQATQBTAF8ARABFAEMAIgAsACIAQQBTAFQAUgBPAF8ATwBSAEIASQBUAF8AQQBYAEkAUwAiACwAIgBBAFMAVABSAE8AXwBPAFIAQgBJAFQAXwBQAEUAUgBJAE8ARAAiACwAIgBBAFMAVABSAE8AXwBPAFIAQgBJAFQAXwBTAFUATQBfAE0AQQBTAFMARQBTACIALAAiAEEAUwBUAFIATwBfAE8AUgBCAEkAVABfAFMATwBMAFYARQBSACIALAAiAEcAZQBuAGUAcgBhAGwALgBSAEUAQwBJAFAAIgAsACIARwBlAG4AZQByAGEAbAAuAEYAUgBBAEMAIgAsACIARwBlAG4AZQByAGEAbAAuAFIATwBPAFQAIgAsACIARwBlAG4AZQByAGEAbAAuAEYATwBSAE0AVQBMAEEAXwBUAEUAWABUACIALAAiAEcAZQBuAGUAcgBhAGwALgBSAE8AVQBOAEQAXwBGAEkAWAAiAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAE0ARABZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>